<commit_message>
modification of (submit_json_data, update_score, update_highest_possible_scores, update_total_max_quarterly, validate_score)
</commit_message>
<xml_diff>
--- a/Migrade_v.1.2/temp.xlsx
+++ b/Migrade_v.1.2/temp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN51"/>
+  <dimension ref="A1:AN57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -782,7 +782,7 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr">
         <is>
-          <t>2017 - 2018</t>
+          <t>2019 - 2020</t>
         </is>
       </c>
       <c r="T4" t="inlineStr"/>
@@ -791,7 +791,7 @@
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Grade </t>
+          <t xml:space="preserve">Grade Level </t>
         </is>
       </c>
       <c r="Y4" t="inlineStr"/>
@@ -799,7 +799,7 @@
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>Grade 5</t>
+          <t>Grade 6</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr"/>
@@ -813,7 +813,7 @@
       <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>EARTH</t>
+          <t>GALILEO</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr"/>
@@ -853,7 +853,7 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Age as of August 31st</t>
+          <t>AGE as of 1st Friday June</t>
         </is>
       </c>
       <c r="K5" t="inlineStr"/>
@@ -975,7 +975,7 @@
       <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mother's Maiden Name (Last Name, First Name, Middle </t>
+          <t>Mother's Maiden Name (Last Name, First Name, Middle Name)</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr"/>
@@ -1002,13 +1002,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>164512110014</t>
+          <t>164512130171</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>BORLAGDAN, ALFIE BISMAR</t>
+          <t>ANIBAN,LEO JELLY, TINAPAY</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -1021,13 +1021,13 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>05-18-2005</t>
+          <t>09-23-2008</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K7" t="inlineStr"/>
@@ -1069,7 +1069,7 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>BORLAGDAN, ALLAN GOLEMLEM</t>
+          <t>ANIBAN, LEO BUTAL</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr"/>
@@ -1077,7 +1077,7 @@
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>BISMAR,CARMENCITA,BLANQUEZA,</t>
+          <t>TINAPAY,JILL,BAJADI,</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr"/>
@@ -1092,13 +1092,13 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>164512130010</t>
+          <t>164512130045</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>BORLAGDAN, RJ BISMAR</t>
+          <t>ASILO,RAIN JUSTINE, MERCADO</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -1111,13 +1111,13 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>11-11-2006</t>
+          <t>05-20-2007</t>
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K8" t="inlineStr"/>
@@ -1136,7 +1136,7 @@
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R8" t="inlineStr"/>
@@ -1159,7 +1159,7 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>BORLAGDAN, ALLAN GOLEMLEM</t>
+          <t>ASILO, CHRISTOPHER SALILICAN</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr"/>
@@ -1167,7 +1167,7 @@
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>BISMAR,CARMENCITA,BLANQUEZA,</t>
+          <t>MERCADO,MARICEL,HERNANDEZ,</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr"/>
@@ -1182,13 +1182,13 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>136907120127</t>
+          <t>424663150037</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CAMBE, RALPH LOUIE ARAGON</t>
+          <t>CAMBE,SEAN DAVE, ARAGON</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -1201,13 +1201,13 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>03-02-2007</t>
+          <t>03-15-2008</t>
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K9" t="inlineStr"/>
@@ -1267,22 +1267,18 @@
       <c r="AK9" t="inlineStr"/>
       <c r="AL9" t="inlineStr"/>
       <c r="AM9" t="inlineStr"/>
-      <c r="AN9" t="inlineStr">
-        <is>
-          <t>T/I DATE:2017-06-05</t>
-        </is>
-      </c>
+      <c r="AN9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>164512130016</t>
+          <t>164512140032</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CAONES, JAYRUS CARL LACANIN</t>
+          <t>CARANAY,JHAYCEE CARL, CORDERO</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -1295,7 +1291,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>08-25-2006</t>
+          <t>11-25-2007</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
@@ -1343,7 +1339,7 @@
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>CAONES, JAYZON NUNAY</t>
+          <t>CARANAY, ROGELIO JR CABOTAJE</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr"/>
@@ -1351,7 +1347,7 @@
       <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="inlineStr">
         <is>
-          <t>LACANIN,JERLYN,BELO,</t>
+          <t>CORDERO,NORMA,ALIDO,</t>
         </is>
       </c>
       <c r="AG10" t="inlineStr"/>
@@ -1366,13 +1362,13 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>164512120011</t>
+          <t>164512140029</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CELESTE, ANDREW ACE ESPINOSA</t>
+          <t>CASTRO,ICHIRO, MENDOZA</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -1385,7 +1381,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>02-09-2007</t>
+          <t>09-08-2008</t>
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
@@ -1410,7 +1406,7 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>PLATERO</t>
         </is>
       </c>
       <c r="R11" t="inlineStr"/>
@@ -1433,7 +1429,7 @@
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>CELESTE, ALEJANDRO SARVIDA</t>
+          <t>CASTRO, SEVERLINO ABAPO</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr"/>
@@ -1441,7 +1437,7 @@
       <c r="AE11" t="inlineStr"/>
       <c r="AF11" t="inlineStr">
         <is>
-          <t>ESPINOSA,LORENA,ALBERTO,</t>
+          <t>MENDOZA,ALICIA,ZULUETA,</t>
         </is>
       </c>
       <c r="AG11" t="inlineStr"/>
@@ -1456,13 +1452,13 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>164512130047</t>
+          <t>164512150094</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CUPANG, CHRISTIAN ZAMORA</t>
+          <t>CAYLAO,DAYNE, VIÑA</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -1475,13 +1471,13 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>06-21-2007</t>
+          <t>03-17-2007</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K12" t="inlineStr"/>
@@ -1500,7 +1496,7 @@
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>PLATERO</t>
         </is>
       </c>
       <c r="R12" t="inlineStr"/>
@@ -1523,7 +1519,7 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>CUPANG, ANTONIO CRISMUNDO JR</t>
+          <t>CAYLAO, DANZEL CIPRIANO</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr"/>
@@ -1531,7 +1527,7 @@
       <c r="AE12" t="inlineStr"/>
       <c r="AF12" t="inlineStr">
         <is>
-          <t>ZAMORA,TERESITA,ALING,</t>
+          <t>VIÑA,CAREN,CRUZ,</t>
         </is>
       </c>
       <c r="AG12" t="inlineStr"/>
@@ -1546,13 +1542,13 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>108226120133</t>
+          <t>164512130131</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>GABATIN, KING TYRON GILBERT AMORTIZADO</t>
+          <t>CHAN,JHON RHAYNE, REPELAR</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -1565,13 +1561,13 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>11-10-2004</t>
+          <t>01-16-2008</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K13" t="inlineStr"/>
@@ -1613,7 +1609,7 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>GABATIN, TEOFILO TACSIAT</t>
+          <t>CHAN, JONATHAN ALICARTE</t>
         </is>
       </c>
       <c r="AC13" t="inlineStr"/>
@@ -1621,7 +1617,7 @@
       <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="inlineStr">
         <is>
-          <t>AMORTIZADO,MARIA LOURDES,CAPUQUIAN,</t>
+          <t>REPELAR,ELENA,ROXAS,</t>
         </is>
       </c>
       <c r="AG13" t="inlineStr"/>
@@ -1636,13 +1632,13 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>164512130022</t>
+          <t>402456150012</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>LAGADI, JHOSUA BUSTAMANTE</t>
+          <t>GETALADO,EARL SAMUEL, CLAVE</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -1655,7 +1651,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>11-08-2006</t>
+          <t>09-10-2008</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -1680,7 +1676,7 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R14" t="inlineStr"/>
@@ -1703,7 +1699,7 @@
       <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>LAGADI, VICENTE GABRIEL JR</t>
+          <t>GETALADO, ERNESTO CERTEZA</t>
         </is>
       </c>
       <c r="AC14" t="inlineStr"/>
@@ -1711,7 +1707,7 @@
       <c r="AE14" t="inlineStr"/>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>BUSTAMANTE,ELIZA,BULARON,</t>
+          <t>CLAVE,SERENIDAD,TABLIZO,</t>
         </is>
       </c>
       <c r="AG14" t="inlineStr"/>
@@ -1726,13 +1722,13 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>112505130003</t>
+          <t>164512130101</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LLANZA, ALFREDO LAYCO JR</t>
+          <t>GLOBIO,MARCKY, GALVAN</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -1745,13 +1741,13 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>09-28-2006</t>
+          <t>03-11-2008</t>
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
@@ -1770,7 +1766,7 @@
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>SANTO NINO</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R15" t="inlineStr"/>
@@ -1791,17 +1787,13 @@
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="inlineStr">
-        <is>
-          <t>LLANZA, ALFREDO CARGALLO SR</t>
-        </is>
-      </c>
+      <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="inlineStr"/>
       <c r="AD15" t="inlineStr"/>
       <c r="AE15" t="inlineStr"/>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>LAYCO,ARCELI,MONTANEZ,</t>
+          <t>GLOBIO,RENITA,GALVAN,</t>
         </is>
       </c>
       <c r="AG15" t="inlineStr"/>
@@ -1811,18 +1803,22 @@
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr"/>
       <c r="AM15" t="inlineStr"/>
-      <c r="AN15" t="inlineStr"/>
+      <c r="AN15" t="inlineStr">
+        <is>
+          <t>DRP "Family Problem"Date:2019/11/04</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>164512130024</t>
+          <t>164512140006</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MALINTAD, JAMES DUMAYO</t>
+          <t>MIRANDA,ANDREI, BIANES</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -1835,13 +1831,13 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>03-05-2007</t>
+          <t>04-29-2007</t>
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
@@ -1860,7 +1856,7 @@
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R16" t="inlineStr"/>
@@ -1883,7 +1879,7 @@
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>MALINTAD, GREMER CAONG</t>
+          <t>MIRANDA, ESTELITO VILLANUEVA</t>
         </is>
       </c>
       <c r="AC16" t="inlineStr"/>
@@ -1891,7 +1887,7 @@
       <c r="AE16" t="inlineStr"/>
       <c r="AF16" t="inlineStr">
         <is>
-          <t>DUMAYO,MINDA,TUMIMO,</t>
+          <t>BIANES,JENNIFER,QUINTUA,</t>
         </is>
       </c>
       <c r="AG16" t="inlineStr"/>
@@ -1901,18 +1897,22 @@
       <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="inlineStr"/>
-      <c r="AN16" t="inlineStr"/>
+      <c r="AN16" t="inlineStr">
+        <is>
+          <t>T/I Pook Elem. Sch. Date:2019-06-03</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>164512130027</t>
+          <t>164512130118</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MATULA, JOHN GABRIEL ZAVALLA</t>
+          <t>NAVAREZ,ANDREI, MONTAÑEZ</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -1925,13 +1925,13 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>09-25-2006</t>
+          <t>07-26-2007</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K17" t="inlineStr"/>
@@ -1973,7 +1973,7 @@
       <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>MATULA, VICTOR GONZALES</t>
+          <t>NAVAREZ, ARNEL NABUHAY</t>
         </is>
       </c>
       <c r="AC17" t="inlineStr"/>
@@ -1981,7 +1981,7 @@
       <c r="AE17" t="inlineStr"/>
       <c r="AF17" t="inlineStr">
         <is>
-          <t>ZAVALLA,FLORENCIA,NILLO,</t>
+          <t>MONTAÑEZ,SUSANA,VILLARIN,</t>
         </is>
       </c>
       <c r="AG17" t="inlineStr"/>
@@ -1996,13 +1996,13 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>164512120051</t>
+          <t>164512100132</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>OLIVEROS, JHONUEL BISMAR</t>
+          <t>SALAYSAY,JOHN LOUIE, FLORES</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -2015,13 +2015,13 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>01-16-2007</t>
+          <t>02-18-2004</t>
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">15 </t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
@@ -2063,7 +2063,7 @@
       <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>OLIVEROS, JOEL AFANTE</t>
+          <t>SALAYSAY, ALFREDO REYES</t>
         </is>
       </c>
       <c r="AC18" t="inlineStr"/>
@@ -2071,7 +2071,7 @@
       <c r="AE18" t="inlineStr"/>
       <c r="AF18" t="inlineStr">
         <is>
-          <t>BLANQUEZA,JANET,BISMAR,</t>
+          <t>FLORES,CECILIA,LOPENA,</t>
         </is>
       </c>
       <c r="AG18" t="inlineStr"/>
@@ -2086,13 +2086,13 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>108474140114</t>
+          <t>108476120166</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>QUILLOSA, MERICK MASAREDO</t>
+          <t>SAMANIEGO,MATTHEW ANDREI, ANGULO</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
@@ -2105,13 +2105,13 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>10-04-2006</t>
+          <t>08-01-2006</t>
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
@@ -2130,7 +2130,7 @@
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R19" t="inlineStr"/>
@@ -2153,7 +2153,7 @@
       <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>QUILLOSA, MARVIN MANLOLO</t>
+          <t>SAMANIEGO, MICHAEL ABUCEJO</t>
         </is>
       </c>
       <c r="AC19" t="inlineStr"/>
@@ -2161,7 +2161,7 @@
       <c r="AE19" t="inlineStr"/>
       <c r="AF19" t="inlineStr">
         <is>
-          <t>MASAREDO,PERLA,ACOSTA,</t>
+          <t>ANGULO,ABIGAIL,GUSTILO,</t>
         </is>
       </c>
       <c r="AG19" t="inlineStr"/>
@@ -2176,13 +2176,13 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>164512130030</t>
+          <t>108426130045</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>SANGYAHON, JUSTINE MAGTAGAD</t>
+          <t>SAN JUAN JR.,ARLY, PLATINO</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
@@ -2195,13 +2195,13 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>09-22-2006</t>
+          <t>09-29-2007</t>
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K20" t="inlineStr"/>
@@ -2243,7 +2243,7 @@
       <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>SANGYAHON, ERLINDO PATRICIO</t>
+          <t>SAN JUAN, ARLY TAPUIC SR</t>
         </is>
       </c>
       <c r="AC20" t="inlineStr"/>
@@ -2251,7 +2251,7 @@
       <c r="AE20" t="inlineStr"/>
       <c r="AF20" t="inlineStr">
         <is>
-          <t>MAGTAGAD,CHERYL,ESPAÑOLA,</t>
+          <t>PLATINO,EVANGELINE,GUILLEN,</t>
         </is>
       </c>
       <c r="AG20" t="inlineStr"/>
@@ -2266,13 +2266,13 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>136775120015</t>
+          <t>164512130091</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
-          <t>SANTOS, ANGELO GALLARDO</t>
+          <t>SANTOS,MARK, BELANO</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>05-15-2007</t>
+          <t>09-05-2008</t>
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
@@ -2333,7 +2333,7 @@
       <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>SANTOS, ARTURO CRUZ</t>
+          <t>SANTOS, ROLANDO BARBOSA</t>
         </is>
       </c>
       <c r="AC21" t="inlineStr"/>
@@ -2341,7 +2341,7 @@
       <c r="AE21" t="inlineStr"/>
       <c r="AF21" t="inlineStr">
         <is>
-          <t>UMALI,GALLARDO,GUADALUPE,</t>
+          <t>BELANO,LIZA,BERIANO,</t>
         </is>
       </c>
       <c r="AG21" t="inlineStr"/>
@@ -2351,22 +2351,18 @@
       <c r="AK21" t="inlineStr"/>
       <c r="AL21" t="inlineStr"/>
       <c r="AM21" t="inlineStr"/>
-      <c r="AN21" t="inlineStr">
-        <is>
-          <t>Pending TI</t>
-        </is>
-      </c>
+      <c r="AN21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>164512120054</t>
+          <t>164512140037</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
-          <t>TABING, RANDEL ABELLA</t>
+          <t>VILLANUEVA,JOSH CYREL, CLASA</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
@@ -2379,13 +2375,13 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>06-16-2007</t>
+          <t>11-09-2007</t>
         </is>
       </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
@@ -2427,7 +2423,7 @@
       <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>TABING, RANDY ESTEBAN</t>
+          <t>VILLANUEVA, PABLITO MARIÑAS</t>
         </is>
       </c>
       <c r="AC22" t="inlineStr"/>
@@ -2435,7 +2431,7 @@
       <c r="AE22" t="inlineStr"/>
       <c r="AF22" t="inlineStr">
         <is>
-          <t>ABELLA,MARIDEL,ENCELAN,</t>
+          <t>CLASA,EVEBERLY,MONTESCO,</t>
         </is>
       </c>
       <c r="AG22" t="inlineStr"/>
@@ -2448,86 +2444,44 @@
       <c r="AN22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>164512120055</t>
-        </is>
+      <c r="A23" t="n">
+        <v>16</v>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
-          <t>VALENCIA, RIN WINZHEL AGUADO</t>
+          <t>&lt;=== TOTAL MALE</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>01-09-2007</t>
-        </is>
-      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">10 </t>
-        </is>
-      </c>
+      <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>Tagalog</t>
-        </is>
-      </c>
+      <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>Christianity</t>
-        </is>
-      </c>
+      <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>ZAPOTE</t>
-        </is>
-      </c>
+      <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>CITY OF BIÑAN</t>
-        </is>
-      </c>
+      <c r="U23" t="inlineStr"/>
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr"/>
-      <c r="X23" t="inlineStr">
-        <is>
-          <t>LAGUNA</t>
-        </is>
-      </c>
+      <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="inlineStr"/>
-      <c r="AB23" t="inlineStr">
-        <is>
-          <t>VALENCIA, CHERWEN MANONGSONG</t>
-        </is>
-      </c>
+      <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="inlineStr"/>
       <c r="AD23" t="inlineStr"/>
       <c r="AE23" t="inlineStr"/>
-      <c r="AF23" t="inlineStr">
-        <is>
-          <t>AGUADO,FRITCHEL,VICTORIO,</t>
-        </is>
-      </c>
+      <c r="AF23" t="inlineStr"/>
       <c r="AG23" t="inlineStr"/>
       <c r="AH23" t="inlineStr"/>
       <c r="AI23" t="inlineStr"/>
@@ -2538,44 +2492,86 @@
       <c r="AN23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>17</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>164512140038</t>
+        </is>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
-          <t>&lt;=== TOTAL MALE</t>
+          <t>ARRESGADO,LEANNE ROSE, CARLOS</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>08-25-2008</t>
+        </is>
+      </c>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr"/>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr"/>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr"/>
-      <c r="X24" t="inlineStr"/>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="inlineStr"/>
-      <c r="AB24" t="inlineStr"/>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>ARRESGADO, JUNARD MALAKARTE</t>
+        </is>
+      </c>
       <c r="AC24" t="inlineStr"/>
       <c r="AD24" t="inlineStr"/>
       <c r="AE24" t="inlineStr"/>
-      <c r="AF24" t="inlineStr"/>
+      <c r="AF24" t="inlineStr">
+        <is>
+          <t>CARLOS,AILEEN,VERANO,</t>
+        </is>
+      </c>
       <c r="AG24" t="inlineStr"/>
       <c r="AH24" t="inlineStr"/>
       <c r="AI24" t="inlineStr"/>
@@ -2588,13 +2584,13 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>164512130075</t>
+          <t>164512140016</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ACILO, CHARLENE DAGUMAN</t>
+          <t>BORCELANGO,DONA LYNN, DAPRINAL</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -2607,7 +2603,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>10-18-2006</t>
+          <t>07-22-2008</t>
         </is>
       </c>
       <c r="I25" t="inlineStr"/>
@@ -2655,7 +2651,7 @@
       <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>ACILO, CHARLITO LOPENA</t>
+          <t>BORCELANGO, DONATO REYES</t>
         </is>
       </c>
       <c r="AC25" t="inlineStr"/>
@@ -2663,7 +2659,7 @@
       <c r="AE25" t="inlineStr"/>
       <c r="AF25" t="inlineStr">
         <is>
-          <t>DAGUMAN,AILENE,ABE,</t>
+          <t>DAPRINAL,JONALINE,ATOR,</t>
         </is>
       </c>
       <c r="AG25" t="inlineStr"/>
@@ -2678,13 +2674,13 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>164512130061</t>
+          <t>164512140017</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
-          <t>BETITO, EURICE ROSACEÑA</t>
+          <t>CAONES,JUSEA MICAH, LACANIN</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
@@ -2697,13 +2693,13 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>05-03-2007</t>
+          <t>01-31-2008</t>
         </is>
       </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K26" t="inlineStr"/>
@@ -2745,7 +2741,7 @@
       <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="inlineStr">
         <is>
-          <t>BETITO, ARMANDO SALAMODING</t>
+          <t>CAONES, JAYZON NUNAY</t>
         </is>
       </c>
       <c r="AC26" t="inlineStr"/>
@@ -2753,7 +2749,7 @@
       <c r="AE26" t="inlineStr"/>
       <c r="AF26" t="inlineStr">
         <is>
-          <t>ROSACENA,REMEDIOS,VILLANUEVA,</t>
+          <t>LACANIN,JERLYN,BELO,</t>
         </is>
       </c>
       <c r="AG26" t="inlineStr"/>
@@ -2768,13 +2764,13 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>164512120064</t>
+          <t>105111130128</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CAFINO, JASMIN CLAIRE CANTIGA</t>
+          <t>CLEMENTE,MARTHA ASHLEE, COLIS</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -2787,7 +2783,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>03-06-2007</t>
+          <t>07-02-2008</t>
         </is>
       </c>
       <c r="I27" t="inlineStr"/>
@@ -2812,7 +2808,7 @@
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R27" t="inlineStr"/>
@@ -2835,7 +2831,7 @@
       <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="inlineStr">
         <is>
-          <t>CAFINO, RODERICK SOREÑO</t>
+          <t>CLEMENTE, RAFAEL KRIS PRONUEVO CLEMENTE</t>
         </is>
       </c>
       <c r="AC27" t="inlineStr"/>
@@ -2843,7 +2839,7 @@
       <c r="AE27" t="inlineStr"/>
       <c r="AF27" t="inlineStr">
         <is>
-          <t>CANTIGA,GRACE,IGNACIO,</t>
+          <t>COLIS,MA NIEVES VALANTINE,CUNANAN,</t>
         </is>
       </c>
       <c r="AG27" t="inlineStr"/>
@@ -2853,18 +2849,22 @@
       <c r="AK27" t="inlineStr"/>
       <c r="AL27" t="inlineStr"/>
       <c r="AM27" t="inlineStr"/>
-      <c r="AN27" t="inlineStr"/>
+      <c r="AN27" t="inlineStr">
+        <is>
+          <t>T/I  San Miguel Elem.Sch.Date:2019-06-03</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>164512120218</t>
+          <t>109850130028</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CLARION, MARY QUEEN MARIEL RAMISO</t>
+          <t>DEL MUNDO,CATHLYN, SALDINO</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
@@ -2877,13 +2877,13 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>10-01-2006</t>
+          <t>11-22-2007</t>
         </is>
       </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K28" t="inlineStr"/>
@@ -2902,7 +2902,7 @@
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R28" t="inlineStr"/>
@@ -2925,7 +2925,7 @@
       <c r="AA28" t="inlineStr"/>
       <c r="AB28" t="inlineStr">
         <is>
-          <t>CLARION, MARCIAL GARRAN</t>
+          <t>DEL MUNDO, JUNE LINGGA</t>
         </is>
       </c>
       <c r="AC28" t="inlineStr"/>
@@ -2933,7 +2933,7 @@
       <c r="AE28" t="inlineStr"/>
       <c r="AF28" t="inlineStr">
         <is>
-          <t>RAMISO,LIEZEL,SIMPO,</t>
+          <t>SALDINO,ANNABELLE,SOLAYAO,</t>
         </is>
       </c>
       <c r="AG28" t="inlineStr"/>
@@ -2948,13 +2948,13 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>164512130029</t>
+          <t>164512130166</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>DIONISO, JHAMAICA ALEGRE</t>
+          <t>DICDICAN,TRISHA ELLAINE, REALON</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>10-25-2005</t>
+          <t>03-01-2008</t>
         </is>
       </c>
       <c r="I29" t="inlineStr"/>
@@ -2992,7 +2992,7 @@
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R29" t="inlineStr"/>
@@ -3015,7 +3015,7 @@
       <c r="AA29" t="inlineStr"/>
       <c r="AB29" t="inlineStr">
         <is>
-          <t>DIONISIO, ROEL CRUZ</t>
+          <t>DICDICAN, RICHARD JIMENEZ</t>
         </is>
       </c>
       <c r="AC29" t="inlineStr"/>
@@ -3023,7 +3023,7 @@
       <c r="AE29" t="inlineStr"/>
       <c r="AF29" t="inlineStr">
         <is>
-          <t>ALEGRE,SHIELA,SAHIRON,</t>
+          <t>REALON,MA CLARISSA,ROLDAN,</t>
         </is>
       </c>
       <c r="AG29" t="inlineStr"/>
@@ -3038,13 +3038,13 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>164512120071</t>
+          <t>164512130124</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ESPINOSA, MIAH JUMAO-AS</t>
+          <t>ESPINAR,ANGIELYN, MARCE</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>12-13-2006</t>
+          <t>07-26-2008</t>
         </is>
       </c>
       <c r="I30" t="inlineStr"/>
@@ -3082,7 +3082,7 @@
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO NINO</t>
         </is>
       </c>
       <c r="R30" t="inlineStr"/>
@@ -3105,7 +3105,7 @@
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr">
         <is>
-          <t>ESPINOSA, BONIFACIO ALVERIO</t>
+          <t>ESPINAR, EDISON FLORALDE</t>
         </is>
       </c>
       <c r="AC30" t="inlineStr"/>
@@ -3113,7 +3113,7 @@
       <c r="AE30" t="inlineStr"/>
       <c r="AF30" t="inlineStr">
         <is>
-          <t>JUMAO-AS,CECILIA,MABATID,</t>
+          <t>MARCE,MARIE GRACE,MONTAÑEZ,</t>
         </is>
       </c>
       <c r="AG30" t="inlineStr"/>
@@ -3128,13 +3128,13 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>164512120033</t>
+          <t>108226120096</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>GABUTAN, ANGIE GOLLAYAN</t>
+          <t>GABATIN,LADY TRISHA, AMORTIZADO</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
@@ -3147,13 +3147,13 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>08-06-2006</t>
+          <t>11-03-2006</t>
         </is>
       </c>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
@@ -3195,7 +3195,7 @@
       <c r="AA31" t="inlineStr"/>
       <c r="AB31" t="inlineStr">
         <is>
-          <t>GABUTAN, ALVE SUMARGO</t>
+          <t>GABATIN, TEOFILO TACSIAT</t>
         </is>
       </c>
       <c r="AC31" t="inlineStr"/>
@@ -3203,7 +3203,7 @@
       <c r="AE31" t="inlineStr"/>
       <c r="AF31" t="inlineStr">
         <is>
-          <t>GOLLAYAN,MARITES,BLANZA,</t>
+          <t>AMORTIZADO,MARIA LOURDES,CAPUQUIAN,</t>
         </is>
       </c>
       <c r="AG31" t="inlineStr"/>
@@ -3218,13 +3218,13 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>164512110030</t>
+          <t>164512130042</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
-          <t>GONZALO, ERICQUEZEN DACASIN</t>
+          <t>JOVEN,JENALEN, MASIKAT</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
@@ -3237,13 +3237,13 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>12-07-2005</t>
+          <t>10-01-2006</t>
         </is>
       </c>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
@@ -3285,7 +3285,7 @@
       <c r="AA32" t="inlineStr"/>
       <c r="AB32" t="inlineStr">
         <is>
-          <t>GONZALO, ERIC TORIO</t>
+          <t>JOVEN, SAMUEL ARCEGA</t>
         </is>
       </c>
       <c r="AC32" t="inlineStr"/>
@@ -3293,7 +3293,7 @@
       <c r="AE32" t="inlineStr"/>
       <c r="AF32" t="inlineStr">
         <is>
-          <t>DACASIN,HEIDE,VERGARA,</t>
+          <t>MASIKAT,CRISTINA,BAYAN,</t>
         </is>
       </c>
       <c r="AG32" t="inlineStr"/>
@@ -3308,13 +3308,13 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>164512130062</t>
+          <t>108407130083</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>HUTALLA, RHIAM CLARIS ESPINOSA</t>
+          <t>MALABAG,ANGELICA, MIRANDA</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
@@ -3327,13 +3327,13 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>01-04-2007</t>
+          <t>12-22-2007</t>
         </is>
       </c>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
@@ -3375,7 +3375,7 @@
       <c r="AA33" t="inlineStr"/>
       <c r="AB33" t="inlineStr">
         <is>
-          <t>HUTALLA, CLARO GONZALES</t>
+          <t>MALABAG, ANGELITO MELICIO</t>
         </is>
       </c>
       <c r="AC33" t="inlineStr"/>
@@ -3383,7 +3383,7 @@
       <c r="AE33" t="inlineStr"/>
       <c r="AF33" t="inlineStr">
         <is>
-          <t>ESPINOSA,MIRIAM,ALMEDA,</t>
+          <t>MIRANDA,MARY ANN,BAYANID,</t>
         </is>
       </c>
       <c r="AG33" t="inlineStr"/>
@@ -3398,13 +3398,13 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>164512130032</t>
+          <t>164512140043</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LLANZA, RUTH MICAH CORPUZ</t>
+          <t>MAMANSAG,JEIAH EUNICE, SERRANO</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>11-24-2006</t>
+          <t>08-09-2008</t>
         </is>
       </c>
       <c r="I34" t="inlineStr"/>
@@ -3442,7 +3442,7 @@
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R34" t="inlineStr"/>
@@ -3465,7 +3465,7 @@
       <c r="AA34" t="inlineStr"/>
       <c r="AB34" t="inlineStr">
         <is>
-          <t>LLANZA, JOSEPH GUEVARRA</t>
+          <t>MAMANSAG, EMMERSON SALCEDO</t>
         </is>
       </c>
       <c r="AC34" t="inlineStr"/>
@@ -3473,7 +3473,7 @@
       <c r="AE34" t="inlineStr"/>
       <c r="AF34" t="inlineStr">
         <is>
-          <t>CORPUZ,CLARISA,BARONIA,</t>
+          <t>SERRANO,GERLIE,VALCOBA,</t>
         </is>
       </c>
       <c r="AG34" t="inlineStr"/>
@@ -3488,13 +3488,13 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>164512130036</t>
+          <t>424638150057</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MACARAIG, MARICRIS SABADO</t>
+          <t>MANALILI,JAMAICA AMOR, ROSALES</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
@@ -3507,13 +3507,13 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>10-16-2007</t>
+          <t>01-21-2008</t>
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr">
         <is>
-          <t xml:space="preserve">9 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
@@ -3532,7 +3532,7 @@
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R35" t="inlineStr"/>
@@ -3555,7 +3555,7 @@
       <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="inlineStr">
         <is>
-          <t>MACARAIG, EDWIN GARCIA</t>
+          <t>MANALILI, JAM ANTHONY CASTILLO</t>
         </is>
       </c>
       <c r="AC35" t="inlineStr"/>
@@ -3563,7 +3563,7 @@
       <c r="AE35" t="inlineStr"/>
       <c r="AF35" t="inlineStr">
         <is>
-          <t>SABADO,MARIA,SARSOZA,</t>
+          <t>ROSALES,RACHEL,MALIBAGO,</t>
         </is>
       </c>
       <c r="AG35" t="inlineStr"/>
@@ -3578,13 +3578,13 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>108231130020</t>
+          <t>164512130089</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MARAÑAN, JERAMIAH ALAHAY</t>
+          <t>MARTINEZ,ASHLEE NICHOLE, SABANAL</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>10-01-2006</t>
+          <t>11-16-2008</t>
         </is>
       </c>
       <c r="I36" t="inlineStr"/>
@@ -3622,7 +3622,7 @@
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R36" t="inlineStr"/>
@@ -3645,7 +3645,7 @@
       <c r="AA36" t="inlineStr"/>
       <c r="AB36" t="inlineStr">
         <is>
-          <t>MARAÑAN, RONNIE CUEME</t>
+          <t>MARTINEZ, MAR JUN BRUCE</t>
         </is>
       </c>
       <c r="AC36" t="inlineStr"/>
@@ -3653,7 +3653,7 @@
       <c r="AE36" t="inlineStr"/>
       <c r="AF36" t="inlineStr">
         <is>
-          <t>TATA,ALAHAY,JOSEPHINE,</t>
+          <t>SABANAL,DESARIE,ALORA,</t>
         </is>
       </c>
       <c r="AG36" t="inlineStr"/>
@@ -3663,22 +3663,18 @@
       <c r="AK36" t="inlineStr"/>
       <c r="AL36" t="inlineStr"/>
       <c r="AM36" t="inlineStr"/>
-      <c r="AN36" t="inlineStr">
-        <is>
-          <t>T/I DATE:2017-06-05</t>
-        </is>
-      </c>
+      <c r="AN36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>164512130037</t>
+          <t>164512140024</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>NAVAL, KRISHA MAY MIRANDA</t>
+          <t>NAVAL,GEARLY SHANE, OCAMPO</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
@@ -3691,13 +3687,13 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>06-01-2007</t>
+          <t>11-03-2007</t>
         </is>
       </c>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
@@ -3739,7 +3735,7 @@
       <c r="AA37" t="inlineStr"/>
       <c r="AB37" t="inlineStr">
         <is>
-          <t>NAVAL, TIBURCIO ALIAS</t>
+          <t>NAVAL, PERFECTO LINGGO</t>
         </is>
       </c>
       <c r="AC37" t="inlineStr"/>
@@ -3747,7 +3743,7 @@
       <c r="AE37" t="inlineStr"/>
       <c r="AF37" t="inlineStr">
         <is>
-          <t>MIRANDA,ERLINDA,RAMOS,</t>
+          <t>ILAITIA,MELANIE,OCAMPO,</t>
         </is>
       </c>
       <c r="AG37" t="inlineStr"/>
@@ -3762,13 +3758,13 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>164512130064</t>
+          <t>164512130194</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
-          <t>NAVAL, ZYDNEY RONQUEZ</t>
+          <t>OLAVARIO,ALLIYAH LORRAINE, GUILLERMO</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
@@ -3781,13 +3777,13 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>11-02-2006</t>
+          <t>07-23-2007</t>
         </is>
       </c>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
@@ -3829,7 +3825,7 @@
       <c r="AA38" t="inlineStr"/>
       <c r="AB38" t="inlineStr">
         <is>
-          <t>NAVAL, FERDINAND DIAGO</t>
+          <t>OLAVARIO, TEODULO NUELAN</t>
         </is>
       </c>
       <c r="AC38" t="inlineStr"/>
@@ -3837,7 +3833,7 @@
       <c r="AE38" t="inlineStr"/>
       <c r="AF38" t="inlineStr">
         <is>
-          <t>RONQUEZ,RIO,CAMACHO,</t>
+          <t>GUILLERMO,IRENE,LIMBAG,</t>
         </is>
       </c>
       <c r="AG38" t="inlineStr"/>
@@ -3852,13 +3848,13 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>164512130038</t>
+          <t>108224130152</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr">
         <is>
-          <t>NAVARRO, ELYZA MAE BERMEJO</t>
+          <t>PUNZALAN,CHANELLE, POSO</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
@@ -3871,7 +3867,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>02-08-2007</t>
+          <t>08-03-2008</t>
         </is>
       </c>
       <c r="I39" t="inlineStr"/>
@@ -3896,7 +3892,7 @@
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R39" t="inlineStr"/>
@@ -3919,7 +3915,7 @@
       <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="inlineStr">
         <is>
-          <t>NAVARRO, RAYMUNDO HALLEGADO</t>
+          <t>PUNZALAN, RAYMOND LISMORAS</t>
         </is>
       </c>
       <c r="AC39" t="inlineStr"/>
@@ -3927,7 +3923,7 @@
       <c r="AE39" t="inlineStr"/>
       <c r="AF39" t="inlineStr">
         <is>
-          <t>BERMEJO,GERALDINE,BERNABE,</t>
+          <t>POSO,CHONA,RAMIREZ,</t>
         </is>
       </c>
       <c r="AG39" t="inlineStr"/>
@@ -3942,13 +3938,13 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>164512130068</t>
+          <t>136908131369</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>PONTIGON, PATRICIA JOY ENCISO</t>
+          <t>ROTUBIO,ALLIANA JALYN, BERONDO</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
@@ -3961,7 +3957,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>11-19-2006</t>
+          <t>07-03-2008</t>
         </is>
       </c>
       <c r="I40" t="inlineStr"/>
@@ -3986,7 +3982,7 @@
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R40" t="inlineStr"/>
@@ -4009,7 +4005,7 @@
       <c r="AA40" t="inlineStr"/>
       <c r="AB40" t="inlineStr">
         <is>
-          <t>PONTIGON, JAIME DATUON</t>
+          <t>ROTUBIO, JAY TOLEDO</t>
         </is>
       </c>
       <c r="AC40" t="inlineStr"/>
@@ -4017,7 +4013,7 @@
       <c r="AE40" t="inlineStr"/>
       <c r="AF40" t="inlineStr">
         <is>
-          <t>ENCISO,JOSEPHINE,MAKATINGRAO,</t>
+          <t>BERONDO,NORMALYN,CORDERO,</t>
         </is>
       </c>
       <c r="AG40" t="inlineStr"/>
@@ -4027,18 +4023,22 @@
       <c r="AK40" t="inlineStr"/>
       <c r="AL40" t="inlineStr"/>
       <c r="AM40" t="inlineStr"/>
-      <c r="AN40" t="inlineStr"/>
+      <c r="AN40" t="inlineStr">
+        <is>
+          <t>T/I Southville IV Elem. Sch.Date:2019-09-02</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>111821090138</t>
+          <t>164512130168</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>RAMIREZ, ELIZA CHRISTINE CARREON</t>
+          <t>SUZON,RYGIN LOVE, GIMENTIZA</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
@@ -4051,13 +4051,13 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>10-10-2003</t>
+          <t>05-20-2008</t>
         </is>
       </c>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr">
         <is>
-          <t xml:space="preserve">13 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
@@ -4076,7 +4076,7 @@
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R41" t="inlineStr"/>
@@ -4099,7 +4099,7 @@
       <c r="AA41" t="inlineStr"/>
       <c r="AB41" t="inlineStr">
         <is>
-          <t>RAMIREZ, ERWIN TORARBA</t>
+          <t>SUZON, GERRY BERCERO</t>
         </is>
       </c>
       <c r="AC41" t="inlineStr"/>
@@ -4107,7 +4107,7 @@
       <c r="AE41" t="inlineStr"/>
       <c r="AF41" t="inlineStr">
         <is>
-          <t>CARREON,NELIA,SARMIENTO,</t>
+          <t>GIMENTIZA,GINA,TUICO,</t>
         </is>
       </c>
       <c r="AG41" t="inlineStr"/>
@@ -4117,22 +4117,18 @@
       <c r="AK41" t="inlineStr"/>
       <c r="AL41" t="inlineStr"/>
       <c r="AM41" t="inlineStr"/>
-      <c r="AN41" t="inlineStr">
-        <is>
-          <t>T/I DATE:2017-06-05</t>
-        </is>
-      </c>
+      <c r="AN41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>164512130040</t>
+          <t>107937130338</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>RIVERA, ANGELINA ELAINE MIRANDA</t>
+          <t>TAVU,RENY DENIEZE, RAMOS</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
@@ -4145,13 +4141,13 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>05-02-2007</t>
+          <t>02-24-2008</t>
         </is>
       </c>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
@@ -4170,7 +4166,7 @@
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R42" t="inlineStr"/>
@@ -4193,7 +4189,7 @@
       <c r="AA42" t="inlineStr"/>
       <c r="AB42" t="inlineStr">
         <is>
-          <t>RIVERA, FERDINAND VILLANUEVA</t>
+          <t>TAVU, RENY RAYMOND VEGA</t>
         </is>
       </c>
       <c r="AC42" t="inlineStr"/>
@@ -4201,7 +4197,7 @@
       <c r="AE42" t="inlineStr"/>
       <c r="AF42" t="inlineStr">
         <is>
-          <t>MIRANDA,SHEILA ROSE,BAYANID,</t>
+          <t>RAMOS,ADELAIDA,SANCHEZ,</t>
         </is>
       </c>
       <c r="AG42" t="inlineStr"/>
@@ -4214,44 +4210,86 @@
       <c r="AN42" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>18</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>164512130105</t>
+        </is>
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>&lt;=== TOTAL FEMALE</t>
+          <t>VARGAS,REIGN BEYONCE, GUILLERMO</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>11-03-2007</t>
+        </is>
+      </c>
       <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr"/>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr"/>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P43" t="inlineStr"/>
-      <c r="Q43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr"/>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr"/>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V43" t="inlineStr"/>
       <c r="W43" t="inlineStr"/>
-      <c r="X43" t="inlineStr"/>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y43" t="inlineStr"/>
       <c r="Z43" t="inlineStr"/>
       <c r="AA43" t="inlineStr"/>
-      <c r="AB43" t="inlineStr"/>
+      <c r="AB43" t="inlineStr">
+        <is>
+          <t>VARGAS, JUSSELLE SARMIENTO</t>
+        </is>
+      </c>
       <c r="AC43" t="inlineStr"/>
       <c r="AD43" t="inlineStr"/>
       <c r="AE43" t="inlineStr"/>
-      <c r="AF43" t="inlineStr"/>
+      <c r="AF43" t="inlineStr">
+        <is>
+          <t>GUILLERMO,ADEL,LIMBAG,</t>
+        </is>
+      </c>
       <c r="AG43" t="inlineStr"/>
       <c r="AH43" t="inlineStr"/>
       <c r="AI43" t="inlineStr"/>
@@ -4263,12 +4301,12 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>&lt;=== COMBINED</t>
+          <t>&lt;=== TOTAL FEMALE</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
@@ -4310,13 +4348,15 @@
       <c r="AN44" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>List and Code of Indicators under REMARKS column</t>
-        </is>
+      <c r="A45" t="n">
+        <v>36</v>
       </c>
       <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr"/>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>&lt;=== COMBINED</t>
+        </is>
+      </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
@@ -4358,42 +4398,22 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Indicator</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Code</t>
-        </is>
-      </c>
+          <t>List and Code of Indicators under REMARKS column</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Required Information</t>
-        </is>
-      </c>
+      <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>Indicator</t>
-        </is>
-      </c>
+      <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>Code</t>
-        </is>
-      </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>Required Information</t>
-        </is>
-      </c>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
@@ -4401,41 +4421,21 @@
       <c r="S46" t="inlineStr"/>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr"/>
-      <c r="V46" t="inlineStr">
-        <is>
-          <t>REGISTERED</t>
-        </is>
-      </c>
+      <c r="V46" t="inlineStr"/>
       <c r="W46" t="inlineStr"/>
       <c r="X46" t="inlineStr"/>
-      <c r="Y46" t="inlineStr">
-        <is>
-          <t>BoSY</t>
-        </is>
-      </c>
-      <c r="Z46" t="inlineStr">
-        <is>
-          <t>EoSY</t>
-        </is>
-      </c>
+      <c r="Y46" t="inlineStr"/>
+      <c r="Z46" t="inlineStr"/>
       <c r="AA46" t="inlineStr"/>
       <c r="AB46" t="inlineStr"/>
       <c r="AC46" t="inlineStr"/>
-      <c r="AD46" t="inlineStr">
-        <is>
-          <t>Prepared by;</t>
-        </is>
-      </c>
+      <c r="AD46" t="inlineStr"/>
       <c r="AE46" t="inlineStr"/>
       <c r="AF46" t="inlineStr"/>
       <c r="AG46" t="inlineStr"/>
       <c r="AH46" t="inlineStr"/>
       <c r="AI46" t="inlineStr"/>
-      <c r="AJ46" t="inlineStr">
-        <is>
-          <t>Certified Correct:</t>
-        </is>
-      </c>
+      <c r="AJ46" t="inlineStr"/>
       <c r="AK46" t="inlineStr"/>
       <c r="AL46" t="inlineStr"/>
       <c r="AM46" t="inlineStr"/>
@@ -4444,27 +4444,18 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Transfered Out
-Transfered In
-Dropped
-</t>
+          <t>Indicator</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>T/O
-T/I
-DRP
-LE</t>
+          <t>Code</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Name of  Public (P) Private (PR) School  &amp; Effectivity Date
-Name of  Public (P) Private (PR) School  &amp; Effectivity Date
-Reason  and Effectivity Date
-Reason (Enrollment beyond 1st Friday of </t>
+          <t>Required Information</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -4473,10 +4464,7 @@
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr">
         <is>
-          <t>CCT Receipient
-Balik Aral
-Learner With Disability
-Accelerated</t>
+          <t>Indicator</t>
         </is>
       </c>
       <c r="J47" t="inlineStr"/>
@@ -4484,18 +4472,12 @@
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr">
         <is>
-          <t>CCT
-B/A
-LWD
-ACL</t>
+          <t>Code</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>CCT Control/reference number &amp; Effectivity Date
-Name of school last attended &amp; Year
-Specify
-Specify Level &amp; Effectivity Data</t>
+          <t>Required Information</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
@@ -4507,23 +4489,27 @@
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr">
         <is>
-          <t>MALE</t>
+          <t>REGISTERED</t>
         </is>
       </c>
       <c r="W47" t="inlineStr"/>
       <c r="X47" t="inlineStr"/>
       <c r="Y47" t="inlineStr">
         <is>
-          <t xml:space="preserve">17 </t>
-        </is>
-      </c>
-      <c r="Z47" t="inlineStr"/>
+          <t>BoSY</t>
+        </is>
+      </c>
+      <c r="Z47" t="inlineStr">
+        <is>
+          <t>EoSY</t>
+        </is>
+      </c>
       <c r="AA47" t="inlineStr"/>
       <c r="AB47" t="inlineStr"/>
       <c r="AC47" t="inlineStr"/>
       <c r="AD47" t="inlineStr">
         <is>
-          <t>LAMBERTO BOLIMA RIVAREZ</t>
+          <t>Prepared by;</t>
         </is>
       </c>
       <c r="AE47" t="inlineStr"/>
@@ -4533,7 +4519,7 @@
       <c r="AI47" t="inlineStr"/>
       <c r="AJ47" t="inlineStr">
         <is>
-          <t>ELSA MONTERERO MANALO</t>
+          <t>Certified Correct:</t>
         </is>
       </c>
       <c r="AK47" t="inlineStr"/>
@@ -4542,20 +4528,62 @@
       <c r="AN47" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr"/>
-      <c r="B48" t="inlineStr"/>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Transfered Out
+Transfered In
+Dropped
+Late Enrollment</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>T/O
+T/I
+DRP
+LE</t>
+        </is>
+      </c>
       <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Name of  Public (P) Private (PR) School  &amp; Effectivity Date
+Name of  Public (P) Private (PR) School  &amp; Effectivity Date
+Reason  and Effectivity Date
+Reason (Enrollment beyond 1st Friday of June)</t>
+        </is>
+      </c>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr"/>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>CCT Receipient
+Balik Aral
+Learner With Disability
+Accelerated</t>
+        </is>
+      </c>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>CCT
+B/A
+LWD
+ACL</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>CCT Control/reference number &amp; Effectivity Date
+Name of school last attended &amp; Year
+Specify
+Specify Level &amp; Effectivity Data</t>
+        </is>
+      </c>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
@@ -4565,19 +4593,23 @@
       <c r="U48" t="inlineStr"/>
       <c r="V48" t="inlineStr">
         <is>
-          <t>FEMALE</t>
+          <t>MALE</t>
         </is>
       </c>
       <c r="W48" t="inlineStr"/>
       <c r="X48" t="inlineStr"/>
-      <c r="Y48" t="inlineStr"/>
-      <c r="Z48" t="inlineStr"/>
+      <c r="Y48" t="n">
+        <v>16</v>
+      </c>
+      <c r="Z48" t="n">
+        <v>15</v>
+      </c>
       <c r="AA48" t="inlineStr"/>
       <c r="AB48" t="inlineStr"/>
       <c r="AC48" t="inlineStr"/>
       <c r="AD48" t="inlineStr">
         <is>
-          <t>(Signature of Adviser over Printed Name)</t>
+          <t>LAMBERTO BOLIMA RIVAREZ</t>
         </is>
       </c>
       <c r="AE48" t="inlineStr"/>
@@ -4587,7 +4619,7 @@
       <c r="AI48" t="inlineStr"/>
       <c r="AJ48" t="inlineStr">
         <is>
-          <t>(Signature of School Head over Printed Name)</t>
+          <t>ELSA MONTERERO MANALO</t>
         </is>
       </c>
       <c r="AK48" t="inlineStr"/>
@@ -4620,9 +4652,7 @@
       <c r="V49" t="inlineStr"/>
       <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr"/>
-      <c r="Y49" t="n">
-        <v>18</v>
-      </c>
+      <c r="Y49" t="inlineStr"/>
       <c r="Z49" t="inlineStr"/>
       <c r="AA49" t="inlineStr"/>
       <c r="AB49" t="inlineStr"/>
@@ -4661,54 +4691,32 @@
       <c r="S50" t="inlineStr"/>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
-      <c r="V50" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
+      <c r="V50" t="inlineStr"/>
       <c r="W50" t="inlineStr"/>
       <c r="X50" t="inlineStr"/>
-      <c r="Y50" t="n">
-        <v>35</v>
-      </c>
+      <c r="Y50" t="inlineStr"/>
       <c r="Z50" t="inlineStr"/>
       <c r="AA50" t="inlineStr"/>
       <c r="AB50" t="inlineStr"/>
       <c r="AC50" t="inlineStr"/>
-      <c r="AD50" t="inlineStr">
-        <is>
-          <t>BoSY Date:</t>
-        </is>
-      </c>
+      <c r="AD50" t="inlineStr"/>
       <c r="AE50" t="inlineStr"/>
       <c r="AF50" t="inlineStr"/>
-      <c r="AG50" t="inlineStr">
-        <is>
-          <t>EoSY Date:</t>
-        </is>
-      </c>
+      <c r="AG50" t="inlineStr"/>
       <c r="AH50" t="inlineStr"/>
       <c r="AI50" t="inlineStr"/>
       <c r="AJ50" t="inlineStr">
         <is>
-          <t>BoSY Date:</t>
+          <t>(Signature of School Head over Printed Name)</t>
         </is>
       </c>
       <c r="AK50" t="inlineStr"/>
       <c r="AL50" t="inlineStr"/>
-      <c r="AM50" t="inlineStr">
-        <is>
-          <t>EoSY Date:</t>
-        </is>
-      </c>
+      <c r="AM50" t="inlineStr"/>
       <c r="AN50" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>Generated on: Tuesday, September 12, 2017</t>
-        </is>
-      </c>
+      <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
@@ -4729,15 +4737,27 @@
       <c r="S51" t="inlineStr"/>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
-      <c r="V51" t="inlineStr"/>
+      <c r="V51" t="inlineStr">
+        <is>
+          <t>FEMALE</t>
+        </is>
+      </c>
       <c r="W51" t="inlineStr"/>
       <c r="X51" t="inlineStr"/>
-      <c r="Y51" t="inlineStr"/>
-      <c r="Z51" t="inlineStr"/>
+      <c r="Y51" t="n">
+        <v>19</v>
+      </c>
+      <c r="Z51" t="n">
+        <v>20</v>
+      </c>
       <c r="AA51" t="inlineStr"/>
       <c r="AB51" t="inlineStr"/>
       <c r="AC51" t="inlineStr"/>
-      <c r="AD51" t="inlineStr"/>
+      <c r="AD51" t="inlineStr">
+        <is>
+          <t>(Signature of Adviser over Printed Name)</t>
+        </is>
+      </c>
       <c r="AE51" t="inlineStr"/>
       <c r="AF51" t="inlineStr"/>
       <c r="AG51" t="inlineStr"/>
@@ -4749,6 +4769,290 @@
       <c r="AM51" t="inlineStr"/>
       <c r="AN51" t="inlineStr"/>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr"/>
+      <c r="R52" t="inlineStr"/>
+      <c r="S52" t="inlineStr"/>
+      <c r="T52" t="inlineStr"/>
+      <c r="U52" t="inlineStr"/>
+      <c r="V52" t="inlineStr"/>
+      <c r="W52" t="inlineStr"/>
+      <c r="X52" t="inlineStr"/>
+      <c r="Y52" t="inlineStr"/>
+      <c r="Z52" t="inlineStr"/>
+      <c r="AA52" t="inlineStr"/>
+      <c r="AB52" t="inlineStr"/>
+      <c r="AC52" t="inlineStr"/>
+      <c r="AD52" t="inlineStr"/>
+      <c r="AE52" t="inlineStr"/>
+      <c r="AF52" t="inlineStr"/>
+      <c r="AG52" t="inlineStr"/>
+      <c r="AH52" t="inlineStr"/>
+      <c r="AI52" t="inlineStr"/>
+      <c r="AJ52" t="inlineStr">
+        <is>
+          <t>BoSY Date:                06-03-2019</t>
+        </is>
+      </c>
+      <c r="AK52" t="inlineStr"/>
+      <c r="AL52" t="inlineStr"/>
+      <c r="AM52" t="inlineStr">
+        <is>
+          <t>EoSY Date:                    04-03-2020</t>
+        </is>
+      </c>
+      <c r="AN52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr"/>
+      <c r="R53" t="inlineStr"/>
+      <c r="S53" t="inlineStr"/>
+      <c r="T53" t="inlineStr"/>
+      <c r="U53" t="inlineStr"/>
+      <c r="V53" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="W53" t="inlineStr"/>
+      <c r="X53" t="inlineStr"/>
+      <c r="Y53" t="n">
+        <v>35</v>
+      </c>
+      <c r="Z53" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA53" t="inlineStr"/>
+      <c r="AB53" t="inlineStr"/>
+      <c r="AC53" t="inlineStr"/>
+      <c r="AD53" t="inlineStr">
+        <is>
+          <t>BoSY Date:                06-03-2019</t>
+        </is>
+      </c>
+      <c r="AE53" t="inlineStr"/>
+      <c r="AF53" t="inlineStr"/>
+      <c r="AG53" t="inlineStr">
+        <is>
+          <t>EoSY Date:                  04-03-2020</t>
+        </is>
+      </c>
+      <c r="AH53" t="inlineStr"/>
+      <c r="AI53" t="inlineStr"/>
+      <c r="AJ53" t="inlineStr"/>
+      <c r="AK53" t="inlineStr"/>
+      <c r="AL53" t="inlineStr"/>
+      <c r="AM53" t="inlineStr"/>
+      <c r="AN53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr"/>
+      <c r="R54" t="inlineStr"/>
+      <c r="S54" t="inlineStr"/>
+      <c r="T54" t="inlineStr"/>
+      <c r="U54" t="inlineStr"/>
+      <c r="V54" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr"/>
+      <c r="Y54" t="inlineStr"/>
+      <c r="Z54" t="inlineStr"/>
+      <c r="AA54" t="inlineStr"/>
+      <c r="AB54" t="inlineStr"/>
+      <c r="AC54" t="inlineStr"/>
+      <c r="AD54" t="inlineStr"/>
+      <c r="AE54" t="inlineStr"/>
+      <c r="AF54" t="inlineStr"/>
+      <c r="AG54" t="inlineStr"/>
+      <c r="AH54" t="inlineStr"/>
+      <c r="AI54" t="inlineStr"/>
+      <c r="AJ54" t="inlineStr"/>
+      <c r="AK54" t="inlineStr"/>
+      <c r="AL54" t="inlineStr"/>
+      <c r="AM54" t="inlineStr"/>
+      <c r="AN54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr"/>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
+      <c r="R55" t="inlineStr"/>
+      <c r="S55" t="inlineStr"/>
+      <c r="T55" t="inlineStr"/>
+      <c r="U55" t="inlineStr"/>
+      <c r="V55" t="inlineStr"/>
+      <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr"/>
+      <c r="Y55" t="inlineStr"/>
+      <c r="Z55" t="inlineStr"/>
+      <c r="AA55" t="inlineStr"/>
+      <c r="AB55" t="inlineStr"/>
+      <c r="AC55" t="inlineStr"/>
+      <c r="AD55" t="inlineStr"/>
+      <c r="AE55" t="inlineStr"/>
+      <c r="AF55" t="inlineStr"/>
+      <c r="AG55" t="inlineStr"/>
+      <c r="AH55" t="inlineStr"/>
+      <c r="AI55" t="inlineStr"/>
+      <c r="AJ55" t="inlineStr"/>
+      <c r="AK55" t="inlineStr"/>
+      <c r="AL55" t="inlineStr"/>
+      <c r="AM55" t="inlineStr"/>
+      <c r="AN55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
+      <c r="R56" t="inlineStr"/>
+      <c r="S56" t="inlineStr"/>
+      <c r="T56" t="inlineStr"/>
+      <c r="U56" t="inlineStr"/>
+      <c r="V56" t="inlineStr"/>
+      <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr"/>
+      <c r="Y56" t="inlineStr"/>
+      <c r="Z56" t="inlineStr"/>
+      <c r="AA56" t="inlineStr"/>
+      <c r="AB56" t="inlineStr"/>
+      <c r="AC56" t="inlineStr"/>
+      <c r="AD56" t="inlineStr"/>
+      <c r="AE56" t="inlineStr"/>
+      <c r="AF56" t="inlineStr"/>
+      <c r="AG56" t="inlineStr"/>
+      <c r="AH56" t="inlineStr"/>
+      <c r="AI56" t="inlineStr"/>
+      <c r="AJ56" t="inlineStr">
+        <is>
+          <t>Generated thru LIS</t>
+        </is>
+      </c>
+      <c r="AK56" t="inlineStr"/>
+      <c r="AL56" t="inlineStr"/>
+      <c r="AM56" t="inlineStr"/>
+      <c r="AN56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Generated on: Saturday, March 21, 2020</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
+      <c r="R57" t="inlineStr"/>
+      <c r="S57" t="inlineStr"/>
+      <c r="T57" t="inlineStr"/>
+      <c r="U57" t="inlineStr"/>
+      <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr"/>
+      <c r="Y57" t="inlineStr"/>
+      <c r="Z57" t="inlineStr"/>
+      <c r="AA57" t="inlineStr"/>
+      <c r="AB57" t="inlineStr"/>
+      <c r="AC57" t="inlineStr"/>
+      <c r="AD57" t="inlineStr"/>
+      <c r="AE57" t="inlineStr"/>
+      <c r="AF57" t="inlineStr"/>
+      <c r="AG57" t="inlineStr"/>
+      <c r="AH57" t="inlineStr"/>
+      <c r="AI57" t="inlineStr"/>
+      <c r="AJ57" t="inlineStr"/>
+      <c r="AK57" t="inlineStr"/>
+      <c r="AL57" t="inlineStr"/>
+      <c r="AM57" t="inlineStr"/>
+      <c r="AN57" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
advisory class (updates correctly)
</commit_message>
<xml_diff>
--- a/Migrade_v.1.2/temp.xlsx
+++ b/Migrade_v.1.2/temp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN57"/>
+  <dimension ref="A1:AN51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -782,7 +782,7 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr">
         <is>
-          <t>2019 - 2020</t>
+          <t>2017 - 2018</t>
         </is>
       </c>
       <c r="T4" t="inlineStr"/>
@@ -791,7 +791,7 @@
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Grade Level </t>
+          <t xml:space="preserve">Grade </t>
         </is>
       </c>
       <c r="Y4" t="inlineStr"/>
@@ -799,7 +799,7 @@
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>Grade 6</t>
+          <t>Grade 5</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr"/>
@@ -813,7 +813,7 @@
       <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>GALILEO</t>
+          <t>EARTH</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr"/>
@@ -853,7 +853,7 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>AGE as of 1st Friday June</t>
+          <t>Age as of August 31st</t>
         </is>
       </c>
       <c r="K5" t="inlineStr"/>
@@ -975,7 +975,7 @@
       <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>Mother's Maiden Name (Last Name, First Name, Middle Name)</t>
+          <t xml:space="preserve">Mother's Maiden Name (Last Name, First Name, Middle </t>
         </is>
       </c>
       <c r="AG6" t="inlineStr"/>
@@ -1002,13 +1002,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>164512130171</t>
+          <t>164512110014</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ANIBAN,LEO JELLY, TINAPAY</t>
+          <t>BORLAGDAN, ALFIE BISMAR</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -1021,13 +1021,13 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>09-23-2008</t>
+          <t>05-18-2005</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K7" t="inlineStr"/>
@@ -1069,7 +1069,7 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>ANIBAN, LEO BUTAL</t>
+          <t>BORLAGDAN, ALLAN GOLEMLEM</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr"/>
@@ -1077,7 +1077,7 @@
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>TINAPAY,JILL,BAJADI,</t>
+          <t>BISMAR,CARMENCITA,BLANQUEZA,</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr"/>
@@ -1092,13 +1092,13 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>164512130045</t>
+          <t>164512130010</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ASILO,RAIN JUSTINE, MERCADO</t>
+          <t>BORLAGDAN, RJ BISMAR</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -1111,13 +1111,13 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>05-20-2007</t>
+          <t>11-11-2006</t>
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K8" t="inlineStr"/>
@@ -1136,7 +1136,7 @@
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R8" t="inlineStr"/>
@@ -1159,7 +1159,7 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>ASILO, CHRISTOPHER SALILICAN</t>
+          <t>BORLAGDAN, ALLAN GOLEMLEM</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr"/>
@@ -1167,7 +1167,7 @@
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>MERCADO,MARICEL,HERNANDEZ,</t>
+          <t>BISMAR,CARMENCITA,BLANQUEZA,</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr"/>
@@ -1182,13 +1182,13 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>424663150037</t>
+          <t>136907120127</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CAMBE,SEAN DAVE, ARAGON</t>
+          <t>CAMBE, RALPH LOUIE ARAGON</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -1201,13 +1201,13 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>03-15-2008</t>
+          <t>03-02-2007</t>
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K9" t="inlineStr"/>
@@ -1267,18 +1267,22 @@
       <c r="AK9" t="inlineStr"/>
       <c r="AL9" t="inlineStr"/>
       <c r="AM9" t="inlineStr"/>
-      <c r="AN9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr">
+        <is>
+          <t>T/I DATE:2017-06-05</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>164512140032</t>
+          <t>164512130016</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CARANAY,JHAYCEE CARL, CORDERO</t>
+          <t>CAONES, JAYRUS CARL LACANIN</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -1291,7 +1295,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>11-25-2007</t>
+          <t>08-25-2006</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
@@ -1339,7 +1343,7 @@
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>CARANAY, ROGELIO JR CABOTAJE</t>
+          <t>CAONES, JAYZON NUNAY</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr"/>
@@ -1347,7 +1351,7 @@
       <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="inlineStr">
         <is>
-          <t>CORDERO,NORMA,ALIDO,</t>
+          <t>LACANIN,JERLYN,BELO,</t>
         </is>
       </c>
       <c r="AG10" t="inlineStr"/>
@@ -1362,13 +1366,13 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>164512140029</t>
+          <t>164512120011</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CASTRO,ICHIRO, MENDOZA</t>
+          <t>CELESTE, ANDREW ACE ESPINOSA</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -1381,7 +1385,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>09-08-2008</t>
+          <t>02-09-2007</t>
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
@@ -1406,7 +1410,7 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>PLATERO</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R11" t="inlineStr"/>
@@ -1429,7 +1433,7 @@
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>CASTRO, SEVERLINO ABAPO</t>
+          <t>CELESTE, ALEJANDRO SARVIDA</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr"/>
@@ -1437,7 +1441,7 @@
       <c r="AE11" t="inlineStr"/>
       <c r="AF11" t="inlineStr">
         <is>
-          <t>MENDOZA,ALICIA,ZULUETA,</t>
+          <t>ESPINOSA,LORENA,ALBERTO,</t>
         </is>
       </c>
       <c r="AG11" t="inlineStr"/>
@@ -1452,13 +1456,13 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>164512150094</t>
+          <t>164512130047</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CAYLAO,DAYNE, VIÑA</t>
+          <t>CUPANG, CHRISTIAN ZAMORA</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -1471,13 +1475,13 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>03-17-2007</t>
+          <t>06-21-2007</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K12" t="inlineStr"/>
@@ -1496,7 +1500,7 @@
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>PLATERO</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R12" t="inlineStr"/>
@@ -1519,7 +1523,7 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>CAYLAO, DANZEL CIPRIANO</t>
+          <t>CUPANG, ANTONIO CRISMUNDO JR</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr"/>
@@ -1527,7 +1531,7 @@
       <c r="AE12" t="inlineStr"/>
       <c r="AF12" t="inlineStr">
         <is>
-          <t>VIÑA,CAREN,CRUZ,</t>
+          <t>ZAMORA,TERESITA,ALING,</t>
         </is>
       </c>
       <c r="AG12" t="inlineStr"/>
@@ -1542,13 +1546,13 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>164512130131</t>
+          <t>108226120133</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CHAN,JHON RHAYNE, REPELAR</t>
+          <t>GABATIN, KING TYRON GILBERT AMORTIZADO</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -1561,13 +1565,13 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>01-16-2008</t>
+          <t>11-10-2004</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K13" t="inlineStr"/>
@@ -1609,7 +1613,7 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>CHAN, JONATHAN ALICARTE</t>
+          <t>GABATIN, TEOFILO TACSIAT</t>
         </is>
       </c>
       <c r="AC13" t="inlineStr"/>
@@ -1617,7 +1621,7 @@
       <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="inlineStr">
         <is>
-          <t>REPELAR,ELENA,ROXAS,</t>
+          <t>AMORTIZADO,MARIA LOURDES,CAPUQUIAN,</t>
         </is>
       </c>
       <c r="AG13" t="inlineStr"/>
@@ -1632,13 +1636,13 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>402456150012</t>
+          <t>164512130022</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>GETALADO,EARL SAMUEL, CLAVE</t>
+          <t>LAGADI, JHOSUA BUSTAMANTE</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -1651,7 +1655,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>09-10-2008</t>
+          <t>11-08-2006</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -1676,7 +1680,7 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R14" t="inlineStr"/>
@@ -1699,7 +1703,7 @@
       <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>GETALADO, ERNESTO CERTEZA</t>
+          <t>LAGADI, VICENTE GABRIEL JR</t>
         </is>
       </c>
       <c r="AC14" t="inlineStr"/>
@@ -1707,7 +1711,7 @@
       <c r="AE14" t="inlineStr"/>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>CLAVE,SERENIDAD,TABLIZO,</t>
+          <t>BUSTAMANTE,ELIZA,BULARON,</t>
         </is>
       </c>
       <c r="AG14" t="inlineStr"/>
@@ -1722,13 +1726,13 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>164512130101</t>
+          <t>112505130003</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>GLOBIO,MARCKY, GALVAN</t>
+          <t>LLANZA, ALFREDO LAYCO JR</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -1741,13 +1745,13 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>03-11-2008</t>
+          <t>09-28-2006</t>
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
@@ -1766,7 +1770,7 @@
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>SANTO NINO</t>
         </is>
       </c>
       <c r="R15" t="inlineStr"/>
@@ -1787,13 +1791,17 @@
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="inlineStr"/>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>LLANZA, ALFREDO CARGALLO SR</t>
+        </is>
+      </c>
       <c r="AC15" t="inlineStr"/>
       <c r="AD15" t="inlineStr"/>
       <c r="AE15" t="inlineStr"/>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>GLOBIO,RENITA,GALVAN,</t>
+          <t>LAYCO,ARCELI,MONTANEZ,</t>
         </is>
       </c>
       <c r="AG15" t="inlineStr"/>
@@ -1803,22 +1811,18 @@
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr"/>
       <c r="AM15" t="inlineStr"/>
-      <c r="AN15" t="inlineStr">
-        <is>
-          <t>DRP "Family Problem"Date:2019/11/04</t>
-        </is>
-      </c>
+      <c r="AN15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>164512140006</t>
+          <t>164512130024</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MIRANDA,ANDREI, BIANES</t>
+          <t>MALINTAD, JAMES DUMAYO</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -1831,13 +1835,13 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>04-29-2007</t>
+          <t>03-05-2007</t>
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
@@ -1856,7 +1860,7 @@
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R16" t="inlineStr"/>
@@ -1879,7 +1883,7 @@
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>MIRANDA, ESTELITO VILLANUEVA</t>
+          <t>MALINTAD, GREMER CAONG</t>
         </is>
       </c>
       <c r="AC16" t="inlineStr"/>
@@ -1887,7 +1891,7 @@
       <c r="AE16" t="inlineStr"/>
       <c r="AF16" t="inlineStr">
         <is>
-          <t>BIANES,JENNIFER,QUINTUA,</t>
+          <t>DUMAYO,MINDA,TUMIMO,</t>
         </is>
       </c>
       <c r="AG16" t="inlineStr"/>
@@ -1897,22 +1901,18 @@
       <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="inlineStr"/>
-      <c r="AN16" t="inlineStr">
-        <is>
-          <t>T/I Pook Elem. Sch. Date:2019-06-03</t>
-        </is>
-      </c>
+      <c r="AN16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>164512130118</t>
+          <t>164512130027</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>NAVAREZ,ANDREI, MONTAÑEZ</t>
+          <t>MATULA, JOHN GABRIEL ZAVALLA</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -1925,13 +1925,13 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>07-26-2007</t>
+          <t>09-25-2006</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K17" t="inlineStr"/>
@@ -1973,7 +1973,7 @@
       <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>NAVAREZ, ARNEL NABUHAY</t>
+          <t>MATULA, VICTOR GONZALES</t>
         </is>
       </c>
       <c r="AC17" t="inlineStr"/>
@@ -1981,7 +1981,7 @@
       <c r="AE17" t="inlineStr"/>
       <c r="AF17" t="inlineStr">
         <is>
-          <t>MONTAÑEZ,SUSANA,VILLARIN,</t>
+          <t>ZAVALLA,FLORENCIA,NILLO,</t>
         </is>
       </c>
       <c r="AG17" t="inlineStr"/>
@@ -1996,13 +1996,13 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>164512100132</t>
+          <t>164512120051</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>SALAYSAY,JOHN LOUIE, FLORES</t>
+          <t>OLIVEROS, JHONUEL BISMAR</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -2015,13 +2015,13 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>02-18-2004</t>
+          <t>01-16-2007</t>
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
-          <t xml:space="preserve">15 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
@@ -2063,7 +2063,7 @@
       <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>SALAYSAY, ALFREDO REYES</t>
+          <t>OLIVEROS, JOEL AFANTE</t>
         </is>
       </c>
       <c r="AC18" t="inlineStr"/>
@@ -2071,7 +2071,7 @@
       <c r="AE18" t="inlineStr"/>
       <c r="AF18" t="inlineStr">
         <is>
-          <t>FLORES,CECILIA,LOPENA,</t>
+          <t>BLANQUEZA,JANET,BISMAR,</t>
         </is>
       </c>
       <c r="AG18" t="inlineStr"/>
@@ -2086,13 +2086,13 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>108476120166</t>
+          <t>108474140114</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>SAMANIEGO,MATTHEW ANDREI, ANGULO</t>
+          <t>QUILLOSA, MERICK MASAREDO</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
@@ -2105,13 +2105,13 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>08-01-2006</t>
+          <t>10-04-2006</t>
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
@@ -2130,7 +2130,7 @@
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R19" t="inlineStr"/>
@@ -2153,7 +2153,7 @@
       <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>SAMANIEGO, MICHAEL ABUCEJO</t>
+          <t>QUILLOSA, MARVIN MANLOLO</t>
         </is>
       </c>
       <c r="AC19" t="inlineStr"/>
@@ -2161,7 +2161,7 @@
       <c r="AE19" t="inlineStr"/>
       <c r="AF19" t="inlineStr">
         <is>
-          <t>ANGULO,ABIGAIL,GUSTILO,</t>
+          <t>MASAREDO,PERLA,ACOSTA,</t>
         </is>
       </c>
       <c r="AG19" t="inlineStr"/>
@@ -2176,13 +2176,13 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>108426130045</t>
+          <t>164512130030</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>SAN JUAN JR.,ARLY, PLATINO</t>
+          <t>SANGYAHON, JUSTINE MAGTAGAD</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
@@ -2195,13 +2195,13 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>09-29-2007</t>
+          <t>09-22-2006</t>
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K20" t="inlineStr"/>
@@ -2243,7 +2243,7 @@
       <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>SAN JUAN, ARLY TAPUIC SR</t>
+          <t>SANGYAHON, ERLINDO PATRICIO</t>
         </is>
       </c>
       <c r="AC20" t="inlineStr"/>
@@ -2251,7 +2251,7 @@
       <c r="AE20" t="inlineStr"/>
       <c r="AF20" t="inlineStr">
         <is>
-          <t>PLATINO,EVANGELINE,GUILLEN,</t>
+          <t>MAGTAGAD,CHERYL,ESPAÑOLA,</t>
         </is>
       </c>
       <c r="AG20" t="inlineStr"/>
@@ -2266,13 +2266,13 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>164512130091</t>
+          <t>136775120015</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
-          <t>SANTOS,MARK, BELANO</t>
+          <t>SANTOS, ANGELO GALLARDO</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>09-05-2008</t>
+          <t>05-15-2007</t>
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
@@ -2333,7 +2333,7 @@
       <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>SANTOS, ROLANDO BARBOSA</t>
+          <t>SANTOS, ARTURO CRUZ</t>
         </is>
       </c>
       <c r="AC21" t="inlineStr"/>
@@ -2341,7 +2341,7 @@
       <c r="AE21" t="inlineStr"/>
       <c r="AF21" t="inlineStr">
         <is>
-          <t>BELANO,LIZA,BERIANO,</t>
+          <t>UMALI,GALLARDO,GUADALUPE,</t>
         </is>
       </c>
       <c r="AG21" t="inlineStr"/>
@@ -2351,18 +2351,22 @@
       <c r="AK21" t="inlineStr"/>
       <c r="AL21" t="inlineStr"/>
       <c r="AM21" t="inlineStr"/>
-      <c r="AN21" t="inlineStr"/>
+      <c r="AN21" t="inlineStr">
+        <is>
+          <t>Pending TI</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>164512140037</t>
+          <t>164512120054</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
-          <t>VILLANUEVA,JOSH CYREL, CLASA</t>
+          <t>TABING, RANDEL ABELLA</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
@@ -2375,13 +2379,13 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>11-09-2007</t>
+          <t>06-16-2007</t>
         </is>
       </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
@@ -2423,7 +2427,7 @@
       <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>VILLANUEVA, PABLITO MARIÑAS</t>
+          <t>TABING, RANDY ESTEBAN</t>
         </is>
       </c>
       <c r="AC22" t="inlineStr"/>
@@ -2431,7 +2435,7 @@
       <c r="AE22" t="inlineStr"/>
       <c r="AF22" t="inlineStr">
         <is>
-          <t>CLASA,EVEBERLY,MONTESCO,</t>
+          <t>ABELLA,MARIDEL,ENCELAN,</t>
         </is>
       </c>
       <c r="AG22" t="inlineStr"/>
@@ -2444,44 +2448,86 @@
       <c r="AN22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>16</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>164512120055</t>
+        </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
-          <t>&lt;=== TOTAL MALE</t>
+          <t>VALENCIA, RIN WINZHEL AGUADO</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>01-09-2007</t>
+        </is>
+      </c>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr"/>
-      <c r="X23" t="inlineStr"/>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="inlineStr"/>
-      <c r="AB23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>VALENCIA, CHERWEN MANONGSONG</t>
+        </is>
+      </c>
       <c r="AC23" t="inlineStr"/>
       <c r="AD23" t="inlineStr"/>
       <c r="AE23" t="inlineStr"/>
-      <c r="AF23" t="inlineStr"/>
+      <c r="AF23" t="inlineStr">
+        <is>
+          <t>AGUADO,FRITCHEL,VICTORIO,</t>
+        </is>
+      </c>
       <c r="AG23" t="inlineStr"/>
       <c r="AH23" t="inlineStr"/>
       <c r="AI23" t="inlineStr"/>
@@ -2492,86 +2538,44 @@
       <c r="AN23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>164512140038</t>
-        </is>
+      <c r="A24" t="n">
+        <v>17</v>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ARRESGADO,LEANNE ROSE, CARLOS</t>
+          <t>&lt;=== TOTAL MALE</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>08-25-2008</t>
-        </is>
-      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t xml:space="preserve">10 </t>
-        </is>
-      </c>
+      <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>Tagalog</t>
-        </is>
-      </c>
+      <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>Christianity</t>
-        </is>
-      </c>
+      <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>ZAPOTE</t>
-        </is>
-      </c>
+      <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>CITY OF BIÑAN</t>
-        </is>
-      </c>
+      <c r="U24" t="inlineStr"/>
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr"/>
-      <c r="X24" t="inlineStr">
-        <is>
-          <t>LAGUNA</t>
-        </is>
-      </c>
+      <c r="X24" t="inlineStr"/>
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="inlineStr"/>
-      <c r="AB24" t="inlineStr">
-        <is>
-          <t>ARRESGADO, JUNARD MALAKARTE</t>
-        </is>
-      </c>
+      <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="inlineStr"/>
       <c r="AD24" t="inlineStr"/>
       <c r="AE24" t="inlineStr"/>
-      <c r="AF24" t="inlineStr">
-        <is>
-          <t>CARLOS,AILEEN,VERANO,</t>
-        </is>
-      </c>
+      <c r="AF24" t="inlineStr"/>
       <c r="AG24" t="inlineStr"/>
       <c r="AH24" t="inlineStr"/>
       <c r="AI24" t="inlineStr"/>
@@ -2584,13 +2588,13 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>164512140016</t>
+          <t>164512130075</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
-          <t>BORCELANGO,DONA LYNN, DAPRINAL</t>
+          <t>ACILO, CHARLENE DAGUMAN</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -2603,7 +2607,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>07-22-2008</t>
+          <t>10-18-2006</t>
         </is>
       </c>
       <c r="I25" t="inlineStr"/>
@@ -2651,7 +2655,7 @@
       <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>BORCELANGO, DONATO REYES</t>
+          <t>ACILO, CHARLITO LOPENA</t>
         </is>
       </c>
       <c r="AC25" t="inlineStr"/>
@@ -2659,7 +2663,7 @@
       <c r="AE25" t="inlineStr"/>
       <c r="AF25" t="inlineStr">
         <is>
-          <t>DAPRINAL,JONALINE,ATOR,</t>
+          <t>DAGUMAN,AILENE,ABE,</t>
         </is>
       </c>
       <c r="AG25" t="inlineStr"/>
@@ -2674,13 +2678,13 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>164512140017</t>
+          <t>164512130061</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CAONES,JUSEA MICAH, LACANIN</t>
+          <t>BETITO, EURICE ROSACEÑA</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
@@ -2693,13 +2697,13 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>01-31-2008</t>
+          <t>05-03-2007</t>
         </is>
       </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K26" t="inlineStr"/>
@@ -2741,7 +2745,7 @@
       <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="inlineStr">
         <is>
-          <t>CAONES, JAYZON NUNAY</t>
+          <t>BETITO, ARMANDO SALAMODING</t>
         </is>
       </c>
       <c r="AC26" t="inlineStr"/>
@@ -2749,7 +2753,7 @@
       <c r="AE26" t="inlineStr"/>
       <c r="AF26" t="inlineStr">
         <is>
-          <t>LACANIN,JERLYN,BELO,</t>
+          <t>ROSACENA,REMEDIOS,VILLANUEVA,</t>
         </is>
       </c>
       <c r="AG26" t="inlineStr"/>
@@ -2764,13 +2768,13 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>105111130128</t>
+          <t>164512120064</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CLEMENTE,MARTHA ASHLEE, COLIS</t>
+          <t>CAFINO, JASMIN CLAIRE CANTIGA</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -2783,7 +2787,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>07-02-2008</t>
+          <t>03-06-2007</t>
         </is>
       </c>
       <c r="I27" t="inlineStr"/>
@@ -2808,7 +2812,7 @@
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R27" t="inlineStr"/>
@@ -2831,7 +2835,7 @@
       <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="inlineStr">
         <is>
-          <t>CLEMENTE, RAFAEL KRIS PRONUEVO CLEMENTE</t>
+          <t>CAFINO, RODERICK SOREÑO</t>
         </is>
       </c>
       <c r="AC27" t="inlineStr"/>
@@ -2839,7 +2843,7 @@
       <c r="AE27" t="inlineStr"/>
       <c r="AF27" t="inlineStr">
         <is>
-          <t>COLIS,MA NIEVES VALANTINE,CUNANAN,</t>
+          <t>CANTIGA,GRACE,IGNACIO,</t>
         </is>
       </c>
       <c r="AG27" t="inlineStr"/>
@@ -2849,22 +2853,18 @@
       <c r="AK27" t="inlineStr"/>
       <c r="AL27" t="inlineStr"/>
       <c r="AM27" t="inlineStr"/>
-      <c r="AN27" t="inlineStr">
-        <is>
-          <t>T/I  San Miguel Elem.Sch.Date:2019-06-03</t>
-        </is>
-      </c>
+      <c r="AN27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>109850130028</t>
+          <t>164512120218</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>DEL MUNDO,CATHLYN, SALDINO</t>
+          <t>CLARION, MARY QUEEN MARIEL RAMISO</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
@@ -2877,13 +2877,13 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>11-22-2007</t>
+          <t>10-01-2006</t>
         </is>
       </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K28" t="inlineStr"/>
@@ -2902,7 +2902,7 @@
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R28" t="inlineStr"/>
@@ -2925,7 +2925,7 @@
       <c r="AA28" t="inlineStr"/>
       <c r="AB28" t="inlineStr">
         <is>
-          <t>DEL MUNDO, JUNE LINGGA</t>
+          <t>CLARION, MARCIAL GARRAN</t>
         </is>
       </c>
       <c r="AC28" t="inlineStr"/>
@@ -2933,7 +2933,7 @@
       <c r="AE28" t="inlineStr"/>
       <c r="AF28" t="inlineStr">
         <is>
-          <t>SALDINO,ANNABELLE,SOLAYAO,</t>
+          <t>RAMISO,LIEZEL,SIMPO,</t>
         </is>
       </c>
       <c r="AG28" t="inlineStr"/>
@@ -2948,13 +2948,13 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>164512130166</t>
+          <t>164512130029</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>DICDICAN,TRISHA ELLAINE, REALON</t>
+          <t>DIONISO, JHAMAICA ALEGRE</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>03-01-2008</t>
+          <t>10-25-2005</t>
         </is>
       </c>
       <c r="I29" t="inlineStr"/>
@@ -2992,7 +2992,7 @@
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R29" t="inlineStr"/>
@@ -3015,7 +3015,7 @@
       <c r="AA29" t="inlineStr"/>
       <c r="AB29" t="inlineStr">
         <is>
-          <t>DICDICAN, RICHARD JIMENEZ</t>
+          <t>DIONISIO, ROEL CRUZ</t>
         </is>
       </c>
       <c r="AC29" t="inlineStr"/>
@@ -3023,7 +3023,7 @@
       <c r="AE29" t="inlineStr"/>
       <c r="AF29" t="inlineStr">
         <is>
-          <t>REALON,MA CLARISSA,ROLDAN,</t>
+          <t>ALEGRE,SHIELA,SAHIRON,</t>
         </is>
       </c>
       <c r="AG29" t="inlineStr"/>
@@ -3038,13 +3038,13 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>164512130124</t>
+          <t>164512120071</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ESPINAR,ANGIELYN, MARCE</t>
+          <t>ESPINOSA, MIAH JUMAO-AS</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>07-26-2008</t>
+          <t>12-13-2006</t>
         </is>
       </c>
       <c r="I30" t="inlineStr"/>
@@ -3082,7 +3082,7 @@
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>SANTO NINO</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R30" t="inlineStr"/>
@@ -3105,7 +3105,7 @@
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr">
         <is>
-          <t>ESPINAR, EDISON FLORALDE</t>
+          <t>ESPINOSA, BONIFACIO ALVERIO</t>
         </is>
       </c>
       <c r="AC30" t="inlineStr"/>
@@ -3113,7 +3113,7 @@
       <c r="AE30" t="inlineStr"/>
       <c r="AF30" t="inlineStr">
         <is>
-          <t>MARCE,MARIE GRACE,MONTAÑEZ,</t>
+          <t>JUMAO-AS,CECILIA,MABATID,</t>
         </is>
       </c>
       <c r="AG30" t="inlineStr"/>
@@ -3128,13 +3128,13 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>108226120096</t>
+          <t>164512120033</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>GABATIN,LADY TRISHA, AMORTIZADO</t>
+          <t>GABUTAN, ANGIE GOLLAYAN</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
@@ -3147,13 +3147,13 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>11-03-2006</t>
+          <t>08-06-2006</t>
         </is>
       </c>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
@@ -3195,7 +3195,7 @@
       <c r="AA31" t="inlineStr"/>
       <c r="AB31" t="inlineStr">
         <is>
-          <t>GABATIN, TEOFILO TACSIAT</t>
+          <t>GABUTAN, ALVE SUMARGO</t>
         </is>
       </c>
       <c r="AC31" t="inlineStr"/>
@@ -3203,7 +3203,7 @@
       <c r="AE31" t="inlineStr"/>
       <c r="AF31" t="inlineStr">
         <is>
-          <t>AMORTIZADO,MARIA LOURDES,CAPUQUIAN,</t>
+          <t>GOLLAYAN,MARITES,BLANZA,</t>
         </is>
       </c>
       <c r="AG31" t="inlineStr"/>
@@ -3218,13 +3218,13 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>164512130042</t>
+          <t>164512110030</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
-          <t>JOVEN,JENALEN, MASIKAT</t>
+          <t>GONZALO, ERICQUEZEN DACASIN</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
@@ -3237,13 +3237,13 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>10-01-2006</t>
+          <t>12-07-2005</t>
         </is>
       </c>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
@@ -3285,7 +3285,7 @@
       <c r="AA32" t="inlineStr"/>
       <c r="AB32" t="inlineStr">
         <is>
-          <t>JOVEN, SAMUEL ARCEGA</t>
+          <t>GONZALO, ERIC TORIO</t>
         </is>
       </c>
       <c r="AC32" t="inlineStr"/>
@@ -3293,7 +3293,7 @@
       <c r="AE32" t="inlineStr"/>
       <c r="AF32" t="inlineStr">
         <is>
-          <t>MASIKAT,CRISTINA,BAYAN,</t>
+          <t>DACASIN,HEIDE,VERGARA,</t>
         </is>
       </c>
       <c r="AG32" t="inlineStr"/>
@@ -3308,13 +3308,13 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>108407130083</t>
+          <t>164512130062</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>MALABAG,ANGELICA, MIRANDA</t>
+          <t>HUTALLA, RHIAM CLARIS ESPINOSA</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
@@ -3327,13 +3327,13 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>12-22-2007</t>
+          <t>01-04-2007</t>
         </is>
       </c>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
@@ -3375,7 +3375,7 @@
       <c r="AA33" t="inlineStr"/>
       <c r="AB33" t="inlineStr">
         <is>
-          <t>MALABAG, ANGELITO MELICIO</t>
+          <t>HUTALLA, CLARO GONZALES</t>
         </is>
       </c>
       <c r="AC33" t="inlineStr"/>
@@ -3383,7 +3383,7 @@
       <c r="AE33" t="inlineStr"/>
       <c r="AF33" t="inlineStr">
         <is>
-          <t>MIRANDA,MARY ANN,BAYANID,</t>
+          <t>ESPINOSA,MIRIAM,ALMEDA,</t>
         </is>
       </c>
       <c r="AG33" t="inlineStr"/>
@@ -3398,13 +3398,13 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>164512140043</t>
+          <t>164512130032</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
-          <t>MAMANSAG,JEIAH EUNICE, SERRANO</t>
+          <t>LLANZA, RUTH MICAH CORPUZ</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>08-09-2008</t>
+          <t>11-24-2006</t>
         </is>
       </c>
       <c r="I34" t="inlineStr"/>
@@ -3442,7 +3442,7 @@
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R34" t="inlineStr"/>
@@ -3465,7 +3465,7 @@
       <c r="AA34" t="inlineStr"/>
       <c r="AB34" t="inlineStr">
         <is>
-          <t>MAMANSAG, EMMERSON SALCEDO</t>
+          <t>LLANZA, JOSEPH GUEVARRA</t>
         </is>
       </c>
       <c r="AC34" t="inlineStr"/>
@@ -3473,7 +3473,7 @@
       <c r="AE34" t="inlineStr"/>
       <c r="AF34" t="inlineStr">
         <is>
-          <t>SERRANO,GERLIE,VALCOBA,</t>
+          <t>CORPUZ,CLARISA,BARONIA,</t>
         </is>
       </c>
       <c r="AG34" t="inlineStr"/>
@@ -3488,13 +3488,13 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>424638150057</t>
+          <t>164512130036</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MANALILI,JAMAICA AMOR, ROSALES</t>
+          <t>MACARAIG, MARICRIS SABADO</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
@@ -3507,13 +3507,13 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>01-21-2008</t>
+          <t>10-16-2007</t>
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">9 </t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
@@ -3532,7 +3532,7 @@
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R35" t="inlineStr"/>
@@ -3555,7 +3555,7 @@
       <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="inlineStr">
         <is>
-          <t>MANALILI, JAM ANTHONY CASTILLO</t>
+          <t>MACARAIG, EDWIN GARCIA</t>
         </is>
       </c>
       <c r="AC35" t="inlineStr"/>
@@ -3563,7 +3563,7 @@
       <c r="AE35" t="inlineStr"/>
       <c r="AF35" t="inlineStr">
         <is>
-          <t>ROSALES,RACHEL,MALIBAGO,</t>
+          <t>SABADO,MARIA,SARSOZA,</t>
         </is>
       </c>
       <c r="AG35" t="inlineStr"/>
@@ -3578,13 +3578,13 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>164512130089</t>
+          <t>108231130020</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MARTINEZ,ASHLEE NICHOLE, SABANAL</t>
+          <t>MARAÑAN, JERAMIAH ALAHAY</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>11-16-2008</t>
+          <t>10-01-2006</t>
         </is>
       </c>
       <c r="I36" t="inlineStr"/>
@@ -3622,7 +3622,7 @@
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R36" t="inlineStr"/>
@@ -3645,7 +3645,7 @@
       <c r="AA36" t="inlineStr"/>
       <c r="AB36" t="inlineStr">
         <is>
-          <t>MARTINEZ, MAR JUN BRUCE</t>
+          <t>MARAÑAN, RONNIE CUEME</t>
         </is>
       </c>
       <c r="AC36" t="inlineStr"/>
@@ -3653,7 +3653,7 @@
       <c r="AE36" t="inlineStr"/>
       <c r="AF36" t="inlineStr">
         <is>
-          <t>SABANAL,DESARIE,ALORA,</t>
+          <t>TATA,ALAHAY,JOSEPHINE,</t>
         </is>
       </c>
       <c r="AG36" t="inlineStr"/>
@@ -3663,18 +3663,22 @@
       <c r="AK36" t="inlineStr"/>
       <c r="AL36" t="inlineStr"/>
       <c r="AM36" t="inlineStr"/>
-      <c r="AN36" t="inlineStr"/>
+      <c r="AN36" t="inlineStr">
+        <is>
+          <t>T/I DATE:2017-06-05</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>164512140024</t>
+          <t>164512130037</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>NAVAL,GEARLY SHANE, OCAMPO</t>
+          <t>NAVAL, KRISHA MAY MIRANDA</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
@@ -3687,13 +3691,13 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>11-03-2007</t>
+          <t>06-01-2007</t>
         </is>
       </c>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
@@ -3735,7 +3739,7 @@
       <c r="AA37" t="inlineStr"/>
       <c r="AB37" t="inlineStr">
         <is>
-          <t>NAVAL, PERFECTO LINGGO</t>
+          <t>NAVAL, TIBURCIO ALIAS</t>
         </is>
       </c>
       <c r="AC37" t="inlineStr"/>
@@ -3743,7 +3747,7 @@
       <c r="AE37" t="inlineStr"/>
       <c r="AF37" t="inlineStr">
         <is>
-          <t>ILAITIA,MELANIE,OCAMPO,</t>
+          <t>MIRANDA,ERLINDA,RAMOS,</t>
         </is>
       </c>
       <c r="AG37" t="inlineStr"/>
@@ -3758,13 +3762,13 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>164512130194</t>
+          <t>164512130064</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
-          <t>OLAVARIO,ALLIYAH LORRAINE, GUILLERMO</t>
+          <t>NAVAL, ZYDNEY RONQUEZ</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
@@ -3777,13 +3781,13 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>07-23-2007</t>
+          <t>11-02-2006</t>
         </is>
       </c>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
@@ -3825,7 +3829,7 @@
       <c r="AA38" t="inlineStr"/>
       <c r="AB38" t="inlineStr">
         <is>
-          <t>OLAVARIO, TEODULO NUELAN</t>
+          <t>NAVAL, FERDINAND DIAGO</t>
         </is>
       </c>
       <c r="AC38" t="inlineStr"/>
@@ -3833,7 +3837,7 @@
       <c r="AE38" t="inlineStr"/>
       <c r="AF38" t="inlineStr">
         <is>
-          <t>GUILLERMO,IRENE,LIMBAG,</t>
+          <t>RONQUEZ,RIO,CAMACHO,</t>
         </is>
       </c>
       <c r="AG38" t="inlineStr"/>
@@ -3848,13 +3852,13 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>108224130152</t>
+          <t>164512130038</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr">
         <is>
-          <t>PUNZALAN,CHANELLE, POSO</t>
+          <t>NAVARRO, ELYZA MAE BERMEJO</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
@@ -3867,7 +3871,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>08-03-2008</t>
+          <t>02-08-2007</t>
         </is>
       </c>
       <c r="I39" t="inlineStr"/>
@@ -3892,7 +3896,7 @@
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R39" t="inlineStr"/>
@@ -3915,7 +3919,7 @@
       <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="inlineStr">
         <is>
-          <t>PUNZALAN, RAYMOND LISMORAS</t>
+          <t>NAVARRO, RAYMUNDO HALLEGADO</t>
         </is>
       </c>
       <c r="AC39" t="inlineStr"/>
@@ -3923,7 +3927,7 @@
       <c r="AE39" t="inlineStr"/>
       <c r="AF39" t="inlineStr">
         <is>
-          <t>POSO,CHONA,RAMIREZ,</t>
+          <t>BERMEJO,GERALDINE,BERNABE,</t>
         </is>
       </c>
       <c r="AG39" t="inlineStr"/>
@@ -3938,13 +3942,13 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>136908131369</t>
+          <t>164512130068</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ROTUBIO,ALLIANA JALYN, BERONDO</t>
+          <t>PONTIGON, PATRICIA JOY ENCISO</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
@@ -3957,7 +3961,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>07-03-2008</t>
+          <t>11-19-2006</t>
         </is>
       </c>
       <c r="I40" t="inlineStr"/>
@@ -3982,7 +3986,7 @@
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R40" t="inlineStr"/>
@@ -4005,7 +4009,7 @@
       <c r="AA40" t="inlineStr"/>
       <c r="AB40" t="inlineStr">
         <is>
-          <t>ROTUBIO, JAY TOLEDO</t>
+          <t>PONTIGON, JAIME DATUON</t>
         </is>
       </c>
       <c r="AC40" t="inlineStr"/>
@@ -4013,7 +4017,7 @@
       <c r="AE40" t="inlineStr"/>
       <c r="AF40" t="inlineStr">
         <is>
-          <t>BERONDO,NORMALYN,CORDERO,</t>
+          <t>ENCISO,JOSEPHINE,MAKATINGRAO,</t>
         </is>
       </c>
       <c r="AG40" t="inlineStr"/>
@@ -4023,22 +4027,18 @@
       <c r="AK40" t="inlineStr"/>
       <c r="AL40" t="inlineStr"/>
       <c r="AM40" t="inlineStr"/>
-      <c r="AN40" t="inlineStr">
-        <is>
-          <t>T/I Southville IV Elem. Sch.Date:2019-09-02</t>
-        </is>
-      </c>
+      <c r="AN40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>164512130168</t>
+          <t>111821090138</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>SUZON,RYGIN LOVE, GIMENTIZA</t>
+          <t>RAMIREZ, ELIZA CHRISTINE CARREON</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
@@ -4051,13 +4051,13 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>05-20-2008</t>
+          <t>10-10-2003</t>
         </is>
       </c>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">13 </t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
@@ -4076,7 +4076,7 @@
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R41" t="inlineStr"/>
@@ -4099,7 +4099,7 @@
       <c r="AA41" t="inlineStr"/>
       <c r="AB41" t="inlineStr">
         <is>
-          <t>SUZON, GERRY BERCERO</t>
+          <t>RAMIREZ, ERWIN TORARBA</t>
         </is>
       </c>
       <c r="AC41" t="inlineStr"/>
@@ -4107,7 +4107,7 @@
       <c r="AE41" t="inlineStr"/>
       <c r="AF41" t="inlineStr">
         <is>
-          <t>GIMENTIZA,GINA,TUICO,</t>
+          <t>CARREON,NELIA,SARMIENTO,</t>
         </is>
       </c>
       <c r="AG41" t="inlineStr"/>
@@ -4117,18 +4117,22 @@
       <c r="AK41" t="inlineStr"/>
       <c r="AL41" t="inlineStr"/>
       <c r="AM41" t="inlineStr"/>
-      <c r="AN41" t="inlineStr"/>
+      <c r="AN41" t="inlineStr">
+        <is>
+          <t>T/I DATE:2017-06-05</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>107937130338</t>
+          <t>164512130040</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>TAVU,RENY DENIEZE, RAMOS</t>
+          <t>RIVERA, ANGELINA ELAINE MIRANDA</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
@@ -4141,13 +4145,13 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>02-24-2008</t>
+          <t>05-02-2007</t>
         </is>
       </c>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
@@ -4166,7 +4170,7 @@
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R42" t="inlineStr"/>
@@ -4189,7 +4193,7 @@
       <c r="AA42" t="inlineStr"/>
       <c r="AB42" t="inlineStr">
         <is>
-          <t>TAVU, RENY RAYMOND VEGA</t>
+          <t>RIVERA, FERDINAND VILLANUEVA</t>
         </is>
       </c>
       <c r="AC42" t="inlineStr"/>
@@ -4197,7 +4201,7 @@
       <c r="AE42" t="inlineStr"/>
       <c r="AF42" t="inlineStr">
         <is>
-          <t>RAMOS,ADELAIDA,SANCHEZ,</t>
+          <t>MIRANDA,SHEILA ROSE,BAYANID,</t>
         </is>
       </c>
       <c r="AG42" t="inlineStr"/>
@@ -4210,86 +4214,44 @@
       <c r="AN42" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>164512130105</t>
-        </is>
+      <c r="A43" t="n">
+        <v>18</v>
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>VARGAS,REIGN BEYONCE, GUILLERMO</t>
+          <t>&lt;=== TOTAL FEMALE</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>11-03-2007</t>
-        </is>
-      </c>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11 </t>
-        </is>
-      </c>
+      <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>Tagalog</t>
-        </is>
-      </c>
+      <c r="L43" t="inlineStr"/>
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>Christianity</t>
-        </is>
-      </c>
+      <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr"/>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>ZAPOTE</t>
-        </is>
-      </c>
+      <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr"/>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr">
-        <is>
-          <t>CITY OF BIÑAN</t>
-        </is>
-      </c>
+      <c r="U43" t="inlineStr"/>
       <c r="V43" t="inlineStr"/>
       <c r="W43" t="inlineStr"/>
-      <c r="X43" t="inlineStr">
-        <is>
-          <t>LAGUNA</t>
-        </is>
-      </c>
+      <c r="X43" t="inlineStr"/>
       <c r="Y43" t="inlineStr"/>
       <c r="Z43" t="inlineStr"/>
       <c r="AA43" t="inlineStr"/>
-      <c r="AB43" t="inlineStr">
-        <is>
-          <t>VARGAS, JUSSELLE SARMIENTO</t>
-        </is>
-      </c>
+      <c r="AB43" t="inlineStr"/>
       <c r="AC43" t="inlineStr"/>
       <c r="AD43" t="inlineStr"/>
       <c r="AE43" t="inlineStr"/>
-      <c r="AF43" t="inlineStr">
-        <is>
-          <t>GUILLERMO,ADEL,LIMBAG,</t>
-        </is>
-      </c>
+      <c r="AF43" t="inlineStr"/>
       <c r="AG43" t="inlineStr"/>
       <c r="AH43" t="inlineStr"/>
       <c r="AI43" t="inlineStr"/>
@@ -4301,12 +4263,12 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>&lt;=== TOTAL FEMALE</t>
+          <t>&lt;=== COMBINED</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
@@ -4348,15 +4310,13 @@
       <c r="AN44" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>36</v>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>List and Code of Indicators under REMARKS column</t>
+        </is>
       </c>
       <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>&lt;=== COMBINED</t>
-        </is>
-      </c>
+      <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
@@ -4398,22 +4358,42 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>List and Code of Indicators under REMARKS column</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr"/>
+          <t>Indicator</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Code</t>
+        </is>
+      </c>
       <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Required Information</t>
+        </is>
+      </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Indicator</t>
+        </is>
+      </c>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>Code</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>Required Information</t>
+        </is>
+      </c>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
@@ -4421,21 +4401,41 @@
       <c r="S46" t="inlineStr"/>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr"/>
-      <c r="V46" t="inlineStr"/>
+      <c r="V46" t="inlineStr">
+        <is>
+          <t>REGISTERED</t>
+        </is>
+      </c>
       <c r="W46" t="inlineStr"/>
       <c r="X46" t="inlineStr"/>
-      <c r="Y46" t="inlineStr"/>
-      <c r="Z46" t="inlineStr"/>
+      <c r="Y46" t="inlineStr">
+        <is>
+          <t>BoSY</t>
+        </is>
+      </c>
+      <c r="Z46" t="inlineStr">
+        <is>
+          <t>EoSY</t>
+        </is>
+      </c>
       <c r="AA46" t="inlineStr"/>
       <c r="AB46" t="inlineStr"/>
       <c r="AC46" t="inlineStr"/>
-      <c r="AD46" t="inlineStr"/>
+      <c r="AD46" t="inlineStr">
+        <is>
+          <t>Prepared by;</t>
+        </is>
+      </c>
       <c r="AE46" t="inlineStr"/>
       <c r="AF46" t="inlineStr"/>
       <c r="AG46" t="inlineStr"/>
       <c r="AH46" t="inlineStr"/>
       <c r="AI46" t="inlineStr"/>
-      <c r="AJ46" t="inlineStr"/>
+      <c r="AJ46" t="inlineStr">
+        <is>
+          <t>Certified Correct:</t>
+        </is>
+      </c>
       <c r="AK46" t="inlineStr"/>
       <c r="AL46" t="inlineStr"/>
       <c r="AM46" t="inlineStr"/>
@@ -4444,18 +4444,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Indicator</t>
+          <t xml:space="preserve">Transfered Out
+Transfered In
+Dropped
+</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Code</t>
+          <t>T/O
+T/I
+DRP
+LE</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Required Information</t>
+          <t xml:space="preserve">Name of  Public (P) Private (PR) School  &amp; Effectivity Date
+Name of  Public (P) Private (PR) School  &amp; Effectivity Date
+Reason  and Effectivity Date
+Reason (Enrollment beyond 1st Friday of </t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -4464,7 +4473,10 @@
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Indicator</t>
+          <t>CCT Receipient
+Balik Aral
+Learner With Disability
+Accelerated</t>
         </is>
       </c>
       <c r="J47" t="inlineStr"/>
@@ -4472,12 +4484,18 @@
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Code</t>
+          <t>CCT
+B/A
+LWD
+ACL</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>Required Information</t>
+          <t>CCT Control/reference number &amp; Effectivity Date
+Name of school last attended &amp; Year
+Specify
+Specify Level &amp; Effectivity Data</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
@@ -4489,27 +4507,23 @@
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr">
         <is>
-          <t>REGISTERED</t>
+          <t>MALE</t>
         </is>
       </c>
       <c r="W47" t="inlineStr"/>
       <c r="X47" t="inlineStr"/>
       <c r="Y47" t="inlineStr">
         <is>
-          <t>BoSY</t>
-        </is>
-      </c>
-      <c r="Z47" t="inlineStr">
-        <is>
-          <t>EoSY</t>
-        </is>
-      </c>
+          <t xml:space="preserve">17 </t>
+        </is>
+      </c>
+      <c r="Z47" t="inlineStr"/>
       <c r="AA47" t="inlineStr"/>
       <c r="AB47" t="inlineStr"/>
       <c r="AC47" t="inlineStr"/>
       <c r="AD47" t="inlineStr">
         <is>
-          <t>Prepared by;</t>
+          <t>LAMBERTO BOLIMA RIVAREZ</t>
         </is>
       </c>
       <c r="AE47" t="inlineStr"/>
@@ -4519,7 +4533,7 @@
       <c r="AI47" t="inlineStr"/>
       <c r="AJ47" t="inlineStr">
         <is>
-          <t>Certified Correct:</t>
+          <t>ELSA MONTERERO MANALO</t>
         </is>
       </c>
       <c r="AK47" t="inlineStr"/>
@@ -4528,62 +4542,20 @@
       <c r="AN47" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Transfered Out
-Transfered In
-Dropped
-Late Enrollment</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>T/O
-T/I
-DRP
-LE</t>
-        </is>
-      </c>
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Name of  Public (P) Private (PR) School  &amp; Effectivity Date
-Name of  Public (P) Private (PR) School  &amp; Effectivity Date
-Reason  and Effectivity Date
-Reason (Enrollment beyond 1st Friday of June)</t>
-        </is>
-      </c>
+      <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>CCT Receipient
-Balik Aral
-Learner With Disability
-Accelerated</t>
-        </is>
-      </c>
+      <c r="I48" t="inlineStr"/>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>CCT
-B/A
-LWD
-ACL</t>
-        </is>
-      </c>
-      <c r="N48" t="inlineStr">
-        <is>
-          <t>CCT Control/reference number &amp; Effectivity Date
-Name of school last attended &amp; Year
-Specify
-Specify Level &amp; Effectivity Data</t>
-        </is>
-      </c>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
@@ -4593,23 +4565,19 @@
       <c r="U48" t="inlineStr"/>
       <c r="V48" t="inlineStr">
         <is>
-          <t>MALE</t>
+          <t>FEMALE</t>
         </is>
       </c>
       <c r="W48" t="inlineStr"/>
       <c r="X48" t="inlineStr"/>
-      <c r="Y48" t="n">
-        <v>16</v>
-      </c>
-      <c r="Z48" t="n">
-        <v>15</v>
-      </c>
+      <c r="Y48" t="inlineStr"/>
+      <c r="Z48" t="inlineStr"/>
       <c r="AA48" t="inlineStr"/>
       <c r="AB48" t="inlineStr"/>
       <c r="AC48" t="inlineStr"/>
       <c r="AD48" t="inlineStr">
         <is>
-          <t>LAMBERTO BOLIMA RIVAREZ</t>
+          <t>(Signature of Adviser over Printed Name)</t>
         </is>
       </c>
       <c r="AE48" t="inlineStr"/>
@@ -4619,7 +4587,7 @@
       <c r="AI48" t="inlineStr"/>
       <c r="AJ48" t="inlineStr">
         <is>
-          <t>ELSA MONTERERO MANALO</t>
+          <t>(Signature of School Head over Printed Name)</t>
         </is>
       </c>
       <c r="AK48" t="inlineStr"/>
@@ -4652,7 +4620,9 @@
       <c r="V49" t="inlineStr"/>
       <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr"/>
-      <c r="Y49" t="inlineStr"/>
+      <c r="Y49" t="n">
+        <v>18</v>
+      </c>
       <c r="Z49" t="inlineStr"/>
       <c r="AA49" t="inlineStr"/>
       <c r="AB49" t="inlineStr"/>
@@ -4691,32 +4661,54 @@
       <c r="S50" t="inlineStr"/>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
-      <c r="V50" t="inlineStr"/>
+      <c r="V50" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
       <c r="W50" t="inlineStr"/>
       <c r="X50" t="inlineStr"/>
-      <c r="Y50" t="inlineStr"/>
+      <c r="Y50" t="n">
+        <v>35</v>
+      </c>
       <c r="Z50" t="inlineStr"/>
       <c r="AA50" t="inlineStr"/>
       <c r="AB50" t="inlineStr"/>
       <c r="AC50" t="inlineStr"/>
-      <c r="AD50" t="inlineStr"/>
+      <c r="AD50" t="inlineStr">
+        <is>
+          <t>BoSY Date:</t>
+        </is>
+      </c>
       <c r="AE50" t="inlineStr"/>
       <c r="AF50" t="inlineStr"/>
-      <c r="AG50" t="inlineStr"/>
+      <c r="AG50" t="inlineStr">
+        <is>
+          <t>EoSY Date:</t>
+        </is>
+      </c>
       <c r="AH50" t="inlineStr"/>
       <c r="AI50" t="inlineStr"/>
       <c r="AJ50" t="inlineStr">
         <is>
-          <t>(Signature of School Head over Printed Name)</t>
+          <t>BoSY Date:</t>
         </is>
       </c>
       <c r="AK50" t="inlineStr"/>
       <c r="AL50" t="inlineStr"/>
-      <c r="AM50" t="inlineStr"/>
+      <c r="AM50" t="inlineStr">
+        <is>
+          <t>EoSY Date:</t>
+        </is>
+      </c>
       <c r="AN50" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr"/>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Generated on: Tuesday, September 12, 2017</t>
+        </is>
+      </c>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
@@ -4737,27 +4729,15 @@
       <c r="S51" t="inlineStr"/>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
-      <c r="V51" t="inlineStr">
-        <is>
-          <t>FEMALE</t>
-        </is>
-      </c>
+      <c r="V51" t="inlineStr"/>
       <c r="W51" t="inlineStr"/>
       <c r="X51" t="inlineStr"/>
-      <c r="Y51" t="n">
-        <v>19</v>
-      </c>
-      <c r="Z51" t="n">
-        <v>20</v>
-      </c>
+      <c r="Y51" t="inlineStr"/>
+      <c r="Z51" t="inlineStr"/>
       <c r="AA51" t="inlineStr"/>
       <c r="AB51" t="inlineStr"/>
       <c r="AC51" t="inlineStr"/>
-      <c r="AD51" t="inlineStr">
-        <is>
-          <t>(Signature of Adviser over Printed Name)</t>
-        </is>
-      </c>
+      <c r="AD51" t="inlineStr"/>
       <c r="AE51" t="inlineStr"/>
       <c r="AF51" t="inlineStr"/>
       <c r="AG51" t="inlineStr"/>
@@ -4769,290 +4749,6 @@
       <c r="AM51" t="inlineStr"/>
       <c r="AN51" t="inlineStr"/>
     </row>
-    <row r="52">
-      <c r="A52" t="inlineStr"/>
-      <c r="B52" t="inlineStr"/>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr"/>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="inlineStr"/>
-      <c r="I52" t="inlineStr"/>
-      <c r="J52" t="inlineStr"/>
-      <c r="K52" t="inlineStr"/>
-      <c r="L52" t="inlineStr"/>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
-      <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr"/>
-      <c r="Q52" t="inlineStr"/>
-      <c r="R52" t="inlineStr"/>
-      <c r="S52" t="inlineStr"/>
-      <c r="T52" t="inlineStr"/>
-      <c r="U52" t="inlineStr"/>
-      <c r="V52" t="inlineStr"/>
-      <c r="W52" t="inlineStr"/>
-      <c r="X52" t="inlineStr"/>
-      <c r="Y52" t="inlineStr"/>
-      <c r="Z52" t="inlineStr"/>
-      <c r="AA52" t="inlineStr"/>
-      <c r="AB52" t="inlineStr"/>
-      <c r="AC52" t="inlineStr"/>
-      <c r="AD52" t="inlineStr"/>
-      <c r="AE52" t="inlineStr"/>
-      <c r="AF52" t="inlineStr"/>
-      <c r="AG52" t="inlineStr"/>
-      <c r="AH52" t="inlineStr"/>
-      <c r="AI52" t="inlineStr"/>
-      <c r="AJ52" t="inlineStr">
-        <is>
-          <t>BoSY Date:                06-03-2019</t>
-        </is>
-      </c>
-      <c r="AK52" t="inlineStr"/>
-      <c r="AL52" t="inlineStr"/>
-      <c r="AM52" t="inlineStr">
-        <is>
-          <t>EoSY Date:                    04-03-2020</t>
-        </is>
-      </c>
-      <c r="AN52" t="inlineStr"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr"/>
-      <c r="B53" t="inlineStr"/>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr"/>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr"/>
-      <c r="J53" t="inlineStr"/>
-      <c r="K53" t="inlineStr"/>
-      <c r="L53" t="inlineStr"/>
-      <c r="M53" t="inlineStr"/>
-      <c r="N53" t="inlineStr"/>
-      <c r="O53" t="inlineStr"/>
-      <c r="P53" t="inlineStr"/>
-      <c r="Q53" t="inlineStr"/>
-      <c r="R53" t="inlineStr"/>
-      <c r="S53" t="inlineStr"/>
-      <c r="T53" t="inlineStr"/>
-      <c r="U53" t="inlineStr"/>
-      <c r="V53" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="W53" t="inlineStr"/>
-      <c r="X53" t="inlineStr"/>
-      <c r="Y53" t="n">
-        <v>35</v>
-      </c>
-      <c r="Z53" t="n">
-        <v>35</v>
-      </c>
-      <c r="AA53" t="inlineStr"/>
-      <c r="AB53" t="inlineStr"/>
-      <c r="AC53" t="inlineStr"/>
-      <c r="AD53" t="inlineStr">
-        <is>
-          <t>BoSY Date:                06-03-2019</t>
-        </is>
-      </c>
-      <c r="AE53" t="inlineStr"/>
-      <c r="AF53" t="inlineStr"/>
-      <c r="AG53" t="inlineStr">
-        <is>
-          <t>EoSY Date:                  04-03-2020</t>
-        </is>
-      </c>
-      <c r="AH53" t="inlineStr"/>
-      <c r="AI53" t="inlineStr"/>
-      <c r="AJ53" t="inlineStr"/>
-      <c r="AK53" t="inlineStr"/>
-      <c r="AL53" t="inlineStr"/>
-      <c r="AM53" t="inlineStr"/>
-      <c r="AN53" t="inlineStr"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr"/>
-      <c r="B54" t="inlineStr"/>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr"/>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr"/>
-      <c r="J54" t="inlineStr"/>
-      <c r="K54" t="inlineStr"/>
-      <c r="L54" t="inlineStr"/>
-      <c r="M54" t="inlineStr"/>
-      <c r="N54" t="inlineStr"/>
-      <c r="O54" t="inlineStr"/>
-      <c r="P54" t="inlineStr"/>
-      <c r="Q54" t="inlineStr"/>
-      <c r="R54" t="inlineStr"/>
-      <c r="S54" t="inlineStr"/>
-      <c r="T54" t="inlineStr"/>
-      <c r="U54" t="inlineStr"/>
-      <c r="V54" t="inlineStr"/>
-      <c r="W54" t="inlineStr"/>
-      <c r="X54" t="inlineStr"/>
-      <c r="Y54" t="inlineStr"/>
-      <c r="Z54" t="inlineStr"/>
-      <c r="AA54" t="inlineStr"/>
-      <c r="AB54" t="inlineStr"/>
-      <c r="AC54" t="inlineStr"/>
-      <c r="AD54" t="inlineStr"/>
-      <c r="AE54" t="inlineStr"/>
-      <c r="AF54" t="inlineStr"/>
-      <c r="AG54" t="inlineStr"/>
-      <c r="AH54" t="inlineStr"/>
-      <c r="AI54" t="inlineStr"/>
-      <c r="AJ54" t="inlineStr"/>
-      <c r="AK54" t="inlineStr"/>
-      <c r="AL54" t="inlineStr"/>
-      <c r="AM54" t="inlineStr"/>
-      <c r="AN54" t="inlineStr"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr"/>
-      <c r="B55" t="inlineStr"/>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr"/>
-      <c r="J55" t="inlineStr"/>
-      <c r="K55" t="inlineStr"/>
-      <c r="L55" t="inlineStr"/>
-      <c r="M55" t="inlineStr"/>
-      <c r="N55" t="inlineStr"/>
-      <c r="O55" t="inlineStr"/>
-      <c r="P55" t="inlineStr"/>
-      <c r="Q55" t="inlineStr"/>
-      <c r="R55" t="inlineStr"/>
-      <c r="S55" t="inlineStr"/>
-      <c r="T55" t="inlineStr"/>
-      <c r="U55" t="inlineStr"/>
-      <c r="V55" t="inlineStr"/>
-      <c r="W55" t="inlineStr"/>
-      <c r="X55" t="inlineStr"/>
-      <c r="Y55" t="inlineStr"/>
-      <c r="Z55" t="inlineStr"/>
-      <c r="AA55" t="inlineStr"/>
-      <c r="AB55" t="inlineStr"/>
-      <c r="AC55" t="inlineStr"/>
-      <c r="AD55" t="inlineStr"/>
-      <c r="AE55" t="inlineStr"/>
-      <c r="AF55" t="inlineStr"/>
-      <c r="AG55" t="inlineStr"/>
-      <c r="AH55" t="inlineStr"/>
-      <c r="AI55" t="inlineStr"/>
-      <c r="AJ55" t="inlineStr"/>
-      <c r="AK55" t="inlineStr"/>
-      <c r="AL55" t="inlineStr"/>
-      <c r="AM55" t="inlineStr"/>
-      <c r="AN55" t="inlineStr"/>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr"/>
-      <c r="B56" t="inlineStr"/>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
-      <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
-      <c r="J56" t="inlineStr"/>
-      <c r="K56" t="inlineStr"/>
-      <c r="L56" t="inlineStr"/>
-      <c r="M56" t="inlineStr"/>
-      <c r="N56" t="inlineStr"/>
-      <c r="O56" t="inlineStr"/>
-      <c r="P56" t="inlineStr"/>
-      <c r="Q56" t="inlineStr"/>
-      <c r="R56" t="inlineStr"/>
-      <c r="S56" t="inlineStr"/>
-      <c r="T56" t="inlineStr"/>
-      <c r="U56" t="inlineStr"/>
-      <c r="V56" t="inlineStr"/>
-      <c r="W56" t="inlineStr"/>
-      <c r="X56" t="inlineStr"/>
-      <c r="Y56" t="inlineStr"/>
-      <c r="Z56" t="inlineStr"/>
-      <c r="AA56" t="inlineStr"/>
-      <c r="AB56" t="inlineStr"/>
-      <c r="AC56" t="inlineStr"/>
-      <c r="AD56" t="inlineStr"/>
-      <c r="AE56" t="inlineStr"/>
-      <c r="AF56" t="inlineStr"/>
-      <c r="AG56" t="inlineStr"/>
-      <c r="AH56" t="inlineStr"/>
-      <c r="AI56" t="inlineStr"/>
-      <c r="AJ56" t="inlineStr">
-        <is>
-          <t>Generated thru LIS</t>
-        </is>
-      </c>
-      <c r="AK56" t="inlineStr"/>
-      <c r="AL56" t="inlineStr"/>
-      <c r="AM56" t="inlineStr"/>
-      <c r="AN56" t="inlineStr"/>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Generated on: Saturday, March 21, 2020</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr"/>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr"/>
-      <c r="J57" t="inlineStr"/>
-      <c r="K57" t="inlineStr"/>
-      <c r="L57" t="inlineStr"/>
-      <c r="M57" t="inlineStr"/>
-      <c r="N57" t="inlineStr"/>
-      <c r="O57" t="inlineStr"/>
-      <c r="P57" t="inlineStr"/>
-      <c r="Q57" t="inlineStr"/>
-      <c r="R57" t="inlineStr"/>
-      <c r="S57" t="inlineStr"/>
-      <c r="T57" t="inlineStr"/>
-      <c r="U57" t="inlineStr"/>
-      <c r="V57" t="inlineStr"/>
-      <c r="W57" t="inlineStr"/>
-      <c r="X57" t="inlineStr"/>
-      <c r="Y57" t="inlineStr"/>
-      <c r="Z57" t="inlineStr"/>
-      <c r="AA57" t="inlineStr"/>
-      <c r="AB57" t="inlineStr"/>
-      <c r="AC57" t="inlineStr"/>
-      <c r="AD57" t="inlineStr"/>
-      <c r="AE57" t="inlineStr"/>
-      <c r="AF57" t="inlineStr"/>
-      <c r="AG57" t="inlineStr"/>
-      <c r="AH57" t="inlineStr"/>
-      <c r="AI57" t="inlineStr"/>
-      <c r="AJ57" t="inlineStr"/>
-      <c r="AK57" t="inlineStr"/>
-      <c r="AL57" t="inlineStr"/>
-      <c r="AM57" t="inlineStr"/>
-      <c r="AN57" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
admin crud, master crud
</commit_message>
<xml_diff>
--- a/Migrade_v.1.2/temp.xlsx
+++ b/Migrade_v.1.2/temp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN51"/>
+  <dimension ref="A1:AN57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -782,7 +782,7 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr">
         <is>
-          <t>2017 - 2018</t>
+          <t>2019 - 2020</t>
         </is>
       </c>
       <c r="T4" t="inlineStr"/>
@@ -791,7 +791,7 @@
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Grade </t>
+          <t xml:space="preserve">Grade Level </t>
         </is>
       </c>
       <c r="Y4" t="inlineStr"/>
@@ -799,7 +799,7 @@
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>Grade 5</t>
+          <t>Grade 6</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr"/>
@@ -813,7 +813,7 @@
       <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>EARTH</t>
+          <t>GALILEO</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr"/>
@@ -853,7 +853,7 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Age as of August 31st</t>
+          <t>AGE as of 1st Friday June</t>
         </is>
       </c>
       <c r="K5" t="inlineStr"/>
@@ -975,7 +975,7 @@
       <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mother's Maiden Name (Last Name, First Name, Middle </t>
+          <t>Mother's Maiden Name (Last Name, First Name, Middle Name)</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr"/>
@@ -1002,13 +1002,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>164512110014</t>
+          <t>164512130171</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>BORLAGDAN, ALFIE BISMAR</t>
+          <t>ANIBAN,LEO JELLY, TINAPAY</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -1021,13 +1021,13 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>05-18-2005</t>
+          <t>09-23-2008</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K7" t="inlineStr"/>
@@ -1069,7 +1069,7 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>BORLAGDAN, ALLAN GOLEMLEM</t>
+          <t>ANIBAN, LEO BUTAL</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr"/>
@@ -1077,7 +1077,7 @@
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>BISMAR,CARMENCITA,BLANQUEZA,</t>
+          <t>TINAPAY,JILL,BAJADI,</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr"/>
@@ -1092,13 +1092,13 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>164512130010</t>
+          <t>164512130045</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>BORLAGDAN, RJ BISMAR</t>
+          <t>ASILO,RAIN JUSTINE, MERCADO</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -1111,13 +1111,13 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>11-11-2006</t>
+          <t>05-20-2007</t>
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K8" t="inlineStr"/>
@@ -1136,7 +1136,7 @@
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R8" t="inlineStr"/>
@@ -1159,7 +1159,7 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>BORLAGDAN, ALLAN GOLEMLEM</t>
+          <t>ASILO, CHRISTOPHER SALILICAN</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr"/>
@@ -1167,7 +1167,7 @@
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>BISMAR,CARMENCITA,BLANQUEZA,</t>
+          <t>MERCADO,MARICEL,HERNANDEZ,</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr"/>
@@ -1182,13 +1182,13 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>136907120127</t>
+          <t>424663150037</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CAMBE, RALPH LOUIE ARAGON</t>
+          <t>CAMBE,SEAN DAVE, ARAGON</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -1201,13 +1201,13 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>03-02-2007</t>
+          <t>03-15-2008</t>
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K9" t="inlineStr"/>
@@ -1267,22 +1267,18 @@
       <c r="AK9" t="inlineStr"/>
       <c r="AL9" t="inlineStr"/>
       <c r="AM9" t="inlineStr"/>
-      <c r="AN9" t="inlineStr">
-        <is>
-          <t>T/I DATE:2017-06-05</t>
-        </is>
-      </c>
+      <c r="AN9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>164512130016</t>
+          <t>164512140032</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CAONES, JAYRUS CARL LACANIN</t>
+          <t>CARANAY,JHAYCEE CARL, CORDERO</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -1295,7 +1291,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>08-25-2006</t>
+          <t>11-25-2007</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
@@ -1343,7 +1339,7 @@
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>CAONES, JAYZON NUNAY</t>
+          <t>CARANAY, ROGELIO JR CABOTAJE</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr"/>
@@ -1351,7 +1347,7 @@
       <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="inlineStr">
         <is>
-          <t>LACANIN,JERLYN,BELO,</t>
+          <t>CORDERO,NORMA,ALIDO,</t>
         </is>
       </c>
       <c r="AG10" t="inlineStr"/>
@@ -1366,13 +1362,13 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>164512120011</t>
+          <t>164512140029</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CELESTE, ANDREW ACE ESPINOSA</t>
+          <t>CASTRO,ICHIRO, MENDOZA</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -1385,7 +1381,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>02-09-2007</t>
+          <t>09-08-2008</t>
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
@@ -1410,7 +1406,7 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>PLATERO</t>
         </is>
       </c>
       <c r="R11" t="inlineStr"/>
@@ -1433,7 +1429,7 @@
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>CELESTE, ALEJANDRO SARVIDA</t>
+          <t>CASTRO, SEVERLINO ABAPO</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr"/>
@@ -1441,7 +1437,7 @@
       <c r="AE11" t="inlineStr"/>
       <c r="AF11" t="inlineStr">
         <is>
-          <t>ESPINOSA,LORENA,ALBERTO,</t>
+          <t>MENDOZA,ALICIA,ZULUETA,</t>
         </is>
       </c>
       <c r="AG11" t="inlineStr"/>
@@ -1456,13 +1452,13 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>164512130047</t>
+          <t>164512150094</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CUPANG, CHRISTIAN ZAMORA</t>
+          <t>CAYLAO,DAYNE, VIÑA</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -1475,13 +1471,13 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>06-21-2007</t>
+          <t>03-17-2007</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K12" t="inlineStr"/>
@@ -1500,7 +1496,7 @@
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>PLATERO</t>
         </is>
       </c>
       <c r="R12" t="inlineStr"/>
@@ -1523,7 +1519,7 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>CUPANG, ANTONIO CRISMUNDO JR</t>
+          <t>CAYLAO, DANZEL CIPRIANO</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr"/>
@@ -1531,7 +1527,7 @@
       <c r="AE12" t="inlineStr"/>
       <c r="AF12" t="inlineStr">
         <is>
-          <t>ZAMORA,TERESITA,ALING,</t>
+          <t>VIÑA,CAREN,CRUZ,</t>
         </is>
       </c>
       <c r="AG12" t="inlineStr"/>
@@ -1546,13 +1542,13 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>108226120133</t>
+          <t>164512130131</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>GABATIN, KING TYRON GILBERT AMORTIZADO</t>
+          <t>CHAN,JHON RHAYNE, REPELAR</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -1565,13 +1561,13 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>11-10-2004</t>
+          <t>01-16-2008</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K13" t="inlineStr"/>
@@ -1613,7 +1609,7 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>GABATIN, TEOFILO TACSIAT</t>
+          <t>CHAN, JONATHAN ALICARTE</t>
         </is>
       </c>
       <c r="AC13" t="inlineStr"/>
@@ -1621,7 +1617,7 @@
       <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="inlineStr">
         <is>
-          <t>AMORTIZADO,MARIA LOURDES,CAPUQUIAN,</t>
+          <t>REPELAR,ELENA,ROXAS,</t>
         </is>
       </c>
       <c r="AG13" t="inlineStr"/>
@@ -1636,13 +1632,13 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>164512130022</t>
+          <t>402456150012</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>LAGADI, JHOSUA BUSTAMANTE</t>
+          <t>GETALADO,EARL SAMUEL, CLAVE</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -1655,7 +1651,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>11-08-2006</t>
+          <t>09-10-2008</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -1680,7 +1676,7 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R14" t="inlineStr"/>
@@ -1703,7 +1699,7 @@
       <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>LAGADI, VICENTE GABRIEL JR</t>
+          <t>GETALADO, ERNESTO CERTEZA</t>
         </is>
       </c>
       <c r="AC14" t="inlineStr"/>
@@ -1711,7 +1707,7 @@
       <c r="AE14" t="inlineStr"/>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>BUSTAMANTE,ELIZA,BULARON,</t>
+          <t>CLAVE,SERENIDAD,TABLIZO,</t>
         </is>
       </c>
       <c r="AG14" t="inlineStr"/>
@@ -1726,13 +1722,13 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>112505130003</t>
+          <t>164512130101</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LLANZA, ALFREDO LAYCO JR</t>
+          <t>GLOBIO,MARCKY, GALVAN</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -1745,13 +1741,13 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>09-28-2006</t>
+          <t>03-11-2008</t>
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
@@ -1770,7 +1766,7 @@
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>SANTO NINO</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R15" t="inlineStr"/>
@@ -1791,17 +1787,13 @@
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="inlineStr">
-        <is>
-          <t>LLANZA, ALFREDO CARGALLO SR</t>
-        </is>
-      </c>
+      <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="inlineStr"/>
       <c r="AD15" t="inlineStr"/>
       <c r="AE15" t="inlineStr"/>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>LAYCO,ARCELI,MONTANEZ,</t>
+          <t>GLOBIO,RENITA,GALVAN,</t>
         </is>
       </c>
       <c r="AG15" t="inlineStr"/>
@@ -1811,18 +1803,22 @@
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr"/>
       <c r="AM15" t="inlineStr"/>
-      <c r="AN15" t="inlineStr"/>
+      <c r="AN15" t="inlineStr">
+        <is>
+          <t>DRP "Family Problem"Date:2019/11/04</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>164512130024</t>
+          <t>164512140006</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MALINTAD, JAMES DUMAYO</t>
+          <t>MIRANDA,ANDREI, BIANES</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -1835,13 +1831,13 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>03-05-2007</t>
+          <t>04-29-2007</t>
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
@@ -1860,7 +1856,7 @@
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R16" t="inlineStr"/>
@@ -1883,7 +1879,7 @@
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>MALINTAD, GREMER CAONG</t>
+          <t>MIRANDA, ESTELITO VILLANUEVA</t>
         </is>
       </c>
       <c r="AC16" t="inlineStr"/>
@@ -1891,7 +1887,7 @@
       <c r="AE16" t="inlineStr"/>
       <c r="AF16" t="inlineStr">
         <is>
-          <t>DUMAYO,MINDA,TUMIMO,</t>
+          <t>BIANES,JENNIFER,QUINTUA,</t>
         </is>
       </c>
       <c r="AG16" t="inlineStr"/>
@@ -1901,18 +1897,22 @@
       <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="inlineStr"/>
-      <c r="AN16" t="inlineStr"/>
+      <c r="AN16" t="inlineStr">
+        <is>
+          <t>T/I Pook Elem. Sch. Date:2019-06-03</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>164512130027</t>
+          <t>164512130118</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MATULA, JOHN GABRIEL ZAVALLA</t>
+          <t>NAVAREZ,ANDREI, MONTAÑEZ</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -1925,13 +1925,13 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>09-25-2006</t>
+          <t>07-26-2007</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K17" t="inlineStr"/>
@@ -1973,7 +1973,7 @@
       <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>MATULA, VICTOR GONZALES</t>
+          <t>NAVAREZ, ARNEL NABUHAY</t>
         </is>
       </c>
       <c r="AC17" t="inlineStr"/>
@@ -1981,7 +1981,7 @@
       <c r="AE17" t="inlineStr"/>
       <c r="AF17" t="inlineStr">
         <is>
-          <t>ZAVALLA,FLORENCIA,NILLO,</t>
+          <t>MONTAÑEZ,SUSANA,VILLARIN,</t>
         </is>
       </c>
       <c r="AG17" t="inlineStr"/>
@@ -1996,13 +1996,13 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>164512120051</t>
+          <t>164512100132</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>OLIVEROS, JHONUEL BISMAR</t>
+          <t>SALAYSAY,JOHN LOUIE, FLORES</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -2015,13 +2015,13 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>01-16-2007</t>
+          <t>02-18-2004</t>
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">15 </t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
@@ -2063,7 +2063,7 @@
       <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>OLIVEROS, JOEL AFANTE</t>
+          <t>SALAYSAY, ALFREDO REYES</t>
         </is>
       </c>
       <c r="AC18" t="inlineStr"/>
@@ -2071,7 +2071,7 @@
       <c r="AE18" t="inlineStr"/>
       <c r="AF18" t="inlineStr">
         <is>
-          <t>BLANQUEZA,JANET,BISMAR,</t>
+          <t>FLORES,CECILIA,LOPENA,</t>
         </is>
       </c>
       <c r="AG18" t="inlineStr"/>
@@ -2086,13 +2086,13 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>108474140114</t>
+          <t>108476120166</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>QUILLOSA, MERICK MASAREDO</t>
+          <t>SAMANIEGO,MATTHEW ANDREI, ANGULO</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
@@ -2105,13 +2105,13 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>10-04-2006</t>
+          <t>08-01-2006</t>
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
@@ -2130,7 +2130,7 @@
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R19" t="inlineStr"/>
@@ -2153,7 +2153,7 @@
       <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>QUILLOSA, MARVIN MANLOLO</t>
+          <t>SAMANIEGO, MICHAEL ABUCEJO</t>
         </is>
       </c>
       <c r="AC19" t="inlineStr"/>
@@ -2161,7 +2161,7 @@
       <c r="AE19" t="inlineStr"/>
       <c r="AF19" t="inlineStr">
         <is>
-          <t>MASAREDO,PERLA,ACOSTA,</t>
+          <t>ANGULO,ABIGAIL,GUSTILO,</t>
         </is>
       </c>
       <c r="AG19" t="inlineStr"/>
@@ -2176,13 +2176,13 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>164512130030</t>
+          <t>108426130045</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>SANGYAHON, JUSTINE MAGTAGAD</t>
+          <t>SAN JUAN JR.,ARLY, PLATINO</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
@@ -2195,13 +2195,13 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>09-22-2006</t>
+          <t>09-29-2007</t>
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K20" t="inlineStr"/>
@@ -2243,7 +2243,7 @@
       <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>SANGYAHON, ERLINDO PATRICIO</t>
+          <t>SAN JUAN, ARLY TAPUIC SR</t>
         </is>
       </c>
       <c r="AC20" t="inlineStr"/>
@@ -2251,7 +2251,7 @@
       <c r="AE20" t="inlineStr"/>
       <c r="AF20" t="inlineStr">
         <is>
-          <t>MAGTAGAD,CHERYL,ESPAÑOLA,</t>
+          <t>PLATINO,EVANGELINE,GUILLEN,</t>
         </is>
       </c>
       <c r="AG20" t="inlineStr"/>
@@ -2266,13 +2266,13 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>136775120015</t>
+          <t>164512130091</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
-          <t>SANTOS, ANGELO GALLARDO</t>
+          <t>SANTOS,MARK, BELANO</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>05-15-2007</t>
+          <t>09-05-2008</t>
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
@@ -2333,7 +2333,7 @@
       <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>SANTOS, ARTURO CRUZ</t>
+          <t>SANTOS, ROLANDO BARBOSA</t>
         </is>
       </c>
       <c r="AC21" t="inlineStr"/>
@@ -2341,7 +2341,7 @@
       <c r="AE21" t="inlineStr"/>
       <c r="AF21" t="inlineStr">
         <is>
-          <t>UMALI,GALLARDO,GUADALUPE,</t>
+          <t>BELANO,LIZA,BERIANO,</t>
         </is>
       </c>
       <c r="AG21" t="inlineStr"/>
@@ -2351,22 +2351,18 @@
       <c r="AK21" t="inlineStr"/>
       <c r="AL21" t="inlineStr"/>
       <c r="AM21" t="inlineStr"/>
-      <c r="AN21" t="inlineStr">
-        <is>
-          <t>Pending TI</t>
-        </is>
-      </c>
+      <c r="AN21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>164512120054</t>
+          <t>164512140037</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
-          <t>TABING, RANDEL ABELLA</t>
+          <t>VILLANUEVA,JOSH CYREL, CLASA</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
@@ -2379,13 +2375,13 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>06-16-2007</t>
+          <t>11-09-2007</t>
         </is>
       </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
@@ -2427,7 +2423,7 @@
       <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>TABING, RANDY ESTEBAN</t>
+          <t>VILLANUEVA, PABLITO MARIÑAS</t>
         </is>
       </c>
       <c r="AC22" t="inlineStr"/>
@@ -2435,7 +2431,7 @@
       <c r="AE22" t="inlineStr"/>
       <c r="AF22" t="inlineStr">
         <is>
-          <t>ABELLA,MARIDEL,ENCELAN,</t>
+          <t>CLASA,EVEBERLY,MONTESCO,</t>
         </is>
       </c>
       <c r="AG22" t="inlineStr"/>
@@ -2448,86 +2444,44 @@
       <c r="AN22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>164512120055</t>
-        </is>
+      <c r="A23" t="n">
+        <v>16</v>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
-          <t>VALENCIA, RIN WINZHEL AGUADO</t>
+          <t>&lt;=== TOTAL MALE</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>01-09-2007</t>
-        </is>
-      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">10 </t>
-        </is>
-      </c>
+      <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>Tagalog</t>
-        </is>
-      </c>
+      <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>Christianity</t>
-        </is>
-      </c>
+      <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>ZAPOTE</t>
-        </is>
-      </c>
+      <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>CITY OF BIÑAN</t>
-        </is>
-      </c>
+      <c r="U23" t="inlineStr"/>
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr"/>
-      <c r="X23" t="inlineStr">
-        <is>
-          <t>LAGUNA</t>
-        </is>
-      </c>
+      <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="inlineStr"/>
-      <c r="AB23" t="inlineStr">
-        <is>
-          <t>VALENCIA, CHERWEN MANONGSONG</t>
-        </is>
-      </c>
+      <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="inlineStr"/>
       <c r="AD23" t="inlineStr"/>
       <c r="AE23" t="inlineStr"/>
-      <c r="AF23" t="inlineStr">
-        <is>
-          <t>AGUADO,FRITCHEL,VICTORIO,</t>
-        </is>
-      </c>
+      <c r="AF23" t="inlineStr"/>
       <c r="AG23" t="inlineStr"/>
       <c r="AH23" t="inlineStr"/>
       <c r="AI23" t="inlineStr"/>
@@ -2538,44 +2492,86 @@
       <c r="AN23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>17</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>164512140038</t>
+        </is>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
-          <t>&lt;=== TOTAL MALE</t>
+          <t>ARRESGADO,LEANNE ROSE, CARLOS</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>08-25-2008</t>
+        </is>
+      </c>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr"/>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr"/>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr"/>
-      <c r="X24" t="inlineStr"/>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="inlineStr"/>
-      <c r="AB24" t="inlineStr"/>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>ARRESGADO, JUNARD MALAKARTE</t>
+        </is>
+      </c>
       <c r="AC24" t="inlineStr"/>
       <c r="AD24" t="inlineStr"/>
       <c r="AE24" t="inlineStr"/>
-      <c r="AF24" t="inlineStr"/>
+      <c r="AF24" t="inlineStr">
+        <is>
+          <t>CARLOS,AILEEN,VERANO,</t>
+        </is>
+      </c>
       <c r="AG24" t="inlineStr"/>
       <c r="AH24" t="inlineStr"/>
       <c r="AI24" t="inlineStr"/>
@@ -2588,13 +2584,13 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>164512130075</t>
+          <t>164512140016</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ACILO, CHARLENE DAGUMAN</t>
+          <t>BORCELANGO,DONA LYNN, DAPRINAL</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -2607,7 +2603,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>10-18-2006</t>
+          <t>07-22-2008</t>
         </is>
       </c>
       <c r="I25" t="inlineStr"/>
@@ -2655,7 +2651,7 @@
       <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>ACILO, CHARLITO LOPENA</t>
+          <t>BORCELANGO, DONATO REYES</t>
         </is>
       </c>
       <c r="AC25" t="inlineStr"/>
@@ -2663,7 +2659,7 @@
       <c r="AE25" t="inlineStr"/>
       <c r="AF25" t="inlineStr">
         <is>
-          <t>DAGUMAN,AILENE,ABE,</t>
+          <t>DAPRINAL,JONALINE,ATOR,</t>
         </is>
       </c>
       <c r="AG25" t="inlineStr"/>
@@ -2678,13 +2674,13 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>164512130061</t>
+          <t>164512140017</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
-          <t>BETITO, EURICE ROSACEÑA</t>
+          <t>CAONES,JUSEA MICAH, LACANIN</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
@@ -2697,13 +2693,13 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>05-03-2007</t>
+          <t>01-31-2008</t>
         </is>
       </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K26" t="inlineStr"/>
@@ -2745,7 +2741,7 @@
       <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="inlineStr">
         <is>
-          <t>BETITO, ARMANDO SALAMODING</t>
+          <t>CAONES, JAYZON NUNAY</t>
         </is>
       </c>
       <c r="AC26" t="inlineStr"/>
@@ -2753,7 +2749,7 @@
       <c r="AE26" t="inlineStr"/>
       <c r="AF26" t="inlineStr">
         <is>
-          <t>ROSACENA,REMEDIOS,VILLANUEVA,</t>
+          <t>LACANIN,JERLYN,BELO,</t>
         </is>
       </c>
       <c r="AG26" t="inlineStr"/>
@@ -2768,13 +2764,13 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>164512120064</t>
+          <t>105111130128</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CAFINO, JASMIN CLAIRE CANTIGA</t>
+          <t>CLEMENTE,MARTHA ASHLEE, COLIS</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -2787,7 +2783,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>03-06-2007</t>
+          <t>07-02-2008</t>
         </is>
       </c>
       <c r="I27" t="inlineStr"/>
@@ -2812,7 +2808,7 @@
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R27" t="inlineStr"/>
@@ -2835,7 +2831,7 @@
       <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="inlineStr">
         <is>
-          <t>CAFINO, RODERICK SOREÑO</t>
+          <t>CLEMENTE, RAFAEL KRIS PRONUEVO CLEMENTE</t>
         </is>
       </c>
       <c r="AC27" t="inlineStr"/>
@@ -2843,7 +2839,7 @@
       <c r="AE27" t="inlineStr"/>
       <c r="AF27" t="inlineStr">
         <is>
-          <t>CANTIGA,GRACE,IGNACIO,</t>
+          <t>COLIS,MA NIEVES VALANTINE,CUNANAN,</t>
         </is>
       </c>
       <c r="AG27" t="inlineStr"/>
@@ -2853,18 +2849,22 @@
       <c r="AK27" t="inlineStr"/>
       <c r="AL27" t="inlineStr"/>
       <c r="AM27" t="inlineStr"/>
-      <c r="AN27" t="inlineStr"/>
+      <c r="AN27" t="inlineStr">
+        <is>
+          <t>T/I  San Miguel Elem.Sch.Date:2019-06-03</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>164512120218</t>
+          <t>109850130028</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CLARION, MARY QUEEN MARIEL RAMISO</t>
+          <t>DEL MUNDO,CATHLYN, SALDINO</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
@@ -2877,13 +2877,13 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>10-01-2006</t>
+          <t>11-22-2007</t>
         </is>
       </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K28" t="inlineStr"/>
@@ -2902,7 +2902,7 @@
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R28" t="inlineStr"/>
@@ -2925,7 +2925,7 @@
       <c r="AA28" t="inlineStr"/>
       <c r="AB28" t="inlineStr">
         <is>
-          <t>CLARION, MARCIAL GARRAN</t>
+          <t>DEL MUNDO, JUNE LINGGA</t>
         </is>
       </c>
       <c r="AC28" t="inlineStr"/>
@@ -2933,7 +2933,7 @@
       <c r="AE28" t="inlineStr"/>
       <c r="AF28" t="inlineStr">
         <is>
-          <t>RAMISO,LIEZEL,SIMPO,</t>
+          <t>SALDINO,ANNABELLE,SOLAYAO,</t>
         </is>
       </c>
       <c r="AG28" t="inlineStr"/>
@@ -2948,13 +2948,13 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>164512130029</t>
+          <t>164512130166</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>DIONISO, JHAMAICA ALEGRE</t>
+          <t>DICDICAN,TRISHA ELLAINE, REALON</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>10-25-2005</t>
+          <t>03-01-2008</t>
         </is>
       </c>
       <c r="I29" t="inlineStr"/>
@@ -2992,7 +2992,7 @@
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R29" t="inlineStr"/>
@@ -3015,7 +3015,7 @@
       <c r="AA29" t="inlineStr"/>
       <c r="AB29" t="inlineStr">
         <is>
-          <t>DIONISIO, ROEL CRUZ</t>
+          <t>DICDICAN, RICHARD JIMENEZ</t>
         </is>
       </c>
       <c r="AC29" t="inlineStr"/>
@@ -3023,7 +3023,7 @@
       <c r="AE29" t="inlineStr"/>
       <c r="AF29" t="inlineStr">
         <is>
-          <t>ALEGRE,SHIELA,SAHIRON,</t>
+          <t>REALON,MA CLARISSA,ROLDAN,</t>
         </is>
       </c>
       <c r="AG29" t="inlineStr"/>
@@ -3038,13 +3038,13 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>164512120071</t>
+          <t>164512130124</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ESPINOSA, MIAH JUMAO-AS</t>
+          <t>ESPINAR,ANGIELYN, MARCE</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>12-13-2006</t>
+          <t>07-26-2008</t>
         </is>
       </c>
       <c r="I30" t="inlineStr"/>
@@ -3082,7 +3082,7 @@
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO NINO</t>
         </is>
       </c>
       <c r="R30" t="inlineStr"/>
@@ -3105,7 +3105,7 @@
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr">
         <is>
-          <t>ESPINOSA, BONIFACIO ALVERIO</t>
+          <t>ESPINAR, EDISON FLORALDE</t>
         </is>
       </c>
       <c r="AC30" t="inlineStr"/>
@@ -3113,7 +3113,7 @@
       <c r="AE30" t="inlineStr"/>
       <c r="AF30" t="inlineStr">
         <is>
-          <t>JUMAO-AS,CECILIA,MABATID,</t>
+          <t>MARCE,MARIE GRACE,MONTAÑEZ,</t>
         </is>
       </c>
       <c r="AG30" t="inlineStr"/>
@@ -3128,13 +3128,13 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>164512120033</t>
+          <t>108226120096</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>GABUTAN, ANGIE GOLLAYAN</t>
+          <t>GABATIN,LADY TRISHA, AMORTIZADO</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
@@ -3147,13 +3147,13 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>08-06-2006</t>
+          <t>11-03-2006</t>
         </is>
       </c>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
@@ -3195,7 +3195,7 @@
       <c r="AA31" t="inlineStr"/>
       <c r="AB31" t="inlineStr">
         <is>
-          <t>GABUTAN, ALVE SUMARGO</t>
+          <t>GABATIN, TEOFILO TACSIAT</t>
         </is>
       </c>
       <c r="AC31" t="inlineStr"/>
@@ -3203,7 +3203,7 @@
       <c r="AE31" t="inlineStr"/>
       <c r="AF31" t="inlineStr">
         <is>
-          <t>GOLLAYAN,MARITES,BLANZA,</t>
+          <t>AMORTIZADO,MARIA LOURDES,CAPUQUIAN,</t>
         </is>
       </c>
       <c r="AG31" t="inlineStr"/>
@@ -3218,13 +3218,13 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>164512110030</t>
+          <t>164512130042</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
-          <t>GONZALO, ERICQUEZEN DACASIN</t>
+          <t>JOVEN,JENALEN, MASIKAT</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
@@ -3237,13 +3237,13 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>12-07-2005</t>
+          <t>10-01-2006</t>
         </is>
       </c>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
@@ -3285,7 +3285,7 @@
       <c r="AA32" t="inlineStr"/>
       <c r="AB32" t="inlineStr">
         <is>
-          <t>GONZALO, ERIC TORIO</t>
+          <t>JOVEN, SAMUEL ARCEGA</t>
         </is>
       </c>
       <c r="AC32" t="inlineStr"/>
@@ -3293,7 +3293,7 @@
       <c r="AE32" t="inlineStr"/>
       <c r="AF32" t="inlineStr">
         <is>
-          <t>DACASIN,HEIDE,VERGARA,</t>
+          <t>MASIKAT,CRISTINA,BAYAN,</t>
         </is>
       </c>
       <c r="AG32" t="inlineStr"/>
@@ -3308,13 +3308,13 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>164512130062</t>
+          <t>108407130083</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>HUTALLA, RHIAM CLARIS ESPINOSA</t>
+          <t>MALABAG,ANGELICA, MIRANDA</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
@@ -3327,13 +3327,13 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>01-04-2007</t>
+          <t>12-22-2007</t>
         </is>
       </c>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
@@ -3375,7 +3375,7 @@
       <c r="AA33" t="inlineStr"/>
       <c r="AB33" t="inlineStr">
         <is>
-          <t>HUTALLA, CLARO GONZALES</t>
+          <t>MALABAG, ANGELITO MELICIO</t>
         </is>
       </c>
       <c r="AC33" t="inlineStr"/>
@@ -3383,7 +3383,7 @@
       <c r="AE33" t="inlineStr"/>
       <c r="AF33" t="inlineStr">
         <is>
-          <t>ESPINOSA,MIRIAM,ALMEDA,</t>
+          <t>MIRANDA,MARY ANN,BAYANID,</t>
         </is>
       </c>
       <c r="AG33" t="inlineStr"/>
@@ -3398,13 +3398,13 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>164512130032</t>
+          <t>164512140043</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LLANZA, RUTH MICAH CORPUZ</t>
+          <t>MAMANSAG,JEIAH EUNICE, SERRANO</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>11-24-2006</t>
+          <t>08-09-2008</t>
         </is>
       </c>
       <c r="I34" t="inlineStr"/>
@@ -3442,7 +3442,7 @@
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R34" t="inlineStr"/>
@@ -3465,7 +3465,7 @@
       <c r="AA34" t="inlineStr"/>
       <c r="AB34" t="inlineStr">
         <is>
-          <t>LLANZA, JOSEPH GUEVARRA</t>
+          <t>MAMANSAG, EMMERSON SALCEDO</t>
         </is>
       </c>
       <c r="AC34" t="inlineStr"/>
@@ -3473,7 +3473,7 @@
       <c r="AE34" t="inlineStr"/>
       <c r="AF34" t="inlineStr">
         <is>
-          <t>CORPUZ,CLARISA,BARONIA,</t>
+          <t>SERRANO,GERLIE,VALCOBA,</t>
         </is>
       </c>
       <c r="AG34" t="inlineStr"/>
@@ -3488,13 +3488,13 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>164512130036</t>
+          <t>424638150057</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MACARAIG, MARICRIS SABADO</t>
+          <t>MANALILI,JAMAICA AMOR, ROSALES</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
@@ -3507,13 +3507,13 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>10-16-2007</t>
+          <t>01-21-2008</t>
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr">
         <is>
-          <t xml:space="preserve">9 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
@@ -3532,7 +3532,7 @@
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R35" t="inlineStr"/>
@@ -3555,7 +3555,7 @@
       <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="inlineStr">
         <is>
-          <t>MACARAIG, EDWIN GARCIA</t>
+          <t>MANALILI, JAM ANTHONY CASTILLO</t>
         </is>
       </c>
       <c r="AC35" t="inlineStr"/>
@@ -3563,7 +3563,7 @@
       <c r="AE35" t="inlineStr"/>
       <c r="AF35" t="inlineStr">
         <is>
-          <t>SABADO,MARIA,SARSOZA,</t>
+          <t>ROSALES,RACHEL,MALIBAGO,</t>
         </is>
       </c>
       <c r="AG35" t="inlineStr"/>
@@ -3578,13 +3578,13 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>108231130020</t>
+          <t>164512130089</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MARAÑAN, JERAMIAH ALAHAY</t>
+          <t>MARTINEZ,ASHLEE NICHOLE, SABANAL</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>10-01-2006</t>
+          <t>11-16-2008</t>
         </is>
       </c>
       <c r="I36" t="inlineStr"/>
@@ -3622,7 +3622,7 @@
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R36" t="inlineStr"/>
@@ -3645,7 +3645,7 @@
       <c r="AA36" t="inlineStr"/>
       <c r="AB36" t="inlineStr">
         <is>
-          <t>MARAÑAN, RONNIE CUEME</t>
+          <t>MARTINEZ, MAR JUN BRUCE</t>
         </is>
       </c>
       <c r="AC36" t="inlineStr"/>
@@ -3653,7 +3653,7 @@
       <c r="AE36" t="inlineStr"/>
       <c r="AF36" t="inlineStr">
         <is>
-          <t>TATA,ALAHAY,JOSEPHINE,</t>
+          <t>SABANAL,DESARIE,ALORA,</t>
         </is>
       </c>
       <c r="AG36" t="inlineStr"/>
@@ -3663,22 +3663,18 @@
       <c r="AK36" t="inlineStr"/>
       <c r="AL36" t="inlineStr"/>
       <c r="AM36" t="inlineStr"/>
-      <c r="AN36" t="inlineStr">
-        <is>
-          <t>T/I DATE:2017-06-05</t>
-        </is>
-      </c>
+      <c r="AN36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>164512130037</t>
+          <t>164512140024</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>NAVAL, KRISHA MAY MIRANDA</t>
+          <t>NAVAL,GEARLY SHANE, OCAMPO</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
@@ -3691,13 +3687,13 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>06-01-2007</t>
+          <t>11-03-2007</t>
         </is>
       </c>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
@@ -3739,7 +3735,7 @@
       <c r="AA37" t="inlineStr"/>
       <c r="AB37" t="inlineStr">
         <is>
-          <t>NAVAL, TIBURCIO ALIAS</t>
+          <t>NAVAL, PERFECTO LINGGO</t>
         </is>
       </c>
       <c r="AC37" t="inlineStr"/>
@@ -3747,7 +3743,7 @@
       <c r="AE37" t="inlineStr"/>
       <c r="AF37" t="inlineStr">
         <is>
-          <t>MIRANDA,ERLINDA,RAMOS,</t>
+          <t>ILAITIA,MELANIE,OCAMPO,</t>
         </is>
       </c>
       <c r="AG37" t="inlineStr"/>
@@ -3762,13 +3758,13 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>164512130064</t>
+          <t>164512130194</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
-          <t>NAVAL, ZYDNEY RONQUEZ</t>
+          <t>OLAVARIO,ALLIYAH LORRAINE, GUILLERMO</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
@@ -3781,13 +3777,13 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>11-02-2006</t>
+          <t>07-23-2007</t>
         </is>
       </c>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
@@ -3829,7 +3825,7 @@
       <c r="AA38" t="inlineStr"/>
       <c r="AB38" t="inlineStr">
         <is>
-          <t>NAVAL, FERDINAND DIAGO</t>
+          <t>OLAVARIO, TEODULO NUELAN</t>
         </is>
       </c>
       <c r="AC38" t="inlineStr"/>
@@ -3837,7 +3833,7 @@
       <c r="AE38" t="inlineStr"/>
       <c r="AF38" t="inlineStr">
         <is>
-          <t>RONQUEZ,RIO,CAMACHO,</t>
+          <t>GUILLERMO,IRENE,LIMBAG,</t>
         </is>
       </c>
       <c r="AG38" t="inlineStr"/>
@@ -3852,13 +3848,13 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>164512130038</t>
+          <t>108224130152</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr">
         <is>
-          <t>NAVARRO, ELYZA MAE BERMEJO</t>
+          <t>PUNZALAN,CHANELLE, POSO</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
@@ -3871,7 +3867,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>02-08-2007</t>
+          <t>08-03-2008</t>
         </is>
       </c>
       <c r="I39" t="inlineStr"/>
@@ -3896,7 +3892,7 @@
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R39" t="inlineStr"/>
@@ -3919,7 +3915,7 @@
       <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="inlineStr">
         <is>
-          <t>NAVARRO, RAYMUNDO HALLEGADO</t>
+          <t>PUNZALAN, RAYMOND LISMORAS</t>
         </is>
       </c>
       <c r="AC39" t="inlineStr"/>
@@ -3927,7 +3923,7 @@
       <c r="AE39" t="inlineStr"/>
       <c r="AF39" t="inlineStr">
         <is>
-          <t>BERMEJO,GERALDINE,BERNABE,</t>
+          <t>POSO,CHONA,RAMIREZ,</t>
         </is>
       </c>
       <c r="AG39" t="inlineStr"/>
@@ -3942,13 +3938,13 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>164512130068</t>
+          <t>136908131369</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>PONTIGON, PATRICIA JOY ENCISO</t>
+          <t>ROTUBIO,ALLIANA JALYN, BERONDO</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
@@ -3961,7 +3957,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>11-19-2006</t>
+          <t>07-03-2008</t>
         </is>
       </c>
       <c r="I40" t="inlineStr"/>
@@ -3986,7 +3982,7 @@
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R40" t="inlineStr"/>
@@ -4009,7 +4005,7 @@
       <c r="AA40" t="inlineStr"/>
       <c r="AB40" t="inlineStr">
         <is>
-          <t>PONTIGON, JAIME DATUON</t>
+          <t>ROTUBIO, JAY TOLEDO</t>
         </is>
       </c>
       <c r="AC40" t="inlineStr"/>
@@ -4017,7 +4013,7 @@
       <c r="AE40" t="inlineStr"/>
       <c r="AF40" t="inlineStr">
         <is>
-          <t>ENCISO,JOSEPHINE,MAKATINGRAO,</t>
+          <t>BERONDO,NORMALYN,CORDERO,</t>
         </is>
       </c>
       <c r="AG40" t="inlineStr"/>
@@ -4027,18 +4023,22 @@
       <c r="AK40" t="inlineStr"/>
       <c r="AL40" t="inlineStr"/>
       <c r="AM40" t="inlineStr"/>
-      <c r="AN40" t="inlineStr"/>
+      <c r="AN40" t="inlineStr">
+        <is>
+          <t>T/I Southville IV Elem. Sch.Date:2019-09-02</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>111821090138</t>
+          <t>164512130168</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>RAMIREZ, ELIZA CHRISTINE CARREON</t>
+          <t>SUZON,RYGIN LOVE, GIMENTIZA</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
@@ -4051,13 +4051,13 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>10-10-2003</t>
+          <t>05-20-2008</t>
         </is>
       </c>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr">
         <is>
-          <t xml:space="preserve">13 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
@@ -4076,7 +4076,7 @@
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R41" t="inlineStr"/>
@@ -4099,7 +4099,7 @@
       <c r="AA41" t="inlineStr"/>
       <c r="AB41" t="inlineStr">
         <is>
-          <t>RAMIREZ, ERWIN TORARBA</t>
+          <t>SUZON, GERRY BERCERO</t>
         </is>
       </c>
       <c r="AC41" t="inlineStr"/>
@@ -4107,7 +4107,7 @@
       <c r="AE41" t="inlineStr"/>
       <c r="AF41" t="inlineStr">
         <is>
-          <t>CARREON,NELIA,SARMIENTO,</t>
+          <t>GIMENTIZA,GINA,TUICO,</t>
         </is>
       </c>
       <c r="AG41" t="inlineStr"/>
@@ -4117,22 +4117,18 @@
       <c r="AK41" t="inlineStr"/>
       <c r="AL41" t="inlineStr"/>
       <c r="AM41" t="inlineStr"/>
-      <c r="AN41" t="inlineStr">
-        <is>
-          <t>T/I DATE:2017-06-05</t>
-        </is>
-      </c>
+      <c r="AN41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>164512130040</t>
+          <t>107937130338</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>RIVERA, ANGELINA ELAINE MIRANDA</t>
+          <t>TAVU,RENY DENIEZE, RAMOS</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
@@ -4145,13 +4141,13 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>05-02-2007</t>
+          <t>02-24-2008</t>
         </is>
       </c>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
@@ -4170,7 +4166,7 @@
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R42" t="inlineStr"/>
@@ -4193,7 +4189,7 @@
       <c r="AA42" t="inlineStr"/>
       <c r="AB42" t="inlineStr">
         <is>
-          <t>RIVERA, FERDINAND VILLANUEVA</t>
+          <t>TAVU, RENY RAYMOND VEGA</t>
         </is>
       </c>
       <c r="AC42" t="inlineStr"/>
@@ -4201,7 +4197,7 @@
       <c r="AE42" t="inlineStr"/>
       <c r="AF42" t="inlineStr">
         <is>
-          <t>MIRANDA,SHEILA ROSE,BAYANID,</t>
+          <t>RAMOS,ADELAIDA,SANCHEZ,</t>
         </is>
       </c>
       <c r="AG42" t="inlineStr"/>
@@ -4214,44 +4210,86 @@
       <c r="AN42" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>18</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>164512130105</t>
+        </is>
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>&lt;=== TOTAL FEMALE</t>
+          <t>VARGAS,REIGN BEYONCE, GUILLERMO</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>11-03-2007</t>
+        </is>
+      </c>
       <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr"/>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr"/>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P43" t="inlineStr"/>
-      <c r="Q43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr"/>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr"/>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V43" t="inlineStr"/>
       <c r="W43" t="inlineStr"/>
-      <c r="X43" t="inlineStr"/>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y43" t="inlineStr"/>
       <c r="Z43" t="inlineStr"/>
       <c r="AA43" t="inlineStr"/>
-      <c r="AB43" t="inlineStr"/>
+      <c r="AB43" t="inlineStr">
+        <is>
+          <t>VARGAS, JUSSELLE SARMIENTO</t>
+        </is>
+      </c>
       <c r="AC43" t="inlineStr"/>
       <c r="AD43" t="inlineStr"/>
       <c r="AE43" t="inlineStr"/>
-      <c r="AF43" t="inlineStr"/>
+      <c r="AF43" t="inlineStr">
+        <is>
+          <t>GUILLERMO,ADEL,LIMBAG,</t>
+        </is>
+      </c>
       <c r="AG43" t="inlineStr"/>
       <c r="AH43" t="inlineStr"/>
       <c r="AI43" t="inlineStr"/>
@@ -4263,12 +4301,12 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>&lt;=== COMBINED</t>
+          <t>&lt;=== TOTAL FEMALE</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
@@ -4310,13 +4348,15 @@
       <c r="AN44" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>List and Code of Indicators under REMARKS column</t>
-        </is>
+      <c r="A45" t="n">
+        <v>36</v>
       </c>
       <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr"/>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>&lt;=== COMBINED</t>
+        </is>
+      </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
@@ -4358,42 +4398,22 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Indicator</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Code</t>
-        </is>
-      </c>
+          <t>List and Code of Indicators under REMARKS column</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Required Information</t>
-        </is>
-      </c>
+      <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>Indicator</t>
-        </is>
-      </c>
+      <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>Code</t>
-        </is>
-      </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>Required Information</t>
-        </is>
-      </c>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
@@ -4401,41 +4421,21 @@
       <c r="S46" t="inlineStr"/>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr"/>
-      <c r="V46" t="inlineStr">
-        <is>
-          <t>REGISTERED</t>
-        </is>
-      </c>
+      <c r="V46" t="inlineStr"/>
       <c r="W46" t="inlineStr"/>
       <c r="X46" t="inlineStr"/>
-      <c r="Y46" t="inlineStr">
-        <is>
-          <t>BoSY</t>
-        </is>
-      </c>
-      <c r="Z46" t="inlineStr">
-        <is>
-          <t>EoSY</t>
-        </is>
-      </c>
+      <c r="Y46" t="inlineStr"/>
+      <c r="Z46" t="inlineStr"/>
       <c r="AA46" t="inlineStr"/>
       <c r="AB46" t="inlineStr"/>
       <c r="AC46" t="inlineStr"/>
-      <c r="AD46" t="inlineStr">
-        <is>
-          <t>Prepared by;</t>
-        </is>
-      </c>
+      <c r="AD46" t="inlineStr"/>
       <c r="AE46" t="inlineStr"/>
       <c r="AF46" t="inlineStr"/>
       <c r="AG46" t="inlineStr"/>
       <c r="AH46" t="inlineStr"/>
       <c r="AI46" t="inlineStr"/>
-      <c r="AJ46" t="inlineStr">
-        <is>
-          <t>Certified Correct:</t>
-        </is>
-      </c>
+      <c r="AJ46" t="inlineStr"/>
       <c r="AK46" t="inlineStr"/>
       <c r="AL46" t="inlineStr"/>
       <c r="AM46" t="inlineStr"/>
@@ -4444,27 +4444,18 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Transfered Out
-Transfered In
-Dropped
-</t>
+          <t>Indicator</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>T/O
-T/I
-DRP
-LE</t>
+          <t>Code</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Name of  Public (P) Private (PR) School  &amp; Effectivity Date
-Name of  Public (P) Private (PR) School  &amp; Effectivity Date
-Reason  and Effectivity Date
-Reason (Enrollment beyond 1st Friday of </t>
+          <t>Required Information</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -4473,10 +4464,7 @@
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr">
         <is>
-          <t>CCT Receipient
-Balik Aral
-Learner With Disability
-Accelerated</t>
+          <t>Indicator</t>
         </is>
       </c>
       <c r="J47" t="inlineStr"/>
@@ -4484,18 +4472,12 @@
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr">
         <is>
-          <t>CCT
-B/A
-LWD
-ACL</t>
+          <t>Code</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>CCT Control/reference number &amp; Effectivity Date
-Name of school last attended &amp; Year
-Specify
-Specify Level &amp; Effectivity Data</t>
+          <t>Required Information</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
@@ -4507,23 +4489,27 @@
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr">
         <is>
-          <t>MALE</t>
+          <t>REGISTERED</t>
         </is>
       </c>
       <c r="W47" t="inlineStr"/>
       <c r="X47" t="inlineStr"/>
       <c r="Y47" t="inlineStr">
         <is>
-          <t xml:space="preserve">17 </t>
-        </is>
-      </c>
-      <c r="Z47" t="inlineStr"/>
+          <t>BoSY</t>
+        </is>
+      </c>
+      <c r="Z47" t="inlineStr">
+        <is>
+          <t>EoSY</t>
+        </is>
+      </c>
       <c r="AA47" t="inlineStr"/>
       <c r="AB47" t="inlineStr"/>
       <c r="AC47" t="inlineStr"/>
       <c r="AD47" t="inlineStr">
         <is>
-          <t>LAMBERTO BOLIMA RIVAREZ</t>
+          <t>Prepared by;</t>
         </is>
       </c>
       <c r="AE47" t="inlineStr"/>
@@ -4533,7 +4519,7 @@
       <c r="AI47" t="inlineStr"/>
       <c r="AJ47" t="inlineStr">
         <is>
-          <t>ELSA MONTERERO MANALO</t>
+          <t>Certified Correct:</t>
         </is>
       </c>
       <c r="AK47" t="inlineStr"/>
@@ -4542,20 +4528,62 @@
       <c r="AN47" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr"/>
-      <c r="B48" t="inlineStr"/>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Transfered Out
+Transfered In
+Dropped
+Late Enrollment</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>T/O
+T/I
+DRP
+LE</t>
+        </is>
+      </c>
       <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Name of  Public (P) Private (PR) School  &amp; Effectivity Date
+Name of  Public (P) Private (PR) School  &amp; Effectivity Date
+Reason  and Effectivity Date
+Reason (Enrollment beyond 1st Friday of June)</t>
+        </is>
+      </c>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr"/>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>CCT Receipient
+Balik Aral
+Learner With Disability
+Accelerated</t>
+        </is>
+      </c>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>CCT
+B/A
+LWD
+ACL</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>CCT Control/reference number &amp; Effectivity Date
+Name of school last attended &amp; Year
+Specify
+Specify Level &amp; Effectivity Data</t>
+        </is>
+      </c>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
@@ -4565,19 +4593,23 @@
       <c r="U48" t="inlineStr"/>
       <c r="V48" t="inlineStr">
         <is>
-          <t>FEMALE</t>
+          <t>MALE</t>
         </is>
       </c>
       <c r="W48" t="inlineStr"/>
       <c r="X48" t="inlineStr"/>
-      <c r="Y48" t="inlineStr"/>
-      <c r="Z48" t="inlineStr"/>
+      <c r="Y48" t="n">
+        <v>16</v>
+      </c>
+      <c r="Z48" t="n">
+        <v>15</v>
+      </c>
       <c r="AA48" t="inlineStr"/>
       <c r="AB48" t="inlineStr"/>
       <c r="AC48" t="inlineStr"/>
       <c r="AD48" t="inlineStr">
         <is>
-          <t>(Signature of Adviser over Printed Name)</t>
+          <t>LAMBERTO BOLIMA RIVAREZ</t>
         </is>
       </c>
       <c r="AE48" t="inlineStr"/>
@@ -4587,7 +4619,7 @@
       <c r="AI48" t="inlineStr"/>
       <c r="AJ48" t="inlineStr">
         <is>
-          <t>(Signature of School Head over Printed Name)</t>
+          <t>ELSA MONTERERO MANALO</t>
         </is>
       </c>
       <c r="AK48" t="inlineStr"/>
@@ -4620,9 +4652,7 @@
       <c r="V49" t="inlineStr"/>
       <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr"/>
-      <c r="Y49" t="n">
-        <v>18</v>
-      </c>
+      <c r="Y49" t="inlineStr"/>
       <c r="Z49" t="inlineStr"/>
       <c r="AA49" t="inlineStr"/>
       <c r="AB49" t="inlineStr"/>
@@ -4661,54 +4691,32 @@
       <c r="S50" t="inlineStr"/>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
-      <c r="V50" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
+      <c r="V50" t="inlineStr"/>
       <c r="W50" t="inlineStr"/>
       <c r="X50" t="inlineStr"/>
-      <c r="Y50" t="n">
-        <v>35</v>
-      </c>
+      <c r="Y50" t="inlineStr"/>
       <c r="Z50" t="inlineStr"/>
       <c r="AA50" t="inlineStr"/>
       <c r="AB50" t="inlineStr"/>
       <c r="AC50" t="inlineStr"/>
-      <c r="AD50" t="inlineStr">
-        <is>
-          <t>BoSY Date:</t>
-        </is>
-      </c>
+      <c r="AD50" t="inlineStr"/>
       <c r="AE50" t="inlineStr"/>
       <c r="AF50" t="inlineStr"/>
-      <c r="AG50" t="inlineStr">
-        <is>
-          <t>EoSY Date:</t>
-        </is>
-      </c>
+      <c r="AG50" t="inlineStr"/>
       <c r="AH50" t="inlineStr"/>
       <c r="AI50" t="inlineStr"/>
       <c r="AJ50" t="inlineStr">
         <is>
-          <t>BoSY Date:</t>
+          <t>(Signature of School Head over Printed Name)</t>
         </is>
       </c>
       <c r="AK50" t="inlineStr"/>
       <c r="AL50" t="inlineStr"/>
-      <c r="AM50" t="inlineStr">
-        <is>
-          <t>EoSY Date:</t>
-        </is>
-      </c>
+      <c r="AM50" t="inlineStr"/>
       <c r="AN50" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>Generated on: Tuesday, September 12, 2017</t>
-        </is>
-      </c>
+      <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
@@ -4729,15 +4737,27 @@
       <c r="S51" t="inlineStr"/>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
-      <c r="V51" t="inlineStr"/>
+      <c r="V51" t="inlineStr">
+        <is>
+          <t>FEMALE</t>
+        </is>
+      </c>
       <c r="W51" t="inlineStr"/>
       <c r="X51" t="inlineStr"/>
-      <c r="Y51" t="inlineStr"/>
-      <c r="Z51" t="inlineStr"/>
+      <c r="Y51" t="n">
+        <v>19</v>
+      </c>
+      <c r="Z51" t="n">
+        <v>20</v>
+      </c>
       <c r="AA51" t="inlineStr"/>
       <c r="AB51" t="inlineStr"/>
       <c r="AC51" t="inlineStr"/>
-      <c r="AD51" t="inlineStr"/>
+      <c r="AD51" t="inlineStr">
+        <is>
+          <t>(Signature of Adviser over Printed Name)</t>
+        </is>
+      </c>
       <c r="AE51" t="inlineStr"/>
       <c r="AF51" t="inlineStr"/>
       <c r="AG51" t="inlineStr"/>
@@ -4749,6 +4769,290 @@
       <c r="AM51" t="inlineStr"/>
       <c r="AN51" t="inlineStr"/>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr"/>
+      <c r="R52" t="inlineStr"/>
+      <c r="S52" t="inlineStr"/>
+      <c r="T52" t="inlineStr"/>
+      <c r="U52" t="inlineStr"/>
+      <c r="V52" t="inlineStr"/>
+      <c r="W52" t="inlineStr"/>
+      <c r="X52" t="inlineStr"/>
+      <c r="Y52" t="inlineStr"/>
+      <c r="Z52" t="inlineStr"/>
+      <c r="AA52" t="inlineStr"/>
+      <c r="AB52" t="inlineStr"/>
+      <c r="AC52" t="inlineStr"/>
+      <c r="AD52" t="inlineStr"/>
+      <c r="AE52" t="inlineStr"/>
+      <c r="AF52" t="inlineStr"/>
+      <c r="AG52" t="inlineStr"/>
+      <c r="AH52" t="inlineStr"/>
+      <c r="AI52" t="inlineStr"/>
+      <c r="AJ52" t="inlineStr">
+        <is>
+          <t>BoSY Date:                06-03-2019</t>
+        </is>
+      </c>
+      <c r="AK52" t="inlineStr"/>
+      <c r="AL52" t="inlineStr"/>
+      <c r="AM52" t="inlineStr">
+        <is>
+          <t>EoSY Date:                    04-03-2020</t>
+        </is>
+      </c>
+      <c r="AN52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr"/>
+      <c r="R53" t="inlineStr"/>
+      <c r="S53" t="inlineStr"/>
+      <c r="T53" t="inlineStr"/>
+      <c r="U53" t="inlineStr"/>
+      <c r="V53" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="W53" t="inlineStr"/>
+      <c r="X53" t="inlineStr"/>
+      <c r="Y53" t="n">
+        <v>35</v>
+      </c>
+      <c r="Z53" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA53" t="inlineStr"/>
+      <c r="AB53" t="inlineStr"/>
+      <c r="AC53" t="inlineStr"/>
+      <c r="AD53" t="inlineStr">
+        <is>
+          <t>BoSY Date:                06-03-2019</t>
+        </is>
+      </c>
+      <c r="AE53" t="inlineStr"/>
+      <c r="AF53" t="inlineStr"/>
+      <c r="AG53" t="inlineStr">
+        <is>
+          <t>EoSY Date:                  04-03-2020</t>
+        </is>
+      </c>
+      <c r="AH53" t="inlineStr"/>
+      <c r="AI53" t="inlineStr"/>
+      <c r="AJ53" t="inlineStr"/>
+      <c r="AK53" t="inlineStr"/>
+      <c r="AL53" t="inlineStr"/>
+      <c r="AM53" t="inlineStr"/>
+      <c r="AN53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr"/>
+      <c r="R54" t="inlineStr"/>
+      <c r="S54" t="inlineStr"/>
+      <c r="T54" t="inlineStr"/>
+      <c r="U54" t="inlineStr"/>
+      <c r="V54" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr"/>
+      <c r="Y54" t="inlineStr"/>
+      <c r="Z54" t="inlineStr"/>
+      <c r="AA54" t="inlineStr"/>
+      <c r="AB54" t="inlineStr"/>
+      <c r="AC54" t="inlineStr"/>
+      <c r="AD54" t="inlineStr"/>
+      <c r="AE54" t="inlineStr"/>
+      <c r="AF54" t="inlineStr"/>
+      <c r="AG54" t="inlineStr"/>
+      <c r="AH54" t="inlineStr"/>
+      <c r="AI54" t="inlineStr"/>
+      <c r="AJ54" t="inlineStr"/>
+      <c r="AK54" t="inlineStr"/>
+      <c r="AL54" t="inlineStr"/>
+      <c r="AM54" t="inlineStr"/>
+      <c r="AN54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr"/>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
+      <c r="R55" t="inlineStr"/>
+      <c r="S55" t="inlineStr"/>
+      <c r="T55" t="inlineStr"/>
+      <c r="U55" t="inlineStr"/>
+      <c r="V55" t="inlineStr"/>
+      <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr"/>
+      <c r="Y55" t="inlineStr"/>
+      <c r="Z55" t="inlineStr"/>
+      <c r="AA55" t="inlineStr"/>
+      <c r="AB55" t="inlineStr"/>
+      <c r="AC55" t="inlineStr"/>
+      <c r="AD55" t="inlineStr"/>
+      <c r="AE55" t="inlineStr"/>
+      <c r="AF55" t="inlineStr"/>
+      <c r="AG55" t="inlineStr"/>
+      <c r="AH55" t="inlineStr"/>
+      <c r="AI55" t="inlineStr"/>
+      <c r="AJ55" t="inlineStr"/>
+      <c r="AK55" t="inlineStr"/>
+      <c r="AL55" t="inlineStr"/>
+      <c r="AM55" t="inlineStr"/>
+      <c r="AN55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
+      <c r="R56" t="inlineStr"/>
+      <c r="S56" t="inlineStr"/>
+      <c r="T56" t="inlineStr"/>
+      <c r="U56" t="inlineStr"/>
+      <c r="V56" t="inlineStr"/>
+      <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr"/>
+      <c r="Y56" t="inlineStr"/>
+      <c r="Z56" t="inlineStr"/>
+      <c r="AA56" t="inlineStr"/>
+      <c r="AB56" t="inlineStr"/>
+      <c r="AC56" t="inlineStr"/>
+      <c r="AD56" t="inlineStr"/>
+      <c r="AE56" t="inlineStr"/>
+      <c r="AF56" t="inlineStr"/>
+      <c r="AG56" t="inlineStr"/>
+      <c r="AH56" t="inlineStr"/>
+      <c r="AI56" t="inlineStr"/>
+      <c r="AJ56" t="inlineStr">
+        <is>
+          <t>Generated thru LIS</t>
+        </is>
+      </c>
+      <c r="AK56" t="inlineStr"/>
+      <c r="AL56" t="inlineStr"/>
+      <c r="AM56" t="inlineStr"/>
+      <c r="AN56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Generated on: Saturday, March 21, 2020</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
+      <c r="R57" t="inlineStr"/>
+      <c r="S57" t="inlineStr"/>
+      <c r="T57" t="inlineStr"/>
+      <c r="U57" t="inlineStr"/>
+      <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr"/>
+      <c r="Y57" t="inlineStr"/>
+      <c r="Z57" t="inlineStr"/>
+      <c r="AA57" t="inlineStr"/>
+      <c r="AB57" t="inlineStr"/>
+      <c r="AC57" t="inlineStr"/>
+      <c r="AD57" t="inlineStr"/>
+      <c r="AE57" t="inlineStr"/>
+      <c r="AF57" t="inlineStr"/>
+      <c r="AG57" t="inlineStr"/>
+      <c r="AH57" t="inlineStr"/>
+      <c r="AI57" t="inlineStr"/>
+      <c r="AJ57" t="inlineStr"/>
+      <c r="AK57" t="inlineStr"/>
+      <c r="AL57" t="inlineStr"/>
+      <c r="AM57" t="inlineStr"/>
+      <c r="AN57" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
approving of mt , some inbox ui
</commit_message>
<xml_diff>
--- a/Migrade_v.1.2/temp.xlsx
+++ b/Migrade_v.1.2/temp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN57"/>
+  <dimension ref="A1:AN51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -782,7 +782,7 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr">
         <is>
-          <t>2019 - 2020</t>
+          <t>2017 - 2018</t>
         </is>
       </c>
       <c r="T4" t="inlineStr"/>
@@ -791,7 +791,7 @@
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Grade Level </t>
+          <t xml:space="preserve">Grade </t>
         </is>
       </c>
       <c r="Y4" t="inlineStr"/>
@@ -799,7 +799,7 @@
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>Grade 6</t>
+          <t>Grade 5</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr"/>
@@ -813,7 +813,7 @@
       <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>GALILEO</t>
+          <t>EARTH</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr"/>
@@ -853,7 +853,7 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>AGE as of 1st Friday June</t>
+          <t>Age as of August 31st</t>
         </is>
       </c>
       <c r="K5" t="inlineStr"/>
@@ -975,7 +975,7 @@
       <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>Mother's Maiden Name (Last Name, First Name, Middle Name)</t>
+          <t xml:space="preserve">Mother's Maiden Name (Last Name, First Name, Middle </t>
         </is>
       </c>
       <c r="AG6" t="inlineStr"/>
@@ -1002,13 +1002,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>164512130171</t>
+          <t>164512110014</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ANIBAN,LEO JELLY, TINAPAY</t>
+          <t>BORLAGDAN, ALFIE BISMAR</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -1021,13 +1021,13 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>09-23-2008</t>
+          <t>05-18-2005</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K7" t="inlineStr"/>
@@ -1069,7 +1069,7 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>ANIBAN, LEO BUTAL</t>
+          <t>BORLAGDAN, ALLAN GOLEMLEM</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr"/>
@@ -1077,7 +1077,7 @@
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>TINAPAY,JILL,BAJADI,</t>
+          <t>BISMAR,CARMENCITA,BLANQUEZA,</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr"/>
@@ -1092,13 +1092,13 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>164512130045</t>
+          <t>164512130010</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ASILO,RAIN JUSTINE, MERCADO</t>
+          <t>BORLAGDAN, RJ BISMAR</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -1111,13 +1111,13 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>05-20-2007</t>
+          <t>11-11-2006</t>
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K8" t="inlineStr"/>
@@ -1136,7 +1136,7 @@
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R8" t="inlineStr"/>
@@ -1159,7 +1159,7 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>ASILO, CHRISTOPHER SALILICAN</t>
+          <t>BORLAGDAN, ALLAN GOLEMLEM</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr"/>
@@ -1167,7 +1167,7 @@
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>MERCADO,MARICEL,HERNANDEZ,</t>
+          <t>BISMAR,CARMENCITA,BLANQUEZA,</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr"/>
@@ -1182,13 +1182,13 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>424663150037</t>
+          <t>136907120127</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CAMBE,SEAN DAVE, ARAGON</t>
+          <t>CAMBE, RALPH LOUIE ARAGON</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -1201,13 +1201,13 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>03-15-2008</t>
+          <t>03-02-2007</t>
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K9" t="inlineStr"/>
@@ -1267,18 +1267,22 @@
       <c r="AK9" t="inlineStr"/>
       <c r="AL9" t="inlineStr"/>
       <c r="AM9" t="inlineStr"/>
-      <c r="AN9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr">
+        <is>
+          <t>T/I DATE:2017-06-05</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>164512140032</t>
+          <t>164512130016</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CARANAY,JHAYCEE CARL, CORDERO</t>
+          <t>CAONES, JAYRUS CARL LACANIN</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -1291,7 +1295,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>11-25-2007</t>
+          <t>08-25-2006</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
@@ -1339,7 +1343,7 @@
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>CARANAY, ROGELIO JR CABOTAJE</t>
+          <t>CAONES, JAYZON NUNAY</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr"/>
@@ -1347,7 +1351,7 @@
       <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="inlineStr">
         <is>
-          <t>CORDERO,NORMA,ALIDO,</t>
+          <t>LACANIN,JERLYN,BELO,</t>
         </is>
       </c>
       <c r="AG10" t="inlineStr"/>
@@ -1362,13 +1366,13 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>164512140029</t>
+          <t>164512120011</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CASTRO,ICHIRO, MENDOZA</t>
+          <t>CELESTE, ANDREW ACE ESPINOSA</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -1381,7 +1385,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>09-08-2008</t>
+          <t>02-09-2007</t>
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
@@ -1406,7 +1410,7 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>PLATERO</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R11" t="inlineStr"/>
@@ -1429,7 +1433,7 @@
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>CASTRO, SEVERLINO ABAPO</t>
+          <t>CELESTE, ALEJANDRO SARVIDA</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr"/>
@@ -1437,7 +1441,7 @@
       <c r="AE11" t="inlineStr"/>
       <c r="AF11" t="inlineStr">
         <is>
-          <t>MENDOZA,ALICIA,ZULUETA,</t>
+          <t>ESPINOSA,LORENA,ALBERTO,</t>
         </is>
       </c>
       <c r="AG11" t="inlineStr"/>
@@ -1452,13 +1456,13 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>164512150094</t>
+          <t>164512130047</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CAYLAO,DAYNE, VIÑA</t>
+          <t>CUPANG, CHRISTIAN ZAMORA</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -1471,13 +1475,13 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>03-17-2007</t>
+          <t>06-21-2007</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K12" t="inlineStr"/>
@@ -1496,7 +1500,7 @@
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>PLATERO</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R12" t="inlineStr"/>
@@ -1519,7 +1523,7 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>CAYLAO, DANZEL CIPRIANO</t>
+          <t>CUPANG, ANTONIO CRISMUNDO JR</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr"/>
@@ -1527,7 +1531,7 @@
       <c r="AE12" t="inlineStr"/>
       <c r="AF12" t="inlineStr">
         <is>
-          <t>VIÑA,CAREN,CRUZ,</t>
+          <t>ZAMORA,TERESITA,ALING,</t>
         </is>
       </c>
       <c r="AG12" t="inlineStr"/>
@@ -1542,13 +1546,13 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>164512130131</t>
+          <t>108226120133</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CHAN,JHON RHAYNE, REPELAR</t>
+          <t>GABATIN, KING TYRON GILBERT AMORTIZADO</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -1561,13 +1565,13 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>01-16-2008</t>
+          <t>11-10-2004</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K13" t="inlineStr"/>
@@ -1609,7 +1613,7 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>CHAN, JONATHAN ALICARTE</t>
+          <t>GABATIN, TEOFILO TACSIAT</t>
         </is>
       </c>
       <c r="AC13" t="inlineStr"/>
@@ -1617,7 +1621,7 @@
       <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="inlineStr">
         <is>
-          <t>REPELAR,ELENA,ROXAS,</t>
+          <t>AMORTIZADO,MARIA LOURDES,CAPUQUIAN,</t>
         </is>
       </c>
       <c r="AG13" t="inlineStr"/>
@@ -1632,13 +1636,13 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>402456150012</t>
+          <t>164512130022</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>GETALADO,EARL SAMUEL, CLAVE</t>
+          <t>LAGADI, JHOSUA BUSTAMANTE</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -1651,7 +1655,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>09-10-2008</t>
+          <t>11-08-2006</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -1676,7 +1680,7 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R14" t="inlineStr"/>
@@ -1699,7 +1703,7 @@
       <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>GETALADO, ERNESTO CERTEZA</t>
+          <t>LAGADI, VICENTE GABRIEL JR</t>
         </is>
       </c>
       <c r="AC14" t="inlineStr"/>
@@ -1707,7 +1711,7 @@
       <c r="AE14" t="inlineStr"/>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>CLAVE,SERENIDAD,TABLIZO,</t>
+          <t>BUSTAMANTE,ELIZA,BULARON,</t>
         </is>
       </c>
       <c r="AG14" t="inlineStr"/>
@@ -1722,13 +1726,13 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>164512130101</t>
+          <t>112505130003</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>GLOBIO,MARCKY, GALVAN</t>
+          <t>LLANZA, ALFREDO LAYCO JR</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -1741,13 +1745,13 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>03-11-2008</t>
+          <t>09-28-2006</t>
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
@@ -1766,7 +1770,7 @@
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>SANTO NINO</t>
         </is>
       </c>
       <c r="R15" t="inlineStr"/>
@@ -1787,13 +1791,17 @@
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="inlineStr"/>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>LLANZA, ALFREDO CARGALLO SR</t>
+        </is>
+      </c>
       <c r="AC15" t="inlineStr"/>
       <c r="AD15" t="inlineStr"/>
       <c r="AE15" t="inlineStr"/>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>GLOBIO,RENITA,GALVAN,</t>
+          <t>LAYCO,ARCELI,MONTANEZ,</t>
         </is>
       </c>
       <c r="AG15" t="inlineStr"/>
@@ -1803,22 +1811,18 @@
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr"/>
       <c r="AM15" t="inlineStr"/>
-      <c r="AN15" t="inlineStr">
-        <is>
-          <t>DRP "Family Problem"Date:2019/11/04</t>
-        </is>
-      </c>
+      <c r="AN15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>164512140006</t>
+          <t>164512130024</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MIRANDA,ANDREI, BIANES</t>
+          <t>MALINTAD, JAMES DUMAYO</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -1831,13 +1835,13 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>04-29-2007</t>
+          <t>03-05-2007</t>
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
@@ -1856,7 +1860,7 @@
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R16" t="inlineStr"/>
@@ -1879,7 +1883,7 @@
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>MIRANDA, ESTELITO VILLANUEVA</t>
+          <t>MALINTAD, GREMER CAONG</t>
         </is>
       </c>
       <c r="AC16" t="inlineStr"/>
@@ -1887,7 +1891,7 @@
       <c r="AE16" t="inlineStr"/>
       <c r="AF16" t="inlineStr">
         <is>
-          <t>BIANES,JENNIFER,QUINTUA,</t>
+          <t>DUMAYO,MINDA,TUMIMO,</t>
         </is>
       </c>
       <c r="AG16" t="inlineStr"/>
@@ -1897,22 +1901,18 @@
       <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="inlineStr"/>
-      <c r="AN16" t="inlineStr">
-        <is>
-          <t>T/I Pook Elem. Sch. Date:2019-06-03</t>
-        </is>
-      </c>
+      <c r="AN16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>164512130118</t>
+          <t>164512130027</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>NAVAREZ,ANDREI, MONTAÑEZ</t>
+          <t>MATULA, JOHN GABRIEL ZAVALLA</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -1925,13 +1925,13 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>07-26-2007</t>
+          <t>09-25-2006</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K17" t="inlineStr"/>
@@ -1973,7 +1973,7 @@
       <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>NAVAREZ, ARNEL NABUHAY</t>
+          <t>MATULA, VICTOR GONZALES</t>
         </is>
       </c>
       <c r="AC17" t="inlineStr"/>
@@ -1981,7 +1981,7 @@
       <c r="AE17" t="inlineStr"/>
       <c r="AF17" t="inlineStr">
         <is>
-          <t>MONTAÑEZ,SUSANA,VILLARIN,</t>
+          <t>ZAVALLA,FLORENCIA,NILLO,</t>
         </is>
       </c>
       <c r="AG17" t="inlineStr"/>
@@ -1996,13 +1996,13 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>164512100132</t>
+          <t>164512120051</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>SALAYSAY,JOHN LOUIE, FLORES</t>
+          <t>OLIVEROS, JHONUEL BISMAR</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -2015,13 +2015,13 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>02-18-2004</t>
+          <t>01-16-2007</t>
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
-          <t xml:space="preserve">15 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
@@ -2063,7 +2063,7 @@
       <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>SALAYSAY, ALFREDO REYES</t>
+          <t>OLIVEROS, JOEL AFANTE</t>
         </is>
       </c>
       <c r="AC18" t="inlineStr"/>
@@ -2071,7 +2071,7 @@
       <c r="AE18" t="inlineStr"/>
       <c r="AF18" t="inlineStr">
         <is>
-          <t>FLORES,CECILIA,LOPENA,</t>
+          <t>BLANQUEZA,JANET,BISMAR,</t>
         </is>
       </c>
       <c r="AG18" t="inlineStr"/>
@@ -2086,13 +2086,13 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>108476120166</t>
+          <t>108474140114</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>SAMANIEGO,MATTHEW ANDREI, ANGULO</t>
+          <t>QUILLOSA, MERICK MASAREDO</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
@@ -2105,13 +2105,13 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>08-01-2006</t>
+          <t>10-04-2006</t>
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
@@ -2130,7 +2130,7 @@
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R19" t="inlineStr"/>
@@ -2153,7 +2153,7 @@
       <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>SAMANIEGO, MICHAEL ABUCEJO</t>
+          <t>QUILLOSA, MARVIN MANLOLO</t>
         </is>
       </c>
       <c r="AC19" t="inlineStr"/>
@@ -2161,7 +2161,7 @@
       <c r="AE19" t="inlineStr"/>
       <c r="AF19" t="inlineStr">
         <is>
-          <t>ANGULO,ABIGAIL,GUSTILO,</t>
+          <t>MASAREDO,PERLA,ACOSTA,</t>
         </is>
       </c>
       <c r="AG19" t="inlineStr"/>
@@ -2176,13 +2176,13 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>108426130045</t>
+          <t>164512130030</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>SAN JUAN JR.,ARLY, PLATINO</t>
+          <t>SANGYAHON, JUSTINE MAGTAGAD</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
@@ -2195,13 +2195,13 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>09-29-2007</t>
+          <t>09-22-2006</t>
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K20" t="inlineStr"/>
@@ -2243,7 +2243,7 @@
       <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>SAN JUAN, ARLY TAPUIC SR</t>
+          <t>SANGYAHON, ERLINDO PATRICIO</t>
         </is>
       </c>
       <c r="AC20" t="inlineStr"/>
@@ -2251,7 +2251,7 @@
       <c r="AE20" t="inlineStr"/>
       <c r="AF20" t="inlineStr">
         <is>
-          <t>PLATINO,EVANGELINE,GUILLEN,</t>
+          <t>MAGTAGAD,CHERYL,ESPAÑOLA,</t>
         </is>
       </c>
       <c r="AG20" t="inlineStr"/>
@@ -2266,13 +2266,13 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>164512130091</t>
+          <t>136775120015</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
-          <t>SANTOS,MARK, BELANO</t>
+          <t>SANTOS, ANGELO GALLARDO</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>09-05-2008</t>
+          <t>05-15-2007</t>
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
@@ -2333,7 +2333,7 @@
       <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>SANTOS, ROLANDO BARBOSA</t>
+          <t>SANTOS, ARTURO CRUZ</t>
         </is>
       </c>
       <c r="AC21" t="inlineStr"/>
@@ -2341,7 +2341,7 @@
       <c r="AE21" t="inlineStr"/>
       <c r="AF21" t="inlineStr">
         <is>
-          <t>BELANO,LIZA,BERIANO,</t>
+          <t>UMALI,GALLARDO,GUADALUPE,</t>
         </is>
       </c>
       <c r="AG21" t="inlineStr"/>
@@ -2351,18 +2351,22 @@
       <c r="AK21" t="inlineStr"/>
       <c r="AL21" t="inlineStr"/>
       <c r="AM21" t="inlineStr"/>
-      <c r="AN21" t="inlineStr"/>
+      <c r="AN21" t="inlineStr">
+        <is>
+          <t>Pending TI</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>164512140037</t>
+          <t>164512120054</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
-          <t>VILLANUEVA,JOSH CYREL, CLASA</t>
+          <t>TABING, RANDEL ABELLA</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
@@ -2375,13 +2379,13 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>11-09-2007</t>
+          <t>06-16-2007</t>
         </is>
       </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
@@ -2423,7 +2427,7 @@
       <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>VILLANUEVA, PABLITO MARIÑAS</t>
+          <t>TABING, RANDY ESTEBAN</t>
         </is>
       </c>
       <c r="AC22" t="inlineStr"/>
@@ -2431,7 +2435,7 @@
       <c r="AE22" t="inlineStr"/>
       <c r="AF22" t="inlineStr">
         <is>
-          <t>CLASA,EVEBERLY,MONTESCO,</t>
+          <t>ABELLA,MARIDEL,ENCELAN,</t>
         </is>
       </c>
       <c r="AG22" t="inlineStr"/>
@@ -2444,44 +2448,86 @@
       <c r="AN22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>16</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>164512120055</t>
+        </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
-          <t>&lt;=== TOTAL MALE</t>
+          <t>VALENCIA, RIN WINZHEL AGUADO</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>01-09-2007</t>
+        </is>
+      </c>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr"/>
-      <c r="X23" t="inlineStr"/>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="inlineStr"/>
-      <c r="AB23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>VALENCIA, CHERWEN MANONGSONG</t>
+        </is>
+      </c>
       <c r="AC23" t="inlineStr"/>
       <c r="AD23" t="inlineStr"/>
       <c r="AE23" t="inlineStr"/>
-      <c r="AF23" t="inlineStr"/>
+      <c r="AF23" t="inlineStr">
+        <is>
+          <t>AGUADO,FRITCHEL,VICTORIO,</t>
+        </is>
+      </c>
       <c r="AG23" t="inlineStr"/>
       <c r="AH23" t="inlineStr"/>
       <c r="AI23" t="inlineStr"/>
@@ -2492,86 +2538,44 @@
       <c r="AN23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>164512140038</t>
-        </is>
+      <c r="A24" t="n">
+        <v>17</v>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ARRESGADO,LEANNE ROSE, CARLOS</t>
+          <t>&lt;=== TOTAL MALE</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>08-25-2008</t>
-        </is>
-      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t xml:space="preserve">10 </t>
-        </is>
-      </c>
+      <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>Tagalog</t>
-        </is>
-      </c>
+      <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>Christianity</t>
-        </is>
-      </c>
+      <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>ZAPOTE</t>
-        </is>
-      </c>
+      <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>CITY OF BIÑAN</t>
-        </is>
-      </c>
+      <c r="U24" t="inlineStr"/>
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr"/>
-      <c r="X24" t="inlineStr">
-        <is>
-          <t>LAGUNA</t>
-        </is>
-      </c>
+      <c r="X24" t="inlineStr"/>
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="inlineStr"/>
-      <c r="AB24" t="inlineStr">
-        <is>
-          <t>ARRESGADO, JUNARD MALAKARTE</t>
-        </is>
-      </c>
+      <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="inlineStr"/>
       <c r="AD24" t="inlineStr"/>
       <c r="AE24" t="inlineStr"/>
-      <c r="AF24" t="inlineStr">
-        <is>
-          <t>CARLOS,AILEEN,VERANO,</t>
-        </is>
-      </c>
+      <c r="AF24" t="inlineStr"/>
       <c r="AG24" t="inlineStr"/>
       <c r="AH24" t="inlineStr"/>
       <c r="AI24" t="inlineStr"/>
@@ -2584,13 +2588,13 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>164512140016</t>
+          <t>164512130075</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
-          <t>BORCELANGO,DONA LYNN, DAPRINAL</t>
+          <t>ACILO, CHARLENE DAGUMAN</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -2603,7 +2607,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>07-22-2008</t>
+          <t>10-18-2006</t>
         </is>
       </c>
       <c r="I25" t="inlineStr"/>
@@ -2651,7 +2655,7 @@
       <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>BORCELANGO, DONATO REYES</t>
+          <t>ACILO, CHARLITO LOPENA</t>
         </is>
       </c>
       <c r="AC25" t="inlineStr"/>
@@ -2659,7 +2663,7 @@
       <c r="AE25" t="inlineStr"/>
       <c r="AF25" t="inlineStr">
         <is>
-          <t>DAPRINAL,JONALINE,ATOR,</t>
+          <t>DAGUMAN,AILENE,ABE,</t>
         </is>
       </c>
       <c r="AG25" t="inlineStr"/>
@@ -2674,13 +2678,13 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>164512140017</t>
+          <t>164512130061</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CAONES,JUSEA MICAH, LACANIN</t>
+          <t>BETITO, EURICE ROSACEÑA</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
@@ -2693,13 +2697,13 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>01-31-2008</t>
+          <t>05-03-2007</t>
         </is>
       </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K26" t="inlineStr"/>
@@ -2741,7 +2745,7 @@
       <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="inlineStr">
         <is>
-          <t>CAONES, JAYZON NUNAY</t>
+          <t>BETITO, ARMANDO SALAMODING</t>
         </is>
       </c>
       <c r="AC26" t="inlineStr"/>
@@ -2749,7 +2753,7 @@
       <c r="AE26" t="inlineStr"/>
       <c r="AF26" t="inlineStr">
         <is>
-          <t>LACANIN,JERLYN,BELO,</t>
+          <t>ROSACENA,REMEDIOS,VILLANUEVA,</t>
         </is>
       </c>
       <c r="AG26" t="inlineStr"/>
@@ -2764,13 +2768,13 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>105111130128</t>
+          <t>164512120064</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CLEMENTE,MARTHA ASHLEE, COLIS</t>
+          <t>CAFINO, JASMIN CLAIRE CANTIGA</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -2783,7 +2787,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>07-02-2008</t>
+          <t>03-06-2007</t>
         </is>
       </c>
       <c r="I27" t="inlineStr"/>
@@ -2808,7 +2812,7 @@
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R27" t="inlineStr"/>
@@ -2831,7 +2835,7 @@
       <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="inlineStr">
         <is>
-          <t>CLEMENTE, RAFAEL KRIS PRONUEVO CLEMENTE</t>
+          <t>CAFINO, RODERICK SOREÑO</t>
         </is>
       </c>
       <c r="AC27" t="inlineStr"/>
@@ -2839,7 +2843,7 @@
       <c r="AE27" t="inlineStr"/>
       <c r="AF27" t="inlineStr">
         <is>
-          <t>COLIS,MA NIEVES VALANTINE,CUNANAN,</t>
+          <t>CANTIGA,GRACE,IGNACIO,</t>
         </is>
       </c>
       <c r="AG27" t="inlineStr"/>
@@ -2849,22 +2853,18 @@
       <c r="AK27" t="inlineStr"/>
       <c r="AL27" t="inlineStr"/>
       <c r="AM27" t="inlineStr"/>
-      <c r="AN27" t="inlineStr">
-        <is>
-          <t>T/I  San Miguel Elem.Sch.Date:2019-06-03</t>
-        </is>
-      </c>
+      <c r="AN27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>109850130028</t>
+          <t>164512120218</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>DEL MUNDO,CATHLYN, SALDINO</t>
+          <t>CLARION, MARY QUEEN MARIEL RAMISO</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
@@ -2877,13 +2877,13 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>11-22-2007</t>
+          <t>10-01-2006</t>
         </is>
       </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K28" t="inlineStr"/>
@@ -2902,7 +2902,7 @@
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R28" t="inlineStr"/>
@@ -2925,7 +2925,7 @@
       <c r="AA28" t="inlineStr"/>
       <c r="AB28" t="inlineStr">
         <is>
-          <t>DEL MUNDO, JUNE LINGGA</t>
+          <t>CLARION, MARCIAL GARRAN</t>
         </is>
       </c>
       <c r="AC28" t="inlineStr"/>
@@ -2933,7 +2933,7 @@
       <c r="AE28" t="inlineStr"/>
       <c r="AF28" t="inlineStr">
         <is>
-          <t>SALDINO,ANNABELLE,SOLAYAO,</t>
+          <t>RAMISO,LIEZEL,SIMPO,</t>
         </is>
       </c>
       <c r="AG28" t="inlineStr"/>
@@ -2948,13 +2948,13 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>164512130166</t>
+          <t>164512130029</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>DICDICAN,TRISHA ELLAINE, REALON</t>
+          <t>DIONISO, JHAMAICA ALEGRE</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>03-01-2008</t>
+          <t>10-25-2005</t>
         </is>
       </c>
       <c r="I29" t="inlineStr"/>
@@ -2992,7 +2992,7 @@
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R29" t="inlineStr"/>
@@ -3015,7 +3015,7 @@
       <c r="AA29" t="inlineStr"/>
       <c r="AB29" t="inlineStr">
         <is>
-          <t>DICDICAN, RICHARD JIMENEZ</t>
+          <t>DIONISIO, ROEL CRUZ</t>
         </is>
       </c>
       <c r="AC29" t="inlineStr"/>
@@ -3023,7 +3023,7 @@
       <c r="AE29" t="inlineStr"/>
       <c r="AF29" t="inlineStr">
         <is>
-          <t>REALON,MA CLARISSA,ROLDAN,</t>
+          <t>ALEGRE,SHIELA,SAHIRON,</t>
         </is>
       </c>
       <c r="AG29" t="inlineStr"/>
@@ -3038,13 +3038,13 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>164512130124</t>
+          <t>164512120071</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ESPINAR,ANGIELYN, MARCE</t>
+          <t>ESPINOSA, MIAH JUMAO-AS</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>07-26-2008</t>
+          <t>12-13-2006</t>
         </is>
       </c>
       <c r="I30" t="inlineStr"/>
@@ -3082,7 +3082,7 @@
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>SANTO NINO</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R30" t="inlineStr"/>
@@ -3105,7 +3105,7 @@
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr">
         <is>
-          <t>ESPINAR, EDISON FLORALDE</t>
+          <t>ESPINOSA, BONIFACIO ALVERIO</t>
         </is>
       </c>
       <c r="AC30" t="inlineStr"/>
@@ -3113,7 +3113,7 @@
       <c r="AE30" t="inlineStr"/>
       <c r="AF30" t="inlineStr">
         <is>
-          <t>MARCE,MARIE GRACE,MONTAÑEZ,</t>
+          <t>JUMAO-AS,CECILIA,MABATID,</t>
         </is>
       </c>
       <c r="AG30" t="inlineStr"/>
@@ -3128,13 +3128,13 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>108226120096</t>
+          <t>164512120033</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>GABATIN,LADY TRISHA, AMORTIZADO</t>
+          <t>GABUTAN, ANGIE GOLLAYAN</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
@@ -3147,13 +3147,13 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>11-03-2006</t>
+          <t>08-06-2006</t>
         </is>
       </c>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
@@ -3195,7 +3195,7 @@
       <c r="AA31" t="inlineStr"/>
       <c r="AB31" t="inlineStr">
         <is>
-          <t>GABATIN, TEOFILO TACSIAT</t>
+          <t>GABUTAN, ALVE SUMARGO</t>
         </is>
       </c>
       <c r="AC31" t="inlineStr"/>
@@ -3203,7 +3203,7 @@
       <c r="AE31" t="inlineStr"/>
       <c r="AF31" t="inlineStr">
         <is>
-          <t>AMORTIZADO,MARIA LOURDES,CAPUQUIAN,</t>
+          <t>GOLLAYAN,MARITES,BLANZA,</t>
         </is>
       </c>
       <c r="AG31" t="inlineStr"/>
@@ -3218,13 +3218,13 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>164512130042</t>
+          <t>164512110030</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
-          <t>JOVEN,JENALEN, MASIKAT</t>
+          <t>GONZALO, ERICQUEZEN DACASIN</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
@@ -3237,13 +3237,13 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>10-01-2006</t>
+          <t>12-07-2005</t>
         </is>
       </c>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
@@ -3285,7 +3285,7 @@
       <c r="AA32" t="inlineStr"/>
       <c r="AB32" t="inlineStr">
         <is>
-          <t>JOVEN, SAMUEL ARCEGA</t>
+          <t>GONZALO, ERIC TORIO</t>
         </is>
       </c>
       <c r="AC32" t="inlineStr"/>
@@ -3293,7 +3293,7 @@
       <c r="AE32" t="inlineStr"/>
       <c r="AF32" t="inlineStr">
         <is>
-          <t>MASIKAT,CRISTINA,BAYAN,</t>
+          <t>DACASIN,HEIDE,VERGARA,</t>
         </is>
       </c>
       <c r="AG32" t="inlineStr"/>
@@ -3308,13 +3308,13 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>108407130083</t>
+          <t>164512130062</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>MALABAG,ANGELICA, MIRANDA</t>
+          <t>HUTALLA, RHIAM CLARIS ESPINOSA</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
@@ -3327,13 +3327,13 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>12-22-2007</t>
+          <t>01-04-2007</t>
         </is>
       </c>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
@@ -3375,7 +3375,7 @@
       <c r="AA33" t="inlineStr"/>
       <c r="AB33" t="inlineStr">
         <is>
-          <t>MALABAG, ANGELITO MELICIO</t>
+          <t>HUTALLA, CLARO GONZALES</t>
         </is>
       </c>
       <c r="AC33" t="inlineStr"/>
@@ -3383,7 +3383,7 @@
       <c r="AE33" t="inlineStr"/>
       <c r="AF33" t="inlineStr">
         <is>
-          <t>MIRANDA,MARY ANN,BAYANID,</t>
+          <t>ESPINOSA,MIRIAM,ALMEDA,</t>
         </is>
       </c>
       <c r="AG33" t="inlineStr"/>
@@ -3398,13 +3398,13 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>164512140043</t>
+          <t>164512130032</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
-          <t>MAMANSAG,JEIAH EUNICE, SERRANO</t>
+          <t>LLANZA, RUTH MICAH CORPUZ</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>08-09-2008</t>
+          <t>11-24-2006</t>
         </is>
       </c>
       <c r="I34" t="inlineStr"/>
@@ -3442,7 +3442,7 @@
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R34" t="inlineStr"/>
@@ -3465,7 +3465,7 @@
       <c r="AA34" t="inlineStr"/>
       <c r="AB34" t="inlineStr">
         <is>
-          <t>MAMANSAG, EMMERSON SALCEDO</t>
+          <t>LLANZA, JOSEPH GUEVARRA</t>
         </is>
       </c>
       <c r="AC34" t="inlineStr"/>
@@ -3473,7 +3473,7 @@
       <c r="AE34" t="inlineStr"/>
       <c r="AF34" t="inlineStr">
         <is>
-          <t>SERRANO,GERLIE,VALCOBA,</t>
+          <t>CORPUZ,CLARISA,BARONIA,</t>
         </is>
       </c>
       <c r="AG34" t="inlineStr"/>
@@ -3488,13 +3488,13 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>424638150057</t>
+          <t>164512130036</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MANALILI,JAMAICA AMOR, ROSALES</t>
+          <t>MACARAIG, MARICRIS SABADO</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
@@ -3507,13 +3507,13 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>01-21-2008</t>
+          <t>10-16-2007</t>
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">9 </t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
@@ -3532,7 +3532,7 @@
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R35" t="inlineStr"/>
@@ -3555,7 +3555,7 @@
       <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="inlineStr">
         <is>
-          <t>MANALILI, JAM ANTHONY CASTILLO</t>
+          <t>MACARAIG, EDWIN GARCIA</t>
         </is>
       </c>
       <c r="AC35" t="inlineStr"/>
@@ -3563,7 +3563,7 @@
       <c r="AE35" t="inlineStr"/>
       <c r="AF35" t="inlineStr">
         <is>
-          <t>ROSALES,RACHEL,MALIBAGO,</t>
+          <t>SABADO,MARIA,SARSOZA,</t>
         </is>
       </c>
       <c r="AG35" t="inlineStr"/>
@@ -3578,13 +3578,13 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>164512130089</t>
+          <t>108231130020</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MARTINEZ,ASHLEE NICHOLE, SABANAL</t>
+          <t>MARAÑAN, JERAMIAH ALAHAY</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>11-16-2008</t>
+          <t>10-01-2006</t>
         </is>
       </c>
       <c r="I36" t="inlineStr"/>
@@ -3622,7 +3622,7 @@
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R36" t="inlineStr"/>
@@ -3645,7 +3645,7 @@
       <c r="AA36" t="inlineStr"/>
       <c r="AB36" t="inlineStr">
         <is>
-          <t>MARTINEZ, MAR JUN BRUCE</t>
+          <t>MARAÑAN, RONNIE CUEME</t>
         </is>
       </c>
       <c r="AC36" t="inlineStr"/>
@@ -3653,7 +3653,7 @@
       <c r="AE36" t="inlineStr"/>
       <c r="AF36" t="inlineStr">
         <is>
-          <t>SABANAL,DESARIE,ALORA,</t>
+          <t>TATA,ALAHAY,JOSEPHINE,</t>
         </is>
       </c>
       <c r="AG36" t="inlineStr"/>
@@ -3663,18 +3663,22 @@
       <c r="AK36" t="inlineStr"/>
       <c r="AL36" t="inlineStr"/>
       <c r="AM36" t="inlineStr"/>
-      <c r="AN36" t="inlineStr"/>
+      <c r="AN36" t="inlineStr">
+        <is>
+          <t>T/I DATE:2017-06-05</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>164512140024</t>
+          <t>164512130037</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>NAVAL,GEARLY SHANE, OCAMPO</t>
+          <t>NAVAL, KRISHA MAY MIRANDA</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
@@ -3687,13 +3691,13 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>11-03-2007</t>
+          <t>06-01-2007</t>
         </is>
       </c>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
@@ -3735,7 +3739,7 @@
       <c r="AA37" t="inlineStr"/>
       <c r="AB37" t="inlineStr">
         <is>
-          <t>NAVAL, PERFECTO LINGGO</t>
+          <t>NAVAL, TIBURCIO ALIAS</t>
         </is>
       </c>
       <c r="AC37" t="inlineStr"/>
@@ -3743,7 +3747,7 @@
       <c r="AE37" t="inlineStr"/>
       <c r="AF37" t="inlineStr">
         <is>
-          <t>ILAITIA,MELANIE,OCAMPO,</t>
+          <t>MIRANDA,ERLINDA,RAMOS,</t>
         </is>
       </c>
       <c r="AG37" t="inlineStr"/>
@@ -3758,13 +3762,13 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>164512130194</t>
+          <t>164512130064</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
-          <t>OLAVARIO,ALLIYAH LORRAINE, GUILLERMO</t>
+          <t>NAVAL, ZYDNEY RONQUEZ</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
@@ -3777,13 +3781,13 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>07-23-2007</t>
+          <t>11-02-2006</t>
         </is>
       </c>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
@@ -3825,7 +3829,7 @@
       <c r="AA38" t="inlineStr"/>
       <c r="AB38" t="inlineStr">
         <is>
-          <t>OLAVARIO, TEODULO NUELAN</t>
+          <t>NAVAL, FERDINAND DIAGO</t>
         </is>
       </c>
       <c r="AC38" t="inlineStr"/>
@@ -3833,7 +3837,7 @@
       <c r="AE38" t="inlineStr"/>
       <c r="AF38" t="inlineStr">
         <is>
-          <t>GUILLERMO,IRENE,LIMBAG,</t>
+          <t>RONQUEZ,RIO,CAMACHO,</t>
         </is>
       </c>
       <c r="AG38" t="inlineStr"/>
@@ -3848,13 +3852,13 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>108224130152</t>
+          <t>164512130038</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr">
         <is>
-          <t>PUNZALAN,CHANELLE, POSO</t>
+          <t>NAVARRO, ELYZA MAE BERMEJO</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
@@ -3867,7 +3871,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>08-03-2008</t>
+          <t>02-08-2007</t>
         </is>
       </c>
       <c r="I39" t="inlineStr"/>
@@ -3892,7 +3896,7 @@
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R39" t="inlineStr"/>
@@ -3915,7 +3919,7 @@
       <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="inlineStr">
         <is>
-          <t>PUNZALAN, RAYMOND LISMORAS</t>
+          <t>NAVARRO, RAYMUNDO HALLEGADO</t>
         </is>
       </c>
       <c r="AC39" t="inlineStr"/>
@@ -3923,7 +3927,7 @@
       <c r="AE39" t="inlineStr"/>
       <c r="AF39" t="inlineStr">
         <is>
-          <t>POSO,CHONA,RAMIREZ,</t>
+          <t>BERMEJO,GERALDINE,BERNABE,</t>
         </is>
       </c>
       <c r="AG39" t="inlineStr"/>
@@ -3938,13 +3942,13 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>136908131369</t>
+          <t>164512130068</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ROTUBIO,ALLIANA JALYN, BERONDO</t>
+          <t>PONTIGON, PATRICIA JOY ENCISO</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
@@ -3957,7 +3961,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>07-03-2008</t>
+          <t>11-19-2006</t>
         </is>
       </c>
       <c r="I40" t="inlineStr"/>
@@ -3982,7 +3986,7 @@
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R40" t="inlineStr"/>
@@ -4005,7 +4009,7 @@
       <c r="AA40" t="inlineStr"/>
       <c r="AB40" t="inlineStr">
         <is>
-          <t>ROTUBIO, JAY TOLEDO</t>
+          <t>PONTIGON, JAIME DATUON</t>
         </is>
       </c>
       <c r="AC40" t="inlineStr"/>
@@ -4013,7 +4017,7 @@
       <c r="AE40" t="inlineStr"/>
       <c r="AF40" t="inlineStr">
         <is>
-          <t>BERONDO,NORMALYN,CORDERO,</t>
+          <t>ENCISO,JOSEPHINE,MAKATINGRAO,</t>
         </is>
       </c>
       <c r="AG40" t="inlineStr"/>
@@ -4023,22 +4027,18 @@
       <c r="AK40" t="inlineStr"/>
       <c r="AL40" t="inlineStr"/>
       <c r="AM40" t="inlineStr"/>
-      <c r="AN40" t="inlineStr">
-        <is>
-          <t>T/I Southville IV Elem. Sch.Date:2019-09-02</t>
-        </is>
-      </c>
+      <c r="AN40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>164512130168</t>
+          <t>111821090138</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>SUZON,RYGIN LOVE, GIMENTIZA</t>
+          <t>RAMIREZ, ELIZA CHRISTINE CARREON</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
@@ -4051,13 +4051,13 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>05-20-2008</t>
+          <t>10-10-2003</t>
         </is>
       </c>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">13 </t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
@@ -4076,7 +4076,7 @@
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R41" t="inlineStr"/>
@@ -4099,7 +4099,7 @@
       <c r="AA41" t="inlineStr"/>
       <c r="AB41" t="inlineStr">
         <is>
-          <t>SUZON, GERRY BERCERO</t>
+          <t>RAMIREZ, ERWIN TORARBA</t>
         </is>
       </c>
       <c r="AC41" t="inlineStr"/>
@@ -4107,7 +4107,7 @@
       <c r="AE41" t="inlineStr"/>
       <c r="AF41" t="inlineStr">
         <is>
-          <t>GIMENTIZA,GINA,TUICO,</t>
+          <t>CARREON,NELIA,SARMIENTO,</t>
         </is>
       </c>
       <c r="AG41" t="inlineStr"/>
@@ -4117,18 +4117,22 @@
       <c r="AK41" t="inlineStr"/>
       <c r="AL41" t="inlineStr"/>
       <c r="AM41" t="inlineStr"/>
-      <c r="AN41" t="inlineStr"/>
+      <c r="AN41" t="inlineStr">
+        <is>
+          <t>T/I DATE:2017-06-05</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>107937130338</t>
+          <t>164512130040</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>TAVU,RENY DENIEZE, RAMOS</t>
+          <t>RIVERA, ANGELINA ELAINE MIRANDA</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
@@ -4141,13 +4145,13 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>02-24-2008</t>
+          <t>05-02-2007</t>
         </is>
       </c>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
@@ -4166,7 +4170,7 @@
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R42" t="inlineStr"/>
@@ -4189,7 +4193,7 @@
       <c r="AA42" t="inlineStr"/>
       <c r="AB42" t="inlineStr">
         <is>
-          <t>TAVU, RENY RAYMOND VEGA</t>
+          <t>RIVERA, FERDINAND VILLANUEVA</t>
         </is>
       </c>
       <c r="AC42" t="inlineStr"/>
@@ -4197,7 +4201,7 @@
       <c r="AE42" t="inlineStr"/>
       <c r="AF42" t="inlineStr">
         <is>
-          <t>RAMOS,ADELAIDA,SANCHEZ,</t>
+          <t>MIRANDA,SHEILA ROSE,BAYANID,</t>
         </is>
       </c>
       <c r="AG42" t="inlineStr"/>
@@ -4210,86 +4214,44 @@
       <c r="AN42" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>164512130105</t>
-        </is>
+      <c r="A43" t="n">
+        <v>18</v>
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>VARGAS,REIGN BEYONCE, GUILLERMO</t>
+          <t>&lt;=== TOTAL FEMALE</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>11-03-2007</t>
-        </is>
-      </c>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t xml:space="preserve">11 </t>
-        </is>
-      </c>
+      <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>Tagalog</t>
-        </is>
-      </c>
+      <c r="L43" t="inlineStr"/>
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>Christianity</t>
-        </is>
-      </c>
+      <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr"/>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>ZAPOTE</t>
-        </is>
-      </c>
+      <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr"/>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr">
-        <is>
-          <t>CITY OF BIÑAN</t>
-        </is>
-      </c>
+      <c r="U43" t="inlineStr"/>
       <c r="V43" t="inlineStr"/>
       <c r="W43" t="inlineStr"/>
-      <c r="X43" t="inlineStr">
-        <is>
-          <t>LAGUNA</t>
-        </is>
-      </c>
+      <c r="X43" t="inlineStr"/>
       <c r="Y43" t="inlineStr"/>
       <c r="Z43" t="inlineStr"/>
       <c r="AA43" t="inlineStr"/>
-      <c r="AB43" t="inlineStr">
-        <is>
-          <t>VARGAS, JUSSELLE SARMIENTO</t>
-        </is>
-      </c>
+      <c r="AB43" t="inlineStr"/>
       <c r="AC43" t="inlineStr"/>
       <c r="AD43" t="inlineStr"/>
       <c r="AE43" t="inlineStr"/>
-      <c r="AF43" t="inlineStr">
-        <is>
-          <t>GUILLERMO,ADEL,LIMBAG,</t>
-        </is>
-      </c>
+      <c r="AF43" t="inlineStr"/>
       <c r="AG43" t="inlineStr"/>
       <c r="AH43" t="inlineStr"/>
       <c r="AI43" t="inlineStr"/>
@@ -4301,12 +4263,12 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>&lt;=== TOTAL FEMALE</t>
+          <t>&lt;=== COMBINED</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
@@ -4348,15 +4310,13 @@
       <c r="AN44" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>36</v>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>List and Code of Indicators under REMARKS column</t>
+        </is>
       </c>
       <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>&lt;=== COMBINED</t>
-        </is>
-      </c>
+      <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
@@ -4398,22 +4358,42 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>List and Code of Indicators under REMARKS column</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr"/>
+          <t>Indicator</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Code</t>
+        </is>
+      </c>
       <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Required Information</t>
+        </is>
+      </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Indicator</t>
+        </is>
+      </c>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>Code</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>Required Information</t>
+        </is>
+      </c>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
@@ -4421,21 +4401,41 @@
       <c r="S46" t="inlineStr"/>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr"/>
-      <c r="V46" t="inlineStr"/>
+      <c r="V46" t="inlineStr">
+        <is>
+          <t>REGISTERED</t>
+        </is>
+      </c>
       <c r="W46" t="inlineStr"/>
       <c r="X46" t="inlineStr"/>
-      <c r="Y46" t="inlineStr"/>
-      <c r="Z46" t="inlineStr"/>
+      <c r="Y46" t="inlineStr">
+        <is>
+          <t>BoSY</t>
+        </is>
+      </c>
+      <c r="Z46" t="inlineStr">
+        <is>
+          <t>EoSY</t>
+        </is>
+      </c>
       <c r="AA46" t="inlineStr"/>
       <c r="AB46" t="inlineStr"/>
       <c r="AC46" t="inlineStr"/>
-      <c r="AD46" t="inlineStr"/>
+      <c r="AD46" t="inlineStr">
+        <is>
+          <t>Prepared by;</t>
+        </is>
+      </c>
       <c r="AE46" t="inlineStr"/>
       <c r="AF46" t="inlineStr"/>
       <c r="AG46" t="inlineStr"/>
       <c r="AH46" t="inlineStr"/>
       <c r="AI46" t="inlineStr"/>
-      <c r="AJ46" t="inlineStr"/>
+      <c r="AJ46" t="inlineStr">
+        <is>
+          <t>Certified Correct:</t>
+        </is>
+      </c>
       <c r="AK46" t="inlineStr"/>
       <c r="AL46" t="inlineStr"/>
       <c r="AM46" t="inlineStr"/>
@@ -4444,18 +4444,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Indicator</t>
+          <t xml:space="preserve">Transfered Out
+Transfered In
+Dropped
+</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Code</t>
+          <t>T/O
+T/I
+DRP
+LE</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Required Information</t>
+          <t xml:space="preserve">Name of  Public (P) Private (PR) School  &amp; Effectivity Date
+Name of  Public (P) Private (PR) School  &amp; Effectivity Date
+Reason  and Effectivity Date
+Reason (Enrollment beyond 1st Friday of </t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -4464,7 +4473,10 @@
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Indicator</t>
+          <t>CCT Receipient
+Balik Aral
+Learner With Disability
+Accelerated</t>
         </is>
       </c>
       <c r="J47" t="inlineStr"/>
@@ -4472,12 +4484,18 @@
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Code</t>
+          <t>CCT
+B/A
+LWD
+ACL</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>Required Information</t>
+          <t>CCT Control/reference number &amp; Effectivity Date
+Name of school last attended &amp; Year
+Specify
+Specify Level &amp; Effectivity Data</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
@@ -4489,27 +4507,23 @@
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr">
         <is>
-          <t>REGISTERED</t>
+          <t>MALE</t>
         </is>
       </c>
       <c r="W47" t="inlineStr"/>
       <c r="X47" t="inlineStr"/>
       <c r="Y47" t="inlineStr">
         <is>
-          <t>BoSY</t>
-        </is>
-      </c>
-      <c r="Z47" t="inlineStr">
-        <is>
-          <t>EoSY</t>
-        </is>
-      </c>
+          <t xml:space="preserve">17 </t>
+        </is>
+      </c>
+      <c r="Z47" t="inlineStr"/>
       <c r="AA47" t="inlineStr"/>
       <c r="AB47" t="inlineStr"/>
       <c r="AC47" t="inlineStr"/>
       <c r="AD47" t="inlineStr">
         <is>
-          <t>Prepared by;</t>
+          <t>LAMBERTO BOLIMA RIVAREZ</t>
         </is>
       </c>
       <c r="AE47" t="inlineStr"/>
@@ -4519,7 +4533,7 @@
       <c r="AI47" t="inlineStr"/>
       <c r="AJ47" t="inlineStr">
         <is>
-          <t>Certified Correct:</t>
+          <t>ELSA MONTERERO MANALO</t>
         </is>
       </c>
       <c r="AK47" t="inlineStr"/>
@@ -4528,62 +4542,20 @@
       <c r="AN47" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Transfered Out
-Transfered In
-Dropped
-Late Enrollment</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>T/O
-T/I
-DRP
-LE</t>
-        </is>
-      </c>
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Name of  Public (P) Private (PR) School  &amp; Effectivity Date
-Name of  Public (P) Private (PR) School  &amp; Effectivity Date
-Reason  and Effectivity Date
-Reason (Enrollment beyond 1st Friday of June)</t>
-        </is>
-      </c>
+      <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>CCT Receipient
-Balik Aral
-Learner With Disability
-Accelerated</t>
-        </is>
-      </c>
+      <c r="I48" t="inlineStr"/>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>CCT
-B/A
-LWD
-ACL</t>
-        </is>
-      </c>
-      <c r="N48" t="inlineStr">
-        <is>
-          <t>CCT Control/reference number &amp; Effectivity Date
-Name of school last attended &amp; Year
-Specify
-Specify Level &amp; Effectivity Data</t>
-        </is>
-      </c>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
@@ -4593,23 +4565,19 @@
       <c r="U48" t="inlineStr"/>
       <c r="V48" t="inlineStr">
         <is>
-          <t>MALE</t>
+          <t>FEMALE</t>
         </is>
       </c>
       <c r="W48" t="inlineStr"/>
       <c r="X48" t="inlineStr"/>
-      <c r="Y48" t="n">
-        <v>16</v>
-      </c>
-      <c r="Z48" t="n">
-        <v>15</v>
-      </c>
+      <c r="Y48" t="inlineStr"/>
+      <c r="Z48" t="inlineStr"/>
       <c r="AA48" t="inlineStr"/>
       <c r="AB48" t="inlineStr"/>
       <c r="AC48" t="inlineStr"/>
       <c r="AD48" t="inlineStr">
         <is>
-          <t>LAMBERTO BOLIMA RIVAREZ</t>
+          <t>(Signature of Adviser over Printed Name)</t>
         </is>
       </c>
       <c r="AE48" t="inlineStr"/>
@@ -4619,7 +4587,7 @@
       <c r="AI48" t="inlineStr"/>
       <c r="AJ48" t="inlineStr">
         <is>
-          <t>ELSA MONTERERO MANALO</t>
+          <t>(Signature of School Head over Printed Name)</t>
         </is>
       </c>
       <c r="AK48" t="inlineStr"/>
@@ -4652,7 +4620,9 @@
       <c r="V49" t="inlineStr"/>
       <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr"/>
-      <c r="Y49" t="inlineStr"/>
+      <c r="Y49" t="n">
+        <v>18</v>
+      </c>
       <c r="Z49" t="inlineStr"/>
       <c r="AA49" t="inlineStr"/>
       <c r="AB49" t="inlineStr"/>
@@ -4691,32 +4661,54 @@
       <c r="S50" t="inlineStr"/>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
-      <c r="V50" t="inlineStr"/>
+      <c r="V50" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
       <c r="W50" t="inlineStr"/>
       <c r="X50" t="inlineStr"/>
-      <c r="Y50" t="inlineStr"/>
+      <c r="Y50" t="n">
+        <v>35</v>
+      </c>
       <c r="Z50" t="inlineStr"/>
       <c r="AA50" t="inlineStr"/>
       <c r="AB50" t="inlineStr"/>
       <c r="AC50" t="inlineStr"/>
-      <c r="AD50" t="inlineStr"/>
+      <c r="AD50" t="inlineStr">
+        <is>
+          <t>BoSY Date:</t>
+        </is>
+      </c>
       <c r="AE50" t="inlineStr"/>
       <c r="AF50" t="inlineStr"/>
-      <c r="AG50" t="inlineStr"/>
+      <c r="AG50" t="inlineStr">
+        <is>
+          <t>EoSY Date:</t>
+        </is>
+      </c>
       <c r="AH50" t="inlineStr"/>
       <c r="AI50" t="inlineStr"/>
       <c r="AJ50" t="inlineStr">
         <is>
-          <t>(Signature of School Head over Printed Name)</t>
+          <t>BoSY Date:</t>
         </is>
       </c>
       <c r="AK50" t="inlineStr"/>
       <c r="AL50" t="inlineStr"/>
-      <c r="AM50" t="inlineStr"/>
+      <c r="AM50" t="inlineStr">
+        <is>
+          <t>EoSY Date:</t>
+        </is>
+      </c>
       <c r="AN50" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr"/>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Generated on: Tuesday, September 12, 2017</t>
+        </is>
+      </c>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
@@ -4737,27 +4729,15 @@
       <c r="S51" t="inlineStr"/>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
-      <c r="V51" t="inlineStr">
-        <is>
-          <t>FEMALE</t>
-        </is>
-      </c>
+      <c r="V51" t="inlineStr"/>
       <c r="W51" t="inlineStr"/>
       <c r="X51" t="inlineStr"/>
-      <c r="Y51" t="n">
-        <v>19</v>
-      </c>
-      <c r="Z51" t="n">
-        <v>20</v>
-      </c>
+      <c r="Y51" t="inlineStr"/>
+      <c r="Z51" t="inlineStr"/>
       <c r="AA51" t="inlineStr"/>
       <c r="AB51" t="inlineStr"/>
       <c r="AC51" t="inlineStr"/>
-      <c r="AD51" t="inlineStr">
-        <is>
-          <t>(Signature of Adviser over Printed Name)</t>
-        </is>
-      </c>
+      <c r="AD51" t="inlineStr"/>
       <c r="AE51" t="inlineStr"/>
       <c r="AF51" t="inlineStr"/>
       <c r="AG51" t="inlineStr"/>
@@ -4769,290 +4749,6 @@
       <c r="AM51" t="inlineStr"/>
       <c r="AN51" t="inlineStr"/>
     </row>
-    <row r="52">
-      <c r="A52" t="inlineStr"/>
-      <c r="B52" t="inlineStr"/>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr"/>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="inlineStr"/>
-      <c r="I52" t="inlineStr"/>
-      <c r="J52" t="inlineStr"/>
-      <c r="K52" t="inlineStr"/>
-      <c r="L52" t="inlineStr"/>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
-      <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr"/>
-      <c r="Q52" t="inlineStr"/>
-      <c r="R52" t="inlineStr"/>
-      <c r="S52" t="inlineStr"/>
-      <c r="T52" t="inlineStr"/>
-      <c r="U52" t="inlineStr"/>
-      <c r="V52" t="inlineStr"/>
-      <c r="W52" t="inlineStr"/>
-      <c r="X52" t="inlineStr"/>
-      <c r="Y52" t="inlineStr"/>
-      <c r="Z52" t="inlineStr"/>
-      <c r="AA52" t="inlineStr"/>
-      <c r="AB52" t="inlineStr"/>
-      <c r="AC52" t="inlineStr"/>
-      <c r="AD52" t="inlineStr"/>
-      <c r="AE52" t="inlineStr"/>
-      <c r="AF52" t="inlineStr"/>
-      <c r="AG52" t="inlineStr"/>
-      <c r="AH52" t="inlineStr"/>
-      <c r="AI52" t="inlineStr"/>
-      <c r="AJ52" t="inlineStr">
-        <is>
-          <t>BoSY Date:                06-03-2019</t>
-        </is>
-      </c>
-      <c r="AK52" t="inlineStr"/>
-      <c r="AL52" t="inlineStr"/>
-      <c r="AM52" t="inlineStr">
-        <is>
-          <t>EoSY Date:                    04-03-2020</t>
-        </is>
-      </c>
-      <c r="AN52" t="inlineStr"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr"/>
-      <c r="B53" t="inlineStr"/>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr"/>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr"/>
-      <c r="J53" t="inlineStr"/>
-      <c r="K53" t="inlineStr"/>
-      <c r="L53" t="inlineStr"/>
-      <c r="M53" t="inlineStr"/>
-      <c r="N53" t="inlineStr"/>
-      <c r="O53" t="inlineStr"/>
-      <c r="P53" t="inlineStr"/>
-      <c r="Q53" t="inlineStr"/>
-      <c r="R53" t="inlineStr"/>
-      <c r="S53" t="inlineStr"/>
-      <c r="T53" t="inlineStr"/>
-      <c r="U53" t="inlineStr"/>
-      <c r="V53" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="W53" t="inlineStr"/>
-      <c r="X53" t="inlineStr"/>
-      <c r="Y53" t="n">
-        <v>35</v>
-      </c>
-      <c r="Z53" t="n">
-        <v>35</v>
-      </c>
-      <c r="AA53" t="inlineStr"/>
-      <c r="AB53" t="inlineStr"/>
-      <c r="AC53" t="inlineStr"/>
-      <c r="AD53" t="inlineStr">
-        <is>
-          <t>BoSY Date:                06-03-2019</t>
-        </is>
-      </c>
-      <c r="AE53" t="inlineStr"/>
-      <c r="AF53" t="inlineStr"/>
-      <c r="AG53" t="inlineStr">
-        <is>
-          <t>EoSY Date:                  04-03-2020</t>
-        </is>
-      </c>
-      <c r="AH53" t="inlineStr"/>
-      <c r="AI53" t="inlineStr"/>
-      <c r="AJ53" t="inlineStr"/>
-      <c r="AK53" t="inlineStr"/>
-      <c r="AL53" t="inlineStr"/>
-      <c r="AM53" t="inlineStr"/>
-      <c r="AN53" t="inlineStr"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr"/>
-      <c r="B54" t="inlineStr"/>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr"/>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr"/>
-      <c r="J54" t="inlineStr"/>
-      <c r="K54" t="inlineStr"/>
-      <c r="L54" t="inlineStr"/>
-      <c r="M54" t="inlineStr"/>
-      <c r="N54" t="inlineStr"/>
-      <c r="O54" t="inlineStr"/>
-      <c r="P54" t="inlineStr"/>
-      <c r="Q54" t="inlineStr"/>
-      <c r="R54" t="inlineStr"/>
-      <c r="S54" t="inlineStr"/>
-      <c r="T54" t="inlineStr"/>
-      <c r="U54" t="inlineStr"/>
-      <c r="V54" t="inlineStr"/>
-      <c r="W54" t="inlineStr"/>
-      <c r="X54" t="inlineStr"/>
-      <c r="Y54" t="inlineStr"/>
-      <c r="Z54" t="inlineStr"/>
-      <c r="AA54" t="inlineStr"/>
-      <c r="AB54" t="inlineStr"/>
-      <c r="AC54" t="inlineStr"/>
-      <c r="AD54" t="inlineStr"/>
-      <c r="AE54" t="inlineStr"/>
-      <c r="AF54" t="inlineStr"/>
-      <c r="AG54" t="inlineStr"/>
-      <c r="AH54" t="inlineStr"/>
-      <c r="AI54" t="inlineStr"/>
-      <c r="AJ54" t="inlineStr"/>
-      <c r="AK54" t="inlineStr"/>
-      <c r="AL54" t="inlineStr"/>
-      <c r="AM54" t="inlineStr"/>
-      <c r="AN54" t="inlineStr"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr"/>
-      <c r="B55" t="inlineStr"/>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr"/>
-      <c r="J55" t="inlineStr"/>
-      <c r="K55" t="inlineStr"/>
-      <c r="L55" t="inlineStr"/>
-      <c r="M55" t="inlineStr"/>
-      <c r="N55" t="inlineStr"/>
-      <c r="O55" t="inlineStr"/>
-      <c r="P55" t="inlineStr"/>
-      <c r="Q55" t="inlineStr"/>
-      <c r="R55" t="inlineStr"/>
-      <c r="S55" t="inlineStr"/>
-      <c r="T55" t="inlineStr"/>
-      <c r="U55" t="inlineStr"/>
-      <c r="V55" t="inlineStr"/>
-      <c r="W55" t="inlineStr"/>
-      <c r="X55" t="inlineStr"/>
-      <c r="Y55" t="inlineStr"/>
-      <c r="Z55" t="inlineStr"/>
-      <c r="AA55" t="inlineStr"/>
-      <c r="AB55" t="inlineStr"/>
-      <c r="AC55" t="inlineStr"/>
-      <c r="AD55" t="inlineStr"/>
-      <c r="AE55" t="inlineStr"/>
-      <c r="AF55" t="inlineStr"/>
-      <c r="AG55" t="inlineStr"/>
-      <c r="AH55" t="inlineStr"/>
-      <c r="AI55" t="inlineStr"/>
-      <c r="AJ55" t="inlineStr"/>
-      <c r="AK55" t="inlineStr"/>
-      <c r="AL55" t="inlineStr"/>
-      <c r="AM55" t="inlineStr"/>
-      <c r="AN55" t="inlineStr"/>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr"/>
-      <c r="B56" t="inlineStr"/>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
-      <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
-      <c r="J56" t="inlineStr"/>
-      <c r="K56" t="inlineStr"/>
-      <c r="L56" t="inlineStr"/>
-      <c r="M56" t="inlineStr"/>
-      <c r="N56" t="inlineStr"/>
-      <c r="O56" t="inlineStr"/>
-      <c r="P56" t="inlineStr"/>
-      <c r="Q56" t="inlineStr"/>
-      <c r="R56" t="inlineStr"/>
-      <c r="S56" t="inlineStr"/>
-      <c r="T56" t="inlineStr"/>
-      <c r="U56" t="inlineStr"/>
-      <c r="V56" t="inlineStr"/>
-      <c r="W56" t="inlineStr"/>
-      <c r="X56" t="inlineStr"/>
-      <c r="Y56" t="inlineStr"/>
-      <c r="Z56" t="inlineStr"/>
-      <c r="AA56" t="inlineStr"/>
-      <c r="AB56" t="inlineStr"/>
-      <c r="AC56" t="inlineStr"/>
-      <c r="AD56" t="inlineStr"/>
-      <c r="AE56" t="inlineStr"/>
-      <c r="AF56" t="inlineStr"/>
-      <c r="AG56" t="inlineStr"/>
-      <c r="AH56" t="inlineStr"/>
-      <c r="AI56" t="inlineStr"/>
-      <c r="AJ56" t="inlineStr">
-        <is>
-          <t>Generated thru LIS</t>
-        </is>
-      </c>
-      <c r="AK56" t="inlineStr"/>
-      <c r="AL56" t="inlineStr"/>
-      <c r="AM56" t="inlineStr"/>
-      <c r="AN56" t="inlineStr"/>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Generated on: Saturday, March 21, 2020</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr"/>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr"/>
-      <c r="J57" t="inlineStr"/>
-      <c r="K57" t="inlineStr"/>
-      <c r="L57" t="inlineStr"/>
-      <c r="M57" t="inlineStr"/>
-      <c r="N57" t="inlineStr"/>
-      <c r="O57" t="inlineStr"/>
-      <c r="P57" t="inlineStr"/>
-      <c r="Q57" t="inlineStr"/>
-      <c r="R57" t="inlineStr"/>
-      <c r="S57" t="inlineStr"/>
-      <c r="T57" t="inlineStr"/>
-      <c r="U57" t="inlineStr"/>
-      <c r="V57" t="inlineStr"/>
-      <c r="W57" t="inlineStr"/>
-      <c r="X57" t="inlineStr"/>
-      <c r="Y57" t="inlineStr"/>
-      <c r="Z57" t="inlineStr"/>
-      <c r="AA57" t="inlineStr"/>
-      <c r="AB57" t="inlineStr"/>
-      <c r="AC57" t="inlineStr"/>
-      <c r="AD57" t="inlineStr"/>
-      <c r="AE57" t="inlineStr"/>
-      <c r="AF57" t="inlineStr"/>
-      <c r="AG57" t="inlineStr"/>
-      <c r="AH57" t="inlineStr"/>
-      <c r="AI57" t="inlineStr"/>
-      <c r="AJ57" t="inlineStr"/>
-      <c r="AK57" t="inlineStr"/>
-      <c r="AL57" t="inlineStr"/>
-      <c r="AM57" t="inlineStr"/>
-      <c r="AN57" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
display school year ui fixed
</commit_message>
<xml_diff>
--- a/Migrade_v.1.2/temp.xlsx
+++ b/Migrade_v.1.2/temp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN51"/>
+  <dimension ref="A1:AN57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -782,7 +782,7 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr">
         <is>
-          <t>2017 - 2018</t>
+          <t>2019 - 2020</t>
         </is>
       </c>
       <c r="T4" t="inlineStr"/>
@@ -791,7 +791,7 @@
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Grade </t>
+          <t xml:space="preserve">Grade Level </t>
         </is>
       </c>
       <c r="Y4" t="inlineStr"/>
@@ -799,7 +799,7 @@
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>Grade 5</t>
+          <t>Grade 6</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr"/>
@@ -813,7 +813,7 @@
       <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>EARTH</t>
+          <t>GALILEO</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr"/>
@@ -853,7 +853,7 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Age as of August 31st</t>
+          <t>AGE as of 1st Friday June</t>
         </is>
       </c>
       <c r="K5" t="inlineStr"/>
@@ -975,7 +975,7 @@
       <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mother's Maiden Name (Last Name, First Name, Middle </t>
+          <t>Mother's Maiden Name (Last Name, First Name, Middle Name)</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr"/>
@@ -1002,13 +1002,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>164512110014</t>
+          <t>164512130171</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>BORLAGDAN, ALFIE BISMAR</t>
+          <t>ANIBAN,LEO JELLY, TINAPAY</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -1021,13 +1021,13 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>05-18-2005</t>
+          <t>09-23-2008</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K7" t="inlineStr"/>
@@ -1069,7 +1069,7 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>BORLAGDAN, ALLAN GOLEMLEM</t>
+          <t>ANIBAN, LEO BUTAL</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr"/>
@@ -1077,7 +1077,7 @@
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>BISMAR,CARMENCITA,BLANQUEZA,</t>
+          <t>TINAPAY,JILL,BAJADI,</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr"/>
@@ -1092,13 +1092,13 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>164512130010</t>
+          <t>164512130045</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>BORLAGDAN, RJ BISMAR</t>
+          <t>ASILO,RAIN JUSTINE, MERCADO</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -1111,13 +1111,13 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>11-11-2006</t>
+          <t>05-20-2007</t>
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K8" t="inlineStr"/>
@@ -1136,7 +1136,7 @@
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R8" t="inlineStr"/>
@@ -1159,7 +1159,7 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>BORLAGDAN, ALLAN GOLEMLEM</t>
+          <t>ASILO, CHRISTOPHER SALILICAN</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr"/>
@@ -1167,7 +1167,7 @@
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>BISMAR,CARMENCITA,BLANQUEZA,</t>
+          <t>MERCADO,MARICEL,HERNANDEZ,</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr"/>
@@ -1182,13 +1182,13 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>136907120127</t>
+          <t>424663150037</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CAMBE, RALPH LOUIE ARAGON</t>
+          <t>CAMBE,SEAN DAVE, ARAGON</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -1201,13 +1201,13 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>03-02-2007</t>
+          <t>03-15-2008</t>
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K9" t="inlineStr"/>
@@ -1267,22 +1267,18 @@
       <c r="AK9" t="inlineStr"/>
       <c r="AL9" t="inlineStr"/>
       <c r="AM9" t="inlineStr"/>
-      <c r="AN9" t="inlineStr">
-        <is>
-          <t>T/I DATE:2017-06-05</t>
-        </is>
-      </c>
+      <c r="AN9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>164512130016</t>
+          <t>164512140032</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CAONES, JAYRUS CARL LACANIN</t>
+          <t>CARANAY,JHAYCEE CARL, CORDERO</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -1295,7 +1291,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>08-25-2006</t>
+          <t>11-25-2007</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
@@ -1343,7 +1339,7 @@
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>CAONES, JAYZON NUNAY</t>
+          <t>CARANAY, ROGELIO JR CABOTAJE</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr"/>
@@ -1351,7 +1347,7 @@
       <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="inlineStr">
         <is>
-          <t>LACANIN,JERLYN,BELO,</t>
+          <t>CORDERO,NORMA,ALIDO,</t>
         </is>
       </c>
       <c r="AG10" t="inlineStr"/>
@@ -1366,13 +1362,13 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>164512120011</t>
+          <t>164512140029</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CELESTE, ANDREW ACE ESPINOSA</t>
+          <t>CASTRO,ICHIRO, MENDOZA</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -1385,7 +1381,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>02-09-2007</t>
+          <t>09-08-2008</t>
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
@@ -1410,7 +1406,7 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>PLATERO</t>
         </is>
       </c>
       <c r="R11" t="inlineStr"/>
@@ -1433,7 +1429,7 @@
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>CELESTE, ALEJANDRO SARVIDA</t>
+          <t>CASTRO, SEVERLINO ABAPO</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr"/>
@@ -1441,7 +1437,7 @@
       <c r="AE11" t="inlineStr"/>
       <c r="AF11" t="inlineStr">
         <is>
-          <t>ESPINOSA,LORENA,ALBERTO,</t>
+          <t>MENDOZA,ALICIA,ZULUETA,</t>
         </is>
       </c>
       <c r="AG11" t="inlineStr"/>
@@ -1456,13 +1452,13 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>164512130047</t>
+          <t>164512150094</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CUPANG, CHRISTIAN ZAMORA</t>
+          <t>CAYLAO,DAYNE, VIÑA</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -1475,13 +1471,13 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>06-21-2007</t>
+          <t>03-17-2007</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K12" t="inlineStr"/>
@@ -1500,7 +1496,7 @@
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>PLATERO</t>
         </is>
       </c>
       <c r="R12" t="inlineStr"/>
@@ -1523,7 +1519,7 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>CUPANG, ANTONIO CRISMUNDO JR</t>
+          <t>CAYLAO, DANZEL CIPRIANO</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr"/>
@@ -1531,7 +1527,7 @@
       <c r="AE12" t="inlineStr"/>
       <c r="AF12" t="inlineStr">
         <is>
-          <t>ZAMORA,TERESITA,ALING,</t>
+          <t>VIÑA,CAREN,CRUZ,</t>
         </is>
       </c>
       <c r="AG12" t="inlineStr"/>
@@ -1546,13 +1542,13 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>108226120133</t>
+          <t>164512130131</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>GABATIN, KING TYRON GILBERT AMORTIZADO</t>
+          <t>CHAN,JHON RHAYNE, REPELAR</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -1565,13 +1561,13 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>11-10-2004</t>
+          <t>01-16-2008</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K13" t="inlineStr"/>
@@ -1613,7 +1609,7 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>GABATIN, TEOFILO TACSIAT</t>
+          <t>CHAN, JONATHAN ALICARTE</t>
         </is>
       </c>
       <c r="AC13" t="inlineStr"/>
@@ -1621,7 +1617,7 @@
       <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="inlineStr">
         <is>
-          <t>AMORTIZADO,MARIA LOURDES,CAPUQUIAN,</t>
+          <t>REPELAR,ELENA,ROXAS,</t>
         </is>
       </c>
       <c r="AG13" t="inlineStr"/>
@@ -1636,13 +1632,13 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>164512130022</t>
+          <t>402456150012</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>LAGADI, JHOSUA BUSTAMANTE</t>
+          <t>GETALADO,EARL SAMUEL, CLAVE</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -1655,7 +1651,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>11-08-2006</t>
+          <t>09-10-2008</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -1680,7 +1676,7 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R14" t="inlineStr"/>
@@ -1703,7 +1699,7 @@
       <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>LAGADI, VICENTE GABRIEL JR</t>
+          <t>GETALADO, ERNESTO CERTEZA</t>
         </is>
       </c>
       <c r="AC14" t="inlineStr"/>
@@ -1711,7 +1707,7 @@
       <c r="AE14" t="inlineStr"/>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>BUSTAMANTE,ELIZA,BULARON,</t>
+          <t>CLAVE,SERENIDAD,TABLIZO,</t>
         </is>
       </c>
       <c r="AG14" t="inlineStr"/>
@@ -1726,13 +1722,13 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>112505130003</t>
+          <t>164512130101</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LLANZA, ALFREDO LAYCO JR</t>
+          <t>GLOBIO,MARCKY, GALVAN</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -1745,13 +1741,13 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>09-28-2006</t>
+          <t>03-11-2008</t>
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
@@ -1770,7 +1766,7 @@
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>SANTO NINO</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R15" t="inlineStr"/>
@@ -1791,17 +1787,13 @@
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="inlineStr">
-        <is>
-          <t>LLANZA, ALFREDO CARGALLO SR</t>
-        </is>
-      </c>
+      <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="inlineStr"/>
       <c r="AD15" t="inlineStr"/>
       <c r="AE15" t="inlineStr"/>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>LAYCO,ARCELI,MONTANEZ,</t>
+          <t>GLOBIO,RENITA,GALVAN,</t>
         </is>
       </c>
       <c r="AG15" t="inlineStr"/>
@@ -1811,18 +1803,22 @@
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr"/>
       <c r="AM15" t="inlineStr"/>
-      <c r="AN15" t="inlineStr"/>
+      <c r="AN15" t="inlineStr">
+        <is>
+          <t>DRP "Family Problem"Date:2019/11/04</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>164512130024</t>
+          <t>164512140006</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MALINTAD, JAMES DUMAYO</t>
+          <t>MIRANDA,ANDREI, BIANES</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -1835,13 +1831,13 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>03-05-2007</t>
+          <t>04-29-2007</t>
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
@@ -1860,7 +1856,7 @@
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R16" t="inlineStr"/>
@@ -1883,7 +1879,7 @@
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>MALINTAD, GREMER CAONG</t>
+          <t>MIRANDA, ESTELITO VILLANUEVA</t>
         </is>
       </c>
       <c r="AC16" t="inlineStr"/>
@@ -1891,7 +1887,7 @@
       <c r="AE16" t="inlineStr"/>
       <c r="AF16" t="inlineStr">
         <is>
-          <t>DUMAYO,MINDA,TUMIMO,</t>
+          <t>BIANES,JENNIFER,QUINTUA,</t>
         </is>
       </c>
       <c r="AG16" t="inlineStr"/>
@@ -1901,18 +1897,22 @@
       <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="inlineStr"/>
-      <c r="AN16" t="inlineStr"/>
+      <c r="AN16" t="inlineStr">
+        <is>
+          <t>T/I Pook Elem. Sch. Date:2019-06-03</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>164512130027</t>
+          <t>164512130118</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MATULA, JOHN GABRIEL ZAVALLA</t>
+          <t>NAVAREZ,ANDREI, MONTAÑEZ</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -1925,13 +1925,13 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>09-25-2006</t>
+          <t>07-26-2007</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K17" t="inlineStr"/>
@@ -1973,7 +1973,7 @@
       <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>MATULA, VICTOR GONZALES</t>
+          <t>NAVAREZ, ARNEL NABUHAY</t>
         </is>
       </c>
       <c r="AC17" t="inlineStr"/>
@@ -1981,7 +1981,7 @@
       <c r="AE17" t="inlineStr"/>
       <c r="AF17" t="inlineStr">
         <is>
-          <t>ZAVALLA,FLORENCIA,NILLO,</t>
+          <t>MONTAÑEZ,SUSANA,VILLARIN,</t>
         </is>
       </c>
       <c r="AG17" t="inlineStr"/>
@@ -1996,13 +1996,13 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>164512120051</t>
+          <t>164512100132</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>OLIVEROS, JHONUEL BISMAR</t>
+          <t>SALAYSAY,JOHN LOUIE, FLORES</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -2015,13 +2015,13 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>01-16-2007</t>
+          <t>02-18-2004</t>
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">15 </t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
@@ -2063,7 +2063,7 @@
       <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>OLIVEROS, JOEL AFANTE</t>
+          <t>SALAYSAY, ALFREDO REYES</t>
         </is>
       </c>
       <c r="AC18" t="inlineStr"/>
@@ -2071,7 +2071,7 @@
       <c r="AE18" t="inlineStr"/>
       <c r="AF18" t="inlineStr">
         <is>
-          <t>BLANQUEZA,JANET,BISMAR,</t>
+          <t>FLORES,CECILIA,LOPENA,</t>
         </is>
       </c>
       <c r="AG18" t="inlineStr"/>
@@ -2086,13 +2086,13 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>108474140114</t>
+          <t>108476120166</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>QUILLOSA, MERICK MASAREDO</t>
+          <t>SAMANIEGO,MATTHEW ANDREI, ANGULO</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
@@ -2105,13 +2105,13 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>10-04-2006</t>
+          <t>08-01-2006</t>
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
@@ -2130,7 +2130,7 @@
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R19" t="inlineStr"/>
@@ -2153,7 +2153,7 @@
       <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>QUILLOSA, MARVIN MANLOLO</t>
+          <t>SAMANIEGO, MICHAEL ABUCEJO</t>
         </is>
       </c>
       <c r="AC19" t="inlineStr"/>
@@ -2161,7 +2161,7 @@
       <c r="AE19" t="inlineStr"/>
       <c r="AF19" t="inlineStr">
         <is>
-          <t>MASAREDO,PERLA,ACOSTA,</t>
+          <t>ANGULO,ABIGAIL,GUSTILO,</t>
         </is>
       </c>
       <c r="AG19" t="inlineStr"/>
@@ -2176,13 +2176,13 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>164512130030</t>
+          <t>108426130045</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>SANGYAHON, JUSTINE MAGTAGAD</t>
+          <t>SAN JUAN JR.,ARLY, PLATINO</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
@@ -2195,13 +2195,13 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>09-22-2006</t>
+          <t>09-29-2007</t>
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K20" t="inlineStr"/>
@@ -2243,7 +2243,7 @@
       <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>SANGYAHON, ERLINDO PATRICIO</t>
+          <t>SAN JUAN, ARLY TAPUIC SR</t>
         </is>
       </c>
       <c r="AC20" t="inlineStr"/>
@@ -2251,7 +2251,7 @@
       <c r="AE20" t="inlineStr"/>
       <c r="AF20" t="inlineStr">
         <is>
-          <t>MAGTAGAD,CHERYL,ESPAÑOLA,</t>
+          <t>PLATINO,EVANGELINE,GUILLEN,</t>
         </is>
       </c>
       <c r="AG20" t="inlineStr"/>
@@ -2266,13 +2266,13 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>136775120015</t>
+          <t>164512130091</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
-          <t>SANTOS, ANGELO GALLARDO</t>
+          <t>SANTOS,MARK, BELANO</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>05-15-2007</t>
+          <t>09-05-2008</t>
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
@@ -2333,7 +2333,7 @@
       <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>SANTOS, ARTURO CRUZ</t>
+          <t>SANTOS, ROLANDO BARBOSA</t>
         </is>
       </c>
       <c r="AC21" t="inlineStr"/>
@@ -2341,7 +2341,7 @@
       <c r="AE21" t="inlineStr"/>
       <c r="AF21" t="inlineStr">
         <is>
-          <t>UMALI,GALLARDO,GUADALUPE,</t>
+          <t>BELANO,LIZA,BERIANO,</t>
         </is>
       </c>
       <c r="AG21" t="inlineStr"/>
@@ -2351,22 +2351,18 @@
       <c r="AK21" t="inlineStr"/>
       <c r="AL21" t="inlineStr"/>
       <c r="AM21" t="inlineStr"/>
-      <c r="AN21" t="inlineStr">
-        <is>
-          <t>Pending TI</t>
-        </is>
-      </c>
+      <c r="AN21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>164512120054</t>
+          <t>164512140037</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
-          <t>TABING, RANDEL ABELLA</t>
+          <t>VILLANUEVA,JOSH CYREL, CLASA</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
@@ -2379,13 +2375,13 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>06-16-2007</t>
+          <t>11-09-2007</t>
         </is>
       </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
@@ -2427,7 +2423,7 @@
       <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>TABING, RANDY ESTEBAN</t>
+          <t>VILLANUEVA, PABLITO MARIÑAS</t>
         </is>
       </c>
       <c r="AC22" t="inlineStr"/>
@@ -2435,7 +2431,7 @@
       <c r="AE22" t="inlineStr"/>
       <c r="AF22" t="inlineStr">
         <is>
-          <t>ABELLA,MARIDEL,ENCELAN,</t>
+          <t>CLASA,EVEBERLY,MONTESCO,</t>
         </is>
       </c>
       <c r="AG22" t="inlineStr"/>
@@ -2448,86 +2444,44 @@
       <c r="AN22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>164512120055</t>
-        </is>
+      <c r="A23" t="n">
+        <v>16</v>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
-          <t>VALENCIA, RIN WINZHEL AGUADO</t>
+          <t>&lt;=== TOTAL MALE</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>01-09-2007</t>
-        </is>
-      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">10 </t>
-        </is>
-      </c>
+      <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>Tagalog</t>
-        </is>
-      </c>
+      <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>Christianity</t>
-        </is>
-      </c>
+      <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>ZAPOTE</t>
-        </is>
-      </c>
+      <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>CITY OF BIÑAN</t>
-        </is>
-      </c>
+      <c r="U23" t="inlineStr"/>
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr"/>
-      <c r="X23" t="inlineStr">
-        <is>
-          <t>LAGUNA</t>
-        </is>
-      </c>
+      <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="inlineStr"/>
-      <c r="AB23" t="inlineStr">
-        <is>
-          <t>VALENCIA, CHERWEN MANONGSONG</t>
-        </is>
-      </c>
+      <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="inlineStr"/>
       <c r="AD23" t="inlineStr"/>
       <c r="AE23" t="inlineStr"/>
-      <c r="AF23" t="inlineStr">
-        <is>
-          <t>AGUADO,FRITCHEL,VICTORIO,</t>
-        </is>
-      </c>
+      <c r="AF23" t="inlineStr"/>
       <c r="AG23" t="inlineStr"/>
       <c r="AH23" t="inlineStr"/>
       <c r="AI23" t="inlineStr"/>
@@ -2538,44 +2492,86 @@
       <c r="AN23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>17</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>164512140038</t>
+        </is>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
-          <t>&lt;=== TOTAL MALE</t>
+          <t>ARRESGADO,LEANNE ROSE, CARLOS</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>08-25-2008</t>
+        </is>
+      </c>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr"/>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr"/>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr"/>
-      <c r="X24" t="inlineStr"/>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="inlineStr"/>
-      <c r="AB24" t="inlineStr"/>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>ARRESGADO, JUNARD MALAKARTE</t>
+        </is>
+      </c>
       <c r="AC24" t="inlineStr"/>
       <c r="AD24" t="inlineStr"/>
       <c r="AE24" t="inlineStr"/>
-      <c r="AF24" t="inlineStr"/>
+      <c r="AF24" t="inlineStr">
+        <is>
+          <t>CARLOS,AILEEN,VERANO,</t>
+        </is>
+      </c>
       <c r="AG24" t="inlineStr"/>
       <c r="AH24" t="inlineStr"/>
       <c r="AI24" t="inlineStr"/>
@@ -2588,13 +2584,13 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>164512130075</t>
+          <t>164512140016</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ACILO, CHARLENE DAGUMAN</t>
+          <t>BORCELANGO,DONA LYNN, DAPRINAL</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -2607,7 +2603,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>10-18-2006</t>
+          <t>07-22-2008</t>
         </is>
       </c>
       <c r="I25" t="inlineStr"/>
@@ -2655,7 +2651,7 @@
       <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>ACILO, CHARLITO LOPENA</t>
+          <t>BORCELANGO, DONATO REYES</t>
         </is>
       </c>
       <c r="AC25" t="inlineStr"/>
@@ -2663,7 +2659,7 @@
       <c r="AE25" t="inlineStr"/>
       <c r="AF25" t="inlineStr">
         <is>
-          <t>DAGUMAN,AILENE,ABE,</t>
+          <t>DAPRINAL,JONALINE,ATOR,</t>
         </is>
       </c>
       <c r="AG25" t="inlineStr"/>
@@ -2678,13 +2674,13 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>164512130061</t>
+          <t>164512140017</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
-          <t>BETITO, EURICE ROSACEÑA</t>
+          <t>CAONES,JUSEA MICAH, LACANIN</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
@@ -2697,13 +2693,13 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>05-03-2007</t>
+          <t>01-31-2008</t>
         </is>
       </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K26" t="inlineStr"/>
@@ -2745,7 +2741,7 @@
       <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="inlineStr">
         <is>
-          <t>BETITO, ARMANDO SALAMODING</t>
+          <t>CAONES, JAYZON NUNAY</t>
         </is>
       </c>
       <c r="AC26" t="inlineStr"/>
@@ -2753,7 +2749,7 @@
       <c r="AE26" t="inlineStr"/>
       <c r="AF26" t="inlineStr">
         <is>
-          <t>ROSACENA,REMEDIOS,VILLANUEVA,</t>
+          <t>LACANIN,JERLYN,BELO,</t>
         </is>
       </c>
       <c r="AG26" t="inlineStr"/>
@@ -2768,13 +2764,13 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>164512120064</t>
+          <t>105111130128</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CAFINO, JASMIN CLAIRE CANTIGA</t>
+          <t>CLEMENTE,MARTHA ASHLEE, COLIS</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -2787,7 +2783,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>03-06-2007</t>
+          <t>07-02-2008</t>
         </is>
       </c>
       <c r="I27" t="inlineStr"/>
@@ -2812,7 +2808,7 @@
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R27" t="inlineStr"/>
@@ -2835,7 +2831,7 @@
       <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="inlineStr">
         <is>
-          <t>CAFINO, RODERICK SOREÑO</t>
+          <t>CLEMENTE, RAFAEL KRIS PRONUEVO CLEMENTE</t>
         </is>
       </c>
       <c r="AC27" t="inlineStr"/>
@@ -2843,7 +2839,7 @@
       <c r="AE27" t="inlineStr"/>
       <c r="AF27" t="inlineStr">
         <is>
-          <t>CANTIGA,GRACE,IGNACIO,</t>
+          <t>COLIS,MA NIEVES VALANTINE,CUNANAN,</t>
         </is>
       </c>
       <c r="AG27" t="inlineStr"/>
@@ -2853,18 +2849,22 @@
       <c r="AK27" t="inlineStr"/>
       <c r="AL27" t="inlineStr"/>
       <c r="AM27" t="inlineStr"/>
-      <c r="AN27" t="inlineStr"/>
+      <c r="AN27" t="inlineStr">
+        <is>
+          <t>T/I  San Miguel Elem.Sch.Date:2019-06-03</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>164512120218</t>
+          <t>109850130028</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CLARION, MARY QUEEN MARIEL RAMISO</t>
+          <t>DEL MUNDO,CATHLYN, SALDINO</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
@@ -2877,13 +2877,13 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>10-01-2006</t>
+          <t>11-22-2007</t>
         </is>
       </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K28" t="inlineStr"/>
@@ -2902,7 +2902,7 @@
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R28" t="inlineStr"/>
@@ -2925,7 +2925,7 @@
       <c r="AA28" t="inlineStr"/>
       <c r="AB28" t="inlineStr">
         <is>
-          <t>CLARION, MARCIAL GARRAN</t>
+          <t>DEL MUNDO, JUNE LINGGA</t>
         </is>
       </c>
       <c r="AC28" t="inlineStr"/>
@@ -2933,7 +2933,7 @@
       <c r="AE28" t="inlineStr"/>
       <c r="AF28" t="inlineStr">
         <is>
-          <t>RAMISO,LIEZEL,SIMPO,</t>
+          <t>SALDINO,ANNABELLE,SOLAYAO,</t>
         </is>
       </c>
       <c r="AG28" t="inlineStr"/>
@@ -2948,13 +2948,13 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>164512130029</t>
+          <t>164512130166</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>DIONISO, JHAMAICA ALEGRE</t>
+          <t>DICDICAN,TRISHA ELLAINE, REALON</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>10-25-2005</t>
+          <t>03-01-2008</t>
         </is>
       </c>
       <c r="I29" t="inlineStr"/>
@@ -2992,7 +2992,7 @@
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R29" t="inlineStr"/>
@@ -3015,7 +3015,7 @@
       <c r="AA29" t="inlineStr"/>
       <c r="AB29" t="inlineStr">
         <is>
-          <t>DIONISIO, ROEL CRUZ</t>
+          <t>DICDICAN, RICHARD JIMENEZ</t>
         </is>
       </c>
       <c r="AC29" t="inlineStr"/>
@@ -3023,7 +3023,7 @@
       <c r="AE29" t="inlineStr"/>
       <c r="AF29" t="inlineStr">
         <is>
-          <t>ALEGRE,SHIELA,SAHIRON,</t>
+          <t>REALON,MA CLARISSA,ROLDAN,</t>
         </is>
       </c>
       <c r="AG29" t="inlineStr"/>
@@ -3038,13 +3038,13 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>164512120071</t>
+          <t>164512130124</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ESPINOSA, MIAH JUMAO-AS</t>
+          <t>ESPINAR,ANGIELYN, MARCE</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>12-13-2006</t>
+          <t>07-26-2008</t>
         </is>
       </c>
       <c r="I30" t="inlineStr"/>
@@ -3082,7 +3082,7 @@
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO NINO</t>
         </is>
       </c>
       <c r="R30" t="inlineStr"/>
@@ -3105,7 +3105,7 @@
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr">
         <is>
-          <t>ESPINOSA, BONIFACIO ALVERIO</t>
+          <t>ESPINAR, EDISON FLORALDE</t>
         </is>
       </c>
       <c r="AC30" t="inlineStr"/>
@@ -3113,7 +3113,7 @@
       <c r="AE30" t="inlineStr"/>
       <c r="AF30" t="inlineStr">
         <is>
-          <t>JUMAO-AS,CECILIA,MABATID,</t>
+          <t>MARCE,MARIE GRACE,MONTAÑEZ,</t>
         </is>
       </c>
       <c r="AG30" t="inlineStr"/>
@@ -3128,13 +3128,13 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>164512120033</t>
+          <t>108226120096</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>GABUTAN, ANGIE GOLLAYAN</t>
+          <t>GABATIN,LADY TRISHA, AMORTIZADO</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
@@ -3147,13 +3147,13 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>08-06-2006</t>
+          <t>11-03-2006</t>
         </is>
       </c>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
@@ -3195,7 +3195,7 @@
       <c r="AA31" t="inlineStr"/>
       <c r="AB31" t="inlineStr">
         <is>
-          <t>GABUTAN, ALVE SUMARGO</t>
+          <t>GABATIN, TEOFILO TACSIAT</t>
         </is>
       </c>
       <c r="AC31" t="inlineStr"/>
@@ -3203,7 +3203,7 @@
       <c r="AE31" t="inlineStr"/>
       <c r="AF31" t="inlineStr">
         <is>
-          <t>GOLLAYAN,MARITES,BLANZA,</t>
+          <t>AMORTIZADO,MARIA LOURDES,CAPUQUIAN,</t>
         </is>
       </c>
       <c r="AG31" t="inlineStr"/>
@@ -3218,13 +3218,13 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>164512110030</t>
+          <t>164512130042</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
-          <t>GONZALO, ERICQUEZEN DACASIN</t>
+          <t>JOVEN,JENALEN, MASIKAT</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
@@ -3237,13 +3237,13 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>12-07-2005</t>
+          <t>10-01-2006</t>
         </is>
       </c>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">12 </t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
@@ -3285,7 +3285,7 @@
       <c r="AA32" t="inlineStr"/>
       <c r="AB32" t="inlineStr">
         <is>
-          <t>GONZALO, ERIC TORIO</t>
+          <t>JOVEN, SAMUEL ARCEGA</t>
         </is>
       </c>
       <c r="AC32" t="inlineStr"/>
@@ -3293,7 +3293,7 @@
       <c r="AE32" t="inlineStr"/>
       <c r="AF32" t="inlineStr">
         <is>
-          <t>DACASIN,HEIDE,VERGARA,</t>
+          <t>MASIKAT,CRISTINA,BAYAN,</t>
         </is>
       </c>
       <c r="AG32" t="inlineStr"/>
@@ -3308,13 +3308,13 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>164512130062</t>
+          <t>108407130083</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>HUTALLA, RHIAM CLARIS ESPINOSA</t>
+          <t>MALABAG,ANGELICA, MIRANDA</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
@@ -3327,13 +3327,13 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>01-04-2007</t>
+          <t>12-22-2007</t>
         </is>
       </c>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
@@ -3375,7 +3375,7 @@
       <c r="AA33" t="inlineStr"/>
       <c r="AB33" t="inlineStr">
         <is>
-          <t>HUTALLA, CLARO GONZALES</t>
+          <t>MALABAG, ANGELITO MELICIO</t>
         </is>
       </c>
       <c r="AC33" t="inlineStr"/>
@@ -3383,7 +3383,7 @@
       <c r="AE33" t="inlineStr"/>
       <c r="AF33" t="inlineStr">
         <is>
-          <t>ESPINOSA,MIRIAM,ALMEDA,</t>
+          <t>MIRANDA,MARY ANN,BAYANID,</t>
         </is>
       </c>
       <c r="AG33" t="inlineStr"/>
@@ -3398,13 +3398,13 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>164512130032</t>
+          <t>164512140043</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LLANZA, RUTH MICAH CORPUZ</t>
+          <t>MAMANSAG,JEIAH EUNICE, SERRANO</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>11-24-2006</t>
+          <t>08-09-2008</t>
         </is>
       </c>
       <c r="I34" t="inlineStr"/>
@@ -3442,7 +3442,7 @@
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R34" t="inlineStr"/>
@@ -3465,7 +3465,7 @@
       <c r="AA34" t="inlineStr"/>
       <c r="AB34" t="inlineStr">
         <is>
-          <t>LLANZA, JOSEPH GUEVARRA</t>
+          <t>MAMANSAG, EMMERSON SALCEDO</t>
         </is>
       </c>
       <c r="AC34" t="inlineStr"/>
@@ -3473,7 +3473,7 @@
       <c r="AE34" t="inlineStr"/>
       <c r="AF34" t="inlineStr">
         <is>
-          <t>CORPUZ,CLARISA,BARONIA,</t>
+          <t>SERRANO,GERLIE,VALCOBA,</t>
         </is>
       </c>
       <c r="AG34" t="inlineStr"/>
@@ -3488,13 +3488,13 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>164512130036</t>
+          <t>424638150057</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MACARAIG, MARICRIS SABADO</t>
+          <t>MANALILI,JAMAICA AMOR, ROSALES</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
@@ -3507,13 +3507,13 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>10-16-2007</t>
+          <t>01-21-2008</t>
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr">
         <is>
-          <t xml:space="preserve">9 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
@@ -3532,7 +3532,7 @@
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R35" t="inlineStr"/>
@@ -3555,7 +3555,7 @@
       <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="inlineStr">
         <is>
-          <t>MACARAIG, EDWIN GARCIA</t>
+          <t>MANALILI, JAM ANTHONY CASTILLO</t>
         </is>
       </c>
       <c r="AC35" t="inlineStr"/>
@@ -3563,7 +3563,7 @@
       <c r="AE35" t="inlineStr"/>
       <c r="AF35" t="inlineStr">
         <is>
-          <t>SABADO,MARIA,SARSOZA,</t>
+          <t>ROSALES,RACHEL,MALIBAGO,</t>
         </is>
       </c>
       <c r="AG35" t="inlineStr"/>
@@ -3578,13 +3578,13 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>108231130020</t>
+          <t>164512130089</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MARAÑAN, JERAMIAH ALAHAY</t>
+          <t>MARTINEZ,ASHLEE NICHOLE, SABANAL</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>10-01-2006</t>
+          <t>11-16-2008</t>
         </is>
       </c>
       <c r="I36" t="inlineStr"/>
@@ -3622,7 +3622,7 @@
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R36" t="inlineStr"/>
@@ -3645,7 +3645,7 @@
       <c r="AA36" t="inlineStr"/>
       <c r="AB36" t="inlineStr">
         <is>
-          <t>MARAÑAN, RONNIE CUEME</t>
+          <t>MARTINEZ, MAR JUN BRUCE</t>
         </is>
       </c>
       <c r="AC36" t="inlineStr"/>
@@ -3653,7 +3653,7 @@
       <c r="AE36" t="inlineStr"/>
       <c r="AF36" t="inlineStr">
         <is>
-          <t>TATA,ALAHAY,JOSEPHINE,</t>
+          <t>SABANAL,DESARIE,ALORA,</t>
         </is>
       </c>
       <c r="AG36" t="inlineStr"/>
@@ -3663,22 +3663,18 @@
       <c r="AK36" t="inlineStr"/>
       <c r="AL36" t="inlineStr"/>
       <c r="AM36" t="inlineStr"/>
-      <c r="AN36" t="inlineStr">
-        <is>
-          <t>T/I DATE:2017-06-05</t>
-        </is>
-      </c>
+      <c r="AN36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>164512130037</t>
+          <t>164512140024</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>NAVAL, KRISHA MAY MIRANDA</t>
+          <t>NAVAL,GEARLY SHANE, OCAMPO</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
@@ -3691,13 +3687,13 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>06-01-2007</t>
+          <t>11-03-2007</t>
         </is>
       </c>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
@@ -3739,7 +3735,7 @@
       <c r="AA37" t="inlineStr"/>
       <c r="AB37" t="inlineStr">
         <is>
-          <t>NAVAL, TIBURCIO ALIAS</t>
+          <t>NAVAL, PERFECTO LINGGO</t>
         </is>
       </c>
       <c r="AC37" t="inlineStr"/>
@@ -3747,7 +3743,7 @@
       <c r="AE37" t="inlineStr"/>
       <c r="AF37" t="inlineStr">
         <is>
-          <t>MIRANDA,ERLINDA,RAMOS,</t>
+          <t>ILAITIA,MELANIE,OCAMPO,</t>
         </is>
       </c>
       <c r="AG37" t="inlineStr"/>
@@ -3762,13 +3758,13 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>164512130064</t>
+          <t>164512130194</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
-          <t>NAVAL, ZYDNEY RONQUEZ</t>
+          <t>OLAVARIO,ALLIYAH LORRAINE, GUILLERMO</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
@@ -3781,13 +3777,13 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>11-02-2006</t>
+          <t>07-23-2007</t>
         </is>
       </c>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
@@ -3829,7 +3825,7 @@
       <c r="AA38" t="inlineStr"/>
       <c r="AB38" t="inlineStr">
         <is>
-          <t>NAVAL, FERDINAND DIAGO</t>
+          <t>OLAVARIO, TEODULO NUELAN</t>
         </is>
       </c>
       <c r="AC38" t="inlineStr"/>
@@ -3837,7 +3833,7 @@
       <c r="AE38" t="inlineStr"/>
       <c r="AF38" t="inlineStr">
         <is>
-          <t>RONQUEZ,RIO,CAMACHO,</t>
+          <t>GUILLERMO,IRENE,LIMBAG,</t>
         </is>
       </c>
       <c r="AG38" t="inlineStr"/>
@@ -3852,13 +3848,13 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>164512130038</t>
+          <t>108224130152</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr">
         <is>
-          <t>NAVARRO, ELYZA MAE BERMEJO</t>
+          <t>PUNZALAN,CHANELLE, POSO</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
@@ -3871,7 +3867,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>02-08-2007</t>
+          <t>08-03-2008</t>
         </is>
       </c>
       <c r="I39" t="inlineStr"/>
@@ -3896,7 +3892,7 @@
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R39" t="inlineStr"/>
@@ -3919,7 +3915,7 @@
       <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="inlineStr">
         <is>
-          <t>NAVARRO, RAYMUNDO HALLEGADO</t>
+          <t>PUNZALAN, RAYMOND LISMORAS</t>
         </is>
       </c>
       <c r="AC39" t="inlineStr"/>
@@ -3927,7 +3923,7 @@
       <c r="AE39" t="inlineStr"/>
       <c r="AF39" t="inlineStr">
         <is>
-          <t>BERMEJO,GERALDINE,BERNABE,</t>
+          <t>POSO,CHONA,RAMIREZ,</t>
         </is>
       </c>
       <c r="AG39" t="inlineStr"/>
@@ -3942,13 +3938,13 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>164512130068</t>
+          <t>136908131369</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>PONTIGON, PATRICIA JOY ENCISO</t>
+          <t>ROTUBIO,ALLIANA JALYN, BERONDO</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
@@ -3961,7 +3957,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>11-19-2006</t>
+          <t>07-03-2008</t>
         </is>
       </c>
       <c r="I40" t="inlineStr"/>
@@ -3986,7 +3982,7 @@
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R40" t="inlineStr"/>
@@ -4009,7 +4005,7 @@
       <c r="AA40" t="inlineStr"/>
       <c r="AB40" t="inlineStr">
         <is>
-          <t>PONTIGON, JAIME DATUON</t>
+          <t>ROTUBIO, JAY TOLEDO</t>
         </is>
       </c>
       <c r="AC40" t="inlineStr"/>
@@ -4017,7 +4013,7 @@
       <c r="AE40" t="inlineStr"/>
       <c r="AF40" t="inlineStr">
         <is>
-          <t>ENCISO,JOSEPHINE,MAKATINGRAO,</t>
+          <t>BERONDO,NORMALYN,CORDERO,</t>
         </is>
       </c>
       <c r="AG40" t="inlineStr"/>
@@ -4027,18 +4023,22 @@
       <c r="AK40" t="inlineStr"/>
       <c r="AL40" t="inlineStr"/>
       <c r="AM40" t="inlineStr"/>
-      <c r="AN40" t="inlineStr"/>
+      <c r="AN40" t="inlineStr">
+        <is>
+          <t>T/I Southville IV Elem. Sch.Date:2019-09-02</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>111821090138</t>
+          <t>164512130168</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>RAMIREZ, ELIZA CHRISTINE CARREON</t>
+          <t>SUZON,RYGIN LOVE, GIMENTIZA</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
@@ -4051,13 +4051,13 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>10-10-2003</t>
+          <t>05-20-2008</t>
         </is>
       </c>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr">
         <is>
-          <t xml:space="preserve">13 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
@@ -4076,7 +4076,7 @@
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>SANTO TOMAS (CALABUSO)</t>
+          <t>ZAPOTE</t>
         </is>
       </c>
       <c r="R41" t="inlineStr"/>
@@ -4099,7 +4099,7 @@
       <c r="AA41" t="inlineStr"/>
       <c r="AB41" t="inlineStr">
         <is>
-          <t>RAMIREZ, ERWIN TORARBA</t>
+          <t>SUZON, GERRY BERCERO</t>
         </is>
       </c>
       <c r="AC41" t="inlineStr"/>
@@ -4107,7 +4107,7 @@
       <c r="AE41" t="inlineStr"/>
       <c r="AF41" t="inlineStr">
         <is>
-          <t>CARREON,NELIA,SARMIENTO,</t>
+          <t>GIMENTIZA,GINA,TUICO,</t>
         </is>
       </c>
       <c r="AG41" t="inlineStr"/>
@@ -4117,22 +4117,18 @@
       <c r="AK41" t="inlineStr"/>
       <c r="AL41" t="inlineStr"/>
       <c r="AM41" t="inlineStr"/>
-      <c r="AN41" t="inlineStr">
-        <is>
-          <t>T/I DATE:2017-06-05</t>
-        </is>
-      </c>
+      <c r="AN41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>164512130040</t>
+          <t>107937130338</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>RIVERA, ANGELINA ELAINE MIRANDA</t>
+          <t>TAVU,RENY DENIEZE, RAMOS</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
@@ -4145,13 +4141,13 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>05-02-2007</t>
+          <t>02-24-2008</t>
         </is>
       </c>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
@@ -4170,7 +4166,7 @@
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R42" t="inlineStr"/>
@@ -4193,7 +4189,7 @@
       <c r="AA42" t="inlineStr"/>
       <c r="AB42" t="inlineStr">
         <is>
-          <t>RIVERA, FERDINAND VILLANUEVA</t>
+          <t>TAVU, RENY RAYMOND VEGA</t>
         </is>
       </c>
       <c r="AC42" t="inlineStr"/>
@@ -4201,7 +4197,7 @@
       <c r="AE42" t="inlineStr"/>
       <c r="AF42" t="inlineStr">
         <is>
-          <t>MIRANDA,SHEILA ROSE,BAYANID,</t>
+          <t>RAMOS,ADELAIDA,SANCHEZ,</t>
         </is>
       </c>
       <c r="AG42" t="inlineStr"/>
@@ -4214,44 +4210,86 @@
       <c r="AN42" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>18</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>164512130105</t>
+        </is>
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>&lt;=== TOTAL FEMALE</t>
+          <t>VARGAS,REIGN BEYONCE, GUILLERMO</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>11-03-2007</t>
+        </is>
+      </c>
       <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr"/>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr"/>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P43" t="inlineStr"/>
-      <c r="Q43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr"/>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr"/>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V43" t="inlineStr"/>
       <c r="W43" t="inlineStr"/>
-      <c r="X43" t="inlineStr"/>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y43" t="inlineStr"/>
       <c r="Z43" t="inlineStr"/>
       <c r="AA43" t="inlineStr"/>
-      <c r="AB43" t="inlineStr"/>
+      <c r="AB43" t="inlineStr">
+        <is>
+          <t>VARGAS, JUSSELLE SARMIENTO</t>
+        </is>
+      </c>
       <c r="AC43" t="inlineStr"/>
       <c r="AD43" t="inlineStr"/>
       <c r="AE43" t="inlineStr"/>
-      <c r="AF43" t="inlineStr"/>
+      <c r="AF43" t="inlineStr">
+        <is>
+          <t>GUILLERMO,ADEL,LIMBAG,</t>
+        </is>
+      </c>
       <c r="AG43" t="inlineStr"/>
       <c r="AH43" t="inlineStr"/>
       <c r="AI43" t="inlineStr"/>
@@ -4263,12 +4301,12 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>&lt;=== COMBINED</t>
+          <t>&lt;=== TOTAL FEMALE</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
@@ -4310,13 +4348,15 @@
       <c r="AN44" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>List and Code of Indicators under REMARKS column</t>
-        </is>
+      <c r="A45" t="n">
+        <v>36</v>
       </c>
       <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr"/>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>&lt;=== COMBINED</t>
+        </is>
+      </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
@@ -4358,42 +4398,22 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Indicator</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Code</t>
-        </is>
-      </c>
+          <t>List and Code of Indicators under REMARKS column</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Required Information</t>
-        </is>
-      </c>
+      <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>Indicator</t>
-        </is>
-      </c>
+      <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>Code</t>
-        </is>
-      </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>Required Information</t>
-        </is>
-      </c>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
@@ -4401,41 +4421,21 @@
       <c r="S46" t="inlineStr"/>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr"/>
-      <c r="V46" t="inlineStr">
-        <is>
-          <t>REGISTERED</t>
-        </is>
-      </c>
+      <c r="V46" t="inlineStr"/>
       <c r="W46" t="inlineStr"/>
       <c r="X46" t="inlineStr"/>
-      <c r="Y46" t="inlineStr">
-        <is>
-          <t>BoSY</t>
-        </is>
-      </c>
-      <c r="Z46" t="inlineStr">
-        <is>
-          <t>EoSY</t>
-        </is>
-      </c>
+      <c r="Y46" t="inlineStr"/>
+      <c r="Z46" t="inlineStr"/>
       <c r="AA46" t="inlineStr"/>
       <c r="AB46" t="inlineStr"/>
       <c r="AC46" t="inlineStr"/>
-      <c r="AD46" t="inlineStr">
-        <is>
-          <t>Prepared by;</t>
-        </is>
-      </c>
+      <c r="AD46" t="inlineStr"/>
       <c r="AE46" t="inlineStr"/>
       <c r="AF46" t="inlineStr"/>
       <c r="AG46" t="inlineStr"/>
       <c r="AH46" t="inlineStr"/>
       <c r="AI46" t="inlineStr"/>
-      <c r="AJ46" t="inlineStr">
-        <is>
-          <t>Certified Correct:</t>
-        </is>
-      </c>
+      <c r="AJ46" t="inlineStr"/>
       <c r="AK46" t="inlineStr"/>
       <c r="AL46" t="inlineStr"/>
       <c r="AM46" t="inlineStr"/>
@@ -4444,27 +4444,18 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Transfered Out
-Transfered In
-Dropped
-</t>
+          <t>Indicator</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>T/O
-T/I
-DRP
-LE</t>
+          <t>Code</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Name of  Public (P) Private (PR) School  &amp; Effectivity Date
-Name of  Public (P) Private (PR) School  &amp; Effectivity Date
-Reason  and Effectivity Date
-Reason (Enrollment beyond 1st Friday of </t>
+          <t>Required Information</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -4473,10 +4464,7 @@
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr">
         <is>
-          <t>CCT Receipient
-Balik Aral
-Learner With Disability
-Accelerated</t>
+          <t>Indicator</t>
         </is>
       </c>
       <c r="J47" t="inlineStr"/>
@@ -4484,18 +4472,12 @@
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr">
         <is>
-          <t>CCT
-B/A
-LWD
-ACL</t>
+          <t>Code</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>CCT Control/reference number &amp; Effectivity Date
-Name of school last attended &amp; Year
-Specify
-Specify Level &amp; Effectivity Data</t>
+          <t>Required Information</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
@@ -4507,23 +4489,27 @@
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr">
         <is>
-          <t>MALE</t>
+          <t>REGISTERED</t>
         </is>
       </c>
       <c r="W47" t="inlineStr"/>
       <c r="X47" t="inlineStr"/>
       <c r="Y47" t="inlineStr">
         <is>
-          <t xml:space="preserve">17 </t>
-        </is>
-      </c>
-      <c r="Z47" t="inlineStr"/>
+          <t>BoSY</t>
+        </is>
+      </c>
+      <c r="Z47" t="inlineStr">
+        <is>
+          <t>EoSY</t>
+        </is>
+      </c>
       <c r="AA47" t="inlineStr"/>
       <c r="AB47" t="inlineStr"/>
       <c r="AC47" t="inlineStr"/>
       <c r="AD47" t="inlineStr">
         <is>
-          <t>LAMBERTO BOLIMA RIVAREZ</t>
+          <t>Prepared by;</t>
         </is>
       </c>
       <c r="AE47" t="inlineStr"/>
@@ -4533,7 +4519,7 @@
       <c r="AI47" t="inlineStr"/>
       <c r="AJ47" t="inlineStr">
         <is>
-          <t>ELSA MONTERERO MANALO</t>
+          <t>Certified Correct:</t>
         </is>
       </c>
       <c r="AK47" t="inlineStr"/>
@@ -4542,20 +4528,62 @@
       <c r="AN47" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr"/>
-      <c r="B48" t="inlineStr"/>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Transfered Out
+Transfered In
+Dropped
+Late Enrollment</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>T/O
+T/I
+DRP
+LE</t>
+        </is>
+      </c>
       <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Name of  Public (P) Private (PR) School  &amp; Effectivity Date
+Name of  Public (P) Private (PR) School  &amp; Effectivity Date
+Reason  and Effectivity Date
+Reason (Enrollment beyond 1st Friday of June)</t>
+        </is>
+      </c>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr"/>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>CCT Receipient
+Balik Aral
+Learner With Disability
+Accelerated</t>
+        </is>
+      </c>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>CCT
+B/A
+LWD
+ACL</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>CCT Control/reference number &amp; Effectivity Date
+Name of school last attended &amp; Year
+Specify
+Specify Level &amp; Effectivity Data</t>
+        </is>
+      </c>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
@@ -4565,19 +4593,23 @@
       <c r="U48" t="inlineStr"/>
       <c r="V48" t="inlineStr">
         <is>
-          <t>FEMALE</t>
+          <t>MALE</t>
         </is>
       </c>
       <c r="W48" t="inlineStr"/>
       <c r="X48" t="inlineStr"/>
-      <c r="Y48" t="inlineStr"/>
-      <c r="Z48" t="inlineStr"/>
+      <c r="Y48" t="n">
+        <v>16</v>
+      </c>
+      <c r="Z48" t="n">
+        <v>15</v>
+      </c>
       <c r="AA48" t="inlineStr"/>
       <c r="AB48" t="inlineStr"/>
       <c r="AC48" t="inlineStr"/>
       <c r="AD48" t="inlineStr">
         <is>
-          <t>(Signature of Adviser over Printed Name)</t>
+          <t>LAMBERTO BOLIMA RIVAREZ</t>
         </is>
       </c>
       <c r="AE48" t="inlineStr"/>
@@ -4587,7 +4619,7 @@
       <c r="AI48" t="inlineStr"/>
       <c r="AJ48" t="inlineStr">
         <is>
-          <t>(Signature of School Head over Printed Name)</t>
+          <t>ELSA MONTERERO MANALO</t>
         </is>
       </c>
       <c r="AK48" t="inlineStr"/>
@@ -4620,9 +4652,7 @@
       <c r="V49" t="inlineStr"/>
       <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr"/>
-      <c r="Y49" t="n">
-        <v>18</v>
-      </c>
+      <c r="Y49" t="inlineStr"/>
       <c r="Z49" t="inlineStr"/>
       <c r="AA49" t="inlineStr"/>
       <c r="AB49" t="inlineStr"/>
@@ -4661,54 +4691,32 @@
       <c r="S50" t="inlineStr"/>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
-      <c r="V50" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
+      <c r="V50" t="inlineStr"/>
       <c r="W50" t="inlineStr"/>
       <c r="X50" t="inlineStr"/>
-      <c r="Y50" t="n">
-        <v>35</v>
-      </c>
+      <c r="Y50" t="inlineStr"/>
       <c r="Z50" t="inlineStr"/>
       <c r="AA50" t="inlineStr"/>
       <c r="AB50" t="inlineStr"/>
       <c r="AC50" t="inlineStr"/>
-      <c r="AD50" t="inlineStr">
-        <is>
-          <t>BoSY Date:</t>
-        </is>
-      </c>
+      <c r="AD50" t="inlineStr"/>
       <c r="AE50" t="inlineStr"/>
       <c r="AF50" t="inlineStr"/>
-      <c r="AG50" t="inlineStr">
-        <is>
-          <t>EoSY Date:</t>
-        </is>
-      </c>
+      <c r="AG50" t="inlineStr"/>
       <c r="AH50" t="inlineStr"/>
       <c r="AI50" t="inlineStr"/>
       <c r="AJ50" t="inlineStr">
         <is>
-          <t>BoSY Date:</t>
+          <t>(Signature of School Head over Printed Name)</t>
         </is>
       </c>
       <c r="AK50" t="inlineStr"/>
       <c r="AL50" t="inlineStr"/>
-      <c r="AM50" t="inlineStr">
-        <is>
-          <t>EoSY Date:</t>
-        </is>
-      </c>
+      <c r="AM50" t="inlineStr"/>
       <c r="AN50" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>Generated on: Tuesday, September 12, 2017</t>
-        </is>
-      </c>
+      <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
@@ -4729,15 +4737,27 @@
       <c r="S51" t="inlineStr"/>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
-      <c r="V51" t="inlineStr"/>
+      <c r="V51" t="inlineStr">
+        <is>
+          <t>FEMALE</t>
+        </is>
+      </c>
       <c r="W51" t="inlineStr"/>
       <c r="X51" t="inlineStr"/>
-      <c r="Y51" t="inlineStr"/>
-      <c r="Z51" t="inlineStr"/>
+      <c r="Y51" t="n">
+        <v>19</v>
+      </c>
+      <c r="Z51" t="n">
+        <v>20</v>
+      </c>
       <c r="AA51" t="inlineStr"/>
       <c r="AB51" t="inlineStr"/>
       <c r="AC51" t="inlineStr"/>
-      <c r="AD51" t="inlineStr"/>
+      <c r="AD51" t="inlineStr">
+        <is>
+          <t>(Signature of Adviser over Printed Name)</t>
+        </is>
+      </c>
       <c r="AE51" t="inlineStr"/>
       <c r="AF51" t="inlineStr"/>
       <c r="AG51" t="inlineStr"/>
@@ -4749,6 +4769,290 @@
       <c r="AM51" t="inlineStr"/>
       <c r="AN51" t="inlineStr"/>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr"/>
+      <c r="R52" t="inlineStr"/>
+      <c r="S52" t="inlineStr"/>
+      <c r="T52" t="inlineStr"/>
+      <c r="U52" t="inlineStr"/>
+      <c r="V52" t="inlineStr"/>
+      <c r="W52" t="inlineStr"/>
+      <c r="X52" t="inlineStr"/>
+      <c r="Y52" t="inlineStr"/>
+      <c r="Z52" t="inlineStr"/>
+      <c r="AA52" t="inlineStr"/>
+      <c r="AB52" t="inlineStr"/>
+      <c r="AC52" t="inlineStr"/>
+      <c r="AD52" t="inlineStr"/>
+      <c r="AE52" t="inlineStr"/>
+      <c r="AF52" t="inlineStr"/>
+      <c r="AG52" t="inlineStr"/>
+      <c r="AH52" t="inlineStr"/>
+      <c r="AI52" t="inlineStr"/>
+      <c r="AJ52" t="inlineStr">
+        <is>
+          <t>BoSY Date:                06-03-2019</t>
+        </is>
+      </c>
+      <c r="AK52" t="inlineStr"/>
+      <c r="AL52" t="inlineStr"/>
+      <c r="AM52" t="inlineStr">
+        <is>
+          <t>EoSY Date:                    04-03-2020</t>
+        </is>
+      </c>
+      <c r="AN52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr"/>
+      <c r="R53" t="inlineStr"/>
+      <c r="S53" t="inlineStr"/>
+      <c r="T53" t="inlineStr"/>
+      <c r="U53" t="inlineStr"/>
+      <c r="V53" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="W53" t="inlineStr"/>
+      <c r="X53" t="inlineStr"/>
+      <c r="Y53" t="n">
+        <v>35</v>
+      </c>
+      <c r="Z53" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA53" t="inlineStr"/>
+      <c r="AB53" t="inlineStr"/>
+      <c r="AC53" t="inlineStr"/>
+      <c r="AD53" t="inlineStr">
+        <is>
+          <t>BoSY Date:                06-03-2019</t>
+        </is>
+      </c>
+      <c r="AE53" t="inlineStr"/>
+      <c r="AF53" t="inlineStr"/>
+      <c r="AG53" t="inlineStr">
+        <is>
+          <t>EoSY Date:                  04-03-2020</t>
+        </is>
+      </c>
+      <c r="AH53" t="inlineStr"/>
+      <c r="AI53" t="inlineStr"/>
+      <c r="AJ53" t="inlineStr"/>
+      <c r="AK53" t="inlineStr"/>
+      <c r="AL53" t="inlineStr"/>
+      <c r="AM53" t="inlineStr"/>
+      <c r="AN53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr"/>
+      <c r="R54" t="inlineStr"/>
+      <c r="S54" t="inlineStr"/>
+      <c r="T54" t="inlineStr"/>
+      <c r="U54" t="inlineStr"/>
+      <c r="V54" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr"/>
+      <c r="Y54" t="inlineStr"/>
+      <c r="Z54" t="inlineStr"/>
+      <c r="AA54" t="inlineStr"/>
+      <c r="AB54" t="inlineStr"/>
+      <c r="AC54" t="inlineStr"/>
+      <c r="AD54" t="inlineStr"/>
+      <c r="AE54" t="inlineStr"/>
+      <c r="AF54" t="inlineStr"/>
+      <c r="AG54" t="inlineStr"/>
+      <c r="AH54" t="inlineStr"/>
+      <c r="AI54" t="inlineStr"/>
+      <c r="AJ54" t="inlineStr"/>
+      <c r="AK54" t="inlineStr"/>
+      <c r="AL54" t="inlineStr"/>
+      <c r="AM54" t="inlineStr"/>
+      <c r="AN54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr"/>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
+      <c r="R55" t="inlineStr"/>
+      <c r="S55" t="inlineStr"/>
+      <c r="T55" t="inlineStr"/>
+      <c r="U55" t="inlineStr"/>
+      <c r="V55" t="inlineStr"/>
+      <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr"/>
+      <c r="Y55" t="inlineStr"/>
+      <c r="Z55" t="inlineStr"/>
+      <c r="AA55" t="inlineStr"/>
+      <c r="AB55" t="inlineStr"/>
+      <c r="AC55" t="inlineStr"/>
+      <c r="AD55" t="inlineStr"/>
+      <c r="AE55" t="inlineStr"/>
+      <c r="AF55" t="inlineStr"/>
+      <c r="AG55" t="inlineStr"/>
+      <c r="AH55" t="inlineStr"/>
+      <c r="AI55" t="inlineStr"/>
+      <c r="AJ55" t="inlineStr"/>
+      <c r="AK55" t="inlineStr"/>
+      <c r="AL55" t="inlineStr"/>
+      <c r="AM55" t="inlineStr"/>
+      <c r="AN55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
+      <c r="R56" t="inlineStr"/>
+      <c r="S56" t="inlineStr"/>
+      <c r="T56" t="inlineStr"/>
+      <c r="U56" t="inlineStr"/>
+      <c r="V56" t="inlineStr"/>
+      <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr"/>
+      <c r="Y56" t="inlineStr"/>
+      <c r="Z56" t="inlineStr"/>
+      <c r="AA56" t="inlineStr"/>
+      <c r="AB56" t="inlineStr"/>
+      <c r="AC56" t="inlineStr"/>
+      <c r="AD56" t="inlineStr"/>
+      <c r="AE56" t="inlineStr"/>
+      <c r="AF56" t="inlineStr"/>
+      <c r="AG56" t="inlineStr"/>
+      <c r="AH56" t="inlineStr"/>
+      <c r="AI56" t="inlineStr"/>
+      <c r="AJ56" t="inlineStr">
+        <is>
+          <t>Generated thru LIS</t>
+        </is>
+      </c>
+      <c r="AK56" t="inlineStr"/>
+      <c r="AL56" t="inlineStr"/>
+      <c r="AM56" t="inlineStr"/>
+      <c r="AN56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Generated on: Saturday, March 21, 2020</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
+      <c r="R57" t="inlineStr"/>
+      <c r="S57" t="inlineStr"/>
+      <c r="T57" t="inlineStr"/>
+      <c r="U57" t="inlineStr"/>
+      <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr"/>
+      <c r="Y57" t="inlineStr"/>
+      <c r="Z57" t="inlineStr"/>
+      <c r="AA57" t="inlineStr"/>
+      <c r="AB57" t="inlineStr"/>
+      <c r="AC57" t="inlineStr"/>
+      <c r="AD57" t="inlineStr"/>
+      <c r="AE57" t="inlineStr"/>
+      <c r="AF57" t="inlineStr"/>
+      <c r="AG57" t="inlineStr"/>
+      <c r="AH57" t="inlineStr"/>
+      <c r="AI57" t="inlineStr"/>
+      <c r="AJ57" t="inlineStr"/>
+      <c r="AK57" t="inlineStr"/>
+      <c r="AL57" t="inlineStr"/>
+      <c r="AM57" t="inlineStr"/>
+      <c r="AN57" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
28/03/2024 - 8:59pm (W/ LEARNERS OBSERVATION)
</commit_message>
<xml_diff>
--- a/Migrade_v.1.2/temp.xlsx
+++ b/Migrade_v.1.2/temp.xlsx
@@ -722,7 +722,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>108765</v>
+        <v>108420</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -747,7 +747,7 @@
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr">
         <is>
-          <t>Sta. Rosa City</t>
+          <t>San Pedro City</t>
         </is>
       </c>
       <c r="U3" t="inlineStr"/>
@@ -774,7 +774,7 @@
       <c r="AL3" t="inlineStr"/>
       <c r="AM3" t="inlineStr">
         <is>
-          <t>Sta. Rosa</t>
+          <t>San Pedro</t>
         </is>
       </c>
       <c r="AN3" t="inlineStr"/>
@@ -796,7 +796,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Bagong Buhay Elementary School</t>
+          <t>Cuyab Elementary School</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -818,7 +818,7 @@
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr">
         <is>
-          <t>2015 - 2016</t>
+          <t>2023 - 2024</t>
         </is>
       </c>
       <c r="U4" t="inlineStr"/>
@@ -837,7 +837,7 @@
       <c r="AD4" t="inlineStr"/>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>Grade 2</t>
+          <t>Grade 1</t>
         </is>
       </c>
       <c r="AF4" t="inlineStr"/>
@@ -853,7 +853,7 @@
       <c r="AL4" t="inlineStr"/>
       <c r="AM4" t="inlineStr">
         <is>
-          <t>Antipolo</t>
+          <t>JACINTO</t>
         </is>
       </c>
       <c r="AN4" t="inlineStr"/>
@@ -1062,7 +1062,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ALARIN,JOHN  LLYOD, SALVADOR</t>
+          <t>ALARIN,TRISTAN JAMES, SALVADOR</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -1123,7 +1123,7 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>ALARIN, DANNY TULFO</t>
+          <t>ALARIN, DANNY RAFAEL</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr"/>
@@ -1131,7 +1131,7 @@
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>SALVADOR,PORCELYN FRANCISCO,,</t>
+          <t>SALVADOR,ANGELYN FRANCISCO,,</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr"/>
@@ -1161,7 +1161,7 @@
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ARELLANO,ERICH GABRIEL, ELEANOR</t>
+          <t>ARELLANO,NATHAN GABRIEL, BELLEZA</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -1222,7 +1222,7 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>ARELLANO, MARCIANO ENRIQUE</t>
+          <t>ARELLANO, MANOLITO BELZA</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr"/>
@@ -1230,7 +1230,7 @@
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>ELEANOR,SELENA,SOBERANO,</t>
+          <t>BELLEZA,MELISA,SOBERANO,</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr"/>
@@ -1260,7 +1260,7 @@
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>NERY,ARTHUR, PANGILINAN</t>
+          <t>AZUR,JHONANCE MATTHEW, FEDELES</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -1321,7 +1321,7 @@
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>NERY, WILLI ONG</t>
+          <t>AZUR, EVISON DEAN ERUBAS</t>
         </is>
       </c>
       <c r="AC9" t="inlineStr"/>
@@ -1329,7 +1329,7 @@
       <c r="AE9" t="inlineStr"/>
       <c r="AF9" t="inlineStr">
         <is>
-          <t>PANGILINAN,ANGEL,APRIL,</t>
+          <t>FEDELES,ANALYN,ARRAZ,</t>
         </is>
       </c>
       <c r="AG9" t="inlineStr"/>
@@ -1351,38 +1351,86 @@
       <c r="AS9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>108420220006</t>
+        </is>
+      </c>
       <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>BASBAS,SCOTTIE EURIE, CAPACITE</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>04-15-2017</t>
+        </is>
+      </c>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>BASBAS, EUGENE OMALIN</t>
+        </is>
+      </c>
       <c r="AC10" t="inlineStr"/>
       <c r="AD10" t="inlineStr"/>
       <c r="AE10" t="inlineStr"/>
-      <c r="AF10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>CAPACITE,ROSANNA,DELIMA,</t>
+        </is>
+      </c>
       <c r="AG10" t="inlineStr"/>
       <c r="AH10" t="inlineStr"/>
       <c r="AI10" t="inlineStr"/>
@@ -1394,42 +1442,94 @@
       <c r="AO10" t="inlineStr"/>
       <c r="AP10" t="inlineStr"/>
       <c r="AQ10" t="inlineStr"/>
-      <c r="AR10" t="inlineStr"/>
+      <c r="AR10" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>108420220163</t>
+        </is>
+      </c>
       <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>BAWA-AN,EON DRAKE, MOSTIERA</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>11-17-2016</t>
+        </is>
+      </c>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Filipino</t>
+        </is>
+      </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="inlineStr"/>
-      <c r="AB11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>BAWA-AN, CRISTIAN PILAPIL</t>
+        </is>
+      </c>
       <c r="AC11" t="inlineStr"/>
       <c r="AD11" t="inlineStr"/>
       <c r="AE11" t="inlineStr"/>
-      <c r="AF11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>MOSTIERA,MICHELLE,CARINGAL,</t>
+        </is>
+      </c>
       <c r="AG11" t="inlineStr"/>
       <c r="AH11" t="inlineStr"/>
       <c r="AI11" t="inlineStr"/>
@@ -1441,42 +1541,94 @@
       <c r="AO11" t="inlineStr"/>
       <c r="AP11" t="inlineStr"/>
       <c r="AQ11" t="inlineStr"/>
-      <c r="AR11" t="inlineStr"/>
+      <c r="AR11" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>108420210037</t>
+        </is>
+      </c>
       <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>CAPACETE,JOHN MIGSZ, DIMACULANGAN</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>08-23-2016</t>
+        </is>
+      </c>
       <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
       <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr"/>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X12" t="inlineStr"/>
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="inlineStr"/>
-      <c r="AB12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>CAPACETE, JOHNMEL CHESTER CORNICO</t>
+        </is>
+      </c>
       <c r="AC12" t="inlineStr"/>
       <c r="AD12" t="inlineStr"/>
       <c r="AE12" t="inlineStr"/>
-      <c r="AF12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>DIMACULANGAN,WENDY,YUCSON,</t>
+        </is>
+      </c>
       <c r="AG12" t="inlineStr"/>
       <c r="AH12" t="inlineStr"/>
       <c r="AI12" t="inlineStr"/>
@@ -1488,42 +1640,94 @@
       <c r="AO12" t="inlineStr"/>
       <c r="AP12" t="inlineStr"/>
       <c r="AQ12" t="inlineStr"/>
-      <c r="AR12" t="inlineStr"/>
+      <c r="AR12" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>108420220023</t>
+        </is>
+      </c>
       <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>CASTRO,ACE RAFAEL, LUCIÑADA</t>
+        </is>
+      </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>03-15-2017</t>
+        </is>
+      </c>
       <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="inlineStr"/>
       <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>CASTRO, RAFFY SIBULO</t>
+        </is>
+      </c>
       <c r="AC13" t="inlineStr"/>
       <c r="AD13" t="inlineStr"/>
       <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>LUCIÑADA,ANGELICA,GUEVARRA,</t>
+        </is>
+      </c>
       <c r="AG13" t="inlineStr"/>
       <c r="AH13" t="inlineStr"/>
       <c r="AI13" t="inlineStr"/>
@@ -1535,42 +1739,94 @@
       <c r="AO13" t="inlineStr"/>
       <c r="AP13" t="inlineStr"/>
       <c r="AQ13" t="inlineStr"/>
-      <c r="AR13" t="inlineStr"/>
+      <c r="AR13" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr"/>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>108420220167</t>
+        </is>
+      </c>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>EUSEBIO,CHRISTIAN LOYD, REYES</t>
+        </is>
+      </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>08-27-2016</t>
+        </is>
+      </c>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Filipino</t>
+        </is>
+      </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X14" t="inlineStr"/>
       <c r="Y14" t="inlineStr"/>
       <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="inlineStr"/>
-      <c r="AB14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>EUSEBIO, CHRISTIAN BON</t>
+        </is>
+      </c>
       <c r="AC14" t="inlineStr"/>
       <c r="AD14" t="inlineStr"/>
       <c r="AE14" t="inlineStr"/>
-      <c r="AF14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>REYES,JERELYN,DAUBA,</t>
+        </is>
+      </c>
       <c r="AG14" t="inlineStr"/>
       <c r="AH14" t="inlineStr"/>
       <c r="AI14" t="inlineStr"/>
@@ -1582,42 +1838,94 @@
       <c r="AO14" t="inlineStr"/>
       <c r="AP14" t="inlineStr"/>
       <c r="AQ14" t="inlineStr"/>
-      <c r="AR14" t="inlineStr"/>
+      <c r="AR14" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>108420220102</t>
+        </is>
+      </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>GASGAS,MARK DENNIS, LUMABAD</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>05-26-2013</t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr"/>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X15" t="inlineStr"/>
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="inlineStr"/>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>GASGAS, DANTE MACASAYA</t>
+        </is>
+      </c>
       <c r="AC15" t="inlineStr"/>
       <c r="AD15" t="inlineStr"/>
       <c r="AE15" t="inlineStr"/>
-      <c r="AF15" t="inlineStr"/>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>LUMABAD,AIDA,CARATERO,</t>
+        </is>
+      </c>
       <c r="AG15" t="inlineStr"/>
       <c r="AH15" t="inlineStr"/>
       <c r="AI15" t="inlineStr"/>
@@ -1629,42 +1937,94 @@
       <c r="AO15" t="inlineStr"/>
       <c r="AP15" t="inlineStr"/>
       <c r="AQ15" t="inlineStr"/>
-      <c r="AR15" t="inlineStr"/>
+      <c r="AR15" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr"/>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>108420210042</t>
+        </is>
+      </c>
       <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>HAMOR,YHURIE LORENCE, ALBOR</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>02-04-2016</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
       <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr"/>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X16" t="inlineStr"/>
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="inlineStr"/>
-      <c r="AB16" t="inlineStr"/>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>HAMOR, WILFREDO SINCHONGCO</t>
+        </is>
+      </c>
       <c r="AC16" t="inlineStr"/>
       <c r="AD16" t="inlineStr"/>
       <c r="AE16" t="inlineStr"/>
-      <c r="AF16" t="inlineStr"/>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>ALBOR,MICHELLE,HUTALLA,</t>
+        </is>
+      </c>
       <c r="AG16" t="inlineStr"/>
       <c r="AH16" t="inlineStr"/>
       <c r="AI16" t="inlineStr"/>
@@ -1676,7 +2036,11 @@
       <c r="AO16" t="inlineStr"/>
       <c r="AP16" t="inlineStr"/>
       <c r="AQ16" t="inlineStr"/>
-      <c r="AR16" t="inlineStr"/>
+      <c r="AR16" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS16" t="inlineStr">
         <is>
           <t>T/I DATE:2023-08-29</t>
@@ -1684,38 +2048,86 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr"/>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>108420220013</t>
+        </is>
+      </c>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>JUCUTAN,CALEB MATTEO, ELOMINA</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>10-29-2016</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
       <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V17" t="inlineStr"/>
-      <c r="W17" t="inlineStr"/>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X17" t="inlineStr"/>
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="inlineStr"/>
       <c r="AA17" t="inlineStr"/>
-      <c r="AB17" t="inlineStr"/>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>JUCUTAN, PATRICK ARELLANO</t>
+        </is>
+      </c>
       <c r="AC17" t="inlineStr"/>
       <c r="AD17" t="inlineStr"/>
       <c r="AE17" t="inlineStr"/>
-      <c r="AF17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>ELOMINA,CATHLENE KAYE,MIRONDO,</t>
+        </is>
+      </c>
       <c r="AG17" t="inlineStr"/>
       <c r="AH17" t="inlineStr"/>
       <c r="AI17" t="inlineStr"/>
@@ -1727,42 +2139,94 @@
       <c r="AO17" t="inlineStr"/>
       <c r="AP17" t="inlineStr"/>
       <c r="AQ17" t="inlineStr"/>
-      <c r="AR17" t="inlineStr"/>
+      <c r="AR17" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>108420220014</t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>LEONORA,RAMCEL, NAVARRO</t>
+        </is>
+      </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>04-13-2017</t>
+        </is>
+      </c>
       <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="inlineStr"/>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
-      <c r="U18" t="inlineStr"/>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V18" t="inlineStr"/>
-      <c r="W18" t="inlineStr"/>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X18" t="inlineStr"/>
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="inlineStr"/>
       <c r="AA18" t="inlineStr"/>
-      <c r="AB18" t="inlineStr"/>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>LEONORA, RAMIE CATALAN</t>
+        </is>
+      </c>
       <c r="AC18" t="inlineStr"/>
       <c r="AD18" t="inlineStr"/>
       <c r="AE18" t="inlineStr"/>
-      <c r="AF18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>NAVARRO,MARICEL,VILLARUEL,</t>
+        </is>
+      </c>
       <c r="AG18" t="inlineStr"/>
       <c r="AH18" t="inlineStr"/>
       <c r="AI18" t="inlineStr"/>
@@ -1774,42 +2238,94 @@
       <c r="AO18" t="inlineStr"/>
       <c r="AP18" t="inlineStr"/>
       <c r="AQ18" t="inlineStr"/>
-      <c r="AR18" t="inlineStr"/>
+      <c r="AR18" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>108420220015</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>LIZARDA,RYAN CHARLES, TEMPROSA</t>
+        </is>
+      </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>09-12-2016</t>
+        </is>
+      </c>
       <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
       <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr"/>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr"/>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V19" t="inlineStr"/>
-      <c r="W19" t="inlineStr"/>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X19" t="inlineStr"/>
       <c r="Y19" t="inlineStr"/>
       <c r="Z19" t="inlineStr"/>
       <c r="AA19" t="inlineStr"/>
-      <c r="AB19" t="inlineStr"/>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>LIZARDA, RYAN HALAYAHAY</t>
+        </is>
+      </c>
       <c r="AC19" t="inlineStr"/>
       <c r="AD19" t="inlineStr"/>
       <c r="AE19" t="inlineStr"/>
-      <c r="AF19" t="inlineStr"/>
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>TEMPROSA,CARMELA,MERILO,</t>
+        </is>
+      </c>
       <c r="AG19" t="inlineStr"/>
       <c r="AH19" t="inlineStr"/>
       <c r="AI19" t="inlineStr"/>
@@ -1821,42 +2337,94 @@
       <c r="AO19" t="inlineStr"/>
       <c r="AP19" t="inlineStr"/>
       <c r="AQ19" t="inlineStr"/>
-      <c r="AR19" t="inlineStr"/>
+      <c r="AR19" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr"/>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>108420220057</t>
+        </is>
+      </c>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>LUMABAS,TRISTAN, GABRIEL</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>07-05-2016</t>
+        </is>
+      </c>
       <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr"/>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V20" t="inlineStr"/>
-      <c r="W20" t="inlineStr"/>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X20" t="inlineStr"/>
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr"/>
       <c r="AA20" t="inlineStr"/>
-      <c r="AB20" t="inlineStr"/>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>LUMABAS, EDISON GUILIERMO</t>
+        </is>
+      </c>
       <c r="AC20" t="inlineStr"/>
       <c r="AD20" t="inlineStr"/>
       <c r="AE20" t="inlineStr"/>
-      <c r="AF20" t="inlineStr"/>
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>GABRIEL,PRINCES,MARQUEZ,</t>
+        </is>
+      </c>
       <c r="AG20" t="inlineStr"/>
       <c r="AH20" t="inlineStr"/>
       <c r="AI20" t="inlineStr"/>
@@ -1868,42 +2436,94 @@
       <c r="AO20" t="inlineStr"/>
       <c r="AP20" t="inlineStr"/>
       <c r="AQ20" t="inlineStr"/>
-      <c r="AR20" t="inlineStr"/>
+      <c r="AR20" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>123979220014</t>
+        </is>
+      </c>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NACARIO,GILBERT, ESTRADA</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>03-19-2017</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Waray</t>
+        </is>
+      </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr"/>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr"/>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V21" t="inlineStr"/>
-      <c r="W21" t="inlineStr"/>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X21" t="inlineStr"/>
       <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr"/>
       <c r="AA21" t="inlineStr"/>
-      <c r="AB21" t="inlineStr"/>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>NACARIO, GERALD MAGLINTE</t>
+        </is>
+      </c>
       <c r="AC21" t="inlineStr"/>
       <c r="AD21" t="inlineStr"/>
       <c r="AE21" t="inlineStr"/>
-      <c r="AF21" t="inlineStr"/>
+      <c r="AF21" t="inlineStr">
+        <is>
+          <t>ESTRADA,BABAY AN LOU,CAATILLO,</t>
+        </is>
+      </c>
       <c r="AG21" t="inlineStr"/>
       <c r="AH21" t="inlineStr"/>
       <c r="AI21" t="inlineStr"/>
@@ -1915,7 +2535,11 @@
       <c r="AO21" t="inlineStr"/>
       <c r="AP21" t="inlineStr"/>
       <c r="AQ21" t="inlineStr"/>
-      <c r="AR21" t="inlineStr"/>
+      <c r="AR21" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS21" t="inlineStr">
         <is>
           <t>T/I DATE:2023-12-04</t>
@@ -1923,38 +2547,86 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>108420220058</t>
+        </is>
+      </c>
       <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>PANGANIBAN,JONARD LUCAS, ENCISO</t>
+        </is>
+      </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>09-04-2016</t>
+        </is>
+      </c>
       <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
       <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
-      <c r="R22" t="inlineStr"/>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr"/>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V22" t="inlineStr"/>
-      <c r="W22" t="inlineStr"/>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X22" t="inlineStr"/>
       <c r="Y22" t="inlineStr"/>
       <c r="Z22" t="inlineStr"/>
       <c r="AA22" t="inlineStr"/>
-      <c r="AB22" t="inlineStr"/>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>PANGANIBAN, JONAR DEFEO</t>
+        </is>
+      </c>
       <c r="AC22" t="inlineStr"/>
       <c r="AD22" t="inlineStr"/>
       <c r="AE22" t="inlineStr"/>
-      <c r="AF22" t="inlineStr"/>
+      <c r="AF22" t="inlineStr">
+        <is>
+          <t>ENCISO,ROWENA,PRESTOZA,</t>
+        </is>
+      </c>
       <c r="AG22" t="inlineStr"/>
       <c r="AH22" t="inlineStr"/>
       <c r="AI22" t="inlineStr"/>
@@ -1966,42 +2638,94 @@
       <c r="AO22" t="inlineStr"/>
       <c r="AP22" t="inlineStr"/>
       <c r="AQ22" t="inlineStr"/>
-      <c r="AR22" t="inlineStr"/>
+      <c r="AR22" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>108420210203</t>
+        </is>
+      </c>
       <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>PELARIO,SOL DAVE, DOROTEO</t>
+        </is>
+      </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>02-03-2016</t>
+        </is>
+      </c>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
       <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr"/>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V23" t="inlineStr"/>
-      <c r="W23" t="inlineStr"/>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="inlineStr"/>
-      <c r="AB23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>PELARIO, SOLIETO TRASMIL</t>
+        </is>
+      </c>
       <c r="AC23" t="inlineStr"/>
       <c r="AD23" t="inlineStr"/>
       <c r="AE23" t="inlineStr"/>
-      <c r="AF23" t="inlineStr"/>
+      <c r="AF23" t="inlineStr">
+        <is>
+          <t>DOROTEO,MA THERESA,DELA CRUZ,</t>
+        </is>
+      </c>
       <c r="AG23" t="inlineStr"/>
       <c r="AH23" t="inlineStr"/>
       <c r="AI23" t="inlineStr"/>
@@ -2013,42 +2737,94 @@
       <c r="AO23" t="inlineStr"/>
       <c r="AP23" t="inlineStr"/>
       <c r="AQ23" t="inlineStr"/>
-      <c r="AR23" t="inlineStr"/>
+      <c r="AR23" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr"/>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>108420220139</t>
+        </is>
+      </c>
       <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>RIVA,MARC NICHOLAI, NAVALTA</t>
+        </is>
+      </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>08-12-2017</t>
+        </is>
+      </c>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr"/>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="inlineStr"/>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr"/>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V24" t="inlineStr"/>
-      <c r="W24" t="inlineStr"/>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X24" t="inlineStr"/>
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="inlineStr"/>
-      <c r="AB24" t="inlineStr"/>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>RIVA, MARCO POLO LIZARDA</t>
+        </is>
+      </c>
       <c r="AC24" t="inlineStr"/>
       <c r="AD24" t="inlineStr"/>
       <c r="AE24" t="inlineStr"/>
-      <c r="AF24" t="inlineStr"/>
+      <c r="AF24" t="inlineStr">
+        <is>
+          <t>NAVALTA,JOY,GABION,</t>
+        </is>
+      </c>
       <c r="AG24" t="inlineStr"/>
       <c r="AH24" t="inlineStr"/>
       <c r="AI24" t="inlineStr"/>
@@ -2060,42 +2836,94 @@
       <c r="AO24" t="inlineStr"/>
       <c r="AP24" t="inlineStr"/>
       <c r="AQ24" t="inlineStr"/>
-      <c r="AR24" t="inlineStr"/>
+      <c r="AR24" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr"/>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>108420220189</t>
+        </is>
+      </c>
       <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>SANTOS,AKIYO, PASTIDIO</t>
+        </is>
+      </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>05-24-2014</t>
+        </is>
+      </c>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">9 </t>
+        </is>
+      </c>
       <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Filipino</t>
+        </is>
+      </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr"/>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
-      <c r="R25" t="inlineStr"/>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
-      <c r="U25" t="inlineStr"/>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V25" t="inlineStr"/>
-      <c r="W25" t="inlineStr"/>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X25" t="inlineStr"/>
       <c r="Y25" t="inlineStr"/>
       <c r="Z25" t="inlineStr"/>
       <c r="AA25" t="inlineStr"/>
-      <c r="AB25" t="inlineStr"/>
+      <c r="AB25" t="inlineStr">
+        <is>
+          <t>SANTOS, ALLAN SORALBO</t>
+        </is>
+      </c>
       <c r="AC25" t="inlineStr"/>
       <c r="AD25" t="inlineStr"/>
       <c r="AE25" t="inlineStr"/>
-      <c r="AF25" t="inlineStr"/>
+      <c r="AF25" t="inlineStr">
+        <is>
+          <t>PASTIDIO,MARNELLI,DELA CRUZ,</t>
+        </is>
+      </c>
       <c r="AG25" t="inlineStr"/>
       <c r="AH25" t="inlineStr"/>
       <c r="AI25" t="inlineStr"/>
@@ -2107,42 +2935,94 @@
       <c r="AO25" t="inlineStr"/>
       <c r="AP25" t="inlineStr"/>
       <c r="AQ25" t="inlineStr"/>
-      <c r="AR25" t="inlineStr"/>
+      <c r="AR25" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr"/>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>108420220063</t>
+        </is>
+      </c>
       <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>TUICO,MACKY AXEL, VIAJE</t>
+        </is>
+      </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>12-22-2014</t>
+        </is>
+      </c>
       <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">8 </t>
+        </is>
+      </c>
       <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr"/>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="inlineStr"/>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
-      <c r="U26" t="inlineStr"/>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V26" t="inlineStr"/>
-      <c r="W26" t="inlineStr"/>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="inlineStr"/>
       <c r="Z26" t="inlineStr"/>
       <c r="AA26" t="inlineStr"/>
-      <c r="AB26" t="inlineStr"/>
+      <c r="AB26" t="inlineStr">
+        <is>
+          <t>TUICO, RAYMARK RECTIN</t>
+        </is>
+      </c>
       <c r="AC26" t="inlineStr"/>
       <c r="AD26" t="inlineStr"/>
       <c r="AE26" t="inlineStr"/>
-      <c r="AF26" t="inlineStr"/>
+      <c r="AF26" t="inlineStr">
+        <is>
+          <t>VIAJE,MYRA,BONITA,</t>
+        </is>
+      </c>
       <c r="AG26" t="inlineStr"/>
       <c r="AH26" t="inlineStr"/>
       <c r="AI26" t="inlineStr"/>
@@ -2154,42 +3034,94 @@
       <c r="AO26" t="inlineStr"/>
       <c r="AP26" t="inlineStr"/>
       <c r="AQ26" t="inlineStr"/>
-      <c r="AR26" t="inlineStr"/>
+      <c r="AR26" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr"/>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>108420220065</t>
+        </is>
+      </c>
       <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ZAMORA,JAMES LEONARD, BEN</t>
+        </is>
+      </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>04-26-2016</t>
+        </is>
+      </c>
       <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
       <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr"/>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
-      <c r="R27" t="inlineStr"/>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr"/>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V27" t="inlineStr"/>
-      <c r="W27" t="inlineStr"/>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X27" t="inlineStr"/>
       <c r="Y27" t="inlineStr"/>
       <c r="Z27" t="inlineStr"/>
       <c r="AA27" t="inlineStr"/>
-      <c r="AB27" t="inlineStr"/>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>ZAMORA, FERNNADO PAMADOR</t>
+        </is>
+      </c>
       <c r="AC27" t="inlineStr"/>
       <c r="AD27" t="inlineStr"/>
       <c r="AE27" t="inlineStr"/>
-      <c r="AF27" t="inlineStr"/>
+      <c r="AF27" t="inlineStr">
+        <is>
+          <t>BEN,YVONNE,GUITONES,</t>
+        </is>
+      </c>
       <c r="AG27" t="inlineStr"/>
       <c r="AH27" t="inlineStr"/>
       <c r="AI27" t="inlineStr"/>
@@ -2201,12 +3133,16 @@
       <c r="AO27" t="inlineStr"/>
       <c r="AP27" t="inlineStr"/>
       <c r="AQ27" t="inlineStr"/>
-      <c r="AR27" t="inlineStr"/>
+      <c r="AR27" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
@@ -2266,7 +3202,7 @@
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ALMEIDA,HARLEY, ALVIAR</t>
+          <t>ALMEIDA,JAN ROSETTE, ALVIAR</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
@@ -2327,7 +3263,7 @@
       <c r="AA29" t="inlineStr"/>
       <c r="AB29" t="inlineStr">
         <is>
-          <t>ALMEIDA, LUCAS MATRE JR</t>
+          <t>ALMEIDA, ERNESTO MATRE JR</t>
         </is>
       </c>
       <c r="AC29" t="inlineStr"/>
@@ -2335,7 +3271,7 @@
       <c r="AE29" t="inlineStr"/>
       <c r="AF29" t="inlineStr">
         <is>
-          <t>ALVIAR,LESLY,BALESTEROS,</t>
+          <t>ALVIAR,JENNY ROSE,BERGANTIÑOS,</t>
         </is>
       </c>
       <c r="AG29" t="inlineStr"/>
@@ -2365,7 +3301,7 @@
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ALVIAR,ANGELHAN, LINSANGAN</t>
+          <t>ALVIAR,SOFHIA ALEXIS, LINSANGAN</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
@@ -2426,7 +3362,7 @@
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr">
         <is>
-          <t>ALVIAR, HUBERT TIONGKO</t>
+          <t>ALVIAR, MARK ANDREW TIONGKO</t>
         </is>
       </c>
       <c r="AC30" t="inlineStr"/>
@@ -2434,7 +3370,7 @@
       <c r="AE30" t="inlineStr"/>
       <c r="AF30" t="inlineStr">
         <is>
-          <t>LINSANGAN,GINA,OSAKA,</t>
+          <t>LINSANGAN,JENNALYN,CASTRO,</t>
         </is>
       </c>
       <c r="AG30" t="inlineStr"/>
@@ -2456,29 +3392,69 @@
       <c r="AS30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr"/>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>108420220067</t>
+        </is>
+      </c>
       <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr"/>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>AUSTRIA,CARA ISABELLA, -</t>
+        </is>
+      </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>05-19-2017</t>
+        </is>
+      </c>
       <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr"/>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="inlineStr"/>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr"/>
-      <c r="U31" t="inlineStr"/>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V31" t="inlineStr"/>
-      <c r="W31" t="inlineStr"/>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X31" t="inlineStr"/>
       <c r="Y31" t="inlineStr"/>
       <c r="Z31" t="inlineStr"/>
@@ -2487,7 +3463,11 @@
       <c r="AC31" t="inlineStr"/>
       <c r="AD31" t="inlineStr"/>
       <c r="AE31" t="inlineStr"/>
-      <c r="AF31" t="inlineStr"/>
+      <c r="AF31" t="inlineStr">
+        <is>
+          <t>AUSTRIA,KATE,ESCUDERO,</t>
+        </is>
+      </c>
       <c r="AG31" t="inlineStr"/>
       <c r="AH31" t="inlineStr"/>
       <c r="AI31" t="inlineStr"/>
@@ -2499,42 +3479,94 @@
       <c r="AO31" t="inlineStr"/>
       <c r="AP31" t="inlineStr"/>
       <c r="AQ31" t="inlineStr"/>
-      <c r="AR31" t="inlineStr"/>
+      <c r="AR31" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr"/>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>108222220023</t>
+        </is>
+      </c>
       <c r="B32" t="inlineStr"/>
-      <c r="C32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>BELICINA,MARIA ANGELICA, AGUSTIN</t>
+        </is>
+      </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>06-21-2016</t>
+        </is>
+      </c>
       <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
       <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr"/>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr"/>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr"/>
-      <c r="U32" t="inlineStr"/>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V32" t="inlineStr"/>
-      <c r="W32" t="inlineStr"/>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X32" t="inlineStr"/>
       <c r="Y32" t="inlineStr"/>
       <c r="Z32" t="inlineStr"/>
       <c r="AA32" t="inlineStr"/>
-      <c r="AB32" t="inlineStr"/>
+      <c r="AB32" t="inlineStr">
+        <is>
+          <t>BELICINA, JASON BAAY</t>
+        </is>
+      </c>
       <c r="AC32" t="inlineStr"/>
       <c r="AD32" t="inlineStr"/>
       <c r="AE32" t="inlineStr"/>
-      <c r="AF32" t="inlineStr"/>
+      <c r="AF32" t="inlineStr">
+        <is>
+          <t>AGUSTIN,MARY JANE,PILAPIL,</t>
+        </is>
+      </c>
       <c r="AG32" t="inlineStr"/>
       <c r="AH32" t="inlineStr"/>
       <c r="AI32" t="inlineStr"/>
@@ -2546,7 +3578,11 @@
       <c r="AO32" t="inlineStr"/>
       <c r="AP32" t="inlineStr"/>
       <c r="AQ32" t="inlineStr"/>
-      <c r="AR32" t="inlineStr"/>
+      <c r="AR32" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS32" t="inlineStr">
         <is>
           <t>T/I DATE:2023-08-29</t>
@@ -2554,38 +3590,86 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr"/>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>108420220083</t>
+        </is>
+      </c>
       <c r="B33" t="inlineStr"/>
-      <c r="C33" t="inlineStr"/>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>BUENAFLOR,ZAVINA CHARLAINE, ARGANDA</t>
+        </is>
+      </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>06-12-2017</t>
+        </is>
+      </c>
       <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr"/>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr"/>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr"/>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr"/>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V33" t="inlineStr"/>
-      <c r="W33" t="inlineStr"/>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X33" t="inlineStr"/>
       <c r="Y33" t="inlineStr"/>
       <c r="Z33" t="inlineStr"/>
       <c r="AA33" t="inlineStr"/>
-      <c r="AB33" t="inlineStr"/>
+      <c r="AB33" t="inlineStr">
+        <is>
+          <t>BUENAFLOR, CHARLES IRVIN ROMERO</t>
+        </is>
+      </c>
       <c r="AC33" t="inlineStr"/>
       <c r="AD33" t="inlineStr"/>
       <c r="AE33" t="inlineStr"/>
-      <c r="AF33" t="inlineStr"/>
+      <c r="AF33" t="inlineStr">
+        <is>
+          <t>ARGANDA,PRINCESS,CASTRO,</t>
+        </is>
+      </c>
       <c r="AG33" t="inlineStr"/>
       <c r="AH33" t="inlineStr"/>
       <c r="AI33" t="inlineStr"/>
@@ -2597,42 +3681,94 @@
       <c r="AO33" t="inlineStr"/>
       <c r="AP33" t="inlineStr"/>
       <c r="AQ33" t="inlineStr"/>
-      <c r="AR33" t="inlineStr"/>
+      <c r="AR33" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS33" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr"/>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>108420220035</t>
+        </is>
+      </c>
       <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr"/>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>CURAMPEZ,REYNA MAE, SABAULAN</t>
+        </is>
+      </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>09-24-2015</t>
+        </is>
+      </c>
       <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr"/>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">8 </t>
+        </is>
+      </c>
       <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr"/>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr"/>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="inlineStr"/>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr"/>
-      <c r="U34" t="inlineStr"/>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V34" t="inlineStr"/>
-      <c r="W34" t="inlineStr"/>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X34" t="inlineStr"/>
       <c r="Y34" t="inlineStr"/>
       <c r="Z34" t="inlineStr"/>
       <c r="AA34" t="inlineStr"/>
-      <c r="AB34" t="inlineStr"/>
+      <c r="AB34" t="inlineStr">
+        <is>
+          <t>CURAMPEZ, ELBERTO ESPINOSA</t>
+        </is>
+      </c>
       <c r="AC34" t="inlineStr"/>
       <c r="AD34" t="inlineStr"/>
       <c r="AE34" t="inlineStr"/>
-      <c r="AF34" t="inlineStr"/>
+      <c r="AF34" t="inlineStr">
+        <is>
+          <t>SABAULAN,ANGELA,GILBUENA,</t>
+        </is>
+      </c>
       <c r="AG34" t="inlineStr"/>
       <c r="AH34" t="inlineStr"/>
       <c r="AI34" t="inlineStr"/>
@@ -2644,42 +3780,94 @@
       <c r="AO34" t="inlineStr"/>
       <c r="AP34" t="inlineStr"/>
       <c r="AQ34" t="inlineStr"/>
-      <c r="AR34" t="inlineStr"/>
+      <c r="AR34" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS34" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr"/>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>108420220144</t>
+        </is>
+      </c>
       <c r="B35" t="inlineStr"/>
-      <c r="C35" t="inlineStr"/>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>DE LARA,MICHAELLA ZHAI, WATIWAT</t>
+        </is>
+      </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>02-04-2017</t>
+        </is>
+      </c>
       <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr"/>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr"/>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
-      <c r="R35" t="inlineStr"/>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr"/>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V35" t="inlineStr"/>
-      <c r="W35" t="inlineStr"/>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X35" t="inlineStr"/>
       <c r="Y35" t="inlineStr"/>
       <c r="Z35" t="inlineStr"/>
       <c r="AA35" t="inlineStr"/>
-      <c r="AB35" t="inlineStr"/>
+      <c r="AB35" t="inlineStr">
+        <is>
+          <t>DE LARA, JHASON FAILANO</t>
+        </is>
+      </c>
       <c r="AC35" t="inlineStr"/>
       <c r="AD35" t="inlineStr"/>
       <c r="AE35" t="inlineStr"/>
-      <c r="AF35" t="inlineStr"/>
+      <c r="AF35" t="inlineStr">
+        <is>
+          <t>WATIWAT,MERLYN,AREGLADO,</t>
+        </is>
+      </c>
       <c r="AG35" t="inlineStr"/>
       <c r="AH35" t="inlineStr"/>
       <c r="AI35" t="inlineStr"/>
@@ -2691,42 +3879,94 @@
       <c r="AO35" t="inlineStr"/>
       <c r="AP35" t="inlineStr"/>
       <c r="AQ35" t="inlineStr"/>
-      <c r="AR35" t="inlineStr"/>
+      <c r="AR35" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS35" t="inlineStr"/>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr"/>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>108420190150</t>
+        </is>
+      </c>
       <c r="B36" t="inlineStr"/>
-      <c r="C36" t="inlineStr"/>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>DUHINA,PRINCESS ANN, VILLENA</t>
+        </is>
+      </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>07-11-2014</t>
+        </is>
+      </c>
       <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">9 </t>
+        </is>
+      </c>
       <c r="K36" t="inlineStr"/>
-      <c r="L36" t="inlineStr"/>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr"/>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="inlineStr"/>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr"/>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V36" t="inlineStr"/>
-      <c r="W36" t="inlineStr"/>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X36" t="inlineStr"/>
       <c r="Y36" t="inlineStr"/>
       <c r="Z36" t="inlineStr"/>
       <c r="AA36" t="inlineStr"/>
-      <c r="AB36" t="inlineStr"/>
+      <c r="AB36" t="inlineStr">
+        <is>
+          <t>DUHINA, MARTH POLICARPIO</t>
+        </is>
+      </c>
       <c r="AC36" t="inlineStr"/>
       <c r="AD36" t="inlineStr"/>
       <c r="AE36" t="inlineStr"/>
-      <c r="AF36" t="inlineStr"/>
+      <c r="AF36" t="inlineStr">
+        <is>
+          <t>VILLENA,RENELYN,CABANIG,</t>
+        </is>
+      </c>
       <c r="AG36" t="inlineStr"/>
       <c r="AH36" t="inlineStr"/>
       <c r="AI36" t="inlineStr"/>
@@ -2738,42 +3978,94 @@
       <c r="AO36" t="inlineStr"/>
       <c r="AP36" t="inlineStr"/>
       <c r="AQ36" t="inlineStr"/>
-      <c r="AR36" t="inlineStr"/>
+      <c r="AR36" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS36" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr"/>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>108420220179</t>
+        </is>
+      </c>
       <c r="B37" t="inlineStr"/>
-      <c r="C37" t="inlineStr"/>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>FELIX,ADALINE MARIZZ, JAMISAL</t>
+        </is>
+      </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>04-18-2017</t>
+        </is>
+      </c>
       <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr"/>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr"/>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>Filipino</t>
+        </is>
+      </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr"/>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr"/>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S37" t="inlineStr"/>
       <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr"/>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V37" t="inlineStr"/>
-      <c r="W37" t="inlineStr"/>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X37" t="inlineStr"/>
       <c r="Y37" t="inlineStr"/>
       <c r="Z37" t="inlineStr"/>
       <c r="AA37" t="inlineStr"/>
-      <c r="AB37" t="inlineStr"/>
+      <c r="AB37" t="inlineStr">
+        <is>
+          <t>FELIX, MARVIN NAVAREZ</t>
+        </is>
+      </c>
       <c r="AC37" t="inlineStr"/>
       <c r="AD37" t="inlineStr"/>
       <c r="AE37" t="inlineStr"/>
-      <c r="AF37" t="inlineStr"/>
+      <c r="AF37" t="inlineStr">
+        <is>
+          <t>JAMISAL,CLARIZZA,GARCIA,</t>
+        </is>
+      </c>
       <c r="AG37" t="inlineStr"/>
       <c r="AH37" t="inlineStr"/>
       <c r="AI37" t="inlineStr"/>
@@ -2785,42 +4077,94 @@
       <c r="AO37" t="inlineStr"/>
       <c r="AP37" t="inlineStr"/>
       <c r="AQ37" t="inlineStr"/>
-      <c r="AR37" t="inlineStr"/>
+      <c r="AR37" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS37" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr"/>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>175015220005</t>
+        </is>
+      </c>
       <c r="B38" t="inlineStr"/>
-      <c r="C38" t="inlineStr"/>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>GARILAO,RHONGEN, LUMABAD</t>
+        </is>
+      </c>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>05-02-2016</t>
+        </is>
+      </c>
       <c r="I38" t="inlineStr"/>
-      <c r="J38" t="inlineStr"/>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
       <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Bikol</t>
+        </is>
+      </c>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
-      <c r="O38" t="inlineStr"/>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="inlineStr"/>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S38" t="inlineStr"/>
       <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr"/>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V38" t="inlineStr"/>
-      <c r="W38" t="inlineStr"/>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X38" t="inlineStr"/>
       <c r="Y38" t="inlineStr"/>
       <c r="Z38" t="inlineStr"/>
       <c r="AA38" t="inlineStr"/>
-      <c r="AB38" t="inlineStr"/>
+      <c r="AB38" t="inlineStr">
+        <is>
+          <t>GARILAO, RONALD DEGUIA</t>
+        </is>
+      </c>
       <c r="AC38" t="inlineStr"/>
       <c r="AD38" t="inlineStr"/>
       <c r="AE38" t="inlineStr"/>
-      <c r="AF38" t="inlineStr"/>
+      <c r="AF38" t="inlineStr">
+        <is>
+          <t>LUMABAD,JENNIFER,CARATERO,</t>
+        </is>
+      </c>
       <c r="AG38" t="inlineStr"/>
       <c r="AH38" t="inlineStr"/>
       <c r="AI38" t="inlineStr"/>
@@ -2832,33 +4176,77 @@
       <c r="AO38" t="inlineStr"/>
       <c r="AP38" t="inlineStr"/>
       <c r="AQ38" t="inlineStr"/>
-      <c r="AR38" t="inlineStr"/>
+      <c r="AR38" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS38" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr"/>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>108420220038</t>
+        </is>
+      </c>
       <c r="B39" t="inlineStr"/>
-      <c r="C39" t="inlineStr"/>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>LAPUT,ZHIA JUSMINE, -</t>
+        </is>
+      </c>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>07-06-2017</t>
+        </is>
+      </c>
       <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr"/>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K39" t="inlineStr"/>
-      <c r="L39" t="inlineStr"/>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
-      <c r="O39" t="inlineStr"/>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
-      <c r="R39" t="inlineStr"/>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S39" t="inlineStr"/>
       <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr"/>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V39" t="inlineStr"/>
-      <c r="W39" t="inlineStr"/>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X39" t="inlineStr"/>
       <c r="Y39" t="inlineStr"/>
       <c r="Z39" t="inlineStr"/>
@@ -2867,7 +4255,11 @@
       <c r="AC39" t="inlineStr"/>
       <c r="AD39" t="inlineStr"/>
       <c r="AE39" t="inlineStr"/>
-      <c r="AF39" t="inlineStr"/>
+      <c r="AF39" t="inlineStr">
+        <is>
+          <t>LAPUT,JEANILYN,LINGO,</t>
+        </is>
+      </c>
       <c r="AG39" t="inlineStr"/>
       <c r="AH39" t="inlineStr"/>
       <c r="AI39" t="inlineStr"/>
@@ -2879,42 +4271,94 @@
       <c r="AO39" t="inlineStr"/>
       <c r="AP39" t="inlineStr"/>
       <c r="AQ39" t="inlineStr"/>
-      <c r="AR39" t="inlineStr"/>
+      <c r="AR39" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS39" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr"/>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>408391220011</t>
+        </is>
+      </c>
       <c r="B40" t="inlineStr"/>
-      <c r="C40" t="inlineStr"/>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>MACHADO,ATHARA EUNIZE, AMION</t>
+        </is>
+      </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>05-31-2017</t>
+        </is>
+      </c>
       <c r="I40" t="inlineStr"/>
-      <c r="J40" t="inlineStr"/>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K40" t="inlineStr"/>
-      <c r="L40" t="inlineStr"/>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr"/>
-      <c r="O40" t="inlineStr"/>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
-      <c r="R40" t="inlineStr"/>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S40" t="inlineStr"/>
       <c r="T40" t="inlineStr"/>
-      <c r="U40" t="inlineStr"/>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V40" t="inlineStr"/>
-      <c r="W40" t="inlineStr"/>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X40" t="inlineStr"/>
       <c r="Y40" t="inlineStr"/>
       <c r="Z40" t="inlineStr"/>
       <c r="AA40" t="inlineStr"/>
-      <c r="AB40" t="inlineStr"/>
+      <c r="AB40" t="inlineStr">
+        <is>
+          <t>MACHADO, KEVIN EUGENE GONZALES</t>
+        </is>
+      </c>
       <c r="AC40" t="inlineStr"/>
       <c r="AD40" t="inlineStr"/>
       <c r="AE40" t="inlineStr"/>
-      <c r="AF40" t="inlineStr"/>
+      <c r="AF40" t="inlineStr">
+        <is>
+          <t>AMION,GLADYS,RAMOS,</t>
+        </is>
+      </c>
       <c r="AG40" t="inlineStr"/>
       <c r="AH40" t="inlineStr"/>
       <c r="AI40" t="inlineStr"/>
@@ -2926,7 +4370,11 @@
       <c r="AO40" t="inlineStr"/>
       <c r="AP40" t="inlineStr"/>
       <c r="AQ40" t="inlineStr"/>
-      <c r="AR40" t="inlineStr"/>
+      <c r="AR40" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS40" t="inlineStr">
         <is>
           <t>T/I DATE:2023-08-29</t>
@@ -2934,38 +4382,86 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr"/>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>108420220075</t>
+        </is>
+      </c>
       <c r="B41" t="inlineStr"/>
-      <c r="C41" t="inlineStr"/>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>MAYO,QUEEN ELLIE, MARTIN</t>
+        </is>
+      </c>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>10-15-2016</t>
+        </is>
+      </c>
       <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 </t>
+        </is>
+      </c>
       <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr"/>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr"/>
-      <c r="O41" t="inlineStr"/>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr"/>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S41" t="inlineStr"/>
       <c r="T41" t="inlineStr"/>
-      <c r="U41" t="inlineStr"/>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V41" t="inlineStr"/>
-      <c r="W41" t="inlineStr"/>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X41" t="inlineStr"/>
       <c r="Y41" t="inlineStr"/>
       <c r="Z41" t="inlineStr"/>
       <c r="AA41" t="inlineStr"/>
-      <c r="AB41" t="inlineStr"/>
+      <c r="AB41" t="inlineStr">
+        <is>
+          <t>MAYO, ALBIN SAPANG</t>
+        </is>
+      </c>
       <c r="AC41" t="inlineStr"/>
       <c r="AD41" t="inlineStr"/>
       <c r="AE41" t="inlineStr"/>
-      <c r="AF41" t="inlineStr"/>
+      <c r="AF41" t="inlineStr">
+        <is>
+          <t>MARTIN,QUENNIE,BALANI,</t>
+        </is>
+      </c>
       <c r="AG41" t="inlineStr"/>
       <c r="AH41" t="inlineStr"/>
       <c r="AI41" t="inlineStr"/>
@@ -2977,42 +4473,94 @@
       <c r="AO41" t="inlineStr"/>
       <c r="AP41" t="inlineStr"/>
       <c r="AQ41" t="inlineStr"/>
-      <c r="AR41" t="inlineStr"/>
+      <c r="AR41" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr"/>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>108420220122</t>
+        </is>
+      </c>
       <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr"/>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>MOJICA,LORAINE, CALPE</t>
+        </is>
+      </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>12-20-2016</t>
+        </is>
+      </c>
       <c r="I42" t="inlineStr"/>
-      <c r="J42" t="inlineStr"/>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr"/>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr"/>
-      <c r="O42" t="inlineStr"/>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
-      <c r="R42" t="inlineStr"/>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S42" t="inlineStr"/>
       <c r="T42" t="inlineStr"/>
-      <c r="U42" t="inlineStr"/>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V42" t="inlineStr"/>
-      <c r="W42" t="inlineStr"/>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X42" t="inlineStr"/>
       <c r="Y42" t="inlineStr"/>
       <c r="Z42" t="inlineStr"/>
       <c r="AA42" t="inlineStr"/>
-      <c r="AB42" t="inlineStr"/>
+      <c r="AB42" t="inlineStr">
+        <is>
+          <t>MOJICA, FEDELINO BANDAL</t>
+        </is>
+      </c>
       <c r="AC42" t="inlineStr"/>
       <c r="AD42" t="inlineStr"/>
       <c r="AE42" t="inlineStr"/>
-      <c r="AF42" t="inlineStr"/>
+      <c r="AF42" t="inlineStr">
+        <is>
+          <t>CALPE,GEMMA,MANALANG,</t>
+        </is>
+      </c>
       <c r="AG42" t="inlineStr"/>
       <c r="AH42" t="inlineStr"/>
       <c r="AI42" t="inlineStr"/>
@@ -3024,42 +4572,94 @@
       <c r="AO42" t="inlineStr"/>
       <c r="AP42" t="inlineStr"/>
       <c r="AQ42" t="inlineStr"/>
-      <c r="AR42" t="inlineStr"/>
+      <c r="AR42" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS42" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr"/>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>108420220153</t>
+        </is>
+      </c>
       <c r="B43" t="inlineStr"/>
-      <c r="C43" t="inlineStr"/>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>PAJADAN,AYESHA ANTONETH, ESCUDERO</t>
+        </is>
+      </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>07-16-2017</t>
+        </is>
+      </c>
       <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr"/>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr"/>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P43" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="inlineStr"/>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S43" t="inlineStr"/>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr"/>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V43" t="inlineStr"/>
-      <c r="W43" t="inlineStr"/>
+      <c r="W43" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X43" t="inlineStr"/>
       <c r="Y43" t="inlineStr"/>
       <c r="Z43" t="inlineStr"/>
       <c r="AA43" t="inlineStr"/>
-      <c r="AB43" t="inlineStr"/>
+      <c r="AB43" t="inlineStr">
+        <is>
+          <t>PAJADAN, ANTONIO ANGELEO MENDOZA</t>
+        </is>
+      </c>
       <c r="AC43" t="inlineStr"/>
       <c r="AD43" t="inlineStr"/>
       <c r="AE43" t="inlineStr"/>
-      <c r="AF43" t="inlineStr"/>
+      <c r="AF43" t="inlineStr">
+        <is>
+          <t>ESCUDERO,YVETTE,BUTED,</t>
+        </is>
+      </c>
       <c r="AG43" t="inlineStr"/>
       <c r="AH43" t="inlineStr"/>
       <c r="AI43" t="inlineStr"/>
@@ -3071,42 +4671,94 @@
       <c r="AO43" t="inlineStr"/>
       <c r="AP43" t="inlineStr"/>
       <c r="AQ43" t="inlineStr"/>
-      <c r="AR43" t="inlineStr"/>
+      <c r="AR43" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS43" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr"/>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>108420220078</t>
+        </is>
+      </c>
       <c r="B44" t="inlineStr"/>
-      <c r="C44" t="inlineStr"/>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>PASTIDIO,JAYLEY ELIZE, LORENZO</t>
+        </is>
+      </c>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>10-31-2015</t>
+        </is>
+      </c>
       <c r="I44" t="inlineStr"/>
-      <c r="J44" t="inlineStr"/>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">8 </t>
+        </is>
+      </c>
       <c r="K44" t="inlineStr"/>
-      <c r="L44" t="inlineStr"/>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M44" t="inlineStr"/>
       <c r="N44" t="inlineStr"/>
-      <c r="O44" t="inlineStr"/>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="inlineStr"/>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S44" t="inlineStr"/>
       <c r="T44" t="inlineStr"/>
-      <c r="U44" t="inlineStr"/>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V44" t="inlineStr"/>
-      <c r="W44" t="inlineStr"/>
+      <c r="W44" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X44" t="inlineStr"/>
       <c r="Y44" t="inlineStr"/>
       <c r="Z44" t="inlineStr"/>
       <c r="AA44" t="inlineStr"/>
-      <c r="AB44" t="inlineStr"/>
+      <c r="AB44" t="inlineStr">
+        <is>
+          <t>PASTIDIO, FERDINAND LACDAN</t>
+        </is>
+      </c>
       <c r="AC44" t="inlineStr"/>
       <c r="AD44" t="inlineStr"/>
       <c r="AE44" t="inlineStr"/>
-      <c r="AF44" t="inlineStr"/>
+      <c r="AF44" t="inlineStr">
+        <is>
+          <t>LORENZO,LIEZEL,GUERRERO,</t>
+        </is>
+      </c>
       <c r="AG44" t="inlineStr"/>
       <c r="AH44" t="inlineStr"/>
       <c r="AI44" t="inlineStr"/>
@@ -3118,42 +4770,94 @@
       <c r="AO44" t="inlineStr"/>
       <c r="AP44" t="inlineStr"/>
       <c r="AQ44" t="inlineStr"/>
-      <c r="AR44" t="inlineStr"/>
+      <c r="AR44" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS44" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr"/>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>108420220047</t>
+        </is>
+      </c>
       <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr"/>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>TUICO,MHACY ALEXA, VIAJE</t>
+        </is>
+      </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>12-13-2016</t>
+        </is>
+      </c>
       <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr"/>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K45" t="inlineStr"/>
-      <c r="L45" t="inlineStr"/>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr"/>
-      <c r="O45" t="inlineStr"/>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr"/>
-      <c r="R45" t="inlineStr"/>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S45" t="inlineStr"/>
       <c r="T45" t="inlineStr"/>
-      <c r="U45" t="inlineStr"/>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V45" t="inlineStr"/>
-      <c r="W45" t="inlineStr"/>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X45" t="inlineStr"/>
       <c r="Y45" t="inlineStr"/>
       <c r="Z45" t="inlineStr"/>
       <c r="AA45" t="inlineStr"/>
-      <c r="AB45" t="inlineStr"/>
+      <c r="AB45" t="inlineStr">
+        <is>
+          <t>TUICO, REYMARK RECTIN</t>
+        </is>
+      </c>
       <c r="AC45" t="inlineStr"/>
       <c r="AD45" t="inlineStr"/>
       <c r="AE45" t="inlineStr"/>
-      <c r="AF45" t="inlineStr"/>
+      <c r="AF45" t="inlineStr">
+        <is>
+          <t>VIAJE,MYRA,BONITA,</t>
+        </is>
+      </c>
       <c r="AG45" t="inlineStr"/>
       <c r="AH45" t="inlineStr"/>
       <c r="AI45" t="inlineStr"/>
@@ -3165,42 +4869,94 @@
       <c r="AO45" t="inlineStr"/>
       <c r="AP45" t="inlineStr"/>
       <c r="AQ45" t="inlineStr"/>
-      <c r="AR45" t="inlineStr"/>
+      <c r="AR45" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS45" t="inlineStr"/>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr"/>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>108432220166</t>
+        </is>
+      </c>
       <c r="B46" t="inlineStr"/>
-      <c r="C46" t="inlineStr"/>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>VILLANUEVA,YASSIE, RAMOS</t>
+        </is>
+      </c>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>04-25-2017</t>
+        </is>
+      </c>
       <c r="I46" t="inlineStr"/>
-      <c r="J46" t="inlineStr"/>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K46" t="inlineStr"/>
-      <c r="L46" t="inlineStr"/>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr"/>
-      <c r="O46" t="inlineStr"/>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="inlineStr"/>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S46" t="inlineStr"/>
       <c r="T46" t="inlineStr"/>
-      <c r="U46" t="inlineStr"/>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V46" t="inlineStr"/>
-      <c r="W46" t="inlineStr"/>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X46" t="inlineStr"/>
       <c r="Y46" t="inlineStr"/>
       <c r="Z46" t="inlineStr"/>
       <c r="AA46" t="inlineStr"/>
-      <c r="AB46" t="inlineStr"/>
+      <c r="AB46" t="inlineStr">
+        <is>
+          <t>VILLANUEVA, JESSIE VINLUAN</t>
+        </is>
+      </c>
       <c r="AC46" t="inlineStr"/>
       <c r="AD46" t="inlineStr"/>
       <c r="AE46" t="inlineStr"/>
-      <c r="AF46" t="inlineStr"/>
+      <c r="AF46" t="inlineStr">
+        <is>
+          <t>RAMOS,SARMAINE,CASTAÑARES,</t>
+        </is>
+      </c>
       <c r="AG46" t="inlineStr"/>
       <c r="AH46" t="inlineStr"/>
       <c r="AI46" t="inlineStr"/>
@@ -3212,42 +4968,94 @@
       <c r="AO46" t="inlineStr"/>
       <c r="AP46" t="inlineStr"/>
       <c r="AQ46" t="inlineStr"/>
-      <c r="AR46" t="inlineStr"/>
+      <c r="AR46" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS46" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr"/>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>108420220157</t>
+        </is>
+      </c>
       <c r="B47" t="inlineStr"/>
-      <c r="C47" t="inlineStr"/>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>VOSOTROS,MICIAEL JIA, ECHAVEZ</t>
+        </is>
+      </c>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr"/>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>09-26-2017</t>
+        </is>
+      </c>
       <c r="I47" t="inlineStr"/>
-      <c r="J47" t="inlineStr"/>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 </t>
+        </is>
+      </c>
       <c r="K47" t="inlineStr"/>
-      <c r="L47" t="inlineStr"/>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M47" t="inlineStr"/>
       <c r="N47" t="inlineStr"/>
-      <c r="O47" t="inlineStr"/>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="inlineStr"/>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>CUYAB</t>
+        </is>
+      </c>
       <c r="S47" t="inlineStr"/>
       <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr"/>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>SAN PEDRO</t>
+        </is>
+      </c>
       <c r="V47" t="inlineStr"/>
-      <c r="W47" t="inlineStr"/>
+      <c r="W47" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="X47" t="inlineStr"/>
       <c r="Y47" t="inlineStr"/>
       <c r="Z47" t="inlineStr"/>
       <c r="AA47" t="inlineStr"/>
-      <c r="AB47" t="inlineStr"/>
+      <c r="AB47" t="inlineStr">
+        <is>
+          <t>VOSOTROS, MICHAEL JOE VALENCIA</t>
+        </is>
+      </c>
       <c r="AC47" t="inlineStr"/>
       <c r="AD47" t="inlineStr"/>
       <c r="AE47" t="inlineStr"/>
-      <c r="AF47" t="inlineStr"/>
+      <c r="AF47" t="inlineStr">
+        <is>
+          <t>ECHAVEZ,JIANNE LYANA MARIE,PACO,</t>
+        </is>
+      </c>
       <c r="AG47" t="inlineStr"/>
       <c r="AH47" t="inlineStr"/>
       <c r="AI47" t="inlineStr"/>
@@ -3259,12 +5067,16 @@
       <c r="AO47" t="inlineStr"/>
       <c r="AP47" t="inlineStr"/>
       <c r="AQ47" t="inlineStr"/>
-      <c r="AR47" t="inlineStr"/>
+      <c r="AR47" t="inlineStr">
+        <is>
+          <t>Face to Face</t>
+        </is>
+      </c>
       <c r="AS47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr">
@@ -3317,7 +5129,7 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr">

</xml_diff>

<commit_message>
Error in sf10, generating classrecord, error in new classrecord
</commit_message>
<xml_diff>
--- a/Migrade_v.1.2/temp.xlsx
+++ b/Migrade_v.1.2/temp.xlsx
@@ -692,7 +692,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>876453</v>
+        <v>164512</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -716,7 +716,7 @@
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr">
         <is>
-          <t>Antipolo</t>
+          <t>Binan City</t>
         </is>
       </c>
       <c r="T3" t="inlineStr"/>
@@ -739,7 +739,7 @@
       <c r="AG3" t="inlineStr"/>
       <c r="AH3" t="inlineStr">
         <is>
-          <t>Antipolo</t>
+          <t>Binan</t>
         </is>
       </c>
       <c r="AI3" t="inlineStr"/>
@@ -761,7 +761,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Antipolo ES</t>
+          <t>Zapote ES</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -782,7 +782,7 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr">
         <is>
-          <t>2023 - 2024</t>
+          <t>2019 - 2020</t>
         </is>
       </c>
       <c r="T4" t="inlineStr"/>
@@ -799,7 +799,7 @@
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>Grade 4</t>
+          <t>Grade 6</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr"/>
@@ -813,7 +813,7 @@
       <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>ARCHIMEDES</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr"/>
@@ -1000,13 +1000,15 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>164512137890</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>164512130109</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>PADIOS, YAMEN, O</t>
+          <t>ALORA,RHOME JHAY, NAVAL</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -1019,7 +1021,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>09-23-2008</t>
+          <t>10-04-2008</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
@@ -1067,7 +1069,7 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>RIVALERA, JOHN, H</t>
+          <t>ALORA, JERRY BOMBASI</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr"/>
@@ -1075,7 +1077,7 @@
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>GEROMINO,JILL,BAJADI,</t>
+          <t>NAVAL,CAROL,MIRANDA,</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr"/>
@@ -1088,13 +1090,15 @@
       <c r="AN7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>164512134876</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>164512130164</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CASTO, CHRISTIAN, I</t>
+          <t>BELOLO,JERICK, ZOLETA</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -1107,13 +1111,13 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>05-20-2007</t>
+          <t>07-27-2008</t>
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K8" t="inlineStr"/>
@@ -1155,7 +1159,7 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>BALADIA, SIMSON, T</t>
+          <t>BELOLO, GERRY LACSA</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr"/>
@@ -1163,7 +1167,7 @@
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>QUISIDO,MARICEL,HERNANDEZ,</t>
+          <t>ZOLETA,SHIRLEY,NAVARRO,</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr"/>
@@ -1176,38 +1180,86 @@
       <c r="AN8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>108229120578</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CARREON,JAMES STEVEN, DIALOGO</t>
+        </is>
+      </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>02-10-2007</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">12 </t>
+        </is>
+      </c>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="inlineStr"/>
-      <c r="AB9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>CARREON, RUELITO FLORES</t>
+        </is>
+      </c>
       <c r="AC9" t="inlineStr"/>
       <c r="AD9" t="inlineStr"/>
       <c r="AE9" t="inlineStr"/>
-      <c r="AF9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>DIALOGO,ERLINDA,ESCUETA,</t>
+        </is>
+      </c>
       <c r="AG9" t="inlineStr"/>
       <c r="AH9" t="inlineStr"/>
       <c r="AI9" t="inlineStr"/>
@@ -1218,38 +1270,86 @@
       <c r="AN9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>164512130104</t>
+        </is>
+      </c>
       <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>DAGUIMOL,CLARK KENT, BORNIA</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>04-06-2007</t>
+        </is>
+      </c>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">12 </t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>DAGUIMOL, BENJIE SALVO</t>
+        </is>
+      </c>
       <c r="AC10" t="inlineStr"/>
       <c r="AD10" t="inlineStr"/>
       <c r="AE10" t="inlineStr"/>
-      <c r="AF10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>BORNIA,MELANIE,AMPO,</t>
+        </is>
+      </c>
       <c r="AG10" t="inlineStr"/>
       <c r="AH10" t="inlineStr"/>
       <c r="AI10" t="inlineStr"/>
@@ -1260,38 +1360,86 @@
       <c r="AN10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>106667130014</t>
+        </is>
+      </c>
       <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>DOMINGO,FRANZ RAYMOND, GARCIA</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>08-31-2007</t>
+        </is>
+      </c>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>SANTO TOMAS (CALABUSO)</t>
+        </is>
+      </c>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr"/>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="inlineStr"/>
-      <c r="AB11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>DOMINGO, FERDON DE LEON</t>
+        </is>
+      </c>
       <c r="AC11" t="inlineStr"/>
       <c r="AD11" t="inlineStr"/>
       <c r="AE11" t="inlineStr"/>
-      <c r="AF11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>GARCIA,RELIZA,RAFAEL,</t>
+        </is>
+      </c>
       <c r="AG11" t="inlineStr"/>
       <c r="AH11" t="inlineStr"/>
       <c r="AI11" t="inlineStr"/>
@@ -1302,38 +1450,86 @@
       <c r="AN11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>164512130133</t>
+        </is>
+      </c>
       <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>GABRIEL II,JASON, MERTALLA</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>03-18-2007</t>
+        </is>
+      </c>
       <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">12 </t>
+        </is>
+      </c>
       <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V12" t="inlineStr"/>
       <c r="W12" t="inlineStr"/>
-      <c r="X12" t="inlineStr"/>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="inlineStr"/>
-      <c r="AB12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>GABRIEL, JASON C</t>
+        </is>
+      </c>
       <c r="AC12" t="inlineStr"/>
       <c r="AD12" t="inlineStr"/>
       <c r="AE12" t="inlineStr"/>
-      <c r="AF12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>MERTALLA,NEKISIA,-,</t>
+        </is>
+      </c>
       <c r="AG12" t="inlineStr"/>
       <c r="AH12" t="inlineStr"/>
       <c r="AI12" t="inlineStr"/>
@@ -1344,38 +1540,86 @@
       <c r="AN12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>126231140195</t>
+        </is>
+      </c>
       <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>GORDIONES,PRINCE KIAN, ESCOTO</t>
+        </is>
+      </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>10-20-2007</t>
+        </is>
+      </c>
       <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Cebuano</t>
+        </is>
+      </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>SANTO TOMAS (CALABUSO)</t>
+        </is>
+      </c>
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V13" t="inlineStr"/>
       <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="inlineStr"/>
       <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>GORDIONES, NELSON MAGLANGIT</t>
+        </is>
+      </c>
       <c r="AC13" t="inlineStr"/>
       <c r="AD13" t="inlineStr"/>
       <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>ESCOTO,ROWENA,VASQUES,</t>
+        </is>
+      </c>
       <c r="AG13" t="inlineStr"/>
       <c r="AH13" t="inlineStr"/>
       <c r="AI13" t="inlineStr"/>
@@ -1386,38 +1630,86 @@
       <c r="AN13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr"/>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>107730130068</t>
+        </is>
+      </c>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>MANEJA,NOAH LEXSON, RADAZA</t>
+        </is>
+      </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>04-17-2008</t>
+        </is>
+      </c>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V14" t="inlineStr"/>
       <c r="W14" t="inlineStr"/>
-      <c r="X14" t="inlineStr"/>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y14" t="inlineStr"/>
       <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="inlineStr"/>
-      <c r="AB14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>MANEJA, NELSON CATAPANG</t>
+        </is>
+      </c>
       <c r="AC14" t="inlineStr"/>
       <c r="AD14" t="inlineStr"/>
       <c r="AE14" t="inlineStr"/>
-      <c r="AF14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>RADAZA,FLORENTINA,TAMPUS,</t>
+        </is>
+      </c>
       <c r="AG14" t="inlineStr"/>
       <c r="AH14" t="inlineStr"/>
       <c r="AI14" t="inlineStr"/>
@@ -1428,38 +1720,86 @@
       <c r="AN14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>424663150038</t>
+        </is>
+      </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>NAVAL,RONAN GABRIEL, ULLAY</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>03-29-2008</t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>SANTO TOMAS (CALABUSO)</t>
+        </is>
+      </c>
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V15" t="inlineStr"/>
       <c r="W15" t="inlineStr"/>
-      <c r="X15" t="inlineStr"/>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="inlineStr"/>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>NAVAL, ROMEO CAPUNITAN</t>
+        </is>
+      </c>
       <c r="AC15" t="inlineStr"/>
       <c r="AD15" t="inlineStr"/>
       <c r="AE15" t="inlineStr"/>
-      <c r="AF15" t="inlineStr"/>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>ULLAY,JANET,LOVINO,</t>
+        </is>
+      </c>
       <c r="AG15" t="inlineStr"/>
       <c r="AH15" t="inlineStr"/>
       <c r="AI15" t="inlineStr"/>
@@ -1467,45 +1807,89 @@
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr"/>
       <c r="AM15" t="inlineStr"/>
-      <c r="AN15" t="inlineStr">
-        <is>
-          <t>DRP "Family Problem"Date:2019/11/04</t>
-        </is>
-      </c>
+      <c r="AN15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr"/>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>164512130093</t>
+        </is>
+      </c>
       <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>OLITOQUIT,GABRIEL, DELA CRUZ</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>04-09-2008</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>SAN ANTONIO</t>
+        </is>
+      </c>
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V16" t="inlineStr"/>
       <c r="W16" t="inlineStr"/>
-      <c r="X16" t="inlineStr"/>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="inlineStr"/>
-      <c r="AB16" t="inlineStr"/>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>OLITOQUIT, JOEL ALBO</t>
+        </is>
+      </c>
       <c r="AC16" t="inlineStr"/>
       <c r="AD16" t="inlineStr"/>
       <c r="AE16" t="inlineStr"/>
-      <c r="AF16" t="inlineStr"/>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>DELA CRUZ,MARIBETH,MISSION,</t>
+        </is>
+      </c>
       <c r="AG16" t="inlineStr"/>
       <c r="AH16" t="inlineStr"/>
       <c r="AI16" t="inlineStr"/>
@@ -1513,45 +1897,89 @@
       <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="inlineStr"/>
-      <c r="AN16" t="inlineStr">
-        <is>
-          <t>T/I Pook Elem. Sch. Date:2019-06-03</t>
-        </is>
-      </c>
+      <c r="AN16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr"/>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>164512130113</t>
+        </is>
+      </c>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>PASUOT,JOSHUA, ALMEDA</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>11-16-2008</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V17" t="inlineStr"/>
       <c r="W17" t="inlineStr"/>
-      <c r="X17" t="inlineStr"/>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="inlineStr"/>
       <c r="AA17" t="inlineStr"/>
-      <c r="AB17" t="inlineStr"/>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>PASUOT, JOSEPH NAYNES</t>
+        </is>
+      </c>
       <c r="AC17" t="inlineStr"/>
       <c r="AD17" t="inlineStr"/>
       <c r="AE17" t="inlineStr"/>
-      <c r="AF17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>ALMEDA,SHERYL,BUENAFLOR,</t>
+        </is>
+      </c>
       <c r="AG17" t="inlineStr"/>
       <c r="AH17" t="inlineStr"/>
       <c r="AI17" t="inlineStr"/>
@@ -1562,38 +1990,86 @@
       <c r="AN17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>100964150029</t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>RAQUEDAN,KEITH, PATRIMONIO</t>
+        </is>
+      </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>04-09-2008</t>
+        </is>
+      </c>
       <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Iloko</t>
+        </is>
+      </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>SANTO TOMAS (CALABUSO)</t>
+        </is>
+      </c>
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
-      <c r="U18" t="inlineStr"/>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V18" t="inlineStr"/>
       <c r="W18" t="inlineStr"/>
-      <c r="X18" t="inlineStr"/>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="inlineStr"/>
       <c r="AA18" t="inlineStr"/>
-      <c r="AB18" t="inlineStr"/>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>RAQUEDAN, MARK ANTHONY DUHINO</t>
+        </is>
+      </c>
       <c r="AC18" t="inlineStr"/>
       <c r="AD18" t="inlineStr"/>
       <c r="AE18" t="inlineStr"/>
-      <c r="AF18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>FABRO,GERALDINE,CABURAL,</t>
+        </is>
+      </c>
       <c r="AG18" t="inlineStr"/>
       <c r="AH18" t="inlineStr"/>
       <c r="AI18" t="inlineStr"/>
@@ -1604,38 +2080,86 @@
       <c r="AN18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>136775120015</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>SANTOS,ANGELO, GALLARDO</t>
+        </is>
+      </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>05-15-2007</t>
+        </is>
+      </c>
       <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">12 </t>
+        </is>
+      </c>
       <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr"/>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V19" t="inlineStr"/>
       <c r="W19" t="inlineStr"/>
-      <c r="X19" t="inlineStr"/>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y19" t="inlineStr"/>
       <c r="Z19" t="inlineStr"/>
       <c r="AA19" t="inlineStr"/>
-      <c r="AB19" t="inlineStr"/>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>SANTOS, ARTURO CRUZ</t>
+        </is>
+      </c>
       <c r="AC19" t="inlineStr"/>
       <c r="AD19" t="inlineStr"/>
       <c r="AE19" t="inlineStr"/>
-      <c r="AF19" t="inlineStr"/>
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>UMALI,GALLARDO,GUADALUPE,</t>
+        </is>
+      </c>
       <c r="AG19" t="inlineStr"/>
       <c r="AH19" t="inlineStr"/>
       <c r="AI19" t="inlineStr"/>
@@ -1643,33 +2167,77 @@
       <c r="AK19" t="inlineStr"/>
       <c r="AL19" t="inlineStr"/>
       <c r="AM19" t="inlineStr"/>
-      <c r="AN19" t="inlineStr"/>
+      <c r="AN19" t="inlineStr">
+        <is>
+          <t>T/I DATE:2019-09-02</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr"/>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>164512140011</t>
+        </is>
+      </c>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>SUERO,JOHN ANDRE, TUMIMO</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>01-05-2008</t>
+        </is>
+      </c>
       <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>SANTO TOMAS (CALABUSO)</t>
+        </is>
+      </c>
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V20" t="inlineStr"/>
       <c r="W20" t="inlineStr"/>
-      <c r="X20" t="inlineStr"/>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr"/>
       <c r="AA20" t="inlineStr"/>
@@ -1677,7 +2245,11 @@
       <c r="AC20" t="inlineStr"/>
       <c r="AD20" t="inlineStr"/>
       <c r="AE20" t="inlineStr"/>
-      <c r="AF20" t="inlineStr"/>
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>SUERO,ROSALIE,TUMIMO,</t>
+        </is>
+      </c>
       <c r="AG20" t="inlineStr"/>
       <c r="AH20" t="inlineStr"/>
       <c r="AI20" t="inlineStr"/>
@@ -1688,38 +2260,86 @@
       <c r="AN20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>136884130194</t>
+        </is>
+      </c>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>VERGARA,BRANDON KYLE, DALAQUIT</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>08-06-2008</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr"/>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V21" t="inlineStr"/>
       <c r="W21" t="inlineStr"/>
-      <c r="X21" t="inlineStr"/>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr"/>
       <c r="AA21" t="inlineStr"/>
-      <c r="AB21" t="inlineStr"/>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>VERGARA, RONALD BABON</t>
+        </is>
+      </c>
       <c r="AC21" t="inlineStr"/>
       <c r="AD21" t="inlineStr"/>
       <c r="AE21" t="inlineStr"/>
-      <c r="AF21" t="inlineStr"/>
+      <c r="AF21" t="inlineStr">
+        <is>
+          <t>DALAQUIT,BRENDA,LIGUA,</t>
+        </is>
+      </c>
       <c r="AG21" t="inlineStr"/>
       <c r="AH21" t="inlineStr"/>
       <c r="AI21" t="inlineStr"/>
@@ -1730,38 +2350,86 @@
       <c r="AN21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>108213140455</t>
+        </is>
+      </c>
       <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>VERZOSA,SANTINO JUSTINE, VILLANUEVA</t>
+        </is>
+      </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>05-14-2007</t>
+        </is>
+      </c>
       <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">12 </t>
+        </is>
+      </c>
       <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>PLATERO</t>
+        </is>
+      </c>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr"/>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V22" t="inlineStr"/>
       <c r="W22" t="inlineStr"/>
-      <c r="X22" t="inlineStr"/>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y22" t="inlineStr"/>
       <c r="Z22" t="inlineStr"/>
       <c r="AA22" t="inlineStr"/>
-      <c r="AB22" t="inlineStr"/>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>VERZOSA, LUTGARDO PUNONGBAYAN JR</t>
+        </is>
+      </c>
       <c r="AC22" t="inlineStr"/>
       <c r="AD22" t="inlineStr"/>
       <c r="AE22" t="inlineStr"/>
-      <c r="AF22" t="inlineStr"/>
+      <c r="AF22" t="inlineStr">
+        <is>
+          <t>CASUBUAN,GLORIA,VILLANUEVA,</t>
+        </is>
+      </c>
       <c r="AG22" t="inlineStr"/>
       <c r="AH22" t="inlineStr"/>
       <c r="AI22" t="inlineStr"/>
@@ -1772,44 +2440,86 @@
       <c r="AN22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>2</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>164512130121</t>
+        </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
-          <t>&lt;=== TOTAL MALE</t>
+          <t>VILLANUEVA,DEAN MICHEAL, DE GUZMAN</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>03-11-2008</t>
+        </is>
+      </c>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr"/>
-      <c r="X23" t="inlineStr"/>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="inlineStr"/>
-      <c r="AB23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>VILLANUEVA, JIMMY BOY DELA CRUZ</t>
+        </is>
+      </c>
       <c r="AC23" t="inlineStr"/>
       <c r="AD23" t="inlineStr"/>
       <c r="AE23" t="inlineStr"/>
-      <c r="AF23" t="inlineStr"/>
+      <c r="AF23" t="inlineStr">
+        <is>
+          <t>DE GUZMAN,JOYCE ROANNE,BASULID,</t>
+        </is>
+      </c>
       <c r="AG23" t="inlineStr"/>
       <c r="AH23" t="inlineStr"/>
       <c r="AI23" t="inlineStr"/>
@@ -1821,83 +2531,43 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>164512140987</v>
+        <v>17</v>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
-          <t>MACALAO, JOANNA, V</t>
+          <t>&lt;=== TOTAL MALE</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>08-25-2008</t>
-        </is>
-      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t xml:space="preserve">10 </t>
-        </is>
-      </c>
+      <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>Tagalog</t>
-        </is>
-      </c>
+      <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>Christianity</t>
-        </is>
-      </c>
+      <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>ZAPOTE</t>
-        </is>
-      </c>
+      <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>CITY OF BIÑAN</t>
-        </is>
-      </c>
+      <c r="U24" t="inlineStr"/>
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr"/>
-      <c r="X24" t="inlineStr">
-        <is>
-          <t>LAGUNA</t>
-        </is>
-      </c>
+      <c r="X24" t="inlineStr"/>
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="inlineStr"/>
-      <c r="AB24" t="inlineStr">
-        <is>
-          <t>ARRESGADO, JUNARD MALAKARTE</t>
-        </is>
-      </c>
+      <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="inlineStr"/>
       <c r="AD24" t="inlineStr"/>
       <c r="AE24" t="inlineStr"/>
-      <c r="AF24" t="inlineStr">
-        <is>
-          <t>SEUGUERA,LIEZEL,IBARRA,</t>
-        </is>
-      </c>
+      <c r="AF24" t="inlineStr"/>
       <c r="AG24" t="inlineStr"/>
       <c r="AH24" t="inlineStr"/>
       <c r="AI24" t="inlineStr"/>
@@ -1908,13 +2578,15 @@
       <c r="AN24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>164512141321</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>251501140264</t>
+        </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
-          <t>TEMPROSSA, GIAN, L</t>
+          <t>BAEL,JAMAICA MAE, GLOBIO</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -1927,13 +2599,13 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>07-22-2008</t>
+          <t>02-21-2008</t>
         </is>
       </c>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">11 </t>
         </is>
       </c>
       <c r="K25" t="inlineStr"/>
@@ -1952,7 +2624,7 @@
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>ZAPOTE</t>
+          <t>SANTO TOMAS (CALABUSO)</t>
         </is>
       </c>
       <c r="R25" t="inlineStr"/>
@@ -1975,7 +2647,7 @@
       <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>BORCELANGO, DONATO REYES</t>
+          <t>BAEL, GERALD AFABLE</t>
         </is>
       </c>
       <c r="AC25" t="inlineStr"/>
@@ -1983,7 +2655,7 @@
       <c r="AE25" t="inlineStr"/>
       <c r="AF25" t="inlineStr">
         <is>
-          <t>TOLEDO,NORMA,ALIDO,</t>
+          <t>GLOBIO,RUBYLINDA,GALVAN,</t>
         </is>
       </c>
       <c r="AG25" t="inlineStr"/>
@@ -1996,13 +2668,15 @@
       <c r="AN25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>164512142543</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>126106130232</t>
+        </is>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ABUNDO, MARIE, J</t>
+          <t>BUCOY,SHILLAH MARGARET, JIMENEZ</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
@@ -2015,13 +2689,13 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>01-31-2008</t>
+          <t>07-11-2008</t>
         </is>
       </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">10 </t>
         </is>
       </c>
       <c r="K26" t="inlineStr"/>
@@ -2063,7 +2737,7 @@
       <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="inlineStr">
         <is>
-          <t>CAONES, JAYZON NUNAY</t>
+          <t>BUCOY, ERIC FRANCISCO</t>
         </is>
       </c>
       <c r="AC26" t="inlineStr"/>
@@ -2071,7 +2745,7 @@
       <c r="AE26" t="inlineStr"/>
       <c r="AF26" t="inlineStr">
         <is>
-          <t>PACIO,ALICIA,ZULUETA,</t>
+          <t>JIMENEZ,CHERRY,SANTOS,</t>
         </is>
       </c>
       <c r="AG26" t="inlineStr"/>
@@ -2084,38 +2758,86 @@
       <c r="AN26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr"/>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>108229130500</t>
+        </is>
+      </c>
       <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>DEMECILLO,ANGEL MAE, DALIS</t>
+        </is>
+      </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>09-21-2008</t>
+        </is>
+      </c>
       <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr"/>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P27" t="inlineStr"/>
-      <c r="Q27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>SANTO TOMAS (CALABUSO)</t>
+        </is>
+      </c>
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr"/>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V27" t="inlineStr"/>
       <c r="W27" t="inlineStr"/>
-      <c r="X27" t="inlineStr"/>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y27" t="inlineStr"/>
       <c r="Z27" t="inlineStr"/>
       <c r="AA27" t="inlineStr"/>
-      <c r="AB27" t="inlineStr"/>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>DEMECILLO, ROLANDO LOOD</t>
+        </is>
+      </c>
       <c r="AC27" t="inlineStr"/>
       <c r="AD27" t="inlineStr"/>
       <c r="AE27" t="inlineStr"/>
-      <c r="AF27" t="inlineStr"/>
+      <c r="AF27" t="inlineStr">
+        <is>
+          <t>DALIS,RESELYN,UGAPAY,</t>
+        </is>
+      </c>
       <c r="AG27" t="inlineStr"/>
       <c r="AH27" t="inlineStr"/>
       <c r="AI27" t="inlineStr"/>
@@ -2123,45 +2845,89 @@
       <c r="AK27" t="inlineStr"/>
       <c r="AL27" t="inlineStr"/>
       <c r="AM27" t="inlineStr"/>
-      <c r="AN27" t="inlineStr">
-        <is>
-          <t>T/I  San Miguel Elem.Sch.Date:2019-06-03</t>
-        </is>
-      </c>
+      <c r="AN27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>164512130191</t>
+        </is>
+      </c>
       <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>DIAGO,ASHLEY VENICE, LIMBAG</t>
+        </is>
+      </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>07-17-2008</t>
+        </is>
+      </c>
       <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
-      <c r="O28" t="inlineStr"/>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P28" t="inlineStr"/>
-      <c r="Q28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr"/>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V28" t="inlineStr"/>
       <c r="W28" t="inlineStr"/>
-      <c r="X28" t="inlineStr"/>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y28" t="inlineStr"/>
       <c r="Z28" t="inlineStr"/>
       <c r="AA28" t="inlineStr"/>
-      <c r="AB28" t="inlineStr"/>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>DIAGO, DOMINGO DOROJA JR</t>
+        </is>
+      </c>
       <c r="AC28" t="inlineStr"/>
       <c r="AD28" t="inlineStr"/>
       <c r="AE28" t="inlineStr"/>
-      <c r="AF28" t="inlineStr"/>
+      <c r="AF28" t="inlineStr">
+        <is>
+          <t>LIMBAG,MA MURIEL,ENRIQUEZ,</t>
+        </is>
+      </c>
       <c r="AG28" t="inlineStr"/>
       <c r="AH28" t="inlineStr"/>
       <c r="AI28" t="inlineStr"/>
@@ -2172,38 +2938,86 @@
       <c r="AN28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr"/>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>164512130095</t>
+        </is>
+      </c>
       <c r="B29" t="inlineStr"/>
-      <c r="C29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>DICDICAN,REGINE, JIMENEZ</t>
+        </is>
+      </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>06-25-2008</t>
+        </is>
+      </c>
       <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr"/>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P29" t="inlineStr"/>
-      <c r="Q29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr"/>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V29" t="inlineStr"/>
       <c r="W29" t="inlineStr"/>
-      <c r="X29" t="inlineStr"/>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y29" t="inlineStr"/>
       <c r="Z29" t="inlineStr"/>
       <c r="AA29" t="inlineStr"/>
-      <c r="AB29" t="inlineStr"/>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t>DICDICAN, NARCISO VILLANUEVA</t>
+        </is>
+      </c>
       <c r="AC29" t="inlineStr"/>
       <c r="AD29" t="inlineStr"/>
       <c r="AE29" t="inlineStr"/>
-      <c r="AF29" t="inlineStr"/>
+      <c r="AF29" t="inlineStr">
+        <is>
+          <t>JIMENEZ,AUREA,REYES,</t>
+        </is>
+      </c>
       <c r="AG29" t="inlineStr"/>
       <c r="AH29" t="inlineStr"/>
       <c r="AI29" t="inlineStr"/>
@@ -2214,38 +3028,86 @@
       <c r="AN29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr"/>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>164512100066</t>
+        </is>
+      </c>
       <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>HERMOSO,PAULA, CONDE</t>
+        </is>
+      </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>02-06-2005</t>
+        </is>
+      </c>
       <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">14 </t>
+        </is>
+      </c>
       <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
-      <c r="O30" t="inlineStr"/>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P30" t="inlineStr"/>
-      <c r="Q30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>SANTO TOMAS (CALABUSO)</t>
+        </is>
+      </c>
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr"/>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V30" t="inlineStr"/>
       <c r="W30" t="inlineStr"/>
-      <c r="X30" t="inlineStr"/>
+      <c r="X30" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y30" t="inlineStr"/>
       <c r="Z30" t="inlineStr"/>
       <c r="AA30" t="inlineStr"/>
-      <c r="AB30" t="inlineStr"/>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>HERMOSO, PIO CELON</t>
+        </is>
+      </c>
       <c r="AC30" t="inlineStr"/>
       <c r="AD30" t="inlineStr"/>
       <c r="AE30" t="inlineStr"/>
-      <c r="AF30" t="inlineStr"/>
+      <c r="AF30" t="inlineStr">
+        <is>
+          <t>CONDE,ROSEMARIE,DACUMOS,</t>
+        </is>
+      </c>
       <c r="AG30" t="inlineStr"/>
       <c r="AH30" t="inlineStr"/>
       <c r="AI30" t="inlineStr"/>
@@ -2256,30 +3118,70 @@
       <c r="AN30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr"/>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>108213130324</t>
+        </is>
+      </c>
       <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr"/>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>LANDRITO,PRINCESS, DAVID</t>
+        </is>
+      </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>01-09-2008</t>
+        </is>
+      </c>
       <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr"/>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P31" t="inlineStr"/>
-      <c r="Q31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr"/>
-      <c r="U31" t="inlineStr"/>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V31" t="inlineStr"/>
       <c r="W31" t="inlineStr"/>
-      <c r="X31" t="inlineStr"/>
+      <c r="X31" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y31" t="inlineStr"/>
       <c r="Z31" t="inlineStr"/>
       <c r="AA31" t="inlineStr"/>
@@ -2287,7 +3189,11 @@
       <c r="AC31" t="inlineStr"/>
       <c r="AD31" t="inlineStr"/>
       <c r="AE31" t="inlineStr"/>
-      <c r="AF31" t="inlineStr"/>
+      <c r="AF31" t="inlineStr">
+        <is>
+          <t>LANDRITO,LORENZ MILLECENT,DAVID,</t>
+        </is>
+      </c>
       <c r="AG31" t="inlineStr"/>
       <c r="AH31" t="inlineStr"/>
       <c r="AI31" t="inlineStr"/>
@@ -2298,38 +3204,86 @@
       <c r="AN31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr"/>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>117630130101</t>
+        </is>
+      </c>
       <c r="B32" t="inlineStr"/>
-      <c r="C32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>LARON,CARLEN, MITRA</t>
+        </is>
+      </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>09-16-2008</t>
+        </is>
+      </c>
       <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr"/>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P32" t="inlineStr"/>
-      <c r="Q32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>AYUNGON</t>
+        </is>
+      </c>
       <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr"/>
-      <c r="U32" t="inlineStr"/>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>LA CARLOTA CITY</t>
+        </is>
+      </c>
       <c r="V32" t="inlineStr"/>
       <c r="W32" t="inlineStr"/>
-      <c r="X32" t="inlineStr"/>
+      <c r="X32" t="inlineStr">
+        <is>
+          <t>NEGROS OCCIDENTAL</t>
+        </is>
+      </c>
       <c r="Y32" t="inlineStr"/>
       <c r="Z32" t="inlineStr"/>
       <c r="AA32" t="inlineStr"/>
-      <c r="AB32" t="inlineStr"/>
+      <c r="AB32" t="inlineStr">
+        <is>
+          <t>LARON, CARLOS VALLE</t>
+        </is>
+      </c>
       <c r="AC32" t="inlineStr"/>
       <c r="AD32" t="inlineStr"/>
       <c r="AE32" t="inlineStr"/>
-      <c r="AF32" t="inlineStr"/>
+      <c r="AF32" t="inlineStr">
+        <is>
+          <t>MITRA,ELENITA,ESTOLE,</t>
+        </is>
+      </c>
       <c r="AG32" t="inlineStr"/>
       <c r="AH32" t="inlineStr"/>
       <c r="AI32" t="inlineStr"/>
@@ -2337,41 +3291,93 @@
       <c r="AK32" t="inlineStr"/>
       <c r="AL32" t="inlineStr"/>
       <c r="AM32" t="inlineStr"/>
-      <c r="AN32" t="inlineStr"/>
+      <c r="AN32" t="inlineStr">
+        <is>
+          <t>T/I DATE:2019-06-03</t>
+        </is>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr"/>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>164512130192</t>
+        </is>
+      </c>
       <c r="B33" t="inlineStr"/>
-      <c r="C33" t="inlineStr"/>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>NADURATA,HONEYREY, DE LEON</t>
+        </is>
+      </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>11-15-2007</t>
+        </is>
+      </c>
       <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr"/>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr"/>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P33" t="inlineStr"/>
-      <c r="Q33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr"/>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V33" t="inlineStr"/>
       <c r="W33" t="inlineStr"/>
-      <c r="X33" t="inlineStr"/>
+      <c r="X33" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y33" t="inlineStr"/>
       <c r="Z33" t="inlineStr"/>
       <c r="AA33" t="inlineStr"/>
-      <c r="AB33" t="inlineStr"/>
+      <c r="AB33" t="inlineStr">
+        <is>
+          <t>NADURATA, ROY ALFRED PAREDES</t>
+        </is>
+      </c>
       <c r="AC33" t="inlineStr"/>
       <c r="AD33" t="inlineStr"/>
       <c r="AE33" t="inlineStr"/>
-      <c r="AF33" t="inlineStr"/>
+      <c r="AF33" t="inlineStr">
+        <is>
+          <t>DE LEON,JENNIFFER,VALBUENA,</t>
+        </is>
+      </c>
       <c r="AG33" t="inlineStr"/>
       <c r="AH33" t="inlineStr"/>
       <c r="AI33" t="inlineStr"/>
@@ -2382,38 +3388,86 @@
       <c r="AN33" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr"/>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>164512130097</t>
+        </is>
+      </c>
       <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr"/>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>NAVAL,JASMINE, LIMBAG</t>
+        </is>
+      </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>11-21-2007</t>
+        </is>
+      </c>
       <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr"/>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr"/>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr"/>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P34" t="inlineStr"/>
-      <c r="Q34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr"/>
-      <c r="U34" t="inlineStr"/>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V34" t="inlineStr"/>
       <c r="W34" t="inlineStr"/>
-      <c r="X34" t="inlineStr"/>
+      <c r="X34" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y34" t="inlineStr"/>
       <c r="Z34" t="inlineStr"/>
       <c r="AA34" t="inlineStr"/>
-      <c r="AB34" t="inlineStr"/>
+      <c r="AB34" t="inlineStr">
+        <is>
+          <t>NAVAL, SHERWIN ALORA</t>
+        </is>
+      </c>
       <c r="AC34" t="inlineStr"/>
       <c r="AD34" t="inlineStr"/>
       <c r="AE34" t="inlineStr"/>
-      <c r="AF34" t="inlineStr"/>
+      <c r="AF34" t="inlineStr">
+        <is>
+          <t>LIMBAG,ANGELITA,YUMUL,</t>
+        </is>
+      </c>
       <c r="AG34" t="inlineStr"/>
       <c r="AH34" t="inlineStr"/>
       <c r="AI34" t="inlineStr"/>
@@ -2424,38 +3478,86 @@
       <c r="AN34" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr"/>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>164512130081</t>
+        </is>
+      </c>
       <c r="B35" t="inlineStr"/>
-      <c r="C35" t="inlineStr"/>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>NAVAL,YSABEEL PEARL, RIVERA</t>
+        </is>
+      </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>05-09-2007</t>
+        </is>
+      </c>
       <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">12 </t>
+        </is>
+      </c>
       <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr"/>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr"/>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P35" t="inlineStr"/>
-      <c r="Q35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>SANTO NINO</t>
+        </is>
+      </c>
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr"/>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V35" t="inlineStr"/>
       <c r="W35" t="inlineStr"/>
-      <c r="X35" t="inlineStr"/>
+      <c r="X35" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y35" t="inlineStr"/>
       <c r="Z35" t="inlineStr"/>
       <c r="AA35" t="inlineStr"/>
-      <c r="AB35" t="inlineStr"/>
+      <c r="AB35" t="inlineStr">
+        <is>
+          <t>NAVAL, ISIDRO LINGGO</t>
+        </is>
+      </c>
       <c r="AC35" t="inlineStr"/>
       <c r="AD35" t="inlineStr"/>
       <c r="AE35" t="inlineStr"/>
-      <c r="AF35" t="inlineStr"/>
+      <c r="AF35" t="inlineStr">
+        <is>
+          <t>RIVERA,PERLITA,PARIÑAS,</t>
+        </is>
+      </c>
       <c r="AG35" t="inlineStr"/>
       <c r="AH35" t="inlineStr"/>
       <c r="AI35" t="inlineStr"/>
@@ -2466,38 +3568,86 @@
       <c r="AN35" t="inlineStr"/>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr"/>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>164512140041</t>
+        </is>
+      </c>
       <c r="B36" t="inlineStr"/>
-      <c r="C36" t="inlineStr"/>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ROMERO,GERMAINNE ALYANNA, MARINDUQUE</t>
+        </is>
+      </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>09-04-2008</t>
+        </is>
+      </c>
       <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K36" t="inlineStr"/>
-      <c r="L36" t="inlineStr"/>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr"/>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P36" t="inlineStr"/>
-      <c r="Q36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr"/>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V36" t="inlineStr"/>
       <c r="W36" t="inlineStr"/>
-      <c r="X36" t="inlineStr"/>
+      <c r="X36" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y36" t="inlineStr"/>
       <c r="Z36" t="inlineStr"/>
       <c r="AA36" t="inlineStr"/>
-      <c r="AB36" t="inlineStr"/>
+      <c r="AB36" t="inlineStr">
+        <is>
+          <t>ROMERO JR, ANTONIO SAGALES</t>
+        </is>
+      </c>
       <c r="AC36" t="inlineStr"/>
       <c r="AD36" t="inlineStr"/>
       <c r="AE36" t="inlineStr"/>
-      <c r="AF36" t="inlineStr"/>
+      <c r="AF36" t="inlineStr">
+        <is>
+          <t>MARINDUQUE,GILDA,PAGBUNUCAN,</t>
+        </is>
+      </c>
       <c r="AG36" t="inlineStr"/>
       <c r="AH36" t="inlineStr"/>
       <c r="AI36" t="inlineStr"/>
@@ -2508,38 +3658,86 @@
       <c r="AN36" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr"/>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>164512140042</t>
+        </is>
+      </c>
       <c r="B37" t="inlineStr"/>
-      <c r="C37" t="inlineStr"/>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>ROMERO,GILLIANNE ANDREA, MARINDUQUE</t>
+        </is>
+      </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>09-04-2008</t>
+        </is>
+      </c>
       <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr"/>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr"/>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr"/>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P37" t="inlineStr"/>
-      <c r="Q37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>SANTO TOMAS (CALABUSO)</t>
+        </is>
+      </c>
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr"/>
       <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr"/>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V37" t="inlineStr"/>
       <c r="W37" t="inlineStr"/>
-      <c r="X37" t="inlineStr"/>
+      <c r="X37" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y37" t="inlineStr"/>
       <c r="Z37" t="inlineStr"/>
       <c r="AA37" t="inlineStr"/>
-      <c r="AB37" t="inlineStr"/>
+      <c r="AB37" t="inlineStr">
+        <is>
+          <t>ROMERO JR, ANTONIO SAGALES</t>
+        </is>
+      </c>
       <c r="AC37" t="inlineStr"/>
       <c r="AD37" t="inlineStr"/>
       <c r="AE37" t="inlineStr"/>
-      <c r="AF37" t="inlineStr"/>
+      <c r="AF37" t="inlineStr">
+        <is>
+          <t>MARINDUQUE,GILDA,PAGBUNUCAN,</t>
+        </is>
+      </c>
       <c r="AG37" t="inlineStr"/>
       <c r="AH37" t="inlineStr"/>
       <c r="AI37" t="inlineStr"/>
@@ -2550,38 +3748,86 @@
       <c r="AN37" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr"/>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>164512130103</t>
+        </is>
+      </c>
       <c r="B38" t="inlineStr"/>
-      <c r="C38" t="inlineStr"/>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>SIGUE,FLORENZ MAE, CAHULOGAN</t>
+        </is>
+      </c>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>05-24-2008</t>
+        </is>
+      </c>
       <c r="I38" t="inlineStr"/>
-      <c r="J38" t="inlineStr"/>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
-      <c r="O38" t="inlineStr"/>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P38" t="inlineStr"/>
-      <c r="Q38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr"/>
       <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr"/>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V38" t="inlineStr"/>
       <c r="W38" t="inlineStr"/>
-      <c r="X38" t="inlineStr"/>
+      <c r="X38" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y38" t="inlineStr"/>
       <c r="Z38" t="inlineStr"/>
       <c r="AA38" t="inlineStr"/>
-      <c r="AB38" t="inlineStr"/>
+      <c r="AB38" t="inlineStr">
+        <is>
+          <t>SIGUE, FLORENCIO JR LINGATONG</t>
+        </is>
+      </c>
       <c r="AC38" t="inlineStr"/>
       <c r="AD38" t="inlineStr"/>
       <c r="AE38" t="inlineStr"/>
-      <c r="AF38" t="inlineStr"/>
+      <c r="AF38" t="inlineStr">
+        <is>
+          <t>CAHULOGAN,JOJIE,DUMANGAS,</t>
+        </is>
+      </c>
       <c r="AG38" t="inlineStr"/>
       <c r="AH38" t="inlineStr"/>
       <c r="AI38" t="inlineStr"/>
@@ -2592,38 +3838,86 @@
       <c r="AN38" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr"/>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>164512130088</t>
+        </is>
+      </c>
       <c r="B39" t="inlineStr"/>
-      <c r="C39" t="inlineStr"/>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>SUYU,FRANCINE SHANIA, LUCENIO</t>
+        </is>
+      </c>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>04-20-2008</t>
+        </is>
+      </c>
       <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr"/>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K39" t="inlineStr"/>
-      <c r="L39" t="inlineStr"/>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
-      <c r="O39" t="inlineStr"/>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P39" t="inlineStr"/>
-      <c r="Q39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr"/>
       <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr"/>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V39" t="inlineStr"/>
       <c r="W39" t="inlineStr"/>
-      <c r="X39" t="inlineStr"/>
+      <c r="X39" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y39" t="inlineStr"/>
       <c r="Z39" t="inlineStr"/>
       <c r="AA39" t="inlineStr"/>
-      <c r="AB39" t="inlineStr"/>
+      <c r="AB39" t="inlineStr">
+        <is>
+          <t>SUYU, ROBERTO JR BULAQUI</t>
+        </is>
+      </c>
       <c r="AC39" t="inlineStr"/>
       <c r="AD39" t="inlineStr"/>
       <c r="AE39" t="inlineStr"/>
-      <c r="AF39" t="inlineStr"/>
+      <c r="AF39" t="inlineStr">
+        <is>
+          <t>LUCENIO,MYLENE,SONBESE,</t>
+        </is>
+      </c>
       <c r="AG39" t="inlineStr"/>
       <c r="AH39" t="inlineStr"/>
       <c r="AI39" t="inlineStr"/>
@@ -2634,38 +3928,86 @@
       <c r="AN39" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr"/>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>108213130478</t>
+        </is>
+      </c>
       <c r="B40" t="inlineStr"/>
-      <c r="C40" t="inlineStr"/>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>VERGARA,ALTHEA JOY, WINDAM</t>
+        </is>
+      </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>05-06-2008</t>
+        </is>
+      </c>
       <c r="I40" t="inlineStr"/>
-      <c r="J40" t="inlineStr"/>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K40" t="inlineStr"/>
-      <c r="L40" t="inlineStr"/>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr"/>
-      <c r="O40" t="inlineStr"/>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P40" t="inlineStr"/>
-      <c r="Q40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>SANTO TOMAS (CALABUSO)</t>
+        </is>
+      </c>
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr"/>
       <c r="T40" t="inlineStr"/>
-      <c r="U40" t="inlineStr"/>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V40" t="inlineStr"/>
       <c r="W40" t="inlineStr"/>
-      <c r="X40" t="inlineStr"/>
+      <c r="X40" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y40" t="inlineStr"/>
       <c r="Z40" t="inlineStr"/>
       <c r="AA40" t="inlineStr"/>
-      <c r="AB40" t="inlineStr"/>
+      <c r="AB40" t="inlineStr">
+        <is>
+          <t>VERGARA, TONY DALMINO</t>
+        </is>
+      </c>
       <c r="AC40" t="inlineStr"/>
       <c r="AD40" t="inlineStr"/>
       <c r="AE40" t="inlineStr"/>
-      <c r="AF40" t="inlineStr"/>
+      <c r="AF40" t="inlineStr">
+        <is>
+          <t>WINDAM,ELVIRA,DAGMIL,</t>
+        </is>
+      </c>
       <c r="AG40" t="inlineStr"/>
       <c r="AH40" t="inlineStr"/>
       <c r="AI40" t="inlineStr"/>
@@ -2673,45 +4015,89 @@
       <c r="AK40" t="inlineStr"/>
       <c r="AL40" t="inlineStr"/>
       <c r="AM40" t="inlineStr"/>
-      <c r="AN40" t="inlineStr">
-        <is>
-          <t>T/I Southville IV Elem. Sch.Date:2019-09-02</t>
-        </is>
-      </c>
+      <c r="AN40" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr"/>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>136886140081</t>
+        </is>
+      </c>
       <c r="B41" t="inlineStr"/>
-      <c r="C41" t="inlineStr"/>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>VERGARA,EULYN KEITH, DAIZ</t>
+        </is>
+      </c>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>01-27-2008</t>
+        </is>
+      </c>
       <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11 </t>
+        </is>
+      </c>
       <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr"/>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr"/>
-      <c r="O41" t="inlineStr"/>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P41" t="inlineStr"/>
-      <c r="Q41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>SANTO TOMAS (CALABUSO)</t>
+        </is>
+      </c>
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr"/>
       <c r="T41" t="inlineStr"/>
-      <c r="U41" t="inlineStr"/>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V41" t="inlineStr"/>
       <c r="W41" t="inlineStr"/>
-      <c r="X41" t="inlineStr"/>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y41" t="inlineStr"/>
       <c r="Z41" t="inlineStr"/>
       <c r="AA41" t="inlineStr"/>
-      <c r="AB41" t="inlineStr"/>
+      <c r="AB41" t="inlineStr">
+        <is>
+          <t>VERGARA, EUGENE JAMITO</t>
+        </is>
+      </c>
       <c r="AC41" t="inlineStr"/>
       <c r="AD41" t="inlineStr"/>
       <c r="AE41" t="inlineStr"/>
-      <c r="AF41" t="inlineStr"/>
+      <c r="AF41" t="inlineStr">
+        <is>
+          <t>DAIZ,ANGIELYN,GARCIA,</t>
+        </is>
+      </c>
       <c r="AG41" t="inlineStr"/>
       <c r="AH41" t="inlineStr"/>
       <c r="AI41" t="inlineStr"/>
@@ -2722,38 +4108,86 @@
       <c r="AN41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr"/>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>108462140024</t>
+        </is>
+      </c>
       <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr"/>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>VILLALOBOS,HOLLY MARIE, MARZAN</t>
+        </is>
+      </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>06-30-2008</t>
+        </is>
+      </c>
       <c r="I42" t="inlineStr"/>
-      <c r="J42" t="inlineStr"/>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr"/>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr"/>
-      <c r="O42" t="inlineStr"/>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P42" t="inlineStr"/>
-      <c r="Q42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr"/>
       <c r="T42" t="inlineStr"/>
-      <c r="U42" t="inlineStr"/>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V42" t="inlineStr"/>
       <c r="W42" t="inlineStr"/>
-      <c r="X42" t="inlineStr"/>
+      <c r="X42" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y42" t="inlineStr"/>
       <c r="Z42" t="inlineStr"/>
       <c r="AA42" t="inlineStr"/>
-      <c r="AB42" t="inlineStr"/>
+      <c r="AB42" t="inlineStr">
+        <is>
+          <t>VILLALOBOS, DONDON LLANES</t>
+        </is>
+      </c>
       <c r="AC42" t="inlineStr"/>
       <c r="AD42" t="inlineStr"/>
       <c r="AE42" t="inlineStr"/>
-      <c r="AF42" t="inlineStr"/>
+      <c r="AF42" t="inlineStr">
+        <is>
+          <t>MARZAN,MAE ABEGAEL,SALCEDO,</t>
+        </is>
+      </c>
       <c r="AG42" t="inlineStr"/>
       <c r="AH42" t="inlineStr"/>
       <c r="AI42" t="inlineStr"/>
@@ -2764,38 +4198,86 @@
       <c r="AN42" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr"/>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>164512130117</t>
+        </is>
+      </c>
       <c r="B43" t="inlineStr"/>
-      <c r="C43" t="inlineStr"/>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>YUGOM,YUHHIE, DELA CRUZ</t>
+        </is>
+      </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>10-18-2008</t>
+        </is>
+      </c>
       <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr"/>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 </t>
+        </is>
+      </c>
       <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Tagalog</t>
+        </is>
+      </c>
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr"/>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
       <c r="P43" t="inlineStr"/>
-      <c r="Q43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>ZAPOTE</t>
+        </is>
+      </c>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr"/>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr"/>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>CITY OF BIÑAN</t>
+        </is>
+      </c>
       <c r="V43" t="inlineStr"/>
       <c r="W43" t="inlineStr"/>
-      <c r="X43" t="inlineStr"/>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>LAGUNA</t>
+        </is>
+      </c>
       <c r="Y43" t="inlineStr"/>
       <c r="Z43" t="inlineStr"/>
       <c r="AA43" t="inlineStr"/>
-      <c r="AB43" t="inlineStr"/>
+      <c r="AB43" t="inlineStr">
+        <is>
+          <t>YUGOM, ALFREDO BAGOMBON</t>
+        </is>
+      </c>
       <c r="AC43" t="inlineStr"/>
       <c r="AD43" t="inlineStr"/>
       <c r="AE43" t="inlineStr"/>
-      <c r="AF43" t="inlineStr"/>
+      <c r="AF43" t="inlineStr">
+        <is>
+          <t>DELA CRUZ,MILENE,CAPINING,</t>
+        </is>
+      </c>
       <c r="AG43" t="inlineStr"/>
       <c r="AH43" t="inlineStr"/>
       <c r="AI43" t="inlineStr"/>
@@ -2807,7 +4289,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
@@ -2855,7 +4337,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr">
@@ -3107,15 +4589,13 @@
       <c r="Y48" t="n">
         <v>16</v>
       </c>
-      <c r="Z48" t="n">
-        <v>15</v>
-      </c>
+      <c r="Z48" t="inlineStr"/>
       <c r="AA48" t="inlineStr"/>
       <c r="AB48" t="inlineStr"/>
       <c r="AC48" t="inlineStr"/>
       <c r="AD48" t="inlineStr">
         <is>
-          <t>LAMBERTO BOLIMA RIVAREZ</t>
+          <t>ISSA GARCIA ELIVERA</t>
         </is>
       </c>
       <c r="AE48" t="inlineStr"/>
@@ -3253,9 +4733,7 @@
       <c r="Y51" t="n">
         <v>19</v>
       </c>
-      <c r="Z51" t="n">
-        <v>20</v>
-      </c>
+      <c r="Z51" t="inlineStr"/>
       <c r="AA51" t="inlineStr"/>
       <c r="AB51" t="inlineStr"/>
       <c r="AC51" t="inlineStr"/>
@@ -3313,14 +4791,14 @@
       <c r="AI52" t="inlineStr"/>
       <c r="AJ52" t="inlineStr">
         <is>
-          <t>BoSY Date:                06-03-2019</t>
+          <t>BoSY Date:</t>
         </is>
       </c>
       <c r="AK52" t="inlineStr"/>
       <c r="AL52" t="inlineStr"/>
       <c r="AM52" t="inlineStr">
         <is>
-          <t>EoSY Date:                    04-03-2020</t>
+          <t>EoSY Date:</t>
         </is>
       </c>
       <c r="AN52" t="inlineStr"/>
@@ -3357,22 +4835,20 @@
       <c r="Y53" t="n">
         <v>35</v>
       </c>
-      <c r="Z53" t="n">
-        <v>35</v>
-      </c>
+      <c r="Z53" t="inlineStr"/>
       <c r="AA53" t="inlineStr"/>
       <c r="AB53" t="inlineStr"/>
       <c r="AC53" t="inlineStr"/>
       <c r="AD53" t="inlineStr">
         <is>
-          <t>BoSY Date:                06-03-2019</t>
+          <t>BoSY Date:</t>
         </is>
       </c>
       <c r="AE53" t="inlineStr"/>
       <c r="AF53" t="inlineStr"/>
       <c r="AG53" t="inlineStr">
         <is>
-          <t>EoSY Date:                  04-03-2020</t>
+          <t>EoSY Date:</t>
         </is>
       </c>
       <c r="AH53" t="inlineStr"/>
@@ -3516,7 +4992,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Generated on: Saturday, March 21, 2020</t>
+          <t>Generated on: Monday, March 16, 2020</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>

</xml_diff>

<commit_message>
Page title. Add no data in generation, MAPEH
</commit_message>
<xml_diff>
--- a/Migrade_v.1.2/temp.xlsx
+++ b/Migrade_v.1.2/temp.xlsx
@@ -782,7 +782,7 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr">
         <is>
-          <t>2019 - 2020</t>
+          <t>2023 - 2024</t>
         </is>
       </c>
       <c r="T4" t="inlineStr"/>
@@ -813,7 +813,7 @@
       <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>ARCHIMEDES</t>
+          <t>RED</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr"/>

</xml_diff>